<commit_message>
Ajout commentaires Ineris + tableau de synthèse complété
</commit_message>
<xml_diff>
--- a/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
+++ b/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gcebelieu\Desktop\2024-07-09 - Pleniere GT Risques\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED0122F-629D-4D15-85DF-539EDAEC1912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD48AF64-D870-4098-9B05-51681B809D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28620" yWindow="90" windowWidth="27960" windowHeight="15015" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="540">
   <si>
     <t>Organisme</t>
   </si>
@@ -1291,10 +1291,6 @@
     <t>C'est le cas. Il n'y a pas de règles de topologie spécifique sur ce point dans le standard.</t>
   </si>
   <si>
-    <t>C'est le cas dans le profil PPR sauf quon ne fait pas la distinc tion entre les deux types de bandes particulières.
-Le faut-il ?</t>
-  </si>
-  <si>
     <t>OK, à corriger.
 Cela remet-il en cause la typologie des ouvrages de protection (barrage et digues) ?
 Une référence à la documentation de SIOUH II serait la bienvenue aussi</t>
@@ -1365,9 +1361,6 @@
   </si>
   <si>
     <t>OK pour rajouter la strucutre des tableaux</t>
-  </si>
-  <si>
-    <t>OK cf. précédent</t>
   </si>
   <si>
     <t>OK, à remplacer</t>
@@ -1563,13 +1556,542 @@
 </t>
   </si>
   <si>
+    <t>Cf. ci-dessus</t>
+  </si>
+  <si>
+    <t>Ineris</t>
+  </si>
+  <si>
+    <t>p.106</t>
+  </si>
+  <si>
+    <t>Table perimetre COVADIS mal orthographiée (manque les '_' autour du S)</t>
+  </si>
+  <si>
+    <t>N_PERIMETRE_PPR[NT]_[AAAANNNN]_S_[DDD]</t>
+  </si>
+  <si>
+    <t>p.110</t>
+  </si>
+  <si>
+    <t>Manque crochet gauche CodeGaspar p.110</t>
+  </si>
+  <si>
+    <t>[TypePPR]_[CodeGASPARComplet]_zonealeatechnorapide_[CodeAlea]_s</t>
+  </si>
+  <si>
+    <t>p.111</t>
+  </si>
+  <si>
+    <t>Manque crochet gauche CodeGaspar p.111</t>
+  </si>
+  <si>
+    <t>[TypePPR]_[CodeGASPARComplet]_zonealeatechnolent_[CodeAlea]_s</t>
+  </si>
+  <si>
+    <t>[TypePPR]_[CodeGASPARComplet]_zonealeatechnoprojection_[CodeAlea]_s</t>
+  </si>
+  <si>
+    <t>p.112</t>
+  </si>
+  <si>
+    <t>Manque crochet gauche CodeGaspar p.112</t>
+  </si>
+  <si>
+    <t>[TypePPR]_[CodeGASPARComplet]_zonedangerspecifique_[CodeAlea]_s</t>
+  </si>
+  <si>
+    <t>p.113</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manque crochet gauche CodeGaspar p.113 </t>
+  </si>
+  <si>
+    <t>N_ZONE_REG_PPR[NT]_[AAAANNNN]_[SLP]_[DDD]</t>
+  </si>
+  <si>
+    <t>Pourquoi dans N_ZONE_REG_PPR[NT]_[AAAANNNN]_L_[DDD] on prend L spécifiquement ?</t>
+  </si>
+  <si>
+    <t>p.114</t>
+  </si>
+  <si>
+    <t>Manque crochet gauche CodeGaspar p.114</t>
+  </si>
+  <si>
+    <t>[TypePPR]_[CodeGASPARComplet]_zoneregmultialea fait association entre objets zonage reglementaire et classification des aléas. Or les deux tables existent déjà sous covadis. Pourquoi déclarer impossibilité de réutilisation ? La table multialéa elle-même existe, pourquoi ne pas s’en servir ?</t>
+  </si>
+  <si>
+    <t>Pas de modification simple</t>
+  </si>
+  <si>
+    <t>Pourquoi typologie objet zoneregmultialea ne respecte pas les mêmes capitalisations que pour les autres couches ?</t>
+  </si>
+  <si>
+    <t>ZoneRegMultialea</t>
+  </si>
+  <si>
+    <t>p.115</t>
+  </si>
+  <si>
+    <t>Manque crochet gauche CodeGaspar p.115</t>
+  </si>
+  <si>
+    <t>[TypePPR]_[CodeGASPARComplet]_enjeu_[slp]</t>
+  </si>
+  <si>
+    <t>p.116</t>
+  </si>
+  <si>
+    <t>Manque crochet gauche CodeGaspar p.116</t>
+  </si>
+  <si>
+    <t>[TypePPR]_[CodeGASPARComplet]_originerisque_[slp]</t>
+  </si>
+  <si>
+    <t>p.66</t>
+  </si>
+  <si>
+    <t>perte donnée si taille(ID_GASPAR)&gt;taille(codeprocedure)</t>
+  </si>
+  <si>
+    <t>TEXT(18)</t>
+  </si>
+  <si>
+    <t>p.105</t>
+  </si>
+  <si>
+    <t>pourquoi majuscule sur le P contrairement aux autres clés ?</t>
+  </si>
+  <si>
+    <t>libelleprocedure</t>
+  </si>
+  <si>
+    <t>p.67</t>
+  </si>
+  <si>
+    <t>pourquoi capitalisation P procedure (p.106 uniquement) alors qu'auparavant minuscule ?</t>
+  </si>
+  <si>
+    <t>codeprocedure</t>
+  </si>
+  <si>
+    <t>p.106, 66</t>
+  </si>
+  <si>
+    <t>Pourquoi clé idGASPAR écrite différemment alors que dans les tables COVADIS elle est toujours écrite ID_GASPAR ?</t>
+  </si>
+  <si>
+    <t>ID_GASPAR</t>
+  </si>
+  <si>
+    <t>pourquoi capitalisation sur le P procedure (p.106 uniquement) ?</t>
+  </si>
+  <si>
+    <t>etatprocedure</t>
+  </si>
+  <si>
+    <t>p.106,66</t>
+  </si>
+  <si>
+    <t>p.70, 71, 72</t>
+  </si>
+  <si>
+    <t>TEXT(15)</t>
+  </si>
+  <si>
+    <t>p.70, 71, 72, 75, 77, 79, 80</t>
+  </si>
+  <si>
+    <t>p.70, 71, 72, 75</t>
+  </si>
+  <si>
+    <t>TEXT(7)</t>
+  </si>
+  <si>
+    <t>p.110, 70, 71, 72, 75</t>
+  </si>
+  <si>
+    <t>Nom attribut NIVALEA_ST ne correspond pas à l’attribut COVADIS (ni dans nos spécifications/descriptifs du standard ni dans nos scripts de génération de table)</t>
+  </si>
+  <si>
+    <t>NIVALEA_STD</t>
+  </si>
+  <si>
+    <t>p.79, 80</t>
+  </si>
+  <si>
+    <t>p.77</t>
+  </si>
+  <si>
+    <t>TEXT(50)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Différence longueur significative, attention au passage etatprocedure du .TAB vers le .SHP ou .SHP vers .GPKG (Chaine(2) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>à</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> TEXT(10))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Perte donnée potentielle sur idzonealea (Chaine(15)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>à</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TEXT(8))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Perte donnée potentielle sur codeprocedure (Chaine(18)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>à</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TEXT(16))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Perte donnée potentielle sur typealea (Chaine(7)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>à</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">TEXT(3)) </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Perte donnée potentielle sur idzonereglementaire (Chaine(15)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>à</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TEXT(8))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Perte donnée potentielle sur idrefexterne (Chaine(50)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>à</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TEXT(20))</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">OK sur le principe.
-GeoPackage doit rester la livraison principale visée, la compatibilité avec  Shapefile assurée dans une logique de transition
+GeoPackage doit rester la livraison principale visée et la compatibilité avec  Shapefile assurée dans une logique de transition
 Prévoir une annexe où un paragraphe avec des règles de nommage conformes avec Shapefile
 </t>
   </si>
   <si>
-    <t>Cf. ci-dessus</t>
+    <t>OK sur le principe.
+On peut adopter le même principe que pour le nommange des tables : ppr[nt]_[codeprocedure].gpkg 
+Etant entendu que codeprocedure respecte la nomenclature hors préfixe éventuel ?</t>
+  </si>
+  <si>
+    <t>OK sur le principe. 
+A valdier en GT</t>
+  </si>
+  <si>
+    <t>OK
+à corriger</t>
+  </si>
+  <si>
+    <t>OK
+à corriger
+NB : prévoir plus (ou ne pas mettre de limite) ?</t>
+  </si>
+  <si>
+    <t>cf. commentaire précédent</t>
+  </si>
+  <si>
+    <t>A discuter en GT (cf aussi commentaires BRIL-9 du modèle commun)</t>
+  </si>
+  <si>
+    <t>A discuter. Je ne suis pas sur de comprendre si la demande s'applique aux aléas technos ou naturels et ce qui est demandé exactement ?</t>
+  </si>
+  <si>
+    <t>OK sur le principe  
+Il faudrait aussi dans ce cas modifier le caractère obligatoire des champs idrefexterne et refexterne (comme pour les enjeu), ainsi que l'énumération typrefexterneouvrage (rajouter valeur "aucun")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK sur le principe
+Il faudrait aussi dans ce cas modifier le caractère obligatoire des champs idrefexterne et refexterne </t>
+  </si>
+  <si>
+    <t>OK sur le principe ?
+A discuter :
+- faut-il rajouter un alea "multirisque" ou s'agit-il d'avoir une table qui rassemble toutes les zones d'aléa (avec superposition possibles) ?
+- s'agit-il d'une table toutes zones d'aléas naturels (de référence?)
+- le besoin est-il le même pour les aleéas technos (la strucutre peut varie d'une classe / table à l'autre) ?
+NB : cf. DDT74-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK sur le principe.
+Rajouter les tables d'énumération correspondant aux nomenclatures proposées.
+Simplifier les codes : proposition ?
+</t>
+  </si>
+  <si>
+    <t>OK, à renommer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK sur le principe
+Proposition : "existemesureobligatoire"
+</t>
+  </si>
+  <si>
+    <t>OK, à remplacer
+(NB, le PRECRIT (sans 'S' venait d'une table GASPAR - code d'une sous état)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOK ?
+L'énumération ne propose qu'une seule valeur "Moyen ou modéré" qu'il faut choisir que le risque soit moyen ou modéré selon le type d'aléa considéré. On a essayé d'harmoniser les échelles (cf. p36)
+Cela pose-t-il problème ou faut-il mieux l'expliquer dans le document ?
+</t>
+  </si>
+  <si>
+    <t>OK, sur le principe.
+Peut-on précisier un cas de PPR où nul s'applique et pas très faible ? Ou inversement ?</t>
+  </si>
+  <si>
+    <t>C'est le cas dans le profil PPR sauf quon ne fait pas la distinction entre les deux types de bandes particulières.
+Le faut-il ?</t>
+  </si>
+  <si>
+    <t>NOK ?
+Le code 07 s'applique à des zones reglementées du fait de l'aléa exceptionnel (une réglementation particulière) qu'il est demandé de réprésenter au niveau du zonége reglementaire.
+Le code 08 représente le niveau d'aléa avalanche exceptionnel pour qualifier la zone d'aléa (et peut-être remis en cause éventuellement). 
+A rapprocher de Cf.DDT74-2 et BRIL-9 et discussions plénière</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOK A discuter ?
+Quel est le besoin. Ces zones ne sont elles pas simplement définies par ce qui n'est pas couvert par le zonage reglementaire ?
+Ne risque-t-on pas de rajouter une complexité (géométries) supplémentaire à la couche du zonage réglementaire ?
+Faut-il rapprocher cette remaque de DDT74-14 ?
+</t>
+  </si>
+  <si>
+    <t>OK sur le principe.
+Ce nommage est-il cohérent avec SIOUH2 ? (les anciens libéllés viennent de SIOUH)
+Peut-on rajouter d'autres types d'ouvrages (hors inondation, pour les avalanches par exemple) ?</t>
+  </si>
+  <si>
+    <t>OK sur le principe.
+Cf. commentaire précédent.</t>
+  </si>
+  <si>
+    <t>Le terme "résolution spatiale" est le nom du champ de métadonnées INSPIRE (traduction de "spatialResolution" dans la norme ISO 19115) qui peut être utilisé de différentes façons (résolution ou dénominateur d'échelle).
+On peut préciser différents niveaux d'échelles applicables pour les PPR plutôt que de fixer à 5000 (reprendre le "2000"-"25000" de description du standard) et mettre la valeur adaptée pour chaque jeu de données PPR</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>- OK, à enlever</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Ces informations n'étaient pas indiquées dans l'ancien standard COVADIS. On ne peut donc pas les mentionner dans la partie conversion COAVDIS vers nouveau standard.'</t>
+    </r>
+  </si>
+  <si>
+    <t>C'est une erreur à corriger</t>
+  </si>
+  <si>
+    <t>Oui car le code de l'état est différent.
+NB : peut-être rajouter une table de correspondance entre les deux tables d'états</t>
+  </si>
+  <si>
+    <t>idGASPAR est le nom du champ dans le modèle COAVDIS (partie B). ID_GASPAR est le nom du champ dans l'implémentation sous forme de table (partie C)</t>
+  </si>
+  <si>
+    <t>OK sur le principe
+Il est difficile de documenter l'utilisation de la table multialea COVADIS pour le zonagereglementaire multi alea. On peut indiquer que c'est faisable en donnant des indications algorithmiques (à tenter?)</t>
+  </si>
+  <si>
+    <t>NOK, c'est parce qu'il sagit d'une table (en minuscules) et non d'un classe (il n'y a pas de classe ZoneRegMultiAlea)</t>
+  </si>
+  <si>
+    <t>OK sur le principe. A rapprocher de DDT38-15</t>
+  </si>
+  <si>
+    <t>OK sur le principe.
+Proposer une couhce multialea comme dans les commentaires précédents ?</t>
+  </si>
+  <si>
+    <t>OK, sur le principe
+Par contre, il n'y a pas de procédure PPRT-Multi dans la classification des procédures GASPAR.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK sur le principe
+Mais le type de Procédure PPR-L vient de la classification GASPAR (au même titre qu'on a des PPRN-S, PPRN-I, etc.. Comme sous catégories de procédures PPRN).
+On peut éventuellement étendre cette partie multirisques aux PPRL ?
+</t>
+  </si>
+  <si>
+    <t>OK sur le principe.
+La codification proposées se voulait hiérarchique.
+Solution à trouver pour garder cette hiérarchie en simplifiant</t>
+  </si>
+  <si>
+    <t>Cf. commentaire précédent</t>
+  </si>
+  <si>
+    <t>OK sur le principe
+A-t-on des cas de ce type ?</t>
+  </si>
+  <si>
+    <t>OK sur le principe
+Quelle règle de fusion adopter ?</t>
+  </si>
+  <si>
+    <t>OK sur le principe.
+A voir en fonction du commentaire précédent également</t>
+  </si>
+  <si>
+    <t>OK sur le principe
+A traiter en fonction de la fuision PPRN/PPRL</t>
+  </si>
+  <si>
+    <t>OK
+A rajouter aussi en p80 (dictionnaire des tables)</t>
+  </si>
+  <si>
+    <t>C'est cité dans le guide PPRN comme enjeu incontournable</t>
+  </si>
+  <si>
+    <t>Le guide PPRN fait cette distinction sans doute pour pouvoir faire la distinction au niveau du zonage…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK sur le principe
+Le GT ne s'est pas penché sur la représentation des enjeux car il fallait d'abord s'entendre sur la nomenclature. A terme, cela pourrait faire l'objet d'une extension du standard.
+</t>
+  </si>
+  <si>
+    <t>Oui dans certains cas. Le standard ne précise pas de règle particulière de topologie.</t>
+  </si>
+  <si>
+    <t>OK à rajouter</t>
+  </si>
+  <si>
+    <t>NOK
+Est-il plus simple de copier / coller une couche par type d'aléa  à représenter que de supprimer N couches d'aléas ?</t>
+  </si>
+  <si>
+    <t>OK cf. précédent (1:2000 du coup)</t>
   </si>
 </sst>
 </file>
@@ -1625,12 +2147,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -1658,15 +2174,20 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
-      <color theme="5"/>
+      <color theme="5" tint="-0.249977111117893"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Wingdings"/>
+      <charset val="2"/>
+    </font>
+    <font>
       <sz val="9"/>
-      <color theme="5" tint="-0.249977111117893"/>
+      <color theme="5"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1701,7 +2222,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1733,22 +2254,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1757,16 +2272,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1776,103 +2297,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1932,6 +2356,63 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -1947,6 +2428,26 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2163,6 +2664,26 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2201,35 +2722,35 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E152CA69-C1C4-40F5-84A2-16C1484F79DC}" name="Tableau3" displayName="Tableau3" ref="A1:H20" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:H20" xr:uid="{E152CA69-C1C4-40F5-84A2-16C1484F79DC}"/>
   <tableColumns count="8">
-    <tableColumn id="8" xr3:uid="{FDEDA288-5661-4539-AEBA-9A87C20962E6}" name="Numero" dataDxfId="4">
+    <tableColumn id="8" xr3:uid="{FDEDA288-5661-4539-AEBA-9A87C20962E6}" name="Numero" dataDxfId="18">
       <calculatedColumnFormula>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{635A3DB7-7204-4378-B92A-598A2491845D}" name="Colonne1" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{79A10EF1-8EC6-4A0F-BA8C-3DFA972C0085}" name="Organisme" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{B1796E2E-D6C3-4AA8-BE83-FC4F94A53A8A}" name="Type de commentaire:_x000a_(G)énéral  (M)étier (T)echnique (D)ocument" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{1412256D-CC49-4084-A346-F8B20C24D98A}" name="Page, _x000a_Paragraphe" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{5F39A908-2FFC-40EB-BF7C-360C193B6507}" name="Commentaire" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{D01F9F9F-406C-4050-A108-256D1A81EB43}" name="Modification proposée " dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{2B745299-03CE-435C-B9E5-654FA9CECC38}" name="Décision du GT CNIG Risques" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{635A3DB7-7204-4378-B92A-598A2491845D}" name="Colonne1" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{79A10EF1-8EC6-4A0F-BA8C-3DFA972C0085}" name="Organisme" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{B1796E2E-D6C3-4AA8-BE83-FC4F94A53A8A}" name="Type de commentaire:_x000a_(G)énéral  (M)étier (T)echnique (D)ocument" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{1412256D-CC49-4084-A346-F8B20C24D98A}" name="Page, _x000a_Paragraphe" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{5F39A908-2FFC-40EB-BF7C-360C193B6507}" name="Commentaire" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{D01F9F9F-406C-4050-A108-256D1A81EB43}" name="Modification proposée " dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{2B745299-03CE-435C-B9E5-654FA9CECC38}" name="Décision du GT CNIG Risques" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{847E454C-1CA0-45D6-9F56-3D5FFE89C0F5}" name="Tableau2" displayName="Tableau2" ref="A1:H111" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9">
-  <autoFilter ref="A1:H111" xr:uid="{847E454C-1CA0-45D6-9F56-3D5FFE89C0F5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{847E454C-1CA0-45D6-9F56-3D5FFE89C0F5}" name="Tableau2" displayName="Tableau2" ref="A1:H138" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8">
+  <autoFilter ref="A1:H138" xr:uid="{847E454C-1CA0-45D6-9F56-3D5FFE89C0F5}"/>
   <tableColumns count="8">
-    <tableColumn id="8" xr3:uid="{6862FBA5-3017-4233-B0D4-5BC2462198D0}" name="Colonne2" dataDxfId="3">
+    <tableColumn id="8" xr3:uid="{6862FBA5-3017-4233-B0D4-5BC2462198D0}" name="Colonne2" dataDxfId="7">
       <calculatedColumnFormula>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{A8BB7BB0-4D6B-4A0E-A615-089BDEA55F36}" name="Colonne1" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{81E8B2D7-3970-4344-9966-2E0DDFB404DB}" name="Organisme" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{D152CE9B-5BA5-4879-B7DE-1CBF90027255}" name="Type de commentaire:(G)énéral  (M)étier (T)echnique (D)ocument" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{DE633778-26A0-4BDF-9CA2-36FE6DA84467}" name="Page, Paragraphe" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{378CA86A-0CF7-484A-BD7C-53282B21DE2F}" name="Commentaire" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{38052BD9-6BB2-443C-8278-BB11301B0221}" name="Modification proposée " dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{A2C2771F-6D33-454B-9C1D-FAE8B1231568}" name="Décision du GT CNIG Risques" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{A8BB7BB0-4D6B-4A0E-A615-089BDEA55F36}" name="Colonne1" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{81E8B2D7-3970-4344-9966-2E0DDFB404DB}" name="Organisme" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{D152CE9B-5BA5-4879-B7DE-1CBF90027255}" name="Type de commentaire:(G)énéral  (M)étier (T)echnique (D)ocument" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{DE633778-26A0-4BDF-9CA2-36FE6DA84467}" name="Page, Paragraphe" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{378CA86A-0CF7-484A-BD7C-53282B21DE2F}" name="Commentaire" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{38052BD9-6BB2-443C-8278-BB11301B0221}" name="Modification proposée " dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{A2C2771F-6D33-454B-9C1D-FAE8B1231568}" name="Décision du GT CNIG Risques" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2600,7 +3121,7 @@
       <c r="G2" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="17" t="s">
         <v>351</v>
       </c>
     </row>
@@ -2627,7 +3148,7 @@
       <c r="G3" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="13" t="s">
         <v>352</v>
       </c>
     </row>
@@ -2654,7 +3175,7 @@
       <c r="G4" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="23" t="s">
         <v>355</v>
       </c>
     </row>
@@ -2681,7 +3202,7 @@
       <c r="G5" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="13" t="s">
         <v>353</v>
       </c>
     </row>
@@ -2708,7 +3229,7 @@
       <c r="G6" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="H6" s="17" t="s">
         <v>350</v>
       </c>
     </row>
@@ -2733,7 +3254,7 @@
         <v>323</v>
       </c>
       <c r="G7" s="4"/>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="18" t="s">
         <v>354</v>
       </c>
     </row>
@@ -2760,11 +3281,11 @@
       <c r="G8" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="23" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="92" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-7</v>
@@ -2772,22 +3293,22 @@
       <c r="B9" s="1">
         <v>7</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="13" t="s">
         <v>311</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="13" t="s">
         <v>335</v>
       </c>
-      <c r="H9" s="21" t="s">
+      <c r="H9" s="23" t="s">
         <v>356</v>
       </c>
     </row>
@@ -2814,7 +3335,7 @@
       <c r="G10" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="H10" s="23" t="s">
         <v>358</v>
       </c>
     </row>
@@ -2841,7 +3362,7 @@
       <c r="G11" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="H11" s="21" t="s">
+      <c r="H11" s="23" t="s">
         <v>358</v>
       </c>
     </row>
@@ -2850,7 +3371,7 @@
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-8</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="12">
         <v>8</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -2868,7 +3389,7 @@
       <c r="G12" s="9" t="s">
         <v>315</v>
       </c>
-      <c r="H12" s="21" t="s">
+      <c r="H12" s="23" t="s">
         <v>357</v>
       </c>
     </row>
@@ -2877,7 +3398,7 @@
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>cerema-6</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="12">
         <v>6</v>
       </c>
       <c r="C13" s="9" t="s">
@@ -2895,7 +3416,7 @@
       <c r="G13" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="H13" s="21" t="s">
+      <c r="H13" s="23" t="s">
         <v>359</v>
       </c>
     </row>
@@ -2922,7 +3443,7 @@
       <c r="G14" s="9" t="s">
         <v>336</v>
       </c>
-      <c r="H14" s="21" t="s">
+      <c r="H14" s="23" t="s">
         <v>360</v>
       </c>
     </row>
@@ -2949,7 +3470,7 @@
       <c r="G15" s="4" t="s">
         <v>320</v>
       </c>
-      <c r="H15" s="19" t="s">
+      <c r="H15" s="17" t="s">
         <v>354</v>
       </c>
     </row>
@@ -2976,7 +3497,7 @@
       <c r="G16" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="H16" s="15" t="s">
+      <c r="H16" s="13" t="s">
         <v>361</v>
       </c>
     </row>
@@ -3003,7 +3524,7 @@
       <c r="G17" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="H17" s="19" t="s">
+      <c r="H17" s="17" t="s">
         <v>363</v>
       </c>
     </row>
@@ -3030,11 +3551,11 @@
       <c r="G18" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="H18" s="21" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="57.5" x14ac:dyDescent="0.35">
+      <c r="H18" s="23" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="46" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SDCAP/PONSOH-13</v>
@@ -3057,8 +3578,8 @@
       <c r="G19" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="H19" s="21" t="s">
-        <v>365</v>
+      <c r="H19" s="23" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3082,8 +3603,8 @@
         <v>325</v>
       </c>
       <c r="G20" s="4"/>
-      <c r="H20" s="19" t="s">
-        <v>366</v>
+      <c r="H20" s="17" t="s">
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -3097,17 +3618,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815F14A-19BC-4DCE-8D31-81F595A4B0E7}">
-  <dimension ref="A1:J111"/>
+  <dimension ref="A1:J138"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.6328125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="5.36328125" style="3" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" style="3" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="3.81640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="3" customWidth="1"/>
     <col min="4" max="4" width="16" style="3" customWidth="1"/>
     <col min="5" max="5" width="20.6328125" style="3" customWidth="1"/>
     <col min="6" max="6" width="55.54296875" style="3" customWidth="1"/>
@@ -3117,7 +3638,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>348</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -3163,8 +3684,8 @@
         <v>242</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="23" t="s">
-        <v>377</v>
+      <c r="H2" s="20" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3188,8 +3709,8 @@
         <v>243</v>
       </c>
       <c r="G3" s="4"/>
-      <c r="H3" s="23" t="s">
-        <v>378</v>
+      <c r="H3" s="20" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3213,8 +3734,8 @@
         <v>244</v>
       </c>
       <c r="G4" s="9"/>
-      <c r="H4" s="23" t="s">
-        <v>380</v>
+      <c r="H4" s="20" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="51.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3238,8 +3759,8 @@
         <v>245</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="23" t="s">
-        <v>379</v>
+      <c r="H5" s="20" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="103.5" x14ac:dyDescent="0.35">
@@ -3261,8 +3782,8 @@
         <v>253</v>
       </c>
       <c r="G6" s="4"/>
-      <c r="H6" s="19" t="s">
-        <v>381</v>
+      <c r="H6" s="17" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="46" x14ac:dyDescent="0.35">
@@ -3286,8 +3807,8 @@
       <c r="G7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="15" t="s">
-        <v>382</v>
+      <c r="H7" s="13" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
@@ -3311,8 +3832,8 @@
       <c r="G8" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H8" s="23" t="s">
-        <v>383</v>
+      <c r="H8" s="20" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="23" x14ac:dyDescent="0.35">
@@ -3336,8 +3857,8 @@
       <c r="G9" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="23" t="s">
-        <v>384</v>
+      <c r="H9" s="20" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="65" customHeight="1" x14ac:dyDescent="0.35">
@@ -3363,8 +3884,8 @@
       <c r="G10" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="H10" s="19" t="s">
-        <v>385</v>
+      <c r="H10" s="17" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.35">
@@ -3390,8 +3911,8 @@
       <c r="G11" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="H11" s="19" t="s">
-        <v>386</v>
+      <c r="H11" s="17" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="60.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3417,7 +3938,7 @@
       <c r="G12" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="H12" s="17" t="s">
         <v>350</v>
       </c>
     </row>
@@ -3444,8 +3965,8 @@
       <c r="G13" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="H13" s="19" t="s">
-        <v>387</v>
+      <c r="H13" s="17" t="s">
+        <v>539</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="138" x14ac:dyDescent="0.35">
@@ -3471,8 +3992,8 @@
       <c r="G14" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="H14" s="19" t="s">
-        <v>388</v>
+      <c r="H14" s="17" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
@@ -3498,8 +4019,8 @@
       <c r="G15" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H15" s="19" t="s">
-        <v>389</v>
+      <c r="H15" s="17" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
@@ -3525,11 +4046,11 @@
       <c r="G16" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="H16" s="19" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
+      <c r="H16" s="17" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-4</v>
@@ -3552,11 +4073,11 @@
       <c r="G17" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="H17" s="15" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="23" x14ac:dyDescent="0.35">
+      <c r="H17" s="13" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-4</v>
@@ -3579,11 +4100,11 @@
       <c r="G18" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="H18" s="19" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="57.5" x14ac:dyDescent="0.35">
+      <c r="H18" s="17" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-5</v>
@@ -3606,11 +4127,11 @@
       <c r="G19" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="H19" s="23" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="69" x14ac:dyDescent="0.35">
+      <c r="H19" s="20" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-6</v>
@@ -3633,11 +4154,11 @@
       <c r="G20" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="H20" s="19" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H20" s="17" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-2</v>
@@ -3660,11 +4181,11 @@
       <c r="G21" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="H21" s="19" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H21" s="17" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-3</v>
@@ -3687,11 +4208,11 @@
       <c r="G22" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="H22" s="15" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H22" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-5</v>
@@ -3714,11 +4235,11 @@
       <c r="G23" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="H23" s="19" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+      <c r="H23" s="17" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-4</v>
@@ -3741,11 +4262,11 @@
       <c r="G24" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="H24" s="23" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="23" x14ac:dyDescent="0.35">
+      <c r="H24" s="20" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-5</v>
@@ -3768,11 +4289,11 @@
       <c r="G25" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="H25" s="19" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H25" s="17" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-7</v>
@@ -3795,11 +4316,11 @@
       <c r="G26" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="H26" s="19" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="25" x14ac:dyDescent="0.35">
+      <c r="H26" s="17" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="25" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-6</v>
@@ -3822,11 +4343,11 @@
       <c r="G27" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="H27" s="19" t="s">
+      <c r="H27" s="17" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="92" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-</v>
@@ -3839,7 +4360,7 @@
         <v>16</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>339</v>
@@ -3847,11 +4368,12 @@
       <c r="G28" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="H28" s="23" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H28" s="20" t="s">
+        <v>397</v>
+      </c>
+      <c r="I28" s="19"/>
+    </row>
+    <row r="29" spans="1:9" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-8</v>
@@ -3874,11 +4396,11 @@
       <c r="G29" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="H29" s="19" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H29" s="17" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-9</v>
@@ -3901,11 +4423,11 @@
       <c r="G30" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="H30" s="23" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="57.5" x14ac:dyDescent="0.35">
+      <c r="H30" s="20" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-6</v>
@@ -3928,11 +4450,11 @@
       <c r="G31" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="H31" s="23" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
+      <c r="H31" s="20" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-7</v>
@@ -3955,8 +4477,8 @@
       <c r="G32" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="H32" s="23" t="s">
-        <v>403</v>
+      <c r="H32" s="20" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.35">
@@ -3980,8 +4502,8 @@
         <v>80</v>
       </c>
       <c r="G33" s="4"/>
-      <c r="H33" s="19" t="s">
-        <v>402</v>
+      <c r="H33" s="17" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="57.5" x14ac:dyDescent="0.35">
@@ -4007,8 +4529,8 @@
       <c r="G34" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="H34" s="23" t="s">
-        <v>404</v>
+      <c r="H34" s="20" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4032,8 +4554,8 @@
       <c r="G35" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="H35" s="19" t="s">
-        <v>402</v>
+      <c r="H35" s="17" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
@@ -4059,8 +4581,8 @@
       <c r="G36" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H36" s="15" t="s">
-        <v>405</v>
+      <c r="H36" s="13" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
@@ -4086,8 +4608,8 @@
       <c r="G37" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="H37" s="15" t="s">
-        <v>406</v>
+      <c r="H37" s="13" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
@@ -4103,16 +4625,16 @@
         <v>16</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="H38" s="23" t="s">
-        <v>407</v>
+      <c r="H38" s="20" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="161" x14ac:dyDescent="0.35">
@@ -4128,16 +4650,16 @@
         <v>16</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="H39" s="23" t="s">
-        <v>407</v>
+      <c r="H39" s="20" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="69" x14ac:dyDescent="0.35">
@@ -4163,8 +4685,8 @@
       <c r="G40" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="H40" s="23" t="s">
-        <v>410</v>
+      <c r="H40" s="20" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.35">
@@ -4190,8 +4712,8 @@
       <c r="G41" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="H41" s="23" t="s">
-        <v>411</v>
+      <c r="H41" s="20" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4215,8 +4737,8 @@
         <v>84</v>
       </c>
       <c r="G42" s="4"/>
-      <c r="H42" s="23" t="s">
-        <v>412</v>
+      <c r="H42" s="20" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
@@ -4242,8 +4764,8 @@
       <c r="G43" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H43" s="15" t="s">
-        <v>414</v>
+      <c r="H43" s="13" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.35">
@@ -4269,8 +4791,8 @@
       <c r="G44" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H44" s="23" t="s">
-        <v>415</v>
+      <c r="H44" s="20" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
@@ -4294,8 +4816,8 @@
         <v>102</v>
       </c>
       <c r="G45" s="4"/>
-      <c r="H45" s="23" t="s">
-        <v>416</v>
+      <c r="H45" s="20" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
@@ -4313,7 +4835,7 @@
         <v>16</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>32</v>
@@ -4321,8 +4843,8 @@
       <c r="G46" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H46" s="23" t="s">
-        <v>417</v>
+      <c r="H46" s="20" t="s">
+        <v>415</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4340,7 +4862,7 @@
         <v>16</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>105</v>
@@ -4348,8 +4870,8 @@
       <c r="G47" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="H47" s="23" t="s">
-        <v>416</v>
+      <c r="H47" s="20" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4375,8 +4897,8 @@
       <c r="G48" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H48" s="19" t="s">
-        <v>418</v>
+      <c r="H48" s="17" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="58" customHeight="1" x14ac:dyDescent="0.35">
@@ -4402,8 +4924,8 @@
       <c r="G49" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H49" s="23" t="s">
-        <v>413</v>
+      <c r="H49" s="20" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="57.5" x14ac:dyDescent="0.35">
@@ -4429,8 +4951,8 @@
       <c r="G50" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H50" s="15" t="s">
-        <v>419</v>
+      <c r="H50" s="13" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
@@ -4456,8 +4978,8 @@
       <c r="G51" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="H51" s="19" t="s">
-        <v>394</v>
+      <c r="H51" s="17" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
@@ -4483,8 +5005,8 @@
       <c r="G52" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="H52" s="19" t="s">
-        <v>394</v>
+      <c r="H52" s="17" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="23" x14ac:dyDescent="0.35">
@@ -4510,8 +5032,8 @@
       <c r="G53" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="H53" s="23" t="s">
-        <v>420</v>
+      <c r="H53" s="20" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="36.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4535,8 +5057,8 @@
       <c r="G54" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="H54" s="23" t="s">
-        <v>421</v>
+      <c r="H54" s="20" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.35">
@@ -4560,8 +5082,8 @@
       <c r="G55" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="H55" s="19" t="s">
-        <v>388</v>
+      <c r="H55" s="17" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="57.5" x14ac:dyDescent="0.35">
@@ -4585,8 +5107,8 @@
         <v>89</v>
       </c>
       <c r="G56" s="4"/>
-      <c r="H56" s="15" t="s">
-        <v>424</v>
+      <c r="H56" s="13" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
@@ -4612,8 +5134,8 @@
       <c r="G57" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="H57" s="19" t="s">
-        <v>388</v>
+      <c r="H57" s="17" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="149.5" x14ac:dyDescent="0.35">
@@ -4622,7 +5144,7 @@
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
       </c>
       <c r="B58" s="1"/>
-      <c r="C58" s="17" t="s">
+      <c r="C58" s="15" t="s">
         <v>341</v>
       </c>
       <c r="D58" s="5" t="s">
@@ -4631,12 +5153,12 @@
       <c r="E58" s="5" t="s">
         <v>347</v>
       </c>
-      <c r="F58" s="17" t="s">
+      <c r="F58" s="15" t="s">
         <v>346</v>
       </c>
       <c r="G58" s="4"/>
-      <c r="H58" s="23" t="s">
-        <v>422</v>
+      <c r="H58" s="20" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="46" x14ac:dyDescent="0.35">
@@ -4662,8 +5184,8 @@
       <c r="G59" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="H59" s="23" t="s">
-        <v>423</v>
+      <c r="H59" s="20" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="69" x14ac:dyDescent="0.35">
@@ -4672,7 +5194,7 @@
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
       </c>
       <c r="B60" s="1"/>
-      <c r="C60" s="17" t="s">
+      <c r="C60" s="15" t="s">
         <v>341</v>
       </c>
       <c r="D60" s="5" t="s">
@@ -4681,12 +5203,12 @@
       <c r="E60" s="5" t="s">
         <v>342</v>
       </c>
-      <c r="F60" s="17" t="s">
+      <c r="F60" s="15" t="s">
         <v>345</v>
       </c>
       <c r="G60" s="4"/>
-      <c r="H60" s="23" t="s">
-        <v>427</v>
+      <c r="H60" s="20" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="184" x14ac:dyDescent="0.35">
@@ -4695,7 +5217,7 @@
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
       </c>
       <c r="B61" s="1"/>
-      <c r="C61" s="17" t="s">
+      <c r="C61" s="15" t="s">
         <v>341</v>
       </c>
       <c r="D61" s="5" t="s">
@@ -4708,8 +5230,8 @@
         <v>343</v>
       </c>
       <c r="G61" s="4"/>
-      <c r="H61" s="15" t="s">
-        <v>425</v>
+      <c r="H61" s="13" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="69" x14ac:dyDescent="0.35">
@@ -4735,8 +5257,8 @@
       <c r="G62" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="H62" s="23" t="s">
-        <v>429</v>
+      <c r="H62" s="20" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="46" x14ac:dyDescent="0.35">
@@ -4745,7 +5267,7 @@
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
       </c>
       <c r="B63" s="1"/>
-      <c r="C63" s="17" t="s">
+      <c r="C63" s="15" t="s">
         <v>341</v>
       </c>
       <c r="D63" s="5" t="s">
@@ -4754,12 +5276,12 @@
       <c r="E63" s="5" t="s">
         <v>342</v>
       </c>
-      <c r="F63" s="17" t="s">
+      <c r="F63" s="15" t="s">
         <v>344</v>
       </c>
       <c r="G63" s="4"/>
-      <c r="H63" s="15" t="s">
-        <v>426</v>
+      <c r="H63" s="13" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="46" x14ac:dyDescent="0.35">
@@ -4785,8 +5307,8 @@
       <c r="G64" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="H64" s="23" t="s">
-        <v>428</v>
+      <c r="H64" s="20" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="46" x14ac:dyDescent="0.35">
@@ -4804,7 +5326,7 @@
         <v>11</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F65" s="4" t="s">
         <v>49</v>
@@ -4812,8 +5334,8 @@
       <c r="G65" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H65" s="15" t="s">
-        <v>430</v>
+      <c r="H65" s="13" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="46" x14ac:dyDescent="0.35">
@@ -4831,7 +5353,7 @@
         <v>7</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F66" s="4" t="s">
         <v>52</v>
@@ -4839,8 +5361,8 @@
       <c r="G66" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="H66" s="15" t="s">
-        <v>431</v>
+      <c r="H66" s="13" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="145" x14ac:dyDescent="0.35">
@@ -4866,8 +5388,8 @@
       <c r="G67" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="H67" s="23" t="s">
-        <v>432</v>
+      <c r="H67" s="20" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="88" customHeight="1" x14ac:dyDescent="0.35">
@@ -4893,8 +5415,8 @@
       <c r="G68" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="H68" s="23" t="s">
-        <v>433</v>
+      <c r="H68" s="20" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="103" customHeight="1" x14ac:dyDescent="0.35">
@@ -4920,7 +5442,9 @@
       <c r="G69" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="H69" s="4"/>
+      <c r="H69" s="20" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="70" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="str">
@@ -4945,7 +5469,9 @@
       <c r="G70" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="H70" s="4"/>
+      <c r="H70" s="20" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="71" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="4" t="str">
@@ -4970,90 +5496,98 @@
       <c r="G71" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="H71" s="4"/>
-    </row>
-    <row r="72" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="4" t="str">
+      <c r="H71" s="17" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A72" s="21" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Ineris-14</v>
+      </c>
+      <c r="B72" s="1">
+        <v>14</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="H72" s="20" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A73" s="21" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Ineris-19</v>
+      </c>
+      <c r="B73" s="1">
+        <v>19</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="H73" s="17" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A74" s="21" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Ineris-16</v>
+      </c>
+      <c r="B74" s="1">
+        <v>16</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>467</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="H74" s="17" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-14</v>
       </c>
-      <c r="B72" s="7">
+      <c r="B75" s="7">
         <v>14</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="F72" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="G72" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="H72" s="4"/>
-    </row>
-    <row r="73" spans="1:8" ht="103.5" x14ac:dyDescent="0.35">
-      <c r="A73" s="4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DDT38-15</v>
-      </c>
-      <c r="B73" s="8">
-        <v>15</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="F73" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="G73" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="H73" s="4"/>
-    </row>
-    <row r="74" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DDT38-16</v>
-      </c>
-      <c r="B74" s="8">
-        <v>16</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="D74" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="F74" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="G74" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="H74" s="4"/>
-    </row>
-    <row r="75" spans="1:8" ht="46" x14ac:dyDescent="0.35">
-      <c r="A75" s="4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DDT38-17</v>
-      </c>
-      <c r="B75" s="8">
-        <v>17</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>163</v>
@@ -5062,319 +5596,349 @@
         <v>188</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="H75" s="4"/>
-    </row>
-    <row r="76" spans="1:8" ht="23" x14ac:dyDescent="0.35">
+        <v>273</v>
+      </c>
+      <c r="H75" s="20" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="115" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DDT38-18</v>
+        <v>DDT38-15</v>
       </c>
       <c r="B76" s="8">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>163</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>188</v>
+        <v>16</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>208</v>
+        <v>274</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="H76" s="4"/>
-    </row>
-    <row r="77" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+        <v>275</v>
+      </c>
+      <c r="H76" s="20" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A77" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DDT38-19</v>
-      </c>
-      <c r="B77" s="7">
-        <v>19</v>
+        <v>DDT38-16</v>
+      </c>
+      <c r="B77" s="8">
+        <v>16</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>163</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>190</v>
+        <v>16</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>276</v>
+        <v>202</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="H77" s="4"/>
-    </row>
-    <row r="78" spans="1:8" ht="23" x14ac:dyDescent="0.35">
-      <c r="A78" s="4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DDT38-20</v>
-      </c>
-      <c r="B78" s="7">
-        <v>20</v>
+        <v>203</v>
+      </c>
+      <c r="H77" s="20" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A78" s="21" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Ineris-22</v>
+      </c>
+      <c r="B78" s="1">
+        <v>22</v>
       </c>
       <c r="C78" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>488</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="H78" s="20" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A79" s="21" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Ineris-23</v>
+      </c>
+      <c r="B79" s="1">
+        <v>23</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="H79" s="17" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A80" s="21" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Ineris-24</v>
+      </c>
+      <c r="B80" s="1">
+        <v>24</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>479</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>490</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>480</v>
+      </c>
+      <c r="H80" s="17" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+      <c r="A81" s="4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>DDT38-17</v>
+      </c>
+      <c r="B81" s="8">
+        <v>17</v>
+      </c>
+      <c r="C81" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D78" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E78" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="F78" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="G78" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="H78" s="4"/>
-    </row>
-    <row r="79" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
-      <c r="A79" s="4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DDT38-21</v>
-      </c>
-      <c r="B79" s="8">
-        <v>21</v>
-      </c>
-      <c r="C79" s="4" t="s">
+      <c r="D81" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="G81" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="H81" s="20" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A82" s="4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>DDT38-18</v>
+      </c>
+      <c r="B82" s="8">
+        <v>18</v>
+      </c>
+      <c r="C82" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D79" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="F79" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="G79" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="H79" s="4"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A80" s="4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>Cerema-17</v>
-      </c>
-      <c r="B80" s="1">
-        <v>17</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="D80" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E80" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="F80" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="G80" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="H80" s="4"/>
-    </row>
-    <row r="81" spans="1:8" ht="23" x14ac:dyDescent="0.35">
-      <c r="A81" s="4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DGPR/SRNH/SdcAP/BRIL-16</v>
-      </c>
-      <c r="B81" s="1">
-        <v>16</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D81" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E81" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F81" s="4"/>
-      <c r="G81" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="H81" s="4"/>
-    </row>
-    <row r="82" spans="1:8" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DGPR/SRNH/SdcAP/BRIL-17</v>
-      </c>
-      <c r="B82" s="1">
-        <v>17</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="D82" s="5" t="s">
-        <v>23</v>
+        <v>188</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>90</v>
+        <v>207</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="G82" s="4"/>
-      <c r="H82" s="4"/>
-    </row>
-    <row r="83" spans="1:8" ht="23" x14ac:dyDescent="0.35">
+        <v>208</v>
+      </c>
+      <c r="G82" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="H82" s="20" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A83" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DDT38-22</v>
-      </c>
-      <c r="B83" s="8">
-        <v>22</v>
+        <v>DDT38-19</v>
+      </c>
+      <c r="B83" s="7">
+        <v>19</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>163</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>16</v>
+        <v>190</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="H83" s="4"/>
-    </row>
-    <row r="84" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+        <v>211</v>
+      </c>
+      <c r="H83" s="20" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="23" x14ac:dyDescent="0.35">
       <c r="A84" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DDT38-23</v>
+        <v>DDT38-20</v>
       </c>
       <c r="B84" s="7">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>163</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E84" s="5" t="s">
-        <v>219</v>
+        <v>23</v>
+      </c>
+      <c r="E84" s="10" t="s">
+        <v>210</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="H84" s="4"/>
-    </row>
-    <row r="85" spans="1:8" ht="46" x14ac:dyDescent="0.35">
-      <c r="A85" s="4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DDT38-24</v>
-      </c>
-      <c r="B85" s="7">
-        <v>24</v>
+        <v>213</v>
+      </c>
+      <c r="H84" s="17" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="36.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="21" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Ineris-27</v>
+      </c>
+      <c r="B85" s="1">
+        <v>27</v>
       </c>
       <c r="C85" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>492</v>
+      </c>
+      <c r="G85" s="4" t="s">
+        <v>486</v>
+      </c>
+      <c r="H85" s="20" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A86" s="4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>DDT38-21</v>
+      </c>
+      <c r="B86" s="8">
+        <v>21</v>
+      </c>
+      <c r="C86" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D85" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E85" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="F85" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="G85" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="H85" s="12"/>
-    </row>
-    <row r="86" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DGPR/SRNH/SdCAP/PoNSOH-26</v>
-      </c>
-      <c r="B86" s="1">
+      <c r="D86" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="G86" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="H86" s="20" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="21" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Ineris-26</v>
+      </c>
+      <c r="B87" s="1">
         <v>26</v>
       </c>
-      <c r="C86" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="D86" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E86" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="F86" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="G86" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="H86" s="4"/>
-    </row>
-    <row r="87" spans="1:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DGPR/SRNH/SdCAP/PoNSOH-27</v>
-      </c>
-      <c r="B87" s="1">
-        <v>27</v>
-      </c>
       <c r="C87" s="4" t="s">
-        <v>258</v>
+        <v>431</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>111</v>
+        <v>484</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>112</v>
+        <v>491</v>
       </c>
       <c r="G87" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="H87" s="4"/>
+        <v>477</v>
+      </c>
+      <c r="H87" s="20" t="s">
+        <v>497</v>
+      </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>Cerema-18</v>
+        <v>Cerema-17</v>
       </c>
       <c r="B88" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>114</v>
@@ -5383,583 +5947,1356 @@
         <v>23</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
       <c r="G88" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="H88" s="4"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+        <v>157</v>
+      </c>
+      <c r="H88" s="17" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A89" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>Cerema-19</v>
+        <v>DGPR/SRNH/SdcAP/BRIL-16</v>
       </c>
       <c r="B89" s="1">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>114</v>
+        <v>55</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="F89" s="4" t="s">
-        <v>141</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="F89" s="4"/>
       <c r="G89" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="H89" s="4"/>
-    </row>
-    <row r="90" spans="1:8" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+      <c r="H89" s="17" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DGPR/SRNH/SdcAP/BRIL-18</v>
+        <v>DGPR/SRNH/SdcAP/BRIL-17</v>
       </c>
       <c r="B90" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C90" s="4" t="s">
         <v>55</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>257</v>
+        <v>92</v>
       </c>
       <c r="G90" s="4"/>
-      <c r="H90" s="4"/>
+      <c r="H90" s="13" t="s">
+        <v>508</v>
+      </c>
     </row>
     <row r="91" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A91" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DDT01-1</v>
-      </c>
-      <c r="B91" s="1">
+        <v>DDT38-22</v>
+      </c>
+      <c r="B91" s="8">
+        <v>22</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="G91" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="H91" s="20" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
+      <c r="A92" s="4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>DDT38-23</v>
+      </c>
+      <c r="B92" s="7">
+        <v>23</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="G92" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="H92" s="13" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
+      <c r="A93" s="4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>DDT38-24</v>
+      </c>
+      <c r="B93" s="7">
+        <v>24</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="F93" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="G93" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="H93" s="22" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A94" s="4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>DGPR/SRNH/SdCAP/PoNSOH-26</v>
+      </c>
+      <c r="B94" s="1">
+        <v>26</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G94" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="H94" s="20" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>DGPR/SRNH/SdCAP/PoNSOH-27</v>
+      </c>
+      <c r="B95" s="1">
+        <v>27</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E95" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="G95" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="H95" s="20" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A96" s="4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Cerema-18</v>
+      </c>
+      <c r="B96" s="1">
+        <v>18</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E96" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="G96" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="H96" s="17" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A97" s="4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Cerema-19</v>
+      </c>
+      <c r="B97" s="1">
+        <v>19</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E97" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="F97" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="G97" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="H97" s="17" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="96.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>DGPR/SRNH/SdcAP/BRIL-18</v>
+      </c>
+      <c r="B98" s="1">
+        <v>18</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="G98" s="4"/>
+      <c r="H98" s="20" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A99" s="21" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Ineris-15</v>
+      </c>
+      <c r="B99" s="1">
+        <v>15</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="F99" s="4" t="s">
+        <v>465</v>
+      </c>
+      <c r="G99" s="4" t="s">
+        <v>466</v>
+      </c>
+      <c r="H99" s="17" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="21" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Ineris-1</v>
+      </c>
+      <c r="B100" s="1">
         <v>1</v>
       </c>
-      <c r="C91" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D91" s="5" t="s">
+      <c r="C100" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="D100" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E91" s="5" t="s">
-        <v>371</v>
-      </c>
-      <c r="F91" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="G91" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="H91" s="4"/>
-    </row>
-    <row r="92" spans="1:8" ht="119.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DDT74-6</v>
-      </c>
-      <c r="B92" s="1">
-        <v>6</v>
-      </c>
-      <c r="C92" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D92" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="E92" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="F92" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="G92" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H92" s="4"/>
-    </row>
-    <row r="93" spans="1:8" ht="57.5" x14ac:dyDescent="0.35">
-      <c r="A93" s="4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DDT01-2</v>
-      </c>
-      <c r="B93" s="1">
-        <v>2</v>
-      </c>
-      <c r="C93" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D93" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E93" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="F93" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="G93" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="H93" s="4"/>
-    </row>
-    <row r="94" spans="1:8" ht="46" x14ac:dyDescent="0.35">
-      <c r="A94" s="4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DGPR/SRNH/SdCAP/BRNT-23</v>
-      </c>
-      <c r="B94" s="1">
-        <v>23</v>
-      </c>
-      <c r="C94" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D94" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E94" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="F94" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="G94" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="H94" s="4"/>
-    </row>
-    <row r="95" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>Cerema-20</v>
-      </c>
-      <c r="B95" s="1">
+      <c r="E100" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="F100" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="G100" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="H100" s="17" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="23" x14ac:dyDescent="0.35">
+      <c r="A101" s="21" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Ineris-17</v>
+      </c>
+      <c r="B101" s="1">
+        <v>17</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="G101" s="4" t="s">
+        <v>469</v>
+      </c>
+      <c r="H101" s="17" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A102" s="21" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Ineris-20</v>
+      </c>
+      <c r="B102" s="1">
         <v>20</v>
       </c>
-      <c r="C95" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="D95" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E95" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="F95" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="G95" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="H95" s="4"/>
-    </row>
-    <row r="96" spans="1:8" ht="23" x14ac:dyDescent="0.35">
-      <c r="A96" s="4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DDT38-25</v>
-      </c>
-      <c r="B96" s="7">
-        <v>25</v>
-      </c>
-      <c r="C96" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="D96" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="E96" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="F96" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="G96" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="H96" s="4"/>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A97" s="4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DDT38-26</v>
-      </c>
-      <c r="B97" s="7">
-        <v>26</v>
-      </c>
-      <c r="C97" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="D97" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="E97" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="F97" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="G97" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="H97" s="4"/>
-    </row>
-    <row r="98" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DDT07-1</v>
-      </c>
-      <c r="B98" s="1">
-        <v>1</v>
-      </c>
-      <c r="C98" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D98" s="5" t="s">
+      <c r="C102" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="D102" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E98" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F98" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G98" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H98" s="4"/>
-    </row>
-    <row r="99" spans="1:10" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DGPR/SRNH/SdcAP/BRIL-19</v>
-      </c>
-      <c r="B99" s="1">
-        <v>19</v>
-      </c>
-      <c r="C99" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D99" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E99" s="5" t="s">
-        <v>372</v>
-      </c>
-      <c r="F99" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G99" s="4"/>
-      <c r="H99" s="4"/>
-    </row>
-    <row r="100" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DGPR/SRNH/SdcAP/BRIL-20</v>
-      </c>
-      <c r="B100" s="1">
-        <v>20</v>
-      </c>
-      <c r="C100" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D100" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E100" s="5" t="s">
-        <v>373</v>
-      </c>
-      <c r="F100" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="G100" s="4"/>
-      <c r="H100" s="4"/>
-    </row>
-    <row r="101" spans="1:10" ht="34.5" x14ac:dyDescent="0.35">
-      <c r="A101" s="4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>Cerema-9</v>
-      </c>
-      <c r="B101" s="1">
-        <v>9</v>
-      </c>
-      <c r="C101" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="D101" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E101" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="F101" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="G101" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="H101" s="4"/>
-    </row>
-    <row r="102" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>Cerema-10</v>
-      </c>
-      <c r="B102" s="1">
-        <v>10</v>
-      </c>
-      <c r="C102" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="D102" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="E102" s="5" t="s">
-        <v>137</v>
+        <v>432</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>138</v>
+        <v>473</v>
       </c>
       <c r="G102" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="H102" s="4"/>
-    </row>
-    <row r="103" spans="1:10" ht="23" x14ac:dyDescent="0.35">
-      <c r="A103" s="4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DDT38-27</v>
-      </c>
-      <c r="B103" s="7">
-        <v>27</v>
+        <v>474</v>
+      </c>
+      <c r="H102" s="17" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A103" s="21" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Ineris-21</v>
+      </c>
+      <c r="B103" s="1">
+        <v>21</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>163</v>
+        <v>431</v>
       </c>
       <c r="D103" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="F103" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="G103" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="H103" s="4"/>
-    </row>
-    <row r="104" spans="1:10" ht="23" x14ac:dyDescent="0.35">
-      <c r="A104" s="4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DDT38-28</v>
-      </c>
-      <c r="B104" s="7">
-        <v>28</v>
+        <v>475</v>
+      </c>
+      <c r="F103" s="4" t="s">
+        <v>487</v>
+      </c>
+      <c r="G103" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="H103" s="20" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A104" s="21" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Ineris-18</v>
+      </c>
+      <c r="B104" s="1">
+        <v>18</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>163</v>
+        <v>431</v>
       </c>
       <c r="D104" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>232</v>
+        <v>470</v>
       </c>
       <c r="F104" s="4" t="s">
-        <v>233</v>
+        <v>471</v>
       </c>
       <c r="G104" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="H104" s="13"/>
-    </row>
-    <row r="105" spans="1:10" ht="23" x14ac:dyDescent="0.35">
-      <c r="A105" s="4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DDT38-29</v>
-      </c>
-      <c r="B105" s="7">
-        <v>29</v>
+        <v>472</v>
+      </c>
+      <c r="H104" s="13" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A105" s="21" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Ineris-25</v>
+      </c>
+      <c r="B105" s="1">
+        <v>25</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>163</v>
+        <v>431</v>
       </c>
       <c r="D105" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>235</v>
+        <v>481</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>236</v>
+        <v>482</v>
       </c>
       <c r="G105" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="H105" s="4"/>
-    </row>
-    <row r="106" spans="1:10" ht="34.5" x14ac:dyDescent="0.35">
-      <c r="A106" s="4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DDT74-10</v>
+        <v>483</v>
+      </c>
+      <c r="H105" s="17" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="23" x14ac:dyDescent="0.35">
+      <c r="A106" s="21" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Ineris-2</v>
       </c>
       <c r="B106" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>15</v>
+        <v>431</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E106" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="F106" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="G106" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="H106" s="17" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="23" x14ac:dyDescent="0.35">
+      <c r="A107" s="21" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Ineris-3</v>
+      </c>
+      <c r="B107" s="1">
+        <v>3</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E107" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="F107" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="G107" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="H107" s="17" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="23" x14ac:dyDescent="0.35">
+      <c r="A108" s="21" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Ineris-4</v>
+      </c>
+      <c r="B108" s="1">
+        <v>4</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="D108" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E108" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="F108" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="G108" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="H108" s="17" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+      <c r="A109" s="4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>DDT01-1</v>
+      </c>
+      <c r="B109" s="1">
+        <v>1</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D109" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E109" s="5" t="s">
         <v>370</v>
       </c>
-      <c r="F106" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G106" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H106" s="4"/>
-    </row>
-    <row r="107" spans="1:10" ht="34.5" x14ac:dyDescent="0.35">
-      <c r="A107" s="4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DDT74-11</v>
-      </c>
-      <c r="B107" s="1">
-        <v>11</v>
-      </c>
-      <c r="C107" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D107" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E107" s="5" t="s">
-        <v>370</v>
-      </c>
-      <c r="F107" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G107" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H107" s="4"/>
-    </row>
-    <row r="108" spans="1:10" ht="34.5" x14ac:dyDescent="0.35">
-      <c r="A108" s="4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DDT74-12</v>
-      </c>
-      <c r="B108" s="1">
-        <v>12</v>
-      </c>
-      <c r="C108" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D108" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E108" s="5" t="s">
-        <v>370</v>
-      </c>
-      <c r="F108" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G108" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H108" s="4"/>
-    </row>
-    <row r="109" spans="1:10" ht="23" x14ac:dyDescent="0.35">
-      <c r="A109" s="4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DGPR/SRNH/SdCAP/BRNT-25</v>
-      </c>
-      <c r="B109" s="1">
-        <v>25</v>
-      </c>
-      <c r="C109" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D109" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E109" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F109" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="G109" s="4"/>
-      <c r="H109" s="4"/>
-    </row>
-    <row r="110" spans="1:10" ht="34.5" x14ac:dyDescent="0.35">
-      <c r="A110" s="4" t="str">
-        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DDT74-13</v>
+      <c r="F109" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="G109" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="H109" s="6" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="23" x14ac:dyDescent="0.35">
+      <c r="A110" s="21" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Ineris-5</v>
       </c>
       <c r="B110" s="1">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>15</v>
+        <v>431</v>
       </c>
       <c r="D110" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E110" s="5">
+      <c r="E110" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="F110" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="G110" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="H110" s="17" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A111" s="21" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Ineris-6</v>
+      </c>
+      <c r="B111" s="1">
+        <v>6</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="D111" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E111" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="F111" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="G111" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="H111" s="17" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="23" x14ac:dyDescent="0.35">
+      <c r="A112" s="21" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Ineris-7</v>
+      </c>
+      <c r="B112" s="1">
+        <v>7</v>
+      </c>
+      <c r="C112" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="D112" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E112" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="F112" s="4" t="s">
+        <v>448</v>
+      </c>
+      <c r="G112" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="H112" s="17" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A113" s="21" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Ineris-8</v>
+      </c>
+      <c r="B113" s="1">
+        <v>8</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="D113" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E113" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="F113" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="G113" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="H113" s="17" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" ht="23" x14ac:dyDescent="0.35">
+      <c r="A114" s="21" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Ineris-9</v>
+      </c>
+      <c r="B114" s="1">
+        <v>9</v>
+      </c>
+      <c r="C114" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="D114" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E114" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="F114" s="4" t="s">
+        <v>448</v>
+      </c>
+      <c r="G114" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="H114" s="17" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="57.5" x14ac:dyDescent="0.35">
+      <c r="A115" s="21" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Ineris-10</v>
+      </c>
+      <c r="B115" s="1">
+        <v>10</v>
+      </c>
+      <c r="C115" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="D115" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E115" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="F115" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="G115" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="H115" s="20" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="23" x14ac:dyDescent="0.35">
+      <c r="A116" s="21" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Ineris-11</v>
+      </c>
+      <c r="B116" s="1">
+        <v>11</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="D116" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E116" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="F116" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="G116" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="H116" s="13" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A117" s="21" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Ineris-12</v>
+      </c>
+      <c r="B117" s="1">
+        <v>12</v>
+      </c>
+      <c r="C117" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="D117" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E117" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="F117" s="4" t="s">
+        <v>456</v>
+      </c>
+      <c r="G117" s="4" t="s">
+        <v>457</v>
+      </c>
+      <c r="H117" s="17" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A118" s="21" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Ineris-13</v>
+      </c>
+      <c r="B118" s="1">
+        <v>13</v>
+      </c>
+      <c r="C118" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="D118" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E118" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="F118" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="G118" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="H118" s="17" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="119.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A119" s="4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>DDT74-6</v>
+      </c>
+      <c r="B119" s="1">
+        <v>6</v>
+      </c>
+      <c r="C119" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D119" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="E119" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="F119" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="G119" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H119" s="20" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" ht="57.5" x14ac:dyDescent="0.35">
+      <c r="A120" s="4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>DDT01-2</v>
+      </c>
+      <c r="B120" s="1">
+        <v>2</v>
+      </c>
+      <c r="C120" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D120" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E120" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="F120" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="G120" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="H120" s="20" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+      <c r="A121" s="4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>DGPR/SRNH/SdCAP/BRNT-23</v>
+      </c>
+      <c r="B121" s="1">
+        <v>23</v>
+      </c>
+      <c r="C121" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D121" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E121" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="F121" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G121" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H121" s="20" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A122" s="4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Cerema-20</v>
+      </c>
+      <c r="B122" s="1">
+        <v>20</v>
+      </c>
+      <c r="C122" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D122" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E122" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="F122" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="G122" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="H122" s="20" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A123" s="4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>DDT38-25</v>
+      </c>
+      <c r="B123" s="7">
+        <v>25</v>
+      </c>
+      <c r="C123" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D123" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="E123" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="F123" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="G123" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="H123" s="20" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A124" s="4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>DDT38-26</v>
+      </c>
+      <c r="B124" s="7">
+        <v>26</v>
+      </c>
+      <c r="C124" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D124" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="E124" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="F124" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="G124" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="H124" s="20" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A125" s="4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>DDT07-1</v>
+      </c>
+      <c r="B125" s="1">
+        <v>1</v>
+      </c>
+      <c r="C125" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D125" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E125" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F125" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G125" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H125" s="20" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A126" s="4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>DGPR/SRNH/SdcAP/BRIL-19</v>
+      </c>
+      <c r="B126" s="1">
+        <v>19</v>
+      </c>
+      <c r="C126" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D126" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E126" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="F126" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G126" s="4"/>
+      <c r="H126" s="20" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A127" s="4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>DGPR/SRNH/SdcAP/BRIL-20</v>
+      </c>
+      <c r="B127" s="1">
+        <v>20</v>
+      </c>
+      <c r="C127" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D127" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E127" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="F127" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G127" s="4"/>
+      <c r="H127" s="20" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A128" s="4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Cerema-9</v>
+      </c>
+      <c r="B128" s="1">
+        <v>9</v>
+      </c>
+      <c r="C128" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D128" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E128" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="F128" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G128" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="H128" s="20" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A129" s="4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>Cerema-10</v>
+      </c>
+      <c r="B129" s="1">
+        <v>10</v>
+      </c>
+      <c r="C129" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D129" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E129" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F129" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G129" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="H129" s="20" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" ht="23" x14ac:dyDescent="0.35">
+      <c r="A130" s="4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>DDT38-27</v>
+      </c>
+      <c r="B130" s="7">
+        <v>27</v>
+      </c>
+      <c r="C130" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D130" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E130" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="F130" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="G130" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="H130" s="17" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" ht="23" x14ac:dyDescent="0.35">
+      <c r="A131" s="4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>DDT38-28</v>
+      </c>
+      <c r="B131" s="7">
+        <v>28</v>
+      </c>
+      <c r="C131" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D131" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E131" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="F131" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="G131" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="H131" s="17" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" ht="23" x14ac:dyDescent="0.35">
+      <c r="A132" s="4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>DDT38-29</v>
+      </c>
+      <c r="B132" s="7">
+        <v>29</v>
+      </c>
+      <c r="C132" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D132" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E132" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="F132" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="G132" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="H132" s="17" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A133" s="4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>DDT74-10</v>
+      </c>
+      <c r="B133" s="1">
+        <v>10</v>
+      </c>
+      <c r="C133" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D133" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E133" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="F133" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G133" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H133" s="13" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A134" s="4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>DDT74-11</v>
+      </c>
+      <c r="B134" s="1">
+        <v>11</v>
+      </c>
+      <c r="C134" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D134" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E134" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="F134" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G134" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H134" s="13" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" ht="69" x14ac:dyDescent="0.35">
+      <c r="A135" s="4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>DDT74-12</v>
+      </c>
+      <c r="B135" s="1">
+        <v>12</v>
+      </c>
+      <c r="C135" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D135" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E135" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="F135" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G135" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H135" s="20" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A136" s="4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>DGPR/SRNH/SdCAP/BRNT-25</v>
+      </c>
+      <c r="B136" s="1">
+        <v>25</v>
+      </c>
+      <c r="C136" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D136" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E136" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F136" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G136" s="4"/>
+      <c r="H136" s="13" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A137" s="4" t="str">
+        <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
+        <v>DDT74-13</v>
+      </c>
+      <c r="B137" s="1">
+        <v>13</v>
+      </c>
+      <c r="C137" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D137" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E137" s="5">
         <v>145</v>
       </c>
-      <c r="F110" s="4" t="s">
+      <c r="F137" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G110" s="4" t="s">
+      <c r="G137" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H110" s="4"/>
-    </row>
-    <row r="111" spans="1:10" ht="34.5" x14ac:dyDescent="0.35">
-      <c r="A111" s="4" t="str">
+      <c r="H137" s="17" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A138" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-7</v>
       </c>
-      <c r="B111" s="1">
+      <c r="B138" s="1">
         <v>7</v>
       </c>
-      <c r="C111" s="4" t="s">
+      <c r="C138" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D111" s="5" t="s">
+      <c r="D138" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E111" s="5" t="s">
-        <v>368</v>
-      </c>
-      <c r="F111" s="4" t="s">
+      <c r="E138" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="F138" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G111" s="4" t="s">
+      <c r="G138" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H111" s="4"/>
-      <c r="J111" s="22"/>
+      <c r="H138" s="13" t="s">
+        <v>538</v>
+      </c>
+      <c r="J138" s="19"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Ajout fichier de synthèse des commenntaires apres reunion pleniere
</commit_message>
<xml_diff>
--- a/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
+++ b/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gcebelieu\Desktop\2024-07-09 - Pleniere GT Risques\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD48AF64-D870-4098-9B05-51681B809D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF342CA5-01C3-40D2-B751-35F1A69144CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28620" yWindow="90" windowWidth="27960" windowHeight="15015" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Synthese Modele Commun" sheetId="3" r:id="rId1"/>
@@ -1237,18 +1237,6 @@
     <t>OK (référence COVADIS 1:2000 pour zonages sur plan cadastral)</t>
   </si>
   <si>
-    <t xml:space="preserve">NOK ?
-Cette référence est citée dans le standard PPR
-Les références aux Guides PPR dans le modèle commun sont essentiellement dues aux défintiions.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOK ?
-Pour éviter le doublon avec le standard PPR où cela est écrit
-La partie TRI est écrite ici car le profil TRI n'existe pas encore. Quand il le sera, La partie réglementaire le concernant sera mentionnée dans ce document
-</t>
-  </si>
-  <si>
     <t>OK, à corriger</t>
   </si>
   <si>
@@ -1262,11 +1250,6 @@
 Cette différenciation est plutôt à envisager dans le profil PPR</t>
   </si>
   <si>
-    <t>OK sur le principe. Proposition de synthèse
-"Ce type de procédure couvre les risques naturels liés à la submersion marine, notamment la migration dunaire et pour les PPRL anciens, l’aléa recul du trait de côte et de falaises."
-Question : désormais dans quelle procédure est traitée le recul du trait de côte et de falaises ?</t>
-  </si>
-  <si>
     <t>OK sur le principe cf. après</t>
   </si>
   <si>
@@ -1276,10 +1259,6 @@
     <t>OK, sur le principe. Proposition de synthèse :
 Proposition d’ajouter « Règlement non approuvé » : le document est un règlement qui n’a pas fait l’objet d’une approbation (utilisation dans le cadre d’un PPR ou d’un PAC), et 
 « Zonage réglementaire non approuvé » : le document est un zonage réglementaire qui n’a pas fait l’objet d’une approbation (utilisation dans le cadre d’un PPR ou d’un PAC)</t>
-  </si>
-  <si>
-    <t>NOK ?
-La liste des procédures listées dans le modèle commun est celle des procédures qui font l'objet des Geostandards risques. Les études de danger ne font pas partie du périmètre des Géostandards (même si on représente des éléments qui en sont issus) de ce point de vue..</t>
   </si>
   <si>
     <t xml:space="preserve">OK, pour parler de niveau d'aléa au lieu d'intensité
@@ -1291,11 +1270,6 @@
     <t>C'est le cas. Il n'y a pas de règles de topologie spécifique sur ce point dans le standard.</t>
   </si>
   <si>
-    <t>OK, à corriger.
-Cela remet-il en cause la typologie des ouvrages de protection (barrage et digues) ?
-Une référence à la documentation de SIOUH II serait la bienvenue aussi</t>
-  </si>
-  <si>
     <t>OK. Formulation à trouver</t>
   </si>
   <si>
@@ -1331,9 +1305,6 @@
     <t>p22</t>
   </si>
   <si>
-    <t>Non, à moins qu'il n'y ait une volonté de les transformer en PPR ?</t>
-  </si>
-  <si>
     <t>Cf. montage  actions en cours (projet sweet pepper, accompagnement IGN)</t>
   </si>
   <si>
@@ -1367,21 +1338,6 @@
   </si>
   <si>
     <t>OK, à supprimer</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">OK, référence à rajouter
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(NB : à vérifier si des éléements du standard sont impactés par cette nouvelle référence) ?</t>
-    </r>
   </si>
   <si>
     <t>NOK
@@ -1882,10 +1838,6 @@
 Etant entendu que codeprocedure respecte la nomenclature hors préfixe éventuel ?</t>
   </si>
   <si>
-    <t>OK sur le principe. 
-A valdier en GT</t>
-  </si>
-  <si>
     <t>OK
 à corriger</t>
   </si>
@@ -1948,10 +1900,6 @@
 Peut-on précisier un cas de PPR où nul s'applique et pas très faible ? Ou inversement ?</t>
   </si>
   <si>
-    <t>C'est le cas dans le profil PPR sauf quon ne fait pas la distinction entre les deux types de bandes particulières.
-Le faut-il ?</t>
-  </si>
-  <si>
     <t>NOK ?
 Le code 07 s'applique à des zones reglementées du fait de l'aléa exceptionnel (une réglementation particulière) qu'il est demandé de réprésenter au niveau du zonége reglementaire.
 Le code 08 représente le niveau d'aléa avalanche exceptionnel pour qualifier la zone d'aléa (et peut-être remis en cause éventuellement). 
@@ -1963,11 +1911,6 @@
 Ne risque-t-on pas de rajouter une complexité (géométries) supplémentaire à la couche du zonage réglementaire ?
 Faut-il rapprocher cette remaque de DDT74-14 ?
 </t>
-  </si>
-  <si>
-    <t>OK sur le principe.
-Ce nommage est-il cohérent avec SIOUH2 ? (les anciens libéllés viennent de SIOUH)
-Peut-on rajouter d'autres types d'ouvrages (hors inondation, pour les avalanches par exemple) ?</t>
   </si>
   <si>
     <t>OK sur le principe.
@@ -2092,6 +2035,68 @@
   </si>
   <si>
     <t>OK cf. précédent (1:2000 du coup)</t>
+  </si>
+  <si>
+    <t>OK sur le principe. Proposition de synthèse
+"Ce type de procédure couvre les risques naturels liés à la submersion marine, à la migration dunaire. Certains PPRL anciens traitent de l’aléa recul du trait de côte et de falaises."
+Question : désormais dans quelle procédure est traitée le recul du trait de côte et de falaises ? NB : Procédures d'aménagement portées par les collectivités (dans le cadre des PLU)</t>
+  </si>
+  <si>
+    <t>NOK
+La liste des procédures listées dans le modèle commun est celle des procédures qui font l'objet des Geostandards risques. Les études de danger ne font pas partie du périmètre des Géostandards (même si on représente des éléments qui en sont issus) de ce point de vue..</t>
+  </si>
+  <si>
+    <t>C'est le cas dans le profil PPR sauf quon ne fait pas la distinction entre les deux types de bandes particulières.
+Le faut-il ?
+Proposition Bande particulière + 2 types de bandes particulières</t>
+  </si>
+  <si>
+    <t>OK sur le principe.
+Ce nommage est-il cohérent avec SIOUH2 ? (les anciens libéllés viennent de SIOUH)
+Peut-on rajouter d'autres types d'ouvrages (hors inondation, pour les avalanches par exemple) ?
+- Proposition BRIL (en cours): ouvrages de protection (inondations)" décomposé en AH et SE, et "Autres ouvrages faisant obstacle aux écoulements". A valider avec PONSOH</t>
+  </si>
+  <si>
+    <t>OK, à corriger.
+Cela remet-il en cause la typologie des ouvrages de protection (barrage et digues) ? =&gt; cf. commentaires PPR
+Une référence à la documentation de SIOUH II serait la bienvenue aussi</t>
+  </si>
+  <si>
+    <t>Non, à moins qu'il n'y ait une volonté de les transformer en PPR (cf. Sweet pepper)?
+NB : certains champs obligatoires non renseignés dans PSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK sur le principe. 
+A valdier en GT 
+NB : A vérifier avec le DAGSI (rendre obligatoire les aléas à partir d'une certaine date) ?
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOK
+Cette référence est citée dans le standard PPR
+Les références aux Guides PPR dans le modèle commun sont essentiellement dues aux défintiions.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOK
+Pour éviter le doublon avec le standard PPR où cela est écrit
+La partie TRI est écrite ici car le profil TRI n'existe pas encore. Quand il le sera, La partie réglementaire le concernant sera mentionnée dans ce document
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">OK, référence à rajouter
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(NB : à vérifier si des éléments du standard sont impactés par cette nouvelle référence) ?</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2187,17 +2192,22 @@
     </font>
     <font>
       <sz val="9"/>
-      <color theme="5"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -2224,7 +2234,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2291,6 +2301,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -3053,21 +3064,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939F5930-30D3-43D0-87E8-B00574FE9CE2}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView topLeftCell="D10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.54296875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="14.36328125" style="3" customWidth="1"/>
     <col min="2" max="2" width="11.1796875" style="3" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="21.90625" style="3" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="13.81640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="18.1796875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="63.36328125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="64.36328125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="12" style="3" customWidth="1"/>
+    <col min="5" max="5" width="16.08984375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="49.54296875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="47.6328125" style="3" customWidth="1"/>
     <col min="8" max="8" width="54.81640625" style="3" customWidth="1"/>
     <col min="9" max="16384" width="10.90625" style="3"/>
   </cols>
@@ -3125,7 +3136,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="92" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-2</v>
@@ -3149,10 +3160,10 @@
         <v>332</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="92" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-3</v>
@@ -3176,7 +3187,7 @@
         <v>333</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="75.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3203,7 +3214,7 @@
         <v>305</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>353</v>
+        <v>538</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="89" customHeight="1" x14ac:dyDescent="0.35">
@@ -3255,10 +3266,10 @@
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="18" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="69" x14ac:dyDescent="0.35">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-6</v>
@@ -3281,11 +3292,11 @@
       <c r="G8" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="H8" s="23" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
+      <c r="H8" s="17" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="92" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-7</v>
@@ -3308,8 +3319,8 @@
       <c r="G9" s="13" t="s">
         <v>335</v>
       </c>
-      <c r="H9" s="23" t="s">
-        <v>356</v>
+      <c r="H9" s="17" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3335,8 +3346,8 @@
       <c r="G10" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="H10" s="23" t="s">
-        <v>358</v>
+      <c r="H10" s="17" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -3362,11 +3373,11 @@
       <c r="G11" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="H11" s="23" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="92" x14ac:dyDescent="0.35">
+      <c r="H11" s="17" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="103.5" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-8</v>
@@ -3389,8 +3400,8 @@
       <c r="G12" s="9" t="s">
         <v>315</v>
       </c>
-      <c r="H12" s="23" t="s">
-        <v>357</v>
+      <c r="H12" s="17" t="s">
+        <v>530</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3416,8 +3427,8 @@
       <c r="G13" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="H13" s="23" t="s">
-        <v>359</v>
+      <c r="H13" s="17" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="92" x14ac:dyDescent="0.35">
@@ -3443,8 +3454,8 @@
       <c r="G14" s="9" t="s">
         <v>336</v>
       </c>
-      <c r="H14" s="23" t="s">
-        <v>360</v>
+      <c r="H14" s="17" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="61" customHeight="1" x14ac:dyDescent="0.35">
@@ -3471,10 +3482,10 @@
         <v>320</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="57.5" x14ac:dyDescent="0.35">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="68" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-3</v>
@@ -3498,10 +3509,10 @@
         <v>288</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="77" customHeight="1" x14ac:dyDescent="0.35">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="77" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-4</v>
@@ -3525,10 +3536,10 @@
         <v>291</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="92" x14ac:dyDescent="0.35">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="111" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-5</v>
@@ -3551,11 +3562,11 @@
       <c r="G18" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="H18" s="23" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+      <c r="H18" s="17" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SDCAP/PONSOH-13</v>
@@ -3578,11 +3589,12 @@
       <c r="G19" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="H19" s="23" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H19" s="9" t="s">
+        <v>534</v>
+      </c>
+      <c r="I19" s="24"/>
+    </row>
+    <row r="20" spans="1:9" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/DAPP/BIP-12</v>
@@ -3604,7 +3616,7 @@
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="17" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -3620,8 +3632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815F14A-19BC-4DCE-8D31-81F595A4B0E7}">
   <dimension ref="A1:J138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3630,14 +3642,14 @@
     <col min="2" max="2" width="3.81640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="9.1796875" style="3" customWidth="1"/>
     <col min="4" max="4" width="16" style="3" customWidth="1"/>
-    <col min="5" max="5" width="20.6328125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="55.54296875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="50.36328125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.36328125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="44.08984375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="38" style="3" customWidth="1"/>
     <col min="8" max="8" width="51.81640625" style="3" customWidth="1"/>
     <col min="9" max="16384" width="10.90625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>348</v>
       </c>
@@ -3663,7 +3675,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-2</v>
@@ -3684,11 +3696,12 @@
         <v>242</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="20" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H2" s="9" t="s">
+        <v>535</v>
+      </c>
+      <c r="I2" s="24"/>
+    </row>
+    <row r="3" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-3</v>
@@ -3709,11 +3722,11 @@
         <v>243</v>
       </c>
       <c r="G3" s="4"/>
-      <c r="H3" s="20" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H3" s="9" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-4</v>
@@ -3734,11 +3747,11 @@
         <v>244</v>
       </c>
       <c r="G4" s="9"/>
-      <c r="H4" s="20" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="51.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H4" s="9" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-5</v>
@@ -3759,11 +3772,11 @@
         <v>245</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="20" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="103.5" x14ac:dyDescent="0.35">
+      <c r="H5" s="9" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="118.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP-0</v>
@@ -3783,10 +3796,10 @@
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="17" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-9</v>
@@ -3808,10 +3821,10 @@
         <v>35</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-14</v>
@@ -3833,10 +3846,10 @@
         <v>45</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="23" x14ac:dyDescent="0.35">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-15</v>
@@ -3858,10 +3871,10 @@
         <v>47</v>
       </c>
       <c r="H9" s="20" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="65" customHeight="1" x14ac:dyDescent="0.35">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="74" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-2</v>
@@ -3885,10 +3898,10 @@
         <v>263</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-3</v>
@@ -3912,10 +3925,10 @@
         <v>172</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="60.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="60.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-1</v>
@@ -3942,7 +3955,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-1</v>
@@ -3966,10 +3979,10 @@
         <v>166</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="138" x14ac:dyDescent="0.35">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="161" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-2</v>
@@ -3993,10 +4006,10 @@
         <v>254</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-3</v>
@@ -4020,10 +4033,10 @@
         <v>62</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-1</v>
@@ -4047,10 +4060,10 @@
         <v>117</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-4</v>
@@ -4074,10 +4087,10 @@
         <v>65</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-4</v>
@@ -4101,7 +4114,7 @@
         <v>175</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
@@ -4128,10 +4141,10 @@
         <v>255</v>
       </c>
       <c r="H19" s="20" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-6</v>
@@ -4155,7 +4168,7 @@
         <v>256</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4182,7 +4195,7 @@
         <v>120</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
@@ -4209,10 +4222,10 @@
         <v>122</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-5</v>
@@ -4236,7 +4249,7 @@
         <v>178</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="46" x14ac:dyDescent="0.35">
@@ -4263,7 +4276,7 @@
         <v>260</v>
       </c>
       <c r="H24" s="20" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="23" x14ac:dyDescent="0.35">
@@ -4290,7 +4303,7 @@
         <v>125</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4317,10 +4330,10 @@
         <v>72</v>
       </c>
       <c r="H26" s="17" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="25" x14ac:dyDescent="0.35">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-6</v>
@@ -4344,10 +4357,10 @@
         <v>264</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-</v>
@@ -4360,7 +4373,7 @@
         <v>16</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>339</v>
@@ -4369,7 +4382,7 @@
         <v>340</v>
       </c>
       <c r="H28" s="20" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="I28" s="19"/>
     </row>
@@ -4397,7 +4410,7 @@
         <v>75</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4424,10 +4437,10 @@
         <v>78</v>
       </c>
       <c r="H30" s="20" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-6</v>
@@ -4451,10 +4464,10 @@
         <v>128</v>
       </c>
       <c r="H31" s="20" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-7</v>
@@ -4478,7 +4491,7 @@
         <v>130</v>
       </c>
       <c r="H32" s="20" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.35">
@@ -4503,7 +4516,7 @@
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="17" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="57.5" x14ac:dyDescent="0.35">
@@ -4530,7 +4543,7 @@
         <v>184</v>
       </c>
       <c r="H34" s="20" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4555,7 +4568,7 @@
         <v>82</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
@@ -4582,10 +4595,10 @@
         <v>19</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-21</v>
@@ -4609,10 +4622,10 @@
         <v>99</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="92" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-</v>
@@ -4625,19 +4638,19 @@
         <v>16</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>338</v>
       </c>
       <c r="H38" s="20" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="161" x14ac:dyDescent="0.35">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="207" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-</v>
@@ -4650,19 +4663,19 @@
         <v>16</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>338</v>
       </c>
       <c r="H39" s="20" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="69" x14ac:dyDescent="0.35">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-8</v>
@@ -4686,7 +4699,7 @@
         <v>267</v>
       </c>
       <c r="H40" s="20" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.35">
@@ -4713,7 +4726,7 @@
         <v>133</v>
       </c>
       <c r="H41" s="20" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4738,10 +4751,10 @@
       </c>
       <c r="G42" s="4"/>
       <c r="H42" s="20" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="92" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-4</v>
@@ -4765,7 +4778,7 @@
         <v>26</v>
       </c>
       <c r="H43" s="13" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.35">
@@ -4792,7 +4805,7 @@
         <v>22</v>
       </c>
       <c r="H44" s="20" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
@@ -4817,10 +4830,10 @@
       </c>
       <c r="G45" s="4"/>
       <c r="H45" s="20" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="46" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-8</v>
@@ -4835,7 +4848,7 @@
         <v>16</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>32</v>
@@ -4844,7 +4857,7 @@
         <v>33</v>
       </c>
       <c r="H46" s="20" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4862,7 +4875,7 @@
         <v>16</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>105</v>
@@ -4871,7 +4884,7 @@
         <v>106</v>
       </c>
       <c r="H47" s="20" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4898,7 +4911,7 @@
         <v>25</v>
       </c>
       <c r="H48" s="17" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="58" customHeight="1" x14ac:dyDescent="0.35">
@@ -4924,11 +4937,11 @@
       <c r="G49" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H49" s="20" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="57.5" x14ac:dyDescent="0.35">
+      <c r="H49" s="13" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="69" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT07-2</v>
@@ -4952,7 +4965,7 @@
         <v>14</v>
       </c>
       <c r="H50" s="13" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
@@ -4979,7 +4992,7 @@
         <v>142</v>
       </c>
       <c r="H51" s="17" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
@@ -5006,10 +5019,10 @@
         <v>143</v>
       </c>
       <c r="H52" s="17" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="23" x14ac:dyDescent="0.35">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-13</v>
@@ -5033,7 +5046,7 @@
         <v>145</v>
       </c>
       <c r="H53" s="20" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="36.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5058,7 +5071,7 @@
         <v>87</v>
       </c>
       <c r="H54" s="20" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.35">
@@ -5083,7 +5096,7 @@
         <v>86</v>
       </c>
       <c r="H55" s="17" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="57.5" x14ac:dyDescent="0.35">
@@ -5108,10 +5121,10 @@
       </c>
       <c r="G56" s="4"/>
       <c r="H56" s="13" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="46" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-9</v>
@@ -5135,10 +5148,10 @@
         <v>187</v>
       </c>
       <c r="H57" s="17" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="149.5" x14ac:dyDescent="0.35">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="184" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5158,7 +5171,7 @@
       </c>
       <c r="G58" s="4"/>
       <c r="H58" s="20" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="46" x14ac:dyDescent="0.35">
@@ -5185,10 +5198,10 @@
         <v>148</v>
       </c>
       <c r="H59" s="20" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="69" x14ac:dyDescent="0.35">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="92" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5208,10 +5221,10 @@
       </c>
       <c r="G60" s="4"/>
       <c r="H60" s="20" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="184" x14ac:dyDescent="0.35">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="230" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5231,10 +5244,10 @@
       </c>
       <c r="G61" s="4"/>
       <c r="H61" s="13" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="69" x14ac:dyDescent="0.35">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A62" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-15</v>
@@ -5258,7 +5271,7 @@
         <v>151</v>
       </c>
       <c r="H62" s="20" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="46" x14ac:dyDescent="0.35">
@@ -5281,7 +5294,7 @@
       </c>
       <c r="G63" s="4"/>
       <c r="H63" s="13" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="46" x14ac:dyDescent="0.35">
@@ -5308,7 +5321,7 @@
         <v>154</v>
       </c>
       <c r="H64" s="20" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="46" x14ac:dyDescent="0.35">
@@ -5326,7 +5339,7 @@
         <v>11</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="F65" s="4" t="s">
         <v>49</v>
@@ -5335,7 +5348,7 @@
         <v>50</v>
       </c>
       <c r="H65" s="13" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="46" x14ac:dyDescent="0.35">
@@ -5353,7 +5366,7 @@
         <v>7</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="F66" s="4" t="s">
         <v>52</v>
@@ -5362,10 +5375,10 @@
         <v>53</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="145" x14ac:dyDescent="0.35">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="174" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-10</v>
@@ -5389,7 +5402,7 @@
         <v>270</v>
       </c>
       <c r="H67" s="20" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="88" customHeight="1" x14ac:dyDescent="0.35">
@@ -5416,7 +5429,7 @@
         <v>241</v>
       </c>
       <c r="H68" s="20" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="103" customHeight="1" x14ac:dyDescent="0.35">
@@ -5443,10 +5456,10 @@
         <v>271</v>
       </c>
       <c r="H69" s="20" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-12</v>
@@ -5470,7 +5483,7 @@
         <v>272</v>
       </c>
       <c r="H70" s="20" t="s">
-        <v>495</v>
+        <v>536</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.35">
@@ -5497,7 +5510,7 @@
         <v>197</v>
       </c>
       <c r="H71" s="17" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
@@ -5509,22 +5522,22 @@
         <v>14</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="H72" s="20" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.35">
@@ -5536,22 +5549,22 @@
         <v>19</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="H73" s="17" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.35">
@@ -5563,22 +5576,22 @@
         <v>16</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="H74" s="17" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.35">
@@ -5605,7 +5618,7 @@
         <v>273</v>
       </c>
       <c r="H75" s="20" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="115" customHeight="1" x14ac:dyDescent="0.35">
@@ -5632,7 +5645,7 @@
         <v>275</v>
       </c>
       <c r="H76" s="20" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
@@ -5659,7 +5672,7 @@
         <v>203</v>
       </c>
       <c r="H77" s="20" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
@@ -5671,25 +5684,25 @@
         <v>22</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>488</v>
+        <v>481</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="H78" s="20" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="26" x14ac:dyDescent="0.35">
       <c r="A79" s="21" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-23</v>
@@ -5698,25 +5711,25 @@
         <v>23</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>489</v>
+        <v>482</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="H79" s="17" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="26" x14ac:dyDescent="0.35">
       <c r="A80" s="21" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-24</v>
@@ -5725,22 +5738,22 @@
         <v>24</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
       <c r="F80" s="4" t="s">
+        <v>483</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="H80" s="17" t="s">
         <v>490</v>
-      </c>
-      <c r="G80" s="4" t="s">
-        <v>480</v>
-      </c>
-      <c r="H80" s="17" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="46" x14ac:dyDescent="0.35">
@@ -5767,7 +5780,7 @@
         <v>206</v>
       </c>
       <c r="H81" s="20" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
@@ -5794,10 +5807,10 @@
         <v>209</v>
       </c>
       <c r="H82" s="20" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" ht="57.5" x14ac:dyDescent="0.35">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="69" x14ac:dyDescent="0.35">
       <c r="A83" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-19</v>
@@ -5821,7 +5834,7 @@
         <v>211</v>
       </c>
       <c r="H83" s="20" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="23" x14ac:dyDescent="0.35">
@@ -5848,7 +5861,7 @@
         <v>213</v>
       </c>
       <c r="H84" s="17" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="36.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5860,22 +5873,22 @@
         <v>27</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D85" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E85" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="F85" s="4" t="s">
         <v>485</v>
       </c>
-      <c r="F85" s="4" t="s">
-        <v>492</v>
-      </c>
       <c r="G85" s="4" t="s">
-        <v>486</v>
+        <v>479</v>
       </c>
       <c r="H85" s="20" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
@@ -5902,7 +5915,7 @@
         <v>216</v>
       </c>
       <c r="H86" s="20" t="s">
-        <v>506</v>
+        <v>498</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5914,22 +5927,22 @@
         <v>26</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E87" s="5" t="s">
+        <v>477</v>
+      </c>
+      <c r="F87" s="4" t="s">
         <v>484</v>
       </c>
-      <c r="F87" s="4" t="s">
-        <v>491</v>
-      </c>
       <c r="G87" s="4" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="H87" s="20" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.35">
@@ -5956,7 +5969,7 @@
         <v>157</v>
       </c>
       <c r="H88" s="17" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
@@ -5981,7 +5994,7 @@
         <v>91</v>
       </c>
       <c r="H89" s="17" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6006,7 +6019,7 @@
       </c>
       <c r="G90" s="4"/>
       <c r="H90" s="13" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
@@ -6033,7 +6046,7 @@
         <v>218</v>
       </c>
       <c r="H91" s="20" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
@@ -6060,7 +6073,7 @@
         <v>278</v>
       </c>
       <c r="H92" s="13" t="s">
-        <v>511</v>
+        <v>502</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
@@ -6087,10 +6100,10 @@
         <v>279</v>
       </c>
       <c r="H93" s="22" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.35">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="113" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/PoNSOH-26</v>
@@ -6113,8 +6126,8 @@
       <c r="G94" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="H94" s="20" t="s">
-        <v>513</v>
+      <c r="H94" s="9" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6141,7 +6154,7 @@
         <v>113</v>
       </c>
       <c r="H95" s="20" t="s">
-        <v>514</v>
+        <v>504</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.35">
@@ -6168,7 +6181,7 @@
         <v>143</v>
       </c>
       <c r="H96" s="17" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.35">
@@ -6195,7 +6208,7 @@
         <v>143</v>
       </c>
       <c r="H97" s="17" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="96.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6220,10 +6233,10 @@
       </c>
       <c r="G98" s="4"/>
       <c r="H98" s="20" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="23" x14ac:dyDescent="0.35">
       <c r="A99" s="21" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-15</v>
@@ -6232,22 +6245,22 @@
         <v>15</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D99" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="G99" s="4" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="H99" s="17" t="s">
-        <v>517</v>
+        <v>507</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6259,22 +6272,22 @@
         <v>1</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D100" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="G100" s="4" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="H100" s="17" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="23" x14ac:dyDescent="0.35">
@@ -6286,25 +6299,25 @@
         <v>17</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D101" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="G101" s="4" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="H101" s="17" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="23" x14ac:dyDescent="0.35">
       <c r="A102" s="21" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-20</v>
@@ -6313,25 +6326,25 @@
         <v>20</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D102" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="G102" s="4" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="H102" s="17" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A103" s="21" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-21</v>
@@ -6340,22 +6353,22 @@
         <v>21</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D103" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="F103" s="4" t="s">
-        <v>487</v>
+        <v>480</v>
       </c>
       <c r="G103" s="4" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="H103" s="20" t="s">
-        <v>518</v>
+        <v>508</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
@@ -6367,22 +6380,22 @@
         <v>18</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D104" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="F104" s="4" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="G104" s="4" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="H104" s="13" t="s">
-        <v>519</v>
+        <v>509</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
@@ -6394,22 +6407,22 @@
         <v>25</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D105" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
       <c r="G105" s="4" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
       <c r="H105" s="17" t="s">
-        <v>517</v>
+        <v>507</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="23" x14ac:dyDescent="0.35">
@@ -6421,22 +6434,22 @@
         <v>2</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D106" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="G106" s="4" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="H106" s="17" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="23" x14ac:dyDescent="0.35">
@@ -6448,22 +6461,22 @@
         <v>3</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D107" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="G107" s="4" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="H107" s="17" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="23" x14ac:dyDescent="0.35">
@@ -6475,22 +6488,22 @@
         <v>4</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D108" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="F108" s="4" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="G108" s="4" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="H108" s="17" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="46" x14ac:dyDescent="0.35">
@@ -6508,7 +6521,7 @@
         <v>23</v>
       </c>
       <c r="E109" s="5" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="F109" s="6" t="s">
         <v>249</v>
@@ -6517,7 +6530,7 @@
         <v>250</v>
       </c>
       <c r="H109" s="6" t="s">
-        <v>516</v>
+        <v>506</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="23" x14ac:dyDescent="0.35">
@@ -6529,25 +6542,25 @@
         <v>5</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D110" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="F110" s="4" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="G110" s="4" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="H110" s="17" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="23" x14ac:dyDescent="0.35">
       <c r="A111" s="21" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-6</v>
@@ -6556,25 +6569,25 @@
         <v>6</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D111" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E111" s="5" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="F111" s="4" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="G111" s="4" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="H111" s="17" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" ht="23" x14ac:dyDescent="0.35">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A112" s="21" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-7</v>
@@ -6583,25 +6596,25 @@
         <v>7</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D112" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="F112" s="4" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="G112" s="4" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="H112" s="17" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="23" x14ac:dyDescent="0.35">
       <c r="A113" s="21" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-8</v>
@@ -6610,25 +6623,25 @@
         <v>8</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D113" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="F113" s="4" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="G113" s="4" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="H113" s="17" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" ht="23" x14ac:dyDescent="0.35">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A114" s="21" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-9</v>
@@ -6637,25 +6650,25 @@
         <v>9</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D114" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="F114" s="4" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="G114" s="4" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="H114" s="17" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" ht="57.5" x14ac:dyDescent="0.35">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="69" x14ac:dyDescent="0.35">
       <c r="A115" s="21" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-10</v>
@@ -6664,22 +6677,22 @@
         <v>10</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D115" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="G115" s="4" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="H115" s="20" t="s">
-        <v>520</v>
+        <v>510</v>
       </c>
     </row>
     <row r="116" spans="1:8" ht="23" x14ac:dyDescent="0.35">
@@ -6691,22 +6704,22 @@
         <v>11</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D116" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="F116" s="4" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="G116" s="4" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="H116" s="13" t="s">
-        <v>521</v>
+        <v>511</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.35">
@@ -6718,25 +6731,25 @@
         <v>12</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D117" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="F117" s="4" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="G117" s="4" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="H117" s="17" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" ht="23" x14ac:dyDescent="0.35">
       <c r="A118" s="21" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-13</v>
@@ -6745,22 +6758,22 @@
         <v>13</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D118" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="F118" s="4" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="G118" s="4" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="H118" s="17" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="119" spans="1:8" ht="119.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6778,7 +6791,7 @@
         <v>247</v>
       </c>
       <c r="E119" s="5" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="F119" s="4" t="s">
         <v>248</v>
@@ -6787,7 +6800,7 @@
         <v>29</v>
       </c>
       <c r="H119" s="20" t="s">
-        <v>522</v>
+        <v>512</v>
       </c>
     </row>
     <row r="120" spans="1:8" ht="57.5" x14ac:dyDescent="0.35">
@@ -6805,7 +6818,7 @@
         <v>11</v>
       </c>
       <c r="E120" s="5" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="F120" s="4" t="s">
         <v>251</v>
@@ -6814,10 +6827,10 @@
         <v>252</v>
       </c>
       <c r="H120" s="20" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A121" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-23</v>
@@ -6832,7 +6845,7 @@
         <v>16</v>
       </c>
       <c r="E121" s="5" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="F121" s="4" t="s">
         <v>103</v>
@@ -6841,7 +6854,7 @@
         <v>104</v>
       </c>
       <c r="H121" s="20" t="s">
-        <v>523</v>
+        <v>513</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
@@ -6868,7 +6881,7 @@
         <v>162</v>
       </c>
       <c r="H122" s="20" t="s">
-        <v>525</v>
+        <v>515</v>
       </c>
     </row>
     <row r="123" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
@@ -6895,7 +6908,7 @@
         <v>225</v>
       </c>
       <c r="H123" s="20" t="s">
-        <v>524</v>
+        <v>514</v>
       </c>
     </row>
     <row r="124" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
@@ -6922,7 +6935,7 @@
         <v>228</v>
       </c>
       <c r="H124" s="20" t="s">
-        <v>526</v>
+        <v>516</v>
       </c>
     </row>
     <row r="125" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.35">
@@ -6949,7 +6962,7 @@
         <v>10</v>
       </c>
       <c r="H125" s="20" t="s">
-        <v>527</v>
+        <v>517</v>
       </c>
     </row>
     <row r="126" spans="1:8" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6967,14 +6980,14 @@
         <v>16</v>
       </c>
       <c r="E126" s="5" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="F126" s="4" t="s">
         <v>94</v>
       </c>
       <c r="G126" s="4"/>
       <c r="H126" s="20" t="s">
-        <v>528</v>
+        <v>518</v>
       </c>
     </row>
     <row r="127" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
@@ -6992,17 +7005,17 @@
         <v>16</v>
       </c>
       <c r="E127" s="5" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="F127" s="4" t="s">
         <v>95</v>
       </c>
       <c r="G127" s="4"/>
       <c r="H127" s="20" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" ht="46" x14ac:dyDescent="0.35">
       <c r="A128" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-9</v>
@@ -7026,7 +7039,7 @@
         <v>136</v>
       </c>
       <c r="H128" s="20" t="s">
-        <v>530</v>
+        <v>520</v>
       </c>
     </row>
     <row r="129" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7053,7 +7066,7 @@
         <v>139</v>
       </c>
       <c r="H129" s="20" t="s">
-        <v>531</v>
+        <v>521</v>
       </c>
     </row>
     <row r="130" spans="1:10" ht="23" x14ac:dyDescent="0.35">
@@ -7080,7 +7093,7 @@
         <v>231</v>
       </c>
       <c r="H130" s="17" t="s">
-        <v>532</v>
+        <v>522</v>
       </c>
     </row>
     <row r="131" spans="1:10" ht="23" x14ac:dyDescent="0.35">
@@ -7107,7 +7120,7 @@
         <v>234</v>
       </c>
       <c r="H131" s="17" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="132" spans="1:10" ht="23" x14ac:dyDescent="0.35">
@@ -7134,7 +7147,7 @@
         <v>237</v>
       </c>
       <c r="H132" s="17" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="133" spans="1:10" ht="34.5" x14ac:dyDescent="0.35">
@@ -7152,7 +7165,7 @@
         <v>16</v>
       </c>
       <c r="E133" s="5" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="F133" s="4" t="s">
         <v>36</v>
@@ -7161,10 +7174,10 @@
         <v>37</v>
       </c>
       <c r="H133" s="13" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="134" spans="1:10" ht="34.5" x14ac:dyDescent="0.35">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" ht="46" x14ac:dyDescent="0.35">
       <c r="A134" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-11</v>
@@ -7179,7 +7192,7 @@
         <v>16</v>
       </c>
       <c r="E134" s="5" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="F134" s="4" t="s">
         <v>38</v>
@@ -7188,7 +7201,7 @@
         <v>39</v>
       </c>
       <c r="H134" s="13" t="s">
-        <v>534</v>
+        <v>524</v>
       </c>
     </row>
     <row r="135" spans="1:10" ht="69" x14ac:dyDescent="0.35">
@@ -7206,7 +7219,7 @@
         <v>16</v>
       </c>
       <c r="E135" s="5" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="F135" s="4" t="s">
         <v>40</v>
@@ -7215,7 +7228,7 @@
         <v>41</v>
       </c>
       <c r="H135" s="20" t="s">
-        <v>535</v>
+        <v>525</v>
       </c>
     </row>
     <row r="136" spans="1:10" ht="44" customHeight="1" x14ac:dyDescent="0.35">
@@ -7240,10 +7253,10 @@
       </c>
       <c r="G136" s="4"/>
       <c r="H136" s="13" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="137" spans="1:10" ht="34.5" x14ac:dyDescent="0.35">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" ht="46" x14ac:dyDescent="0.35">
       <c r="A137" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-13</v>
@@ -7267,10 +7280,10 @@
         <v>43</v>
       </c>
       <c r="H137" s="17" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="138" spans="1:10" ht="34.5" x14ac:dyDescent="0.35">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" ht="46" x14ac:dyDescent="0.35">
       <c r="A138" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-7</v>
@@ -7285,7 +7298,7 @@
         <v>7</v>
       </c>
       <c r="E138" s="5" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="F138" s="4" t="s">
         <v>30</v>
@@ -7294,7 +7307,7 @@
         <v>31</v>
       </c>
       <c r="H138" s="13" t="s">
-        <v>538</v>
+        <v>528</v>
       </c>
       <c r="J138" s="19"/>
     </row>

</xml_diff>

<commit_message>
Traitement commentaires modèle commun sauf : DGPR/SRNH/SdcAP/BRIL-7 et DGPR/SRNH/SDCAP/PONSOH-13
</commit_message>
<xml_diff>
--- a/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
+++ b/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Geostandards-Risques\suivi\2024-05_06-Consultation-publique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B41500-8BB6-4E0B-8B7F-52E3093D1FD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0803A9F3-D4D9-4E28-9D59-456DC1C53B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="554">
   <si>
     <t>Organisme</t>
   </si>
@@ -2087,50 +2087,69 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">OK, à corriger.
+    <t>A priori non pour l'instant. 
+=&gt; Envisager de produire un fichier de métadonnées type</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Intégré</t>
+  </si>
+  <si>
+    <t>N.A.</t>
+  </si>
+  <si>
+    <t>intégré</t>
+  </si>
+  <si>
+    <t>intégré (PPR)</t>
+  </si>
+  <si>
+    <t>OK suppression de la référence à l'addenda.</t>
+  </si>
+  <si>
+    <t>OK, à remplacer (et remplacement de la référence à ce document dans par celle au guide en page xx)</t>
+  </si>
+  <si>
+    <t>traité</t>
+  </si>
+  <si>
+    <t>integré</t>
+  </si>
+  <si>
+    <t>cf. commentaires PPR</t>
+  </si>
+  <si>
+    <t>integré (+ carte "approuvée" au lieu de "signée")
++ tables d'énumérations (PPR) + modèle UML + gabarits</t>
+  </si>
+  <si>
+    <t>Vérifier si possibilité de restreindre les valeurs de certains champs au niveau de modèle commun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK, à corriger.
 Cela remet-il en cause la typologie des ouvrages de protection (barrage et digues) ? =&gt; cf. commentaires PPR
 Une référence à la documentation de SIOUH II serait la bienvenue aussi
 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Typologie des ouvrages de protection à modifier. Proposition BRIL (+BRNT ?) à venir</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Non, à moins qu'il n'y ait une volonté de les transformer en PPR (cf. Sweet pepper)?
+  </si>
+  <si>
+    <t>Typologie des ouvrages de protection à modifier. Proposition BRIL (+BRNT ?) à venir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non, à moins qu'il n'y ait une volonté de les transformer en PPR (cf. Sweet pepper)?
 NB : certains champs obligatoires non renseignés dans PSS
 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Ne rendre obligatoire que les thématiques Procédures, Périmètres et Zonage Réglementaire?</t>
-    </r>
-  </si>
-  <si>
-    <t>A priori non pour l'instant. 
-=&gt; Envisager de produire un fichier de métadonnées type</t>
+  </si>
+  <si>
+    <t>Ne rendre obligatoire que les thématiques Procédures, Périmètres et Zonage Réglementaire?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2216,11 +2235,6 @@
       <color theme="1"/>
       <name val="Wingdings"/>
       <charset val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -2321,7 +2335,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2334,10 +2347,13 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2345,7 +2361,45 @@
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="23">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2768,38 +2822,40 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E152CA69-C1C4-40F5-84A2-16C1484F79DC}" name="Tableau3" displayName="Tableau3" ref="A1:H20" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="A1:H20" xr:uid="{E152CA69-C1C4-40F5-84A2-16C1484F79DC}"/>
-  <tableColumns count="8">
-    <tableColumn id="8" xr3:uid="{FDEDA288-5661-4539-AEBA-9A87C20962E6}" name="Numero" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E152CA69-C1C4-40F5-84A2-16C1484F79DC}" name="Tableau3" displayName="Tableau3" ref="A1:I20" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+  <autoFilter ref="A1:I20" xr:uid="{E152CA69-C1C4-40F5-84A2-16C1484F79DC}"/>
+  <tableColumns count="9">
+    <tableColumn id="8" xr3:uid="{FDEDA288-5661-4539-AEBA-9A87C20962E6}" name="Numero" dataDxfId="20">
       <calculatedColumnFormula>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{635A3DB7-7204-4378-B92A-598A2491845D}" name="Colonne1" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{79A10EF1-8EC6-4A0F-BA8C-3DFA972C0085}" name="Organisme" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{B1796E2E-D6C3-4AA8-BE83-FC4F94A53A8A}" name="Type de commentaire:_x000a_(G)énéral  (M)étier (T)echnique (D)ocument" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{1412256D-CC49-4084-A346-F8B20C24D98A}" name="Page, _x000a_Paragraphe" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{5F39A908-2FFC-40EB-BF7C-360C193B6507}" name="Commentaire" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{D01F9F9F-406C-4050-A108-256D1A81EB43}" name="Modification proposée " dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{2B745299-03CE-435C-B9E5-654FA9CECC38}" name="Décision du GT CNIG Risques" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{635A3DB7-7204-4378-B92A-598A2491845D}" name="Colonne1" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{79A10EF1-8EC6-4A0F-BA8C-3DFA972C0085}" name="Organisme" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{B1796E2E-D6C3-4AA8-BE83-FC4F94A53A8A}" name="Type de commentaire:_x000a_(G)énéral  (M)étier (T)echnique (D)ocument" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{1412256D-CC49-4084-A346-F8B20C24D98A}" name="Page, _x000a_Paragraphe" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{5F39A908-2FFC-40EB-BF7C-360C193B6507}" name="Commentaire" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{D01F9F9F-406C-4050-A108-256D1A81EB43}" name="Modification proposée " dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{2B745299-03CE-435C-B9E5-654FA9CECC38}" name="Décision du GT CNIG Risques" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{8675ABB4-B445-45A5-A068-9D591F8235C6}" name="Action" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{847E454C-1CA0-45D6-9F56-3D5FFE89C0F5}" name="Tableau2" displayName="Tableau2" ref="A1:H138" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8">
-  <autoFilter ref="A1:H138" xr:uid="{847E454C-1CA0-45D6-9F56-3D5FFE89C0F5}"/>
-  <tableColumns count="8">
-    <tableColumn id="8" xr3:uid="{6862FBA5-3017-4233-B0D4-5BC2462198D0}" name="Colonne2" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{847E454C-1CA0-45D6-9F56-3D5FFE89C0F5}" name="Tableau2" displayName="Tableau2" ref="A1:I138" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
+  <autoFilter ref="A1:I138" xr:uid="{847E454C-1CA0-45D6-9F56-3D5FFE89C0F5}"/>
+  <tableColumns count="9">
+    <tableColumn id="8" xr3:uid="{6862FBA5-3017-4233-B0D4-5BC2462198D0}" name="Colonne2" dataDxfId="9">
       <calculatedColumnFormula>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{A8BB7BB0-4D6B-4A0E-A615-089BDEA55F36}" name="Colonne1" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{81E8B2D7-3970-4344-9966-2E0DDFB404DB}" name="Organisme" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{D152CE9B-5BA5-4879-B7DE-1CBF90027255}" name="Type de commentaire:(G)énéral  (M)étier (T)echnique (D)ocument" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{DE633778-26A0-4BDF-9CA2-36FE6DA84467}" name="Page, Paragraphe" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{378CA86A-0CF7-484A-BD7C-53282B21DE2F}" name="Commentaire" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{38052BD9-6BB2-443C-8278-BB11301B0221}" name="Modification proposée " dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{A2C2771F-6D33-454B-9C1D-FAE8B1231568}" name="Décision du GT CNIG Risques" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{A8BB7BB0-4D6B-4A0E-A615-089BDEA55F36}" name="Colonne1" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{81E8B2D7-3970-4344-9966-2E0DDFB404DB}" name="Organisme" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{D152CE9B-5BA5-4879-B7DE-1CBF90027255}" name="Type de commentaire:(G)énéral  (M)étier (T)echnique (D)ocument" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{DE633778-26A0-4BDF-9CA2-36FE6DA84467}" name="Page, Paragraphe" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{378CA86A-0CF7-484A-BD7C-53282B21DE2F}" name="Commentaire" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{38052BD9-6BB2-443C-8278-BB11301B0221}" name="Modification proposée " dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{A2C2771F-6D33-454B-9C1D-FAE8B1231568}" name="Décision du GT CNIG Risques" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{039CFFBD-CF12-4001-86EB-ECDCA01C3555}" name="Action" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3102,10 +3158,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939F5930-30D3-43D0-87E8-B00574FE9CE2}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3122,7 +3178,7 @@
     <col min="10" max="16384" width="10.90625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>349</v>
       </c>
@@ -3147,8 +3203,11 @@
       <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="73" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I1" s="2" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="73" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-1</v>
@@ -3174,8 +3233,11 @@
       <c r="H2" s="17" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="92" x14ac:dyDescent="0.35">
+      <c r="I2" s="4" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-2</v>
@@ -3201,8 +3263,11 @@
       <c r="H3" s="13" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="92" x14ac:dyDescent="0.35">
+      <c r="I3" s="4" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-3</v>
@@ -3225,11 +3290,14 @@
       <c r="G4" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="H4" s="23" t="s">
+      <c r="H4" s="17" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="75.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I4" s="4" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="75.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-4</v>
@@ -3255,8 +3323,11 @@
       <c r="H5" s="13" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="89" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I5" s="4" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="89" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-5</v>
@@ -3282,8 +3353,11 @@
       <c r="H6" s="17" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="23" x14ac:dyDescent="0.35">
+      <c r="I6" s="4" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/DAPP/BIP-11</v>
@@ -3307,8 +3381,11 @@
       <c r="H7" s="18" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
+      <c r="I7" s="4" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-6</v>
@@ -3334,8 +3411,11 @@
       <c r="H8" s="17" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="92" x14ac:dyDescent="0.35">
+      <c r="I8" s="4" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-7</v>
@@ -3361,8 +3441,11 @@
       <c r="H9" s="17" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I9" s="24" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-1</v>
@@ -3388,8 +3471,11 @@
       <c r="H10" s="17" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I10" s="4" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-2</v>
@@ -3415,8 +3501,11 @@
       <c r="H11" s="17" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="103.5" x14ac:dyDescent="0.35">
+      <c r="I11" s="4" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-8</v>
@@ -3442,8 +3531,11 @@
       <c r="H12" s="17" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I12" s="4" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>cerema-6</v>
@@ -3469,8 +3561,11 @@
       <c r="H13" s="17" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="92" x14ac:dyDescent="0.35">
+      <c r="I13" s="4" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-9</v>
@@ -3496,8 +3591,11 @@
       <c r="H14" s="17" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="61" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I14" s="4" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="61" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-10</v>
@@ -3523,8 +3621,11 @@
       <c r="H15" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="68" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I15" s="4" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="68" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-3</v>
@@ -3550,8 +3651,11 @@
       <c r="H16" s="13" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="77" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I16" s="4" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="77" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-4</v>
@@ -3577,8 +3681,11 @@
       <c r="H17" s="17" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I17" s="4" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="111" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-5</v>
@@ -3604,8 +3711,11 @@
       <c r="H18" s="17" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I18" s="4" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SDCAP/PONSOH-13</v>
@@ -3628,11 +3738,14 @@
       <c r="G19" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="H19" s="24" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H19" s="25" t="s">
+        <v>550</v>
+      </c>
+      <c r="I19" s="24" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/DAPP/BIP-12</v>
@@ -3655,6 +3768,9 @@
       <c r="G20" s="4"/>
       <c r="H20" s="17" t="s">
         <v>360</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>545</v>
       </c>
     </row>
   </sheetData>
@@ -3671,7 +3787,7 @@
   <dimension ref="A1:I138"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3684,10 +3800,11 @@
     <col min="6" max="6" width="44.08984375" style="3" customWidth="1"/>
     <col min="7" max="7" width="38" style="3" customWidth="1"/>
     <col min="8" max="8" width="51.81640625" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="10.90625" style="3"/>
+    <col min="9" max="9" width="22.26953125" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="10.90625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>348</v>
       </c>
@@ -3712,8 +3829,11 @@
       <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="57.5" x14ac:dyDescent="0.35">
+      <c r="I1" s="16" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-2</v>
@@ -3734,11 +3854,14 @@
         <v>242</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="24" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H2" s="25" t="s">
+        <v>552</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-3</v>
@@ -3759,11 +3882,14 @@
         <v>243</v>
       </c>
       <c r="G3" s="4"/>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="22" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I3" s="4" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-4</v>
@@ -3784,11 +3910,14 @@
         <v>244</v>
       </c>
       <c r="G4" s="9"/>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="22" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I4" s="4" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-5</v>
@@ -3809,11 +3938,12 @@
         <v>245</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="25" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="126.5" x14ac:dyDescent="0.35">
+      <c r="H5" s="22" t="s">
+        <v>537</v>
+      </c>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" ht="126.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP-0</v>
@@ -3835,8 +3965,9 @@
       <c r="H6" s="17" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="57.5" x14ac:dyDescent="0.35">
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-9</v>
@@ -3860,8 +3991,9 @@
       <c r="H7" s="13" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="46" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" ht="46" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-14</v>
@@ -3882,11 +4014,12 @@
       <c r="G8" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="H8" s="19" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="23" x14ac:dyDescent="0.35">
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-15</v>
@@ -3907,11 +4040,12 @@
       <c r="G9" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="H9" s="19" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="74" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" ht="74" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-2</v>
@@ -3937,8 +4071,9 @@
       <c r="H10" s="17" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-3</v>
@@ -3964,8 +4099,9 @@
       <c r="H11" s="17" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="74" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" ht="74" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-1</v>
@@ -3991,8 +4127,11 @@
       <c r="H12" s="17" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I12" s="4" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-1</v>
@@ -4018,8 +4157,11 @@
       <c r="H13" s="17" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="161" x14ac:dyDescent="0.35">
+      <c r="I13" s="4" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="161" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-2</v>
@@ -4043,10 +4185,13 @@
         <v>254</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+        <v>544</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-3</v>
@@ -4070,10 +4215,13 @@
         <v>62</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+        <v>543</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-1</v>
@@ -4099,8 +4247,9 @@
       <c r="H16" s="17" t="s">
         <v>536</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="103.5" x14ac:dyDescent="0.35">
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-4</v>
@@ -4126,8 +4275,9 @@
       <c r="H17" s="13" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-4</v>
@@ -4153,8 +4303,9 @@
       <c r="H18" s="17" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:9" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-5</v>
@@ -4177,11 +4328,12 @@
       <c r="G19" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="H19" s="20" t="s">
+      <c r="H19" s="19" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-6</v>
@@ -4207,8 +4359,9 @@
       <c r="H20" s="17" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:9" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-2</v>
@@ -4234,8 +4387,9 @@
       <c r="H21" s="17" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-3</v>
@@ -4261,8 +4415,9 @@
       <c r="H22" s="13" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="23" x14ac:dyDescent="0.35">
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-5</v>
@@ -4288,8 +4443,9 @@
       <c r="H23" s="17" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+      <c r="I23" s="4"/>
+    </row>
+    <row r="24" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-4</v>
@@ -4312,11 +4468,12 @@
       <c r="G24" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="H24" s="20" t="s">
+      <c r="H24" s="19" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="23" x14ac:dyDescent="0.35">
+      <c r="I24" s="4"/>
+    </row>
+    <row r="25" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-5</v>
@@ -4342,8 +4499,9 @@
       <c r="H25" s="17" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I25" s="4"/>
+    </row>
+    <row r="26" spans="1:9" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-7</v>
@@ -4369,8 +4527,9 @@
       <c r="H26" s="17" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="I26" s="4"/>
+    </row>
+    <row r="27" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-6</v>
@@ -4396,8 +4555,9 @@
       <c r="H27" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="96" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I27" s="4"/>
+    </row>
+    <row r="28" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-</v>
@@ -4418,11 +4578,12 @@
       <c r="G28" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="H28" s="20" t="s">
+      <c r="H28" s="19" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I28" s="4"/>
+    </row>
+    <row r="29" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-8</v>
@@ -4448,8 +4609,9 @@
       <c r="H29" s="17" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I29" s="4"/>
+    </row>
+    <row r="30" spans="1:9" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-9</v>
@@ -4472,11 +4634,12 @@
       <c r="G30" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="H30" s="20" t="s">
+      <c r="H30" s="19" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="69" x14ac:dyDescent="0.35">
+      <c r="I30" s="4"/>
+    </row>
+    <row r="31" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-6</v>
@@ -4499,11 +4662,12 @@
       <c r="G31" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="H31" s="20" t="s">
+      <c r="H31" s="19" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="92" x14ac:dyDescent="0.35">
+      <c r="I31" s="4"/>
+    </row>
+    <row r="32" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-7</v>
@@ -4526,11 +4690,12 @@
       <c r="G32" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="H32" s="20" t="s">
+      <c r="H32" s="19" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I32" s="4"/>
+    </row>
+    <row r="33" spans="1:9" ht="41" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-10</v>
@@ -4554,8 +4719,9 @@
       <c r="H33" s="17" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" ht="57.5" x14ac:dyDescent="0.35">
+      <c r="I33" s="4"/>
+    </row>
+    <row r="34" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-7</v>
@@ -4578,11 +4744,12 @@
       <c r="G34" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="H34" s="20" t="s">
+      <c r="H34" s="19" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I34" s="4"/>
+    </row>
+    <row r="35" spans="1:9" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-11</v>
@@ -4606,8 +4773,9 @@
       <c r="H35" s="17" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
+      <c r="I35" s="4"/>
+    </row>
+    <row r="36" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-1</v>
@@ -4633,8 +4801,9 @@
       <c r="H36" s="13" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I36" s="4"/>
+    </row>
+    <row r="37" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-21</v>
@@ -4660,8 +4829,9 @@
       <c r="H37" s="13" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" ht="92" x14ac:dyDescent="0.35">
+      <c r="I37" s="4"/>
+    </row>
+    <row r="38" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-</v>
@@ -4682,11 +4852,12 @@
       <c r="G38" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="H38" s="20" t="s">
+      <c r="H38" s="19" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" ht="207" x14ac:dyDescent="0.35">
+      <c r="I38" s="4"/>
+    </row>
+    <row r="39" spans="1:9" ht="207" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-</v>
@@ -4707,11 +4878,12 @@
       <c r="G39" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="H39" s="20" t="s">
+      <c r="H39" s="19" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
+      <c r="I39" s="4"/>
+    </row>
+    <row r="40" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-8</v>
@@ -4734,11 +4906,12 @@
       <c r="G40" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="H40" s="20" t="s">
+      <c r="H40" s="19" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I40" s="4"/>
+    </row>
+    <row r="41" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-8</v>
@@ -4761,11 +4934,12 @@
       <c r="G41" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="H41" s="20" t="s">
+      <c r="H41" s="19" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I41" s="4"/>
+    </row>
+    <row r="42" spans="1:9" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-12</v>
@@ -4786,11 +4960,12 @@
         <v>84</v>
       </c>
       <c r="G42" s="4"/>
-      <c r="H42" s="20" t="s">
+      <c r="H42" s="19" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" ht="92" x14ac:dyDescent="0.35">
+      <c r="I42" s="4"/>
+    </row>
+    <row r="43" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-4</v>
@@ -4816,8 +4991,9 @@
       <c r="H43" s="13" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I43" s="4"/>
+    </row>
+    <row r="44" spans="1:9" ht="38" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-2</v>
@@ -4840,11 +5016,12 @@
       <c r="G44" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H44" s="20" t="s">
+      <c r="H44" s="19" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="I44" s="4"/>
+    </row>
+    <row r="45" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/BRNT-22</v>
@@ -4865,11 +5042,12 @@
         <v>102</v>
       </c>
       <c r="G45" s="4"/>
-      <c r="H45" s="20" t="s">
+      <c r="H45" s="19" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+      <c r="I45" s="4"/>
+    </row>
+    <row r="46" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-8</v>
@@ -4892,11 +5070,12 @@
       <c r="G46" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H46" s="20" t="s">
+      <c r="H46" s="19" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I46" s="4"/>
+    </row>
+    <row r="47" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-24</v>
@@ -4919,11 +5098,12 @@
       <c r="G47" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="H47" s="20" t="s">
+      <c r="H47" s="19" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I47" s="4"/>
+    </row>
+    <row r="48" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-3</v>
@@ -4949,8 +5129,9 @@
       <c r="H48" s="17" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I48" s="4"/>
+    </row>
+    <row r="49" spans="1:9" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-5</v>
@@ -4976,8 +5157,9 @@
       <c r="H49" s="13" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" ht="69" x14ac:dyDescent="0.35">
+      <c r="I49" s="4"/>
+    </row>
+    <row r="50" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT07-2</v>
@@ -5003,8 +5185,9 @@
       <c r="H50" s="13" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I50" s="4"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-11</v>
@@ -5030,8 +5213,9 @@
       <c r="H51" s="17" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I51" s="4"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-12</v>
@@ -5057,8 +5241,9 @@
       <c r="H52" s="17" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="I52" s="4"/>
+    </row>
+    <row r="53" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-13</v>
@@ -5081,11 +5266,12 @@
       <c r="G53" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="H53" s="20" t="s">
+      <c r="H53" s="19" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" ht="36.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I53" s="4"/>
+    </row>
+    <row r="54" spans="1:9" ht="36.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-14</v>
@@ -5106,11 +5292,12 @@
       <c r="G54" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="H54" s="20" t="s">
+      <c r="H54" s="19" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I54" s="4"/>
+    </row>
+    <row r="55" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-13</v>
@@ -5134,8 +5321,9 @@
       <c r="H55" s="17" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" ht="57.5" x14ac:dyDescent="0.35">
+      <c r="I55" s="4"/>
+    </row>
+    <row r="56" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-15</v>
@@ -5159,8 +5347,9 @@
       <c r="H56" s="13" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+      <c r="I56" s="4"/>
+    </row>
+    <row r="57" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-9</v>
@@ -5186,8 +5375,9 @@
       <c r="H57" s="17" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" ht="184" x14ac:dyDescent="0.35">
+      <c r="I57" s="4"/>
+    </row>
+    <row r="58" spans="1:9" ht="184" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5206,11 +5396,12 @@
         <v>346</v>
       </c>
       <c r="G58" s="4"/>
-      <c r="H58" s="20" t="s">
+      <c r="H58" s="19" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+      <c r="I58" s="4"/>
+    </row>
+    <row r="59" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-14</v>
@@ -5233,11 +5424,12 @@
       <c r="G59" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="H59" s="20" t="s">
+      <c r="H59" s="19" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" ht="92" x14ac:dyDescent="0.35">
+      <c r="I59" s="4"/>
+    </row>
+    <row r="60" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5256,11 +5448,12 @@
         <v>345</v>
       </c>
       <c r="G60" s="4"/>
-      <c r="H60" s="20" t="s">
+      <c r="H60" s="19" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" ht="230" x14ac:dyDescent="0.35">
+      <c r="I60" s="4"/>
+    </row>
+    <row r="61" spans="1:9" ht="230" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5282,8 +5475,9 @@
       <c r="H61" s="13" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
+      <c r="I61" s="4"/>
+    </row>
+    <row r="62" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A62" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-15</v>
@@ -5306,11 +5500,12 @@
       <c r="G62" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="H62" s="20" t="s">
+      <c r="H62" s="19" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+      <c r="I62" s="4"/>
+    </row>
+    <row r="63" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5332,8 +5527,9 @@
       <c r="H63" s="13" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+      <c r="I63" s="4"/>
+    </row>
+    <row r="64" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A64" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-16</v>
@@ -5356,11 +5552,12 @@
       <c r="G64" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="H64" s="20" t="s">
+      <c r="H64" s="19" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+      <c r="I64" s="4"/>
+    </row>
+    <row r="65" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT01-3</v>
@@ -5386,8 +5583,9 @@
       <c r="H65" s="13" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+      <c r="I65" s="4"/>
+    </row>
+    <row r="66" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDTM 83-1</v>
@@ -5413,8 +5611,9 @@
       <c r="H66" s="13" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" ht="174" x14ac:dyDescent="0.35">
+      <c r="I66" s="4"/>
+    </row>
+    <row r="67" spans="1:9" ht="174" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-10</v>
@@ -5437,11 +5636,12 @@
       <c r="G67" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="H67" s="20" t="s">
+      <c r="H67" s="19" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" ht="88" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I67" s="4"/>
+    </row>
+    <row r="68" spans="1:9" ht="88" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-1</v>
@@ -5464,11 +5664,12 @@
       <c r="G68" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="H68" s="20" t="s">
+      <c r="H68" s="19" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" ht="103" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I68" s="4"/>
+    </row>
+    <row r="69" spans="1:9" ht="103" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-11</v>
@@ -5491,11 +5692,12 @@
       <c r="G69" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="H69" s="20" t="s">
+      <c r="H69" s="19" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I69" s="4"/>
+    </row>
+    <row r="70" spans="1:9" ht="111" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-12</v>
@@ -5518,11 +5720,12 @@
       <c r="G70" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="H70" s="20" t="s">
+      <c r="H70" s="19" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I70" s="4"/>
+    </row>
+    <row r="71" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-13</v>
@@ -5548,9 +5751,10 @@
       <c r="H71" s="17" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
-      <c r="A72" s="21" t="str">
+      <c r="I71" s="4"/>
+    </row>
+    <row r="72" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A72" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-14</v>
       </c>
@@ -5572,12 +5776,13 @@
       <c r="G72" s="4" t="s">
         <v>455</v>
       </c>
-      <c r="H72" s="20" t="s">
+      <c r="H72" s="19" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A73" s="21" t="str">
+      <c r="I72" s="4"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A73" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-19</v>
       </c>
@@ -5602,9 +5807,10 @@
       <c r="H73" s="17" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A74" s="21" t="str">
+      <c r="I73" s="4"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A74" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-16</v>
       </c>
@@ -5629,8 +5835,9 @@
       <c r="H74" s="17" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I74" s="4"/>
+    </row>
+    <row r="75" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-14</v>
@@ -5653,11 +5860,12 @@
       <c r="G75" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="H75" s="20" t="s">
+      <c r="H75" s="19" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" ht="115" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I75" s="4"/>
+    </row>
+    <row r="76" spans="1:9" ht="115" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-15</v>
@@ -5680,11 +5888,12 @@
       <c r="G76" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="H76" s="20" t="s">
+      <c r="H76" s="19" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="I76" s="4"/>
+    </row>
+    <row r="77" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A77" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-16</v>
@@ -5707,12 +5916,13 @@
       <c r="G77" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="H77" s="20" t="s">
+      <c r="H77" s="19" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
-      <c r="A78" s="21" t="str">
+      <c r="I77" s="4"/>
+    </row>
+    <row r="78" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A78" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-22</v>
       </c>
@@ -5734,12 +5944,13 @@
       <c r="G78" s="4" t="s">
         <v>469</v>
       </c>
-      <c r="H78" s="20" t="s">
+      <c r="H78" s="19" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A79" s="21" t="str">
+      <c r="I78" s="4"/>
+    </row>
+    <row r="79" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+      <c r="A79" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-23</v>
       </c>
@@ -5764,9 +5975,10 @@
       <c r="H79" s="17" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A80" s="21" t="str">
+      <c r="I79" s="4"/>
+    </row>
+    <row r="80" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+      <c r="A80" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-24</v>
       </c>
@@ -5791,8 +6003,9 @@
       <c r="H80" s="17" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+      <c r="I80" s="4"/>
+    </row>
+    <row r="81" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A81" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-17</v>
@@ -5815,11 +6028,12 @@
       <c r="G81" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="H81" s="20" t="s">
+      <c r="H81" s="19" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="I81" s="4"/>
+    </row>
+    <row r="82" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A82" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-18</v>
@@ -5842,11 +6056,12 @@
       <c r="G82" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="H82" s="20" t="s">
+      <c r="H82" s="19" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" ht="69" x14ac:dyDescent="0.35">
+      <c r="I82" s="4"/>
+    </row>
+    <row r="83" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A83" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-19</v>
@@ -5869,11 +6084,12 @@
       <c r="G83" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="H83" s="20" t="s">
+      <c r="H83" s="19" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" ht="23" x14ac:dyDescent="0.35">
+      <c r="I83" s="4"/>
+    </row>
+    <row r="84" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A84" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-20</v>
@@ -5899,9 +6115,10 @@
       <c r="H84" s="17" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" ht="36.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="21" t="str">
+      <c r="I84" s="4"/>
+    </row>
+    <row r="85" spans="1:9" ht="36.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-27</v>
       </c>
@@ -5923,11 +6140,12 @@
       <c r="G85" s="4" t="s">
         <v>478</v>
       </c>
-      <c r="H85" s="20" t="s">
+      <c r="H85" s="19" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="I85" s="4"/>
+    </row>
+    <row r="86" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-21</v>
@@ -5950,12 +6168,13 @@
       <c r="G86" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="H86" s="20" t="s">
+      <c r="H86" s="19" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="21" t="str">
+      <c r="I86" s="4"/>
+    </row>
+    <row r="87" spans="1:9" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-26</v>
       </c>
@@ -5977,11 +6196,12 @@
       <c r="G87" s="4" t="s">
         <v>469</v>
       </c>
-      <c r="H87" s="20" t="s">
+      <c r="H87" s="19" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I87" s="4"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-17</v>
@@ -6007,8 +6227,9 @@
       <c r="H88" s="17" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="I88" s="4"/>
+    </row>
+    <row r="89" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A89" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-16</v>
@@ -6032,8 +6253,9 @@
       <c r="H89" s="17" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I89" s="4"/>
+    </row>
+    <row r="90" spans="1:9" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-17</v>
@@ -6057,8 +6279,9 @@
       <c r="H90" s="13" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="I90" s="4"/>
+    </row>
+    <row r="91" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A91" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-22</v>
@@ -6081,11 +6304,12 @@
       <c r="G91" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="H91" s="20" t="s">
+      <c r="H91" s="19" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
+      <c r="I91" s="4"/>
+    </row>
+    <row r="92" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A92" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-23</v>
@@ -6111,8 +6335,9 @@
       <c r="H92" s="13" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
+      <c r="I92" s="4"/>
+    </row>
+    <row r="93" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A93" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-24</v>
@@ -6135,11 +6360,12 @@
       <c r="G93" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="H93" s="22" t="s">
+      <c r="H93" s="21" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" ht="113" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I93" s="4"/>
+    </row>
+    <row r="94" spans="1:9" ht="113" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/PoNSOH-26</v>
@@ -6165,8 +6391,9 @@
       <c r="H94" s="9" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I94" s="4"/>
+    </row>
+    <row r="95" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/PoNSOH-27</v>
@@ -6189,11 +6416,12 @@
       <c r="G95" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="H95" s="20" t="s">
+      <c r="H95" s="19" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I95" s="4"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-18</v>
@@ -6219,8 +6447,9 @@
       <c r="H96" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I96" s="4"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-19</v>
@@ -6246,8 +6475,9 @@
       <c r="H97" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" ht="96.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I97" s="4"/>
+    </row>
+    <row r="98" spans="1:9" ht="96.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-18</v>
@@ -6268,12 +6498,13 @@
         <v>257</v>
       </c>
       <c r="G98" s="4"/>
-      <c r="H98" s="20" t="s">
+      <c r="H98" s="19" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" ht="23" x14ac:dyDescent="0.35">
-      <c r="A99" s="21" t="str">
+      <c r="I98" s="4"/>
+    </row>
+    <row r="99" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="A99" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-15</v>
       </c>
@@ -6298,9 +6529,10 @@
       <c r="H99" s="17" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="21" t="str">
+      <c r="I99" s="4"/>
+    </row>
+    <row r="100" spans="1:9" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-1</v>
       </c>
@@ -6325,9 +6557,10 @@
       <c r="H100" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" ht="23" x14ac:dyDescent="0.35">
-      <c r="A101" s="21" t="str">
+      <c r="I100" s="4"/>
+    </row>
+    <row r="101" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="A101" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-17</v>
       </c>
@@ -6352,9 +6585,10 @@
       <c r="H101" s="17" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" ht="23" x14ac:dyDescent="0.35">
-      <c r="A102" s="21" t="str">
+      <c r="I101" s="4"/>
+    </row>
+    <row r="102" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="A102" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-20</v>
       </c>
@@ -6379,9 +6613,10 @@
       <c r="H102" s="17" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" ht="37.5" x14ac:dyDescent="0.35">
-      <c r="A103" s="21" t="str">
+      <c r="I102" s="4"/>
+    </row>
+    <row r="103" spans="1:9" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="A103" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-21</v>
       </c>
@@ -6403,12 +6638,13 @@
       <c r="G103" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="H103" s="20" t="s">
+      <c r="H103" s="19" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
-      <c r="A104" s="21" t="str">
+      <c r="I103" s="4"/>
+    </row>
+    <row r="104" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A104" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-18</v>
       </c>
@@ -6433,9 +6669,10 @@
       <c r="H104" s="13" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
-      <c r="A105" s="21" t="str">
+      <c r="I104" s="4"/>
+    </row>
+    <row r="105" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A105" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-25</v>
       </c>
@@ -6460,9 +6697,10 @@
       <c r="H105" s="17" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" ht="23" x14ac:dyDescent="0.35">
-      <c r="A106" s="21" t="str">
+      <c r="I105" s="4"/>
+    </row>
+    <row r="106" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="A106" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-2</v>
       </c>
@@ -6487,9 +6725,10 @@
       <c r="H106" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" ht="23" x14ac:dyDescent="0.35">
-      <c r="A107" s="21" t="str">
+      <c r="I106" s="4"/>
+    </row>
+    <row r="107" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="A107" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-3</v>
       </c>
@@ -6514,9 +6753,10 @@
       <c r="H107" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" ht="23" x14ac:dyDescent="0.35">
-      <c r="A108" s="21" t="str">
+      <c r="I107" s="4"/>
+    </row>
+    <row r="108" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="A108" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-4</v>
       </c>
@@ -6541,8 +6781,9 @@
       <c r="H108" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+      <c r="I108" s="4"/>
+    </row>
+    <row r="109" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A109" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT01-1</v>
@@ -6568,9 +6809,10 @@
       <c r="H109" s="6" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" ht="23" x14ac:dyDescent="0.35">
-      <c r="A110" s="21" t="str">
+      <c r="I109" s="4"/>
+    </row>
+    <row r="110" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="A110" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-5</v>
       </c>
@@ -6595,9 +6837,10 @@
       <c r="H110" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" ht="23" x14ac:dyDescent="0.35">
-      <c r="A111" s="21" t="str">
+      <c r="I110" s="4"/>
+    </row>
+    <row r="111" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="A111" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-6</v>
       </c>
@@ -6622,9 +6865,10 @@
       <c r="H111" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
-      <c r="A112" s="21" t="str">
+      <c r="I111" s="4"/>
+    </row>
+    <row r="112" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A112" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-7</v>
       </c>
@@ -6649,9 +6893,10 @@
       <c r="H112" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" ht="23" x14ac:dyDescent="0.35">
-      <c r="A113" s="21" t="str">
+      <c r="I112" s="4"/>
+    </row>
+    <row r="113" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="A113" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-8</v>
       </c>
@@ -6676,9 +6921,10 @@
       <c r="H113" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
-      <c r="A114" s="21" t="str">
+      <c r="I113" s="4"/>
+    </row>
+    <row r="114" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A114" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-9</v>
       </c>
@@ -6703,9 +6949,10 @@
       <c r="H114" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" ht="69" x14ac:dyDescent="0.35">
-      <c r="A115" s="21" t="str">
+      <c r="I114" s="4"/>
+    </row>
+    <row r="115" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+      <c r="A115" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-10</v>
       </c>
@@ -6727,12 +6974,13 @@
       <c r="G115" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="H115" s="20" t="s">
+      <c r="H115" s="19" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="116" spans="1:8" ht="23" x14ac:dyDescent="0.35">
-      <c r="A116" s="21" t="str">
+      <c r="I115" s="4"/>
+    </row>
+    <row r="116" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="A116" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-11</v>
       </c>
@@ -6757,9 +7005,10 @@
       <c r="H116" s="13" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A117" s="21" t="str">
+      <c r="I116" s="4"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A117" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-12</v>
       </c>
@@ -6784,9 +7033,10 @@
       <c r="H117" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" ht="23" x14ac:dyDescent="0.35">
-      <c r="A118" s="21" t="str">
+      <c r="I117" s="4"/>
+    </row>
+    <row r="118" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="A118" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-13</v>
       </c>
@@ -6811,8 +7061,9 @@
       <c r="H118" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" ht="119.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I118" s="4"/>
+    </row>
+    <row r="119" spans="1:9" ht="119.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-6</v>
@@ -6835,11 +7086,12 @@
       <c r="G119" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H119" s="20" t="s">
+      <c r="H119" s="19" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" ht="57.5" x14ac:dyDescent="0.35">
+      <c r="I119" s="4"/>
+    </row>
+    <row r="120" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A120" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT01-2</v>
@@ -6862,11 +7114,12 @@
       <c r="G120" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="H120" s="20" t="s">
+      <c r="H120" s="19" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="121" spans="1:8" ht="57.5" x14ac:dyDescent="0.35">
+      <c r="I120" s="4"/>
+    </row>
+    <row r="121" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A121" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-23</v>
@@ -6889,11 +7142,12 @@
       <c r="G121" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="H121" s="20" t="s">
+      <c r="H121" s="19" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I121" s="4"/>
+    </row>
+    <row r="122" spans="1:9" ht="78" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-20</v>
@@ -6916,11 +7170,12 @@
       <c r="G122" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="H122" s="20" t="s">
+      <c r="H122" s="19" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="I122" s="4"/>
+    </row>
+    <row r="123" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A123" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-25</v>
@@ -6943,11 +7198,12 @@
       <c r="G123" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="H123" s="20" t="s">
+      <c r="H123" s="19" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="124" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="I123" s="4"/>
+    </row>
+    <row r="124" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A124" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-26</v>
@@ -6970,11 +7226,12 @@
       <c r="G124" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="H124" s="20" t="s">
+      <c r="H124" s="19" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="125" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I124" s="4"/>
+    </row>
+    <row r="125" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT07-1</v>
@@ -6997,11 +7254,12 @@
       <c r="G125" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H125" s="20" t="s">
+      <c r="H125" s="19" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="126" spans="1:8" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I125" s="4"/>
+    </row>
+    <row r="126" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-19</v>
@@ -7022,11 +7280,12 @@
         <v>94</v>
       </c>
       <c r="G126" s="4"/>
-      <c r="H126" s="20" t="s">
+      <c r="H126" s="19" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="127" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I126" s="4"/>
+    </row>
+    <row r="127" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-20</v>
@@ -7047,11 +7306,12 @@
         <v>95</v>
       </c>
       <c r="G127" s="4"/>
-      <c r="H127" s="20" t="s">
+      <c r="H127" s="19" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="128" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+      <c r="I127" s="4"/>
+    </row>
+    <row r="128" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A128" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-9</v>
@@ -7074,9 +7334,10 @@
       <c r="G128" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="H128" s="20" t="s">
+      <c r="H128" s="19" t="s">
         <v>519</v>
       </c>
+      <c r="I128" s="4"/>
     </row>
     <row r="129" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="4" t="str">
@@ -7101,9 +7362,10 @@
       <c r="G129" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="H129" s="20" t="s">
+      <c r="H129" s="19" t="s">
         <v>520</v>
       </c>
+      <c r="I129" s="4"/>
     </row>
     <row r="130" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A130" s="4" t="str">
@@ -7131,6 +7393,7 @@
       <c r="H130" s="17" t="s">
         <v>521</v>
       </c>
+      <c r="I130" s="4"/>
     </row>
     <row r="131" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A131" s="4" t="str">
@@ -7158,6 +7421,7 @@
       <c r="H131" s="17" t="s">
         <v>352</v>
       </c>
+      <c r="I131" s="4"/>
     </row>
     <row r="132" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A132" s="4" t="str">
@@ -7185,6 +7449,7 @@
       <c r="H132" s="17" t="s">
         <v>352</v>
       </c>
+      <c r="I132" s="4"/>
     </row>
     <row r="133" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A133" s="4" t="str">
@@ -7212,6 +7477,7 @@
       <c r="H133" s="13" t="s">
         <v>522</v>
       </c>
+      <c r="I133" s="4"/>
     </row>
     <row r="134" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A134" s="4" t="str">
@@ -7239,6 +7505,7 @@
       <c r="H134" s="13" t="s">
         <v>523</v>
       </c>
+      <c r="I134" s="4"/>
     </row>
     <row r="135" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A135" s="4" t="str">
@@ -7263,9 +7530,10 @@
       <c r="G135" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H135" s="20" t="s">
+      <c r="H135" s="19" t="s">
         <v>524</v>
       </c>
+      <c r="I135" s="4"/>
     </row>
     <row r="136" spans="1:9" ht="44" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A136" s="4" t="str">
@@ -7291,6 +7559,7 @@
       <c r="H136" s="13" t="s">
         <v>525</v>
       </c>
+      <c r="I136" s="4"/>
     </row>
     <row r="137" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A137" s="4" t="str">
@@ -7318,6 +7587,7 @@
       <c r="H137" s="17" t="s">
         <v>526</v>
       </c>
+      <c r="I137" s="4"/>
     </row>
     <row r="138" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A138" s="4" t="str">
@@ -7345,7 +7615,7 @@
       <c r="H138" s="13" t="s">
         <v>527</v>
       </c>
-      <c r="I138" s="19"/>
+      <c r="I138" s="23"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
traitement commentaires PPR en cours (DGPR/SRNH/SdcAP/BRIL-8)
</commit_message>
<xml_diff>
--- a/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
+++ b/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Geostandards-Risques\suivi\2024-05_06-Consultation-publique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0803A9F3-D4D9-4E28-9D59-456DC1C53B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7C6796-5E7A-4566-BED7-F693CE65B46F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
+    <workbookView xWindow="29475" yWindow="900" windowWidth="27435" windowHeight="10200" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Synthese Modele Commun" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="560">
   <si>
     <t>Organisme</t>
   </si>
@@ -1334,9 +1334,6 @@
     <t>OK, à remplacer</t>
   </si>
   <si>
-    <t>OK, à supprimer</t>
-  </si>
-  <si>
     <t>NOK
 Cet arrêté est déjà mentionné dans la partie cadre réglementaire</t>
   </si>
@@ -1344,9 +1341,6 @@
     <t>OK, à réordonner</t>
   </si>
   <si>
-    <t>A vérifier</t>
-  </si>
-  <si>
     <t>OK, à modifier</t>
   </si>
   <si>
@@ -1359,14 +1353,6 @@
   <si>
     <t>OK sur le principe
 La formulation "Produire les données métiers des études préalables" ne me semble pas correcte (l'établissement du zonage réglementaire est-il dans la phase d'étude préalable ?)</t>
-  </si>
-  <si>
-    <t>OK, on peut rajouter des liens et le mentionner dans les textes explicatifs</t>
-  </si>
-  <si>
-    <t>A priori, c'est la classe éléments de caracterisation d'aléa qui devrait permettre d'ajouter ces éléments.
-A voir si on peut la rajouter en classe facultative (dans cette version ou une suivante) ?
-Il faudrait la structure de cette table. Où peut-on la trouver ?</t>
   </si>
   <si>
     <t>OK sur le principe.
@@ -2143,6 +2129,49 @@
   </si>
   <si>
     <t>Ne rendre obligatoire que les thématiques Procédures, Périmètres et Zonage Réglementaire?</t>
+  </si>
+  <si>
+    <t>something to do ?</t>
+  </si>
+  <si>
+    <t>A vérifier
+NB : il existe :
+- des PPRN sur Saint-Martin (risque cyclonique et multirsiques)
+- un PPRT sur la Guadeloupe (Baie Mahault)
+Rien sur Saint-Barthélémy, mais il me semble que le code de l'environnement peut aussi s'appliquer à Saint-Barthélémy, non ?</t>
+  </si>
+  <si>
+    <t>OK sur le principe, à modifier
+NB : cartographier l'aléa de référence est trop PPRN-centré =&gt; seulement "cartographier les aléas"</t>
+  </si>
+  <si>
+    <t>intégré (pour la première partie)</t>
+  </si>
+  <si>
+    <t>intégré (pour la partie "du PPR")</t>
+  </si>
+  <si>
+    <t>OK sur le principe. Pour éviter d'aloutrdir le schéma, on mentionne que ce sont les acteurs principaux de l'action qui sont sur le schéma</t>
+  </si>
+  <si>
+    <t>intégré (en accord avec commentaires précédents) + schémas mis à jour</t>
+  </si>
+  <si>
+    <t>intégré + schémas mis à jour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A priori, c'est la classe éléments de caracterisation d'aléa qui devrait permettre d'ajouter ces éléments.
+A voir si on peut la rajouter en classe facultative (dans cette version ou une suivante) ?
+Il faudrait la structure de cette table. Où peut-on la trouver ?
+Cf. :
+-structure LIC (LIGNE ISO COTE HAUTEUR D'EAU) du dictionnaire vigilance inondation du Sandre ? (linéaire)
+- Ligne_iso_cote de la DI (linéaire)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK, sur le principe.
+Reformulation ;  "dont les modalités sont relatives au type d'aléa"
+</t>
   </si>
 </sst>
 </file>
@@ -2362,25 +2391,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="23">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2710,6 +2720,25 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2835,26 +2864,26 @@
     <tableColumn id="5" xr3:uid="{5F39A908-2FFC-40EB-BF7C-360C193B6507}" name="Commentaire" dataDxfId="15"/>
     <tableColumn id="6" xr3:uid="{D01F9F9F-406C-4050-A108-256D1A81EB43}" name="Modification proposée " dataDxfId="14"/>
     <tableColumn id="7" xr3:uid="{2B745299-03CE-435C-B9E5-654FA9CECC38}" name="Décision du GT CNIG Risques" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{8675ABB4-B445-45A5-A068-9D591F8235C6}" name="Action" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{8675ABB4-B445-45A5-A068-9D591F8235C6}" name="Action" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{847E454C-1CA0-45D6-9F56-3D5FFE89C0F5}" name="Tableau2" displayName="Tableau2" ref="A1:I138" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{847E454C-1CA0-45D6-9F56-3D5FFE89C0F5}" name="Tableau2" displayName="Tableau2" ref="A1:I138" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9">
   <autoFilter ref="A1:I138" xr:uid="{847E454C-1CA0-45D6-9F56-3D5FFE89C0F5}"/>
   <tableColumns count="9">
-    <tableColumn id="8" xr3:uid="{6862FBA5-3017-4233-B0D4-5BC2462198D0}" name="Colonne2" dataDxfId="9">
+    <tableColumn id="8" xr3:uid="{6862FBA5-3017-4233-B0D4-5BC2462198D0}" name="Colonne2" dataDxfId="8">
       <calculatedColumnFormula>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{A8BB7BB0-4D6B-4A0E-A615-089BDEA55F36}" name="Colonne1" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{81E8B2D7-3970-4344-9966-2E0DDFB404DB}" name="Organisme" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{D152CE9B-5BA5-4879-B7DE-1CBF90027255}" name="Type de commentaire:(G)énéral  (M)étier (T)echnique (D)ocument" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{DE633778-26A0-4BDF-9CA2-36FE6DA84467}" name="Page, Paragraphe" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{378CA86A-0CF7-484A-BD7C-53282B21DE2F}" name="Commentaire" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{38052BD9-6BB2-443C-8278-BB11301B0221}" name="Modification proposée " dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{A2C2771F-6D33-454B-9C1D-FAE8B1231568}" name="Décision du GT CNIG Risques" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{A8BB7BB0-4D6B-4A0E-A615-089BDEA55F36}" name="Colonne1" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{81E8B2D7-3970-4344-9966-2E0DDFB404DB}" name="Organisme" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{D152CE9B-5BA5-4879-B7DE-1CBF90027255}" name="Type de commentaire:(G)énéral  (M)étier (T)echnique (D)ocument" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{DE633778-26A0-4BDF-9CA2-36FE6DA84467}" name="Page, Paragraphe" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{378CA86A-0CF7-484A-BD7C-53282B21DE2F}" name="Commentaire" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{38052BD9-6BB2-443C-8278-BB11301B0221}" name="Modification proposée " dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{A2C2771F-6D33-454B-9C1D-FAE8B1231568}" name="Décision du GT CNIG Risques" dataDxfId="1"/>
     <tableColumn id="9" xr3:uid="{039CFFBD-CF12-4001-86EB-ECDCA01C3555}" name="Action" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3160,8 +3189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939F5930-30D3-43D0-87E8-B00574FE9CE2}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3204,7 +3233,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="73" customHeight="1" x14ac:dyDescent="0.35">
@@ -3234,7 +3263,7 @@
         <v>351</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="92" x14ac:dyDescent="0.35">
@@ -3261,10 +3290,10 @@
         <v>332</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="92" x14ac:dyDescent="0.35">
@@ -3294,7 +3323,7 @@
         <v>353</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="75.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3321,10 +3350,10 @@
         <v>305</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="89" customHeight="1" x14ac:dyDescent="0.35">
@@ -3354,7 +3383,7 @@
         <v>350</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="23" x14ac:dyDescent="0.35">
@@ -3382,7 +3411,7 @@
         <v>352</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
@@ -3412,7 +3441,7 @@
         <v>358</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="92" x14ac:dyDescent="0.35">
@@ -3442,7 +3471,7 @@
         <v>354</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3472,7 +3501,7 @@
         <v>355</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -3502,7 +3531,7 @@
         <v>355</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
@@ -3529,10 +3558,10 @@
         <v>315</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3562,7 +3591,7 @@
         <v>356</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="92" x14ac:dyDescent="0.35">
@@ -3592,7 +3621,7 @@
         <v>357</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="61" customHeight="1" x14ac:dyDescent="0.35">
@@ -3622,7 +3651,7 @@
         <v>352</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="68" customHeight="1" x14ac:dyDescent="0.35">
@@ -3649,10 +3678,10 @@
         <v>288</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="77" customHeight="1" x14ac:dyDescent="0.35">
@@ -3682,7 +3711,7 @@
         <v>359</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="111" customHeight="1" x14ac:dyDescent="0.35">
@@ -3709,10 +3738,10 @@
         <v>293</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3739,10 +3768,10 @@
         <v>328</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3770,7 +3799,7 @@
         <v>360</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
     </row>
   </sheetData>
@@ -3786,8 +3815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815F14A-19BC-4DCE-8D31-81F595A4B0E7}">
   <dimension ref="A1:I138"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="B31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3830,7 +3859,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="46" x14ac:dyDescent="0.35">
@@ -3855,10 +3884,10 @@
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="25" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3886,7 +3915,7 @@
         <v>371</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3914,7 +3943,7 @@
         <v>372</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="65" customHeight="1" x14ac:dyDescent="0.35">
@@ -3939,9 +3968,11 @@
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="22" t="s">
-        <v>537</v>
-      </c>
-      <c r="I5" s="4"/>
+        <v>533</v>
+      </c>
+      <c r="I5" s="24" t="s">
+        <v>550</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="126.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="str">
@@ -3965,7 +3996,9 @@
       <c r="H6" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="I6" s="4"/>
+      <c r="I6" s="4" t="s">
+        <v>536</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="str">
@@ -3991,7 +4024,9 @@
       <c r="H7" s="13" t="s">
         <v>374</v>
       </c>
-      <c r="I7" s="4"/>
+      <c r="I7" s="4" t="s">
+        <v>536</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="46" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="str">
@@ -4017,7 +4052,7 @@
       <c r="H8" s="19" t="s">
         <v>375</v>
       </c>
-      <c r="I8" s="4"/>
+      <c r="I8" s="24"/>
     </row>
     <row r="9" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="str">
@@ -4043,7 +4078,7 @@
       <c r="H9" s="19" t="s">
         <v>376</v>
       </c>
-      <c r="I9" s="4"/>
+      <c r="I9" s="24"/>
     </row>
     <row r="10" spans="1:9" ht="74" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="str">
@@ -4071,7 +4106,7 @@
       <c r="H10" s="17" t="s">
         <v>377</v>
       </c>
-      <c r="I10" s="4"/>
+      <c r="I10" s="24"/>
     </row>
     <row r="11" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="str">
@@ -4099,7 +4134,7 @@
       <c r="H11" s="17" t="s">
         <v>378</v>
       </c>
-      <c r="I11" s="4"/>
+      <c r="I11" s="24"/>
     </row>
     <row r="12" spans="1:9" ht="74" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="str">
@@ -4128,7 +4163,7 @@
         <v>350</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4155,10 +4190,10 @@
         <v>166</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="161" x14ac:dyDescent="0.35">
@@ -4185,10 +4220,10 @@
         <v>254</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
@@ -4215,10 +4250,10 @@
         <v>62</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
@@ -4245,9 +4280,11 @@
         <v>117</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>536</v>
-      </c>
-      <c r="I16" s="4"/>
+        <v>532</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>537</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="str">
@@ -4273,9 +4310,11 @@
         <v>65</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>381</v>
-      </c>
-      <c r="I17" s="4"/>
+        <v>380</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>536</v>
+      </c>
     </row>
     <row r="18" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="str">
@@ -4301,9 +4340,11 @@
         <v>175</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>382</v>
-      </c>
-      <c r="I18" s="4"/>
+        <v>381</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>537</v>
+      </c>
     </row>
     <row r="19" spans="1:9" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="str">
@@ -4329,9 +4370,11 @@
         <v>255</v>
       </c>
       <c r="H19" s="19" t="s">
-        <v>383</v>
-      </c>
-      <c r="I19" s="4"/>
+        <v>551</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>553</v>
+      </c>
     </row>
     <row r="20" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="str">
@@ -4356,10 +4399,12 @@
       <c r="G20" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="H20" s="17" t="s">
-        <v>384</v>
-      </c>
-      <c r="I20" s="4"/>
+      <c r="H20" s="19" t="s">
+        <v>552</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>537</v>
+      </c>
     </row>
     <row r="21" spans="1:9" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="str">
@@ -4385,9 +4430,11 @@
         <v>120</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>384</v>
-      </c>
-      <c r="I21" s="4"/>
+        <v>382</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>557</v>
+      </c>
     </row>
     <row r="22" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="str">
@@ -4413,11 +4460,13 @@
         <v>122</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>385</v>
-      </c>
-      <c r="I22" s="4"/>
-    </row>
-    <row r="23" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+        <v>383</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-5</v>
@@ -4441,9 +4490,11 @@
         <v>178</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>386</v>
-      </c>
-      <c r="I23" s="4"/>
+        <v>384</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>556</v>
+      </c>
     </row>
     <row r="24" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="str">
@@ -4469,9 +4520,11 @@
         <v>260</v>
       </c>
       <c r="H24" s="19" t="s">
-        <v>387</v>
-      </c>
-      <c r="I24" s="4"/>
+        <v>385</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>554</v>
+      </c>
     </row>
     <row r="25" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="str">
@@ -4497,11 +4550,13 @@
         <v>125</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>386</v>
-      </c>
-      <c r="I25" s="4"/>
-    </row>
-    <row r="26" spans="1:9" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>384</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="71.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-7</v>
@@ -4524,10 +4579,12 @@
       <c r="G26" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="H26" s="17" t="s">
-        <v>388</v>
-      </c>
-      <c r="I26" s="4"/>
+      <c r="H26" s="19" t="s">
+        <v>555</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>537</v>
+      </c>
     </row>
     <row r="27" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="str">
@@ -4555,9 +4612,11 @@
       <c r="H27" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="I27" s="4"/>
-    </row>
-    <row r="28" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I27" s="4" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="115" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-</v>
@@ -4579,9 +4638,9 @@
         <v>340</v>
       </c>
       <c r="H28" s="19" t="s">
-        <v>389</v>
-      </c>
-      <c r="I28" s="4"/>
+        <v>558</v>
+      </c>
+      <c r="I28" s="24"/>
     </row>
     <row r="29" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="str">
@@ -4606,10 +4665,12 @@
       <c r="G29" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="H29" s="17" t="s">
-        <v>380</v>
-      </c>
-      <c r="I29" s="4"/>
+      <c r="H29" s="19" t="s">
+        <v>559</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>537</v>
+      </c>
     </row>
     <row r="30" spans="1:9" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="str">
@@ -4635,7 +4696,7 @@
         <v>78</v>
       </c>
       <c r="H30" s="19" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="I30" s="4"/>
     </row>
@@ -4663,7 +4724,7 @@
         <v>128</v>
       </c>
       <c r="H31" s="19" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="I31" s="4"/>
     </row>
@@ -4691,7 +4752,7 @@
         <v>130</v>
       </c>
       <c r="H32" s="19" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="I32" s="4"/>
     </row>
@@ -4717,7 +4778,7 @@
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="17" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="I33" s="4"/>
     </row>
@@ -4745,7 +4806,7 @@
         <v>184</v>
       </c>
       <c r="H34" s="19" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="I34" s="4"/>
     </row>
@@ -4771,7 +4832,7 @@
         <v>82</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="I35" s="4"/>
     </row>
@@ -4799,7 +4860,7 @@
         <v>19</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I36" s="4"/>
     </row>
@@ -4827,7 +4888,7 @@
         <v>99</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="I37" s="4"/>
     </row>
@@ -4847,13 +4908,13 @@
         <v>369</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>338</v>
       </c>
       <c r="H38" s="19" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="I38" s="4"/>
     </row>
@@ -4873,13 +4934,13 @@
         <v>369</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>338</v>
       </c>
       <c r="H39" s="19" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="I39" s="4"/>
     </row>
@@ -4907,7 +4968,7 @@
         <v>267</v>
       </c>
       <c r="H40" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="I40" s="4"/>
     </row>
@@ -4935,7 +4996,7 @@
         <v>133</v>
       </c>
       <c r="H41" s="19" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="I41" s="4"/>
     </row>
@@ -4961,7 +5022,7 @@
       </c>
       <c r="G42" s="4"/>
       <c r="H42" s="19" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="I42" s="4"/>
     </row>
@@ -4989,7 +5050,7 @@
         <v>26</v>
       </c>
       <c r="H43" s="13" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="I43" s="4"/>
     </row>
@@ -5017,7 +5078,7 @@
         <v>22</v>
       </c>
       <c r="H44" s="19" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="I44" s="4"/>
     </row>
@@ -5043,7 +5104,7 @@
       </c>
       <c r="G45" s="4"/>
       <c r="H45" s="19" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="I45" s="4"/>
     </row>
@@ -5071,7 +5132,7 @@
         <v>33</v>
       </c>
       <c r="H46" s="19" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="I46" s="4"/>
     </row>
@@ -5099,7 +5160,7 @@
         <v>106</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="I47" s="4"/>
     </row>
@@ -5127,7 +5188,7 @@
         <v>25</v>
       </c>
       <c r="H48" s="17" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="I48" s="4"/>
     </row>
@@ -5155,7 +5216,7 @@
         <v>28</v>
       </c>
       <c r="H49" s="13" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="I49" s="4"/>
     </row>
@@ -5183,7 +5244,7 @@
         <v>14</v>
       </c>
       <c r="H50" s="13" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="I50" s="4"/>
     </row>
@@ -5211,7 +5272,7 @@
         <v>142</v>
       </c>
       <c r="H51" s="17" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I51" s="4"/>
     </row>
@@ -5239,7 +5300,7 @@
         <v>143</v>
       </c>
       <c r="H52" s="17" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I52" s="4"/>
     </row>
@@ -5267,7 +5328,7 @@
         <v>145</v>
       </c>
       <c r="H53" s="19" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="I53" s="4"/>
     </row>
@@ -5293,7 +5354,7 @@
         <v>87</v>
       </c>
       <c r="H54" s="19" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="I54" s="4"/>
     </row>
@@ -5345,7 +5406,7 @@
       </c>
       <c r="G56" s="4"/>
       <c r="H56" s="13" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="I56" s="4"/>
     </row>
@@ -5397,7 +5458,7 @@
       </c>
       <c r="G58" s="4"/>
       <c r="H58" s="19" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="I58" s="4"/>
     </row>
@@ -5425,7 +5486,7 @@
         <v>148</v>
       </c>
       <c r="H59" s="19" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="I59" s="4"/>
     </row>
@@ -5449,7 +5510,7 @@
       </c>
       <c r="G60" s="4"/>
       <c r="H60" s="19" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="I60" s="4"/>
     </row>
@@ -5473,7 +5534,7 @@
       </c>
       <c r="G61" s="4"/>
       <c r="H61" s="13" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="I61" s="4"/>
     </row>
@@ -5501,7 +5562,7 @@
         <v>151</v>
       </c>
       <c r="H62" s="19" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="I62" s="4"/>
     </row>
@@ -5525,7 +5586,7 @@
       </c>
       <c r="G63" s="4"/>
       <c r="H63" s="13" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="I63" s="4"/>
     </row>
@@ -5553,7 +5614,7 @@
         <v>154</v>
       </c>
       <c r="H64" s="19" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="I64" s="4"/>
     </row>
@@ -5581,7 +5642,7 @@
         <v>50</v>
       </c>
       <c r="H65" s="13" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="I65" s="4"/>
     </row>
@@ -5609,7 +5670,7 @@
         <v>53</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="I66" s="4"/>
     </row>
@@ -5637,7 +5698,7 @@
         <v>270</v>
       </c>
       <c r="H67" s="19" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="I67" s="4"/>
     </row>
@@ -5665,7 +5726,7 @@
         <v>241</v>
       </c>
       <c r="H68" s="19" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="I68" s="4"/>
     </row>
@@ -5693,7 +5754,7 @@
         <v>271</v>
       </c>
       <c r="H69" s="19" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="I69" s="4"/>
     </row>
@@ -5721,7 +5782,7 @@
         <v>272</v>
       </c>
       <c r="H70" s="19" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="I70" s="4"/>
     </row>
@@ -5749,7 +5810,7 @@
         <v>197</v>
       </c>
       <c r="H71" s="17" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="I71" s="4"/>
     </row>
@@ -5762,22 +5823,22 @@
         <v>14</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H72" s="19" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="I72" s="4"/>
     </row>
@@ -5790,22 +5851,22 @@
         <v>19</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H73" s="17" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="I73" s="4"/>
     </row>
@@ -5818,22 +5879,22 @@
         <v>16</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H74" s="17" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="I74" s="4"/>
     </row>
@@ -5861,7 +5922,7 @@
         <v>273</v>
       </c>
       <c r="H75" s="19" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="I75" s="4"/>
     </row>
@@ -5889,7 +5950,7 @@
         <v>275</v>
       </c>
       <c r="H76" s="19" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="I76" s="4"/>
     </row>
@@ -5917,7 +5978,7 @@
         <v>203</v>
       </c>
       <c r="H77" s="19" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="I77" s="4"/>
     </row>
@@ -5930,22 +5991,22 @@
         <v>22</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="H78" s="19" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="I78" s="4"/>
     </row>
@@ -5958,22 +6019,22 @@
         <v>23</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H79" s="17" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="I79" s="4"/>
     </row>
@@ -5986,22 +6047,22 @@
         <v>24</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="H80" s="17" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="I80" s="4"/>
     </row>
@@ -6029,7 +6090,7 @@
         <v>206</v>
       </c>
       <c r="H81" s="19" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="I81" s="4"/>
     </row>
@@ -6057,7 +6118,7 @@
         <v>209</v>
       </c>
       <c r="H82" s="19" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="I82" s="4"/>
     </row>
@@ -6085,7 +6146,7 @@
         <v>211</v>
       </c>
       <c r="H83" s="19" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="I83" s="4"/>
     </row>
@@ -6113,7 +6174,7 @@
         <v>213</v>
       </c>
       <c r="H84" s="17" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="I84" s="4"/>
     </row>
@@ -6126,22 +6187,22 @@
         <v>27</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D85" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="F85" s="4" t="s">
+        <v>480</v>
+      </c>
+      <c r="G85" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="H85" s="19" t="s">
         <v>484</v>
-      </c>
-      <c r="G85" s="4" t="s">
-        <v>478</v>
-      </c>
-      <c r="H85" s="19" t="s">
-        <v>488</v>
       </c>
       <c r="I85" s="4"/>
     </row>
@@ -6169,7 +6230,7 @@
         <v>216</v>
       </c>
       <c r="H86" s="19" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="I86" s="4"/>
     </row>
@@ -6182,22 +6243,22 @@
         <v>26</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="G87" s="4" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="H87" s="19" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="I87" s="4"/>
     </row>
@@ -6251,7 +6312,7 @@
         <v>91</v>
       </c>
       <c r="H89" s="17" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="I89" s="4"/>
     </row>
@@ -6277,7 +6338,7 @@
       </c>
       <c r="G90" s="4"/>
       <c r="H90" s="13" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="I90" s="4"/>
     </row>
@@ -6305,7 +6366,7 @@
         <v>218</v>
       </c>
       <c r="H91" s="19" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="I91" s="4"/>
     </row>
@@ -6333,7 +6394,7 @@
         <v>278</v>
       </c>
       <c r="H92" s="13" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="I92" s="4"/>
     </row>
@@ -6361,7 +6422,7 @@
         <v>279</v>
       </c>
       <c r="H93" s="21" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="I93" s="4"/>
     </row>
@@ -6389,7 +6450,7 @@
         <v>259</v>
       </c>
       <c r="H94" s="9" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="I94" s="4"/>
     </row>
@@ -6417,7 +6478,7 @@
         <v>113</v>
       </c>
       <c r="H95" s="19" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="I95" s="4"/>
     </row>
@@ -6499,7 +6560,7 @@
       </c>
       <c r="G98" s="4"/>
       <c r="H98" s="19" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="I98" s="4"/>
     </row>
@@ -6512,22 +6573,22 @@
         <v>15</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D99" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="G99" s="4" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="H99" s="17" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="I99" s="4"/>
     </row>
@@ -6540,19 +6601,19 @@
         <v>1</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D100" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="G100" s="4" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="H100" s="17" t="s">
         <v>352</v>
@@ -6568,22 +6629,22 @@
         <v>17</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D101" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="G101" s="4" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="H101" s="17" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="I101" s="4"/>
     </row>
@@ -6596,22 +6657,22 @@
         <v>20</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D102" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="G102" s="4" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="H102" s="17" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="I102" s="4"/>
     </row>
@@ -6624,22 +6685,22 @@
         <v>21</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D103" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="F103" s="4" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="G103" s="4" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="H103" s="19" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="I103" s="4"/>
     </row>
@@ -6652,22 +6713,22 @@
         <v>18</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D104" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="F104" s="4" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="G104" s="4" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="H104" s="13" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="I104" s="4"/>
     </row>
@@ -6680,22 +6741,22 @@
         <v>25</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D105" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="G105" s="4" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="H105" s="17" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="I105" s="4"/>
     </row>
@@ -6708,19 +6769,19 @@
         <v>2</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D106" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="G106" s="4" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="H106" s="17" t="s">
         <v>352</v>
@@ -6736,19 +6797,19 @@
         <v>3</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D107" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="G107" s="4" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="H107" s="17" t="s">
         <v>352</v>
@@ -6764,19 +6825,19 @@
         <v>4</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D108" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="F108" s="4" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="G108" s="4" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="H108" s="17" t="s">
         <v>352</v>
@@ -6807,7 +6868,7 @@
         <v>250</v>
       </c>
       <c r="H109" s="6" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="I109" s="4"/>
     </row>
@@ -6820,19 +6881,19 @@
         <v>5</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D110" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="F110" s="4" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="G110" s="4" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="H110" s="17" t="s">
         <v>352</v>
@@ -6848,19 +6909,19 @@
         <v>6</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D111" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E111" s="5" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="F111" s="4" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="G111" s="4" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="H111" s="17" t="s">
         <v>352</v>
@@ -6876,19 +6937,19 @@
         <v>7</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D112" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="F112" s="4" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="G112" s="4" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="H112" s="17" t="s">
         <v>352</v>
@@ -6904,19 +6965,19 @@
         <v>8</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D113" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="F113" s="4" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="G113" s="4" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="H113" s="17" t="s">
         <v>352</v>
@@ -6932,19 +6993,19 @@
         <v>9</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D114" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="F114" s="4" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="G114" s="4" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="H114" s="17" t="s">
         <v>352</v>
@@ -6960,22 +7021,22 @@
         <v>10</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D115" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="G115" s="4" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="H115" s="19" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="I115" s="4"/>
     </row>
@@ -6988,22 +7049,22 @@
         <v>11</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D116" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E116" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="F116" s="4" t="s">
         <v>441</v>
       </c>
-      <c r="F116" s="4" t="s">
-        <v>445</v>
-      </c>
       <c r="G116" s="4" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="H116" s="13" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="I116" s="4"/>
     </row>
@@ -7016,19 +7077,19 @@
         <v>12</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D117" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="F117" s="4" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="G117" s="4" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="H117" s="17" t="s">
         <v>352</v>
@@ -7044,19 +7105,19 @@
         <v>13</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D118" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="F118" s="4" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="G118" s="4" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="H118" s="17" t="s">
         <v>352</v>
@@ -7087,7 +7148,7 @@
         <v>29</v>
       </c>
       <c r="H119" s="19" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="I119" s="4"/>
     </row>
@@ -7115,7 +7176,7 @@
         <v>252</v>
       </c>
       <c r="H120" s="19" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="I120" s="4"/>
     </row>
@@ -7143,7 +7204,7 @@
         <v>104</v>
       </c>
       <c r="H121" s="19" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="I121" s="4"/>
     </row>
@@ -7171,7 +7232,7 @@
         <v>162</v>
       </c>
       <c r="H122" s="19" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="I122" s="4"/>
     </row>
@@ -7199,7 +7260,7 @@
         <v>225</v>
       </c>
       <c r="H123" s="19" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="I123" s="4"/>
     </row>
@@ -7227,7 +7288,7 @@
         <v>228</v>
       </c>
       <c r="H124" s="19" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="I124" s="4"/>
     </row>
@@ -7255,7 +7316,7 @@
         <v>10</v>
       </c>
       <c r="H125" s="19" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="I125" s="4"/>
     </row>
@@ -7281,7 +7342,7 @@
       </c>
       <c r="G126" s="4"/>
       <c r="H126" s="19" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="I126" s="4"/>
     </row>
@@ -7307,7 +7368,7 @@
       </c>
       <c r="G127" s="4"/>
       <c r="H127" s="19" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="I127" s="4"/>
     </row>
@@ -7335,7 +7396,7 @@
         <v>136</v>
       </c>
       <c r="H128" s="19" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="I128" s="4"/>
     </row>
@@ -7363,7 +7424,7 @@
         <v>139</v>
       </c>
       <c r="H129" s="19" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="I129" s="4"/>
     </row>
@@ -7391,7 +7452,7 @@
         <v>231</v>
       </c>
       <c r="H130" s="17" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="I130" s="4"/>
     </row>
@@ -7475,7 +7536,7 @@
         <v>37</v>
       </c>
       <c r="H133" s="13" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="I133" s="4"/>
     </row>
@@ -7503,7 +7564,7 @@
         <v>39</v>
       </c>
       <c r="H134" s="13" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="I134" s="4"/>
     </row>
@@ -7531,7 +7592,7 @@
         <v>41</v>
       </c>
       <c r="H135" s="19" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="I135" s="4"/>
     </row>
@@ -7557,7 +7618,7 @@
       </c>
       <c r="G136" s="4"/>
       <c r="H136" s="13" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="I136" s="4"/>
     </row>
@@ -7585,7 +7646,7 @@
         <v>43</v>
       </c>
       <c r="H137" s="17" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="I137" s="4"/>
     </row>
@@ -7613,7 +7674,7 @@
         <v>31</v>
       </c>
       <c r="H138" s="13" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="I138" s="23"/>
     </row>

</xml_diff>

<commit_message>
Maj docs plenière 9 juillet
</commit_message>
<xml_diff>
--- a/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
+++ b/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Geostandards-Risques\suivi\2024-05_06-Consultation-publique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7C6796-5E7A-4566-BED7-F693CE65B46F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877C6F1D-6904-41DD-AF51-26087A70F921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29475" yWindow="900" windowWidth="27435" windowHeight="10200" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Synthese Modele Commun" sheetId="3" r:id="rId1"/>
@@ -3815,8 +3815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815F14A-19BC-4DCE-8D31-81F595A4B0E7}">
   <dimension ref="A1:I138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Maj docs plenière 09/07
</commit_message>
<xml_diff>
--- a/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
+++ b/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Geostandards-Risques\suivi\2024-05_06-Consultation-publique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B41500-8BB6-4E0B-8B7F-52E3093D1FD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877C6F1D-6904-41DD-AF51-26087A70F921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Synthese Modele Commun" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="560">
   <si>
     <t>Organisme</t>
   </si>
@@ -1334,9 +1334,6 @@
     <t>OK, à remplacer</t>
   </si>
   <si>
-    <t>OK, à supprimer</t>
-  </si>
-  <si>
     <t>NOK
 Cet arrêté est déjà mentionné dans la partie cadre réglementaire</t>
   </si>
@@ -1344,9 +1341,6 @@
     <t>OK, à réordonner</t>
   </si>
   <si>
-    <t>A vérifier</t>
-  </si>
-  <si>
     <t>OK, à modifier</t>
   </si>
   <si>
@@ -1359,14 +1353,6 @@
   <si>
     <t>OK sur le principe
 La formulation "Produire les données métiers des études préalables" ne me semble pas correcte (l'établissement du zonage réglementaire est-il dans la phase d'étude préalable ?)</t>
-  </si>
-  <si>
-    <t>OK, on peut rajouter des liens et le mentionner dans les textes explicatifs</t>
-  </si>
-  <si>
-    <t>A priori, c'est la classe éléments de caracterisation d'aléa qui devrait permettre d'ajouter ces éléments.
-A voir si on peut la rajouter en classe facultative (dans cette version ou une suivante) ?
-Il faudrait la structure de cette table. Où peut-on la trouver ?</t>
   </si>
   <si>
     <t>OK sur le principe.
@@ -2087,50 +2073,112 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">OK, à corriger.
+    <t>A priori non pour l'instant. 
+=&gt; Envisager de produire un fichier de métadonnées type</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Intégré</t>
+  </si>
+  <si>
+    <t>N.A.</t>
+  </si>
+  <si>
+    <t>intégré</t>
+  </si>
+  <si>
+    <t>intégré (PPR)</t>
+  </si>
+  <si>
+    <t>OK suppression de la référence à l'addenda.</t>
+  </si>
+  <si>
+    <t>OK, à remplacer (et remplacement de la référence à ce document dans par celle au guide en page xx)</t>
+  </si>
+  <si>
+    <t>traité</t>
+  </si>
+  <si>
+    <t>integré</t>
+  </si>
+  <si>
+    <t>cf. commentaires PPR</t>
+  </si>
+  <si>
+    <t>integré (+ carte "approuvée" au lieu de "signée")
++ tables d'énumérations (PPR) + modèle UML + gabarits</t>
+  </si>
+  <si>
+    <t>Vérifier si possibilité de restreindre les valeurs de certains champs au niveau de modèle commun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK, à corriger.
 Cela remet-il en cause la typologie des ouvrages de protection (barrage et digues) ? =&gt; cf. commentaires PPR
 Une référence à la documentation de SIOUH II serait la bienvenue aussi
 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Typologie des ouvrages de protection à modifier. Proposition BRIL (+BRNT ?) à venir</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Non, à moins qu'il n'y ait une volonté de les transformer en PPR (cf. Sweet pepper)?
+  </si>
+  <si>
+    <t>Typologie des ouvrages de protection à modifier. Proposition BRIL (+BRNT ?) à venir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non, à moins qu'il n'y ait une volonté de les transformer en PPR (cf. Sweet pepper)?
 NB : certains champs obligatoires non renseignés dans PSS
 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Ne rendre obligatoire que les thématiques Procédures, Périmètres et Zonage Réglementaire?</t>
-    </r>
-  </si>
-  <si>
-    <t>A priori non pour l'instant. 
-=&gt; Envisager de produire un fichier de métadonnées type</t>
+  </si>
+  <si>
+    <t>Ne rendre obligatoire que les thématiques Procédures, Périmètres et Zonage Réglementaire?</t>
+  </si>
+  <si>
+    <t>something to do ?</t>
+  </si>
+  <si>
+    <t>A vérifier
+NB : il existe :
+- des PPRN sur Saint-Martin (risque cyclonique et multirsiques)
+- un PPRT sur la Guadeloupe (Baie Mahault)
+Rien sur Saint-Barthélémy, mais il me semble que le code de l'environnement peut aussi s'appliquer à Saint-Barthélémy, non ?</t>
+  </si>
+  <si>
+    <t>OK sur le principe, à modifier
+NB : cartographier l'aléa de référence est trop PPRN-centré =&gt; seulement "cartographier les aléas"</t>
+  </si>
+  <si>
+    <t>intégré (pour la première partie)</t>
+  </si>
+  <si>
+    <t>intégré (pour la partie "du PPR")</t>
+  </si>
+  <si>
+    <t>OK sur le principe. Pour éviter d'aloutrdir le schéma, on mentionne que ce sont les acteurs principaux de l'action qui sont sur le schéma</t>
+  </si>
+  <si>
+    <t>intégré (en accord avec commentaires précédents) + schémas mis à jour</t>
+  </si>
+  <si>
+    <t>intégré + schémas mis à jour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A priori, c'est la classe éléments de caracterisation d'aléa qui devrait permettre d'ajouter ces éléments.
+A voir si on peut la rajouter en classe facultative (dans cette version ou une suivante) ?
+Il faudrait la structure de cette table. Où peut-on la trouver ?
+Cf. :
+-structure LIC (LIGNE ISO COTE HAUTEUR D'EAU) du dictionnaire vigilance inondation du Sandre ? (linéaire)
+- Ligne_iso_cote de la DI (linéaire)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK, sur le principe.
+Reformulation ;  "dont les modalités sont relatives au type d'aléa"
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2216,11 +2264,6 @@
       <color theme="1"/>
       <name val="Wingdings"/>
       <charset val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -2321,7 +2364,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2334,10 +2376,13 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2345,7 +2390,26 @@
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="23">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2656,6 +2720,25 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2768,38 +2851,40 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E152CA69-C1C4-40F5-84A2-16C1484F79DC}" name="Tableau3" displayName="Tableau3" ref="A1:H20" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="A1:H20" xr:uid="{E152CA69-C1C4-40F5-84A2-16C1484F79DC}"/>
-  <tableColumns count="8">
-    <tableColumn id="8" xr3:uid="{FDEDA288-5661-4539-AEBA-9A87C20962E6}" name="Numero" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E152CA69-C1C4-40F5-84A2-16C1484F79DC}" name="Tableau3" displayName="Tableau3" ref="A1:I20" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+  <autoFilter ref="A1:I20" xr:uid="{E152CA69-C1C4-40F5-84A2-16C1484F79DC}"/>
+  <tableColumns count="9">
+    <tableColumn id="8" xr3:uid="{FDEDA288-5661-4539-AEBA-9A87C20962E6}" name="Numero" dataDxfId="20">
       <calculatedColumnFormula>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{635A3DB7-7204-4378-B92A-598A2491845D}" name="Colonne1" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{79A10EF1-8EC6-4A0F-BA8C-3DFA972C0085}" name="Organisme" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{B1796E2E-D6C3-4AA8-BE83-FC4F94A53A8A}" name="Type de commentaire:_x000a_(G)énéral  (M)étier (T)echnique (D)ocument" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{1412256D-CC49-4084-A346-F8B20C24D98A}" name="Page, _x000a_Paragraphe" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{5F39A908-2FFC-40EB-BF7C-360C193B6507}" name="Commentaire" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{D01F9F9F-406C-4050-A108-256D1A81EB43}" name="Modification proposée " dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{2B745299-03CE-435C-B9E5-654FA9CECC38}" name="Décision du GT CNIG Risques" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{635A3DB7-7204-4378-B92A-598A2491845D}" name="Colonne1" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{79A10EF1-8EC6-4A0F-BA8C-3DFA972C0085}" name="Organisme" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{B1796E2E-D6C3-4AA8-BE83-FC4F94A53A8A}" name="Type de commentaire:_x000a_(G)énéral  (M)étier (T)echnique (D)ocument" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{1412256D-CC49-4084-A346-F8B20C24D98A}" name="Page, _x000a_Paragraphe" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{5F39A908-2FFC-40EB-BF7C-360C193B6507}" name="Commentaire" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{D01F9F9F-406C-4050-A108-256D1A81EB43}" name="Modification proposée " dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{2B745299-03CE-435C-B9E5-654FA9CECC38}" name="Décision du GT CNIG Risques" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{8675ABB4-B445-45A5-A068-9D591F8235C6}" name="Action" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{847E454C-1CA0-45D6-9F56-3D5FFE89C0F5}" name="Tableau2" displayName="Tableau2" ref="A1:H138" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8">
-  <autoFilter ref="A1:H138" xr:uid="{847E454C-1CA0-45D6-9F56-3D5FFE89C0F5}"/>
-  <tableColumns count="8">
-    <tableColumn id="8" xr3:uid="{6862FBA5-3017-4233-B0D4-5BC2462198D0}" name="Colonne2" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{847E454C-1CA0-45D6-9F56-3D5FFE89C0F5}" name="Tableau2" displayName="Tableau2" ref="A1:I138" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9">
+  <autoFilter ref="A1:I138" xr:uid="{847E454C-1CA0-45D6-9F56-3D5FFE89C0F5}"/>
+  <tableColumns count="9">
+    <tableColumn id="8" xr3:uid="{6862FBA5-3017-4233-B0D4-5BC2462198D0}" name="Colonne2" dataDxfId="8">
       <calculatedColumnFormula>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{A8BB7BB0-4D6B-4A0E-A615-089BDEA55F36}" name="Colonne1" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{81E8B2D7-3970-4344-9966-2E0DDFB404DB}" name="Organisme" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{D152CE9B-5BA5-4879-B7DE-1CBF90027255}" name="Type de commentaire:(G)énéral  (M)étier (T)echnique (D)ocument" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{DE633778-26A0-4BDF-9CA2-36FE6DA84467}" name="Page, Paragraphe" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{378CA86A-0CF7-484A-BD7C-53282B21DE2F}" name="Commentaire" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{38052BD9-6BB2-443C-8278-BB11301B0221}" name="Modification proposée " dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{A2C2771F-6D33-454B-9C1D-FAE8B1231568}" name="Décision du GT CNIG Risques" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{A8BB7BB0-4D6B-4A0E-A615-089BDEA55F36}" name="Colonne1" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{81E8B2D7-3970-4344-9966-2E0DDFB404DB}" name="Organisme" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{D152CE9B-5BA5-4879-B7DE-1CBF90027255}" name="Type de commentaire:(G)énéral  (M)étier (T)echnique (D)ocument" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{DE633778-26A0-4BDF-9CA2-36FE6DA84467}" name="Page, Paragraphe" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{378CA86A-0CF7-484A-BD7C-53282B21DE2F}" name="Commentaire" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{38052BD9-6BB2-443C-8278-BB11301B0221}" name="Modification proposée " dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{A2C2771F-6D33-454B-9C1D-FAE8B1231568}" name="Décision du GT CNIG Risques" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{039CFFBD-CF12-4001-86EB-ECDCA01C3555}" name="Action" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3102,9 +3187,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939F5930-30D3-43D0-87E8-B00574FE9CE2}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
@@ -3122,7 +3207,7 @@
     <col min="10" max="16384" width="10.90625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>349</v>
       </c>
@@ -3147,8 +3232,11 @@
       <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="73" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I1" s="2" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="73" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-1</v>
@@ -3174,8 +3262,11 @@
       <c r="H2" s="17" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="92" x14ac:dyDescent="0.35">
+      <c r="I2" s="4" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-2</v>
@@ -3199,10 +3290,13 @@
         <v>332</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="92" x14ac:dyDescent="0.35">
+        <v>530</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-3</v>
@@ -3225,11 +3319,14 @@
       <c r="G4" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="H4" s="23" t="s">
+      <c r="H4" s="17" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="75.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I4" s="4" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="75.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-4</v>
@@ -3253,10 +3350,13 @@
         <v>305</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="89" customHeight="1" x14ac:dyDescent="0.35">
+        <v>531</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="89" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-5</v>
@@ -3282,8 +3382,11 @@
       <c r="H6" s="17" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="23" x14ac:dyDescent="0.35">
+      <c r="I6" s="4" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/DAPP/BIP-11</v>
@@ -3307,8 +3410,11 @@
       <c r="H7" s="18" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
+      <c r="I7" s="4" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-6</v>
@@ -3334,8 +3440,11 @@
       <c r="H8" s="17" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="92" x14ac:dyDescent="0.35">
+      <c r="I8" s="4" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-7</v>
@@ -3361,8 +3470,11 @@
       <c r="H9" s="17" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I9" s="24" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-1</v>
@@ -3388,8 +3500,11 @@
       <c r="H10" s="17" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I10" s="4" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-2</v>
@@ -3415,8 +3530,11 @@
       <c r="H11" s="17" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="103.5" x14ac:dyDescent="0.35">
+      <c r="I11" s="4" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-8</v>
@@ -3440,10 +3558,13 @@
         <v>315</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>525</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>cerema-6</v>
@@ -3469,8 +3590,11 @@
       <c r="H13" s="17" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="92" x14ac:dyDescent="0.35">
+      <c r="I13" s="4" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-9</v>
@@ -3496,8 +3620,11 @@
       <c r="H14" s="17" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="61" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I14" s="4" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="61" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-10</v>
@@ -3523,8 +3650,11 @@
       <c r="H15" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="68" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I15" s="4" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="68" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-3</v>
@@ -3548,10 +3678,13 @@
         <v>288</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="77" customHeight="1" x14ac:dyDescent="0.35">
+        <v>526</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="77" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-4</v>
@@ -3577,8 +3710,11 @@
       <c r="H17" s="17" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I17" s="4" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="111" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-5</v>
@@ -3602,10 +3738,13 @@
         <v>293</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>527</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SDCAP/PONSOH-13</v>
@@ -3628,11 +3767,14 @@
       <c r="G19" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="H19" s="24" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H19" s="25" t="s">
+        <v>546</v>
+      </c>
+      <c r="I19" s="24" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/DAPP/BIP-12</v>
@@ -3655,6 +3797,9 @@
       <c r="G20" s="4"/>
       <c r="H20" s="17" t="s">
         <v>360</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>541</v>
       </c>
     </row>
   </sheetData>
@@ -3670,8 +3815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815F14A-19BC-4DCE-8D31-81F595A4B0E7}">
   <dimension ref="A1:I138"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3684,10 +3829,11 @@
     <col min="6" max="6" width="44.08984375" style="3" customWidth="1"/>
     <col min="7" max="7" width="38" style="3" customWidth="1"/>
     <col min="8" max="8" width="51.81640625" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="10.90625" style="3"/>
+    <col min="9" max="9" width="22.26953125" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="10.90625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>348</v>
       </c>
@@ -3712,8 +3858,11 @@
       <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="57.5" x14ac:dyDescent="0.35">
+      <c r="I1" s="16" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-2</v>
@@ -3734,11 +3883,14 @@
         <v>242</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="24" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H2" s="25" t="s">
+        <v>548</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-3</v>
@@ -3759,11 +3911,14 @@
         <v>243</v>
       </c>
       <c r="G3" s="4"/>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="22" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I3" s="4" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-4</v>
@@ -3784,11 +3939,14 @@
         <v>244</v>
       </c>
       <c r="G4" s="9"/>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="22" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I4" s="4" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-5</v>
@@ -3809,11 +3967,14 @@
         <v>245</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="25" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="126.5" x14ac:dyDescent="0.35">
+      <c r="H5" s="22" t="s">
+        <v>533</v>
+      </c>
+      <c r="I5" s="24" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="126.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP-0</v>
@@ -3835,8 +3996,11 @@
       <c r="H6" s="17" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="57.5" x14ac:dyDescent="0.35">
+      <c r="I6" s="4" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-9</v>
@@ -3860,8 +4024,11 @@
       <c r="H7" s="13" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="46" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I7" s="4" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="46" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-14</v>
@@ -3882,11 +4049,12 @@
       <c r="G8" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="H8" s="19" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="23" x14ac:dyDescent="0.35">
+      <c r="I8" s="24"/>
+    </row>
+    <row r="9" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-15</v>
@@ -3907,11 +4075,12 @@
       <c r="G9" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="H9" s="19" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="74" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I9" s="24"/>
+    </row>
+    <row r="10" spans="1:9" ht="74" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-2</v>
@@ -3937,8 +4106,9 @@
       <c r="H10" s="17" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I10" s="24"/>
+    </row>
+    <row r="11" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-3</v>
@@ -3964,8 +4134,9 @@
       <c r="H11" s="17" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="74" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I11" s="24"/>
+    </row>
+    <row r="12" spans="1:9" ht="74" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-1</v>
@@ -3991,8 +4162,11 @@
       <c r="H12" s="17" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I12" s="4" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-1</v>
@@ -4016,10 +4190,13 @@
         <v>166</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="161" x14ac:dyDescent="0.35">
+        <v>524</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="161" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-2</v>
@@ -4043,10 +4220,13 @@
         <v>254</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+        <v>540</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-3</v>
@@ -4070,10 +4250,13 @@
         <v>62</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+        <v>539</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-1</v>
@@ -4097,10 +4280,13 @@
         <v>117</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="103.5" x14ac:dyDescent="0.35">
+        <v>532</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-4</v>
@@ -4124,10 +4310,13 @@
         <v>65</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+        <v>380</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-4</v>
@@ -4151,10 +4340,13 @@
         <v>175</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>381</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-5</v>
@@ -4177,11 +4369,14 @@
       <c r="G19" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="H19" s="20" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
+      <c r="H19" s="19" t="s">
+        <v>551</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-6</v>
@@ -4204,11 +4399,14 @@
       <c r="G20" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="H20" s="17" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H20" s="19" t="s">
+        <v>552</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-2</v>
@@ -4232,10 +4430,13 @@
         <v>120</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+        <v>382</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-3</v>
@@ -4259,10 +4460,13 @@
         <v>122</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="23" x14ac:dyDescent="0.35">
+        <v>383</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-5</v>
@@ -4286,10 +4490,13 @@
         <v>178</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+        <v>384</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-4</v>
@@ -4312,11 +4519,14 @@
       <c r="G24" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="H24" s="20" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="23" x14ac:dyDescent="0.35">
+      <c r="H24" s="19" t="s">
+        <v>385</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-5</v>
@@ -4340,10 +4550,13 @@
         <v>125</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>384</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="71.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-7</v>
@@ -4366,11 +4579,14 @@
       <c r="G26" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="H26" s="17" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="H26" s="19" t="s">
+        <v>555</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-6</v>
@@ -4396,8 +4612,11 @@
       <c r="H27" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="96" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I27" s="4" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="115" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-</v>
@@ -4418,11 +4637,12 @@
       <c r="G28" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="H28" s="20" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H28" s="19" t="s">
+        <v>558</v>
+      </c>
+      <c r="I28" s="24"/>
+    </row>
+    <row r="29" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-8</v>
@@ -4445,11 +4665,14 @@
       <c r="G29" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="H29" s="17" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H29" s="19" t="s">
+        <v>559</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-9</v>
@@ -4472,11 +4695,12 @@
       <c r="G30" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="H30" s="20" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="69" x14ac:dyDescent="0.35">
+      <c r="H30" s="19" t="s">
+        <v>386</v>
+      </c>
+      <c r="I30" s="4"/>
+    </row>
+    <row r="31" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-6</v>
@@ -4499,11 +4723,12 @@
       <c r="G31" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="H31" s="20" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="92" x14ac:dyDescent="0.35">
+      <c r="H31" s="19" t="s">
+        <v>387</v>
+      </c>
+      <c r="I31" s="4"/>
+    </row>
+    <row r="32" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-7</v>
@@ -4526,11 +4751,12 @@
       <c r="G32" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="H32" s="20" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H32" s="19" t="s">
+        <v>389</v>
+      </c>
+      <c r="I32" s="4"/>
+    </row>
+    <row r="33" spans="1:9" ht="41" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-10</v>
@@ -4552,10 +4778,11 @@
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="17" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="57.5" x14ac:dyDescent="0.35">
+        <v>388</v>
+      </c>
+      <c r="I33" s="4"/>
+    </row>
+    <row r="34" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-7</v>
@@ -4578,11 +4805,12 @@
       <c r="G34" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="H34" s="20" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H34" s="19" t="s">
+        <v>390</v>
+      </c>
+      <c r="I34" s="4"/>
+    </row>
+    <row r="35" spans="1:9" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-11</v>
@@ -4604,10 +4832,11 @@
         <v>82</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
+        <v>388</v>
+      </c>
+      <c r="I35" s="4"/>
+    </row>
+    <row r="36" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-1</v>
@@ -4631,10 +4860,11 @@
         <v>19</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>391</v>
+      </c>
+      <c r="I36" s="4"/>
+    </row>
+    <row r="37" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-21</v>
@@ -4658,10 +4888,11 @@
         <v>99</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="92" x14ac:dyDescent="0.35">
+        <v>392</v>
+      </c>
+      <c r="I37" s="4"/>
+    </row>
+    <row r="38" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-</v>
@@ -4677,16 +4908,17 @@
         <v>369</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="H38" s="20" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="207" x14ac:dyDescent="0.35">
+      <c r="H38" s="19" t="s">
+        <v>393</v>
+      </c>
+      <c r="I38" s="4"/>
+    </row>
+    <row r="39" spans="1:9" ht="207" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-</v>
@@ -4702,16 +4934,17 @@
         <v>369</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="H39" s="20" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
+      <c r="H39" s="19" t="s">
+        <v>393</v>
+      </c>
+      <c r="I39" s="4"/>
+    </row>
+    <row r="40" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-8</v>
@@ -4734,11 +4967,12 @@
       <c r="G40" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="H40" s="20" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H40" s="19" t="s">
+        <v>396</v>
+      </c>
+      <c r="I40" s="4"/>
+    </row>
+    <row r="41" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-8</v>
@@ -4761,11 +4995,12 @@
       <c r="G41" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="H41" s="20" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H41" s="19" t="s">
+        <v>397</v>
+      </c>
+      <c r="I41" s="4"/>
+    </row>
+    <row r="42" spans="1:9" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-12</v>
@@ -4786,11 +5021,12 @@
         <v>84</v>
       </c>
       <c r="G42" s="4"/>
-      <c r="H42" s="20" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="92" x14ac:dyDescent="0.35">
+      <c r="H42" s="19" t="s">
+        <v>398</v>
+      </c>
+      <c r="I42" s="4"/>
+    </row>
+    <row r="43" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-4</v>
@@ -4814,10 +5050,11 @@
         <v>26</v>
       </c>
       <c r="H43" s="13" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="38" customHeight="1" x14ac:dyDescent="0.35">
+        <v>400</v>
+      </c>
+      <c r="I43" s="4"/>
+    </row>
+    <row r="44" spans="1:9" ht="38" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-2</v>
@@ -4840,11 +5077,12 @@
       <c r="G44" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H44" s="20" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="H44" s="19" t="s">
+        <v>401</v>
+      </c>
+      <c r="I44" s="4"/>
+    </row>
+    <row r="45" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/BRNT-22</v>
@@ -4865,11 +5103,12 @@
         <v>102</v>
       </c>
       <c r="G45" s="4"/>
-      <c r="H45" s="20" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+      <c r="H45" s="19" t="s">
+        <v>402</v>
+      </c>
+      <c r="I45" s="4"/>
+    </row>
+    <row r="46" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-8</v>
@@ -4892,11 +5131,12 @@
       <c r="G46" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H46" s="20" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H46" s="19" t="s">
+        <v>403</v>
+      </c>
+      <c r="I46" s="4"/>
+    </row>
+    <row r="47" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-24</v>
@@ -4919,11 +5159,12 @@
       <c r="G47" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="H47" s="20" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H47" s="19" t="s">
+        <v>402</v>
+      </c>
+      <c r="I47" s="4"/>
+    </row>
+    <row r="48" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-3</v>
@@ -4947,10 +5188,11 @@
         <v>25</v>
       </c>
       <c r="H48" s="17" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+        <v>404</v>
+      </c>
+      <c r="I48" s="4"/>
+    </row>
+    <row r="49" spans="1:9" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-5</v>
@@ -4974,10 +5216,11 @@
         <v>28</v>
       </c>
       <c r="H49" s="13" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="69" x14ac:dyDescent="0.35">
+        <v>399</v>
+      </c>
+      <c r="I49" s="4"/>
+    </row>
+    <row r="50" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT07-2</v>
@@ -5001,10 +5244,11 @@
         <v>14</v>
       </c>
       <c r="H50" s="13" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+        <v>405</v>
+      </c>
+      <c r="I50" s="4"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-11</v>
@@ -5028,10 +5272,11 @@
         <v>142</v>
       </c>
       <c r="H51" s="17" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+        <v>382</v>
+      </c>
+      <c r="I51" s="4"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-12</v>
@@ -5055,10 +5300,11 @@
         <v>143</v>
       </c>
       <c r="H52" s="17" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+        <v>382</v>
+      </c>
+      <c r="I52" s="4"/>
+    </row>
+    <row r="53" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-13</v>
@@ -5081,11 +5327,12 @@
       <c r="G53" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="H53" s="20" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="36.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H53" s="19" t="s">
+        <v>406</v>
+      </c>
+      <c r="I53" s="4"/>
+    </row>
+    <row r="54" spans="1:9" ht="36.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-14</v>
@@ -5106,11 +5353,12 @@
       <c r="G54" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="H54" s="20" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H54" s="19" t="s">
+        <v>407</v>
+      </c>
+      <c r="I54" s="4"/>
+    </row>
+    <row r="55" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-13</v>
@@ -5134,8 +5382,9 @@
       <c r="H55" s="17" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" ht="57.5" x14ac:dyDescent="0.35">
+      <c r="I55" s="4"/>
+    </row>
+    <row r="56" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-15</v>
@@ -5157,10 +5406,11 @@
       </c>
       <c r="G56" s="4"/>
       <c r="H56" s="13" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+        <v>410</v>
+      </c>
+      <c r="I56" s="4"/>
+    </row>
+    <row r="57" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-9</v>
@@ -5186,8 +5436,9 @@
       <c r="H57" s="17" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" ht="184" x14ac:dyDescent="0.35">
+      <c r="I57" s="4"/>
+    </row>
+    <row r="58" spans="1:9" ht="184" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5206,11 +5457,12 @@
         <v>346</v>
       </c>
       <c r="G58" s="4"/>
-      <c r="H58" s="20" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+      <c r="H58" s="19" t="s">
+        <v>408</v>
+      </c>
+      <c r="I58" s="4"/>
+    </row>
+    <row r="59" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-14</v>
@@ -5233,11 +5485,12 @@
       <c r="G59" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="H59" s="20" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="92" x14ac:dyDescent="0.35">
+      <c r="H59" s="19" t="s">
+        <v>409</v>
+      </c>
+      <c r="I59" s="4"/>
+    </row>
+    <row r="60" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5256,11 +5509,12 @@
         <v>345</v>
       </c>
       <c r="G60" s="4"/>
-      <c r="H60" s="20" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="230" x14ac:dyDescent="0.35">
+      <c r="H60" s="19" t="s">
+        <v>413</v>
+      </c>
+      <c r="I60" s="4"/>
+    </row>
+    <row r="61" spans="1:9" ht="230" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5280,10 +5534,11 @@
       </c>
       <c r="G61" s="4"/>
       <c r="H61" s="13" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
+        <v>411</v>
+      </c>
+      <c r="I61" s="4"/>
+    </row>
+    <row r="62" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A62" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-15</v>
@@ -5306,11 +5561,12 @@
       <c r="G62" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="H62" s="20" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+      <c r="H62" s="19" t="s">
+        <v>415</v>
+      </c>
+      <c r="I62" s="4"/>
+    </row>
+    <row r="63" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5330,10 +5586,11 @@
       </c>
       <c r="G63" s="4"/>
       <c r="H63" s="13" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+        <v>412</v>
+      </c>
+      <c r="I63" s="4"/>
+    </row>
+    <row r="64" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A64" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-16</v>
@@ -5356,11 +5613,12 @@
       <c r="G64" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="H64" s="20" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+      <c r="H64" s="19" t="s">
+        <v>414</v>
+      </c>
+      <c r="I64" s="4"/>
+    </row>
+    <row r="65" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT01-3</v>
@@ -5384,10 +5642,11 @@
         <v>50</v>
       </c>
       <c r="H65" s="13" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+        <v>416</v>
+      </c>
+      <c r="I65" s="4"/>
+    </row>
+    <row r="66" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDTM 83-1</v>
@@ -5411,10 +5670,11 @@
         <v>53</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="174" x14ac:dyDescent="0.35">
+        <v>417</v>
+      </c>
+      <c r="I66" s="4"/>
+    </row>
+    <row r="67" spans="1:9" ht="174" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-10</v>
@@ -5437,11 +5697,12 @@
       <c r="G67" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="H67" s="20" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="88" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H67" s="19" t="s">
+        <v>481</v>
+      </c>
+      <c r="I67" s="4"/>
+    </row>
+    <row r="68" spans="1:9" ht="88" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-1</v>
@@ -5464,11 +5725,12 @@
       <c r="G68" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="H68" s="20" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="103" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H68" s="19" t="s">
+        <v>418</v>
+      </c>
+      <c r="I68" s="4"/>
+    </row>
+    <row r="69" spans="1:9" ht="103" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-11</v>
@@ -5491,11 +5753,12 @@
       <c r="G69" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="H69" s="20" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H69" s="19" t="s">
+        <v>482</v>
+      </c>
+      <c r="I69" s="4"/>
+    </row>
+    <row r="70" spans="1:9" ht="111" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-12</v>
@@ -5518,11 +5781,12 @@
       <c r="G70" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="H70" s="20" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H70" s="19" t="s">
+        <v>529</v>
+      </c>
+      <c r="I70" s="4"/>
+    </row>
+    <row r="71" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-13</v>
@@ -5546,11 +5810,12 @@
         <v>197</v>
       </c>
       <c r="H71" s="17" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
-      <c r="A72" s="21" t="str">
+        <v>483</v>
+      </c>
+      <c r="I71" s="4"/>
+    </row>
+    <row r="72" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A72" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-14</v>
       </c>
@@ -5558,26 +5823,27 @@
         <v>14</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>455</v>
-      </c>
-      <c r="H72" s="20" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A73" s="21" t="str">
+        <v>451</v>
+      </c>
+      <c r="H72" s="19" t="s">
+        <v>484</v>
+      </c>
+      <c r="I72" s="4"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A73" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-19</v>
       </c>
@@ -5585,26 +5851,27 @@
         <v>19</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H73" s="17" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A74" s="21" t="str">
+        <v>485</v>
+      </c>
+      <c r="I73" s="4"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A74" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-16</v>
       </c>
@@ -5612,25 +5879,26 @@
         <v>16</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H74" s="17" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.35">
+        <v>485</v>
+      </c>
+      <c r="I74" s="4"/>
+    </row>
+    <row r="75" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-14</v>
@@ -5653,11 +5921,12 @@
       <c r="G75" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="H75" s="20" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" ht="115" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H75" s="19" t="s">
+        <v>486</v>
+      </c>
+      <c r="I75" s="4"/>
+    </row>
+    <row r="76" spans="1:9" ht="115" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-15</v>
@@ -5680,11 +5949,12 @@
       <c r="G76" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="H76" s="20" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="H76" s="19" t="s">
+        <v>490</v>
+      </c>
+      <c r="I76" s="4"/>
+    </row>
+    <row r="77" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A77" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-16</v>
@@ -5707,12 +5977,13 @@
       <c r="G77" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="H77" s="20" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
-      <c r="A78" s="21" t="str">
+      <c r="H77" s="19" t="s">
+        <v>487</v>
+      </c>
+      <c r="I77" s="4"/>
+    </row>
+    <row r="78" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A78" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-22</v>
       </c>
@@ -5720,26 +5991,27 @@
         <v>22</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>469</v>
-      </c>
-      <c r="H78" s="20" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A79" s="21" t="str">
+        <v>465</v>
+      </c>
+      <c r="H78" s="19" t="s">
+        <v>484</v>
+      </c>
+      <c r="I78" s="4"/>
+    </row>
+    <row r="79" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+      <c r="A79" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-23</v>
       </c>
@@ -5747,26 +6019,27 @@
         <v>23</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H79" s="17" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A80" s="21" t="str">
+        <v>485</v>
+      </c>
+      <c r="I79" s="4"/>
+    </row>
+    <row r="80" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+      <c r="A80" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-24</v>
       </c>
@@ -5774,25 +6047,26 @@
         <v>24</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="H80" s="17" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+        <v>485</v>
+      </c>
+      <c r="I80" s="4"/>
+    </row>
+    <row r="81" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A81" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-17</v>
@@ -5815,11 +6089,12 @@
       <c r="G81" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="H81" s="20" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="H81" s="19" t="s">
+        <v>488</v>
+      </c>
+      <c r="I81" s="4"/>
+    </row>
+    <row r="82" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A82" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-18</v>
@@ -5842,11 +6117,12 @@
       <c r="G82" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="H82" s="20" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" ht="69" x14ac:dyDescent="0.35">
+      <c r="H82" s="19" t="s">
+        <v>489</v>
+      </c>
+      <c r="I82" s="4"/>
+    </row>
+    <row r="83" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A83" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-19</v>
@@ -5869,11 +6145,12 @@
       <c r="G83" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="H83" s="20" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" ht="23" x14ac:dyDescent="0.35">
+      <c r="H83" s="19" t="s">
+        <v>491</v>
+      </c>
+      <c r="I83" s="4"/>
+    </row>
+    <row r="84" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A84" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-20</v>
@@ -5897,11 +6174,12 @@
         <v>213</v>
       </c>
       <c r="H84" s="17" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" ht="36.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="21" t="str">
+        <v>492</v>
+      </c>
+      <c r="I84" s="4"/>
+    </row>
+    <row r="85" spans="1:9" ht="36.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-27</v>
       </c>
@@ -5909,25 +6187,26 @@
         <v>27</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D85" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="F85" s="4" t="s">
+        <v>480</v>
+      </c>
+      <c r="G85" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="H85" s="19" t="s">
         <v>484</v>
       </c>
-      <c r="G85" s="4" t="s">
-        <v>478</v>
-      </c>
-      <c r="H85" s="20" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="I85" s="4"/>
+    </row>
+    <row r="86" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-21</v>
@@ -5950,12 +6229,13 @@
       <c r="G86" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="H86" s="20" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="21" t="str">
+      <c r="H86" s="19" t="s">
+        <v>493</v>
+      </c>
+      <c r="I86" s="4"/>
+    </row>
+    <row r="87" spans="1:9" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-26</v>
       </c>
@@ -5963,25 +6243,26 @@
         <v>26</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="G87" s="4" t="s">
-        <v>469</v>
-      </c>
-      <c r="H87" s="20" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+        <v>465</v>
+      </c>
+      <c r="H87" s="19" t="s">
+        <v>484</v>
+      </c>
+      <c r="I87" s="4"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-17</v>
@@ -6007,8 +6288,9 @@
       <c r="H88" s="17" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="I88" s="4"/>
+    </row>
+    <row r="89" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A89" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-16</v>
@@ -6030,10 +6312,11 @@
         <v>91</v>
       </c>
       <c r="H89" s="17" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>494</v>
+      </c>
+      <c r="I89" s="4"/>
+    </row>
+    <row r="90" spans="1:9" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-17</v>
@@ -6055,10 +6338,11 @@
       </c>
       <c r="G90" s="4"/>
       <c r="H90" s="13" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+        <v>495</v>
+      </c>
+      <c r="I90" s="4"/>
+    </row>
+    <row r="91" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A91" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-22</v>
@@ -6081,11 +6365,12 @@
       <c r="G91" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="H91" s="20" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
+      <c r="H91" s="19" t="s">
+        <v>496</v>
+      </c>
+      <c r="I91" s="4"/>
+    </row>
+    <row r="92" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A92" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-23</v>
@@ -6109,10 +6394,11 @@
         <v>278</v>
       </c>
       <c r="H92" s="13" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" ht="80.5" x14ac:dyDescent="0.35">
+        <v>497</v>
+      </c>
+      <c r="I92" s="4"/>
+    </row>
+    <row r="93" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A93" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-24</v>
@@ -6135,11 +6421,12 @@
       <c r="G93" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="H93" s="22" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" ht="113" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H93" s="21" t="s">
+        <v>498</v>
+      </c>
+      <c r="I93" s="4"/>
+    </row>
+    <row r="94" spans="1:9" ht="113" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/PoNSOH-26</v>
@@ -6163,10 +6450,11 @@
         <v>259</v>
       </c>
       <c r="H94" s="9" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>528</v>
+      </c>
+      <c r="I94" s="4"/>
+    </row>
+    <row r="95" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/PoNSOH-27</v>
@@ -6189,11 +6477,12 @@
       <c r="G95" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="H95" s="20" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H95" s="19" t="s">
+        <v>499</v>
+      </c>
+      <c r="I95" s="4"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-18</v>
@@ -6219,8 +6508,9 @@
       <c r="H96" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I96" s="4"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-19</v>
@@ -6246,8 +6536,9 @@
       <c r="H97" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" ht="96.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I97" s="4"/>
+    </row>
+    <row r="98" spans="1:9" ht="96.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-18</v>
@@ -6268,12 +6559,13 @@
         <v>257</v>
       </c>
       <c r="G98" s="4"/>
-      <c r="H98" s="20" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" ht="23" x14ac:dyDescent="0.35">
-      <c r="A99" s="21" t="str">
+      <c r="H98" s="19" t="s">
+        <v>500</v>
+      </c>
+      <c r="I98" s="4"/>
+    </row>
+    <row r="99" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="A99" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-15</v>
       </c>
@@ -6281,26 +6573,27 @@
         <v>15</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D99" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="G99" s="4" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="H99" s="17" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="21" t="str">
+        <v>502</v>
+      </c>
+      <c r="I99" s="4"/>
+    </row>
+    <row r="100" spans="1:9" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-1</v>
       </c>
@@ -6308,26 +6601,27 @@
         <v>1</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D100" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="G100" s="4" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="H100" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" ht="23" x14ac:dyDescent="0.35">
-      <c r="A101" s="21" t="str">
+      <c r="I100" s="4"/>
+    </row>
+    <row r="101" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="A101" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-17</v>
       </c>
@@ -6335,26 +6629,27 @@
         <v>17</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D101" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="G101" s="4" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="H101" s="17" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" ht="23" x14ac:dyDescent="0.35">
-      <c r="A102" s="21" t="str">
+        <v>502</v>
+      </c>
+      <c r="I101" s="4"/>
+    </row>
+    <row r="102" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="A102" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-20</v>
       </c>
@@ -6362,26 +6657,27 @@
         <v>20</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D102" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="G102" s="4" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="H102" s="17" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" ht="37.5" x14ac:dyDescent="0.35">
-      <c r="A103" s="21" t="str">
+        <v>502</v>
+      </c>
+      <c r="I102" s="4"/>
+    </row>
+    <row r="103" spans="1:9" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="A103" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-21</v>
       </c>
@@ -6389,26 +6685,27 @@
         <v>21</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D103" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="F103" s="4" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="G103" s="4" t="s">
-        <v>444</v>
-      </c>
-      <c r="H103" s="20" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
-      <c r="A104" s="21" t="str">
+        <v>440</v>
+      </c>
+      <c r="H103" s="19" t="s">
+        <v>503</v>
+      </c>
+      <c r="I103" s="4"/>
+    </row>
+    <row r="104" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A104" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-18</v>
       </c>
@@ -6416,26 +6713,27 @@
         <v>18</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D104" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="F104" s="4" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="G104" s="4" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="H104" s="13" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
-      <c r="A105" s="21" t="str">
+        <v>504</v>
+      </c>
+      <c r="I104" s="4"/>
+    </row>
+    <row r="105" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A105" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-25</v>
       </c>
@@ -6443,26 +6741,27 @@
         <v>25</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D105" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="G105" s="4" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="H105" s="17" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" ht="23" x14ac:dyDescent="0.35">
-      <c r="A106" s="21" t="str">
+        <v>502</v>
+      </c>
+      <c r="I105" s="4"/>
+    </row>
+    <row r="106" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="A106" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-2</v>
       </c>
@@ -6470,26 +6769,27 @@
         <v>2</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D106" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="G106" s="4" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="H106" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" ht="23" x14ac:dyDescent="0.35">
-      <c r="A107" s="21" t="str">
+      <c r="I106" s="4"/>
+    </row>
+    <row r="107" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="A107" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-3</v>
       </c>
@@ -6497,26 +6797,27 @@
         <v>3</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D107" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="G107" s="4" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="H107" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" ht="23" x14ac:dyDescent="0.35">
-      <c r="A108" s="21" t="str">
+      <c r="I107" s="4"/>
+    </row>
+    <row r="108" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="A108" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-4</v>
       </c>
@@ -6524,25 +6825,26 @@
         <v>4</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D108" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="F108" s="4" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="G108" s="4" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="H108" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+      <c r="I108" s="4"/>
+    </row>
+    <row r="109" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A109" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT01-1</v>
@@ -6566,11 +6868,12 @@
         <v>250</v>
       </c>
       <c r="H109" s="6" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" ht="23" x14ac:dyDescent="0.35">
-      <c r="A110" s="21" t="str">
+        <v>501</v>
+      </c>
+      <c r="I109" s="4"/>
+    </row>
+    <row r="110" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="A110" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-5</v>
       </c>
@@ -6578,26 +6881,27 @@
         <v>5</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D110" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="F110" s="4" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="G110" s="4" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="H110" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" ht="23" x14ac:dyDescent="0.35">
-      <c r="A111" s="21" t="str">
+      <c r="I110" s="4"/>
+    </row>
+    <row r="111" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="A111" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-6</v>
       </c>
@@ -6605,26 +6909,27 @@
         <v>6</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D111" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E111" s="5" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="F111" s="4" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="G111" s="4" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="H111" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
-      <c r="A112" s="21" t="str">
+      <c r="I111" s="4"/>
+    </row>
+    <row r="112" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A112" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-7</v>
       </c>
@@ -6632,26 +6937,27 @@
         <v>7</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D112" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="F112" s="4" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="G112" s="4" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="H112" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" ht="23" x14ac:dyDescent="0.35">
-      <c r="A113" s="21" t="str">
+      <c r="I112" s="4"/>
+    </row>
+    <row r="113" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="A113" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-8</v>
       </c>
@@ -6659,26 +6965,27 @@
         <v>8</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D113" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="F113" s="4" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="G113" s="4" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="H113" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
-      <c r="A114" s="21" t="str">
+      <c r="I113" s="4"/>
+    </row>
+    <row r="114" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="A114" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-9</v>
       </c>
@@ -6686,26 +6993,27 @@
         <v>9</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D114" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="F114" s="4" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="G114" s="4" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="H114" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" ht="69" x14ac:dyDescent="0.35">
-      <c r="A115" s="21" t="str">
+      <c r="I114" s="4"/>
+    </row>
+    <row r="115" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+      <c r="A115" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-10</v>
       </c>
@@ -6713,26 +7021,27 @@
         <v>10</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D115" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="G115" s="4" t="s">
-        <v>444</v>
-      </c>
-      <c r="H115" s="20" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" ht="23" x14ac:dyDescent="0.35">
-      <c r="A116" s="21" t="str">
+        <v>440</v>
+      </c>
+      <c r="H115" s="19" t="s">
+        <v>505</v>
+      </c>
+      <c r="I115" s="4"/>
+    </row>
+    <row r="116" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="A116" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-11</v>
       </c>
@@ -6740,26 +7049,27 @@
         <v>11</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D116" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E116" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="F116" s="4" t="s">
         <v>441</v>
       </c>
-      <c r="F116" s="4" t="s">
-        <v>445</v>
-      </c>
       <c r="G116" s="4" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="H116" s="13" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A117" s="21" t="str">
+        <v>506</v>
+      </c>
+      <c r="I116" s="4"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A117" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-12</v>
       </c>
@@ -6767,26 +7077,27 @@
         <v>12</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D117" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="F117" s="4" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="G117" s="4" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="H117" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" ht="23" x14ac:dyDescent="0.35">
-      <c r="A118" s="21" t="str">
+      <c r="I117" s="4"/>
+    </row>
+    <row r="118" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="A118" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-13</v>
       </c>
@@ -6794,25 +7105,26 @@
         <v>13</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D118" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="F118" s="4" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="G118" s="4" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="H118" s="17" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" ht="119.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I118" s="4"/>
+    </row>
+    <row r="119" spans="1:9" ht="119.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-6</v>
@@ -6835,11 +7147,12 @@
       <c r="G119" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H119" s="20" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" ht="57.5" x14ac:dyDescent="0.35">
+      <c r="H119" s="19" t="s">
+        <v>507</v>
+      </c>
+      <c r="I119" s="4"/>
+    </row>
+    <row r="120" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A120" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT01-2</v>
@@ -6862,11 +7175,12 @@
       <c r="G120" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="H120" s="20" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" ht="57.5" x14ac:dyDescent="0.35">
+      <c r="H120" s="19" t="s">
+        <v>499</v>
+      </c>
+      <c r="I120" s="4"/>
+    </row>
+    <row r="121" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A121" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-23</v>
@@ -6889,11 +7203,12 @@
       <c r="G121" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="H121" s="20" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H121" s="19" t="s">
+        <v>508</v>
+      </c>
+      <c r="I121" s="4"/>
+    </row>
+    <row r="122" spans="1:9" ht="78" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-20</v>
@@ -6916,11 +7231,12 @@
       <c r="G122" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="H122" s="20" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="H122" s="19" t="s">
+        <v>510</v>
+      </c>
+      <c r="I122" s="4"/>
+    </row>
+    <row r="123" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A123" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-25</v>
@@ -6943,11 +7259,12 @@
       <c r="G123" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="H123" s="20" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="H123" s="19" t="s">
+        <v>509</v>
+      </c>
+      <c r="I123" s="4"/>
+    </row>
+    <row r="124" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A124" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-26</v>
@@ -6970,11 +7287,12 @@
       <c r="G124" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="H124" s="20" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H124" s="19" t="s">
+        <v>511</v>
+      </c>
+      <c r="I124" s="4"/>
+    </row>
+    <row r="125" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT07-1</v>
@@ -6997,11 +7315,12 @@
       <c r="G125" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H125" s="20" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H125" s="19" t="s">
+        <v>512</v>
+      </c>
+      <c r="I125" s="4"/>
+    </row>
+    <row r="126" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-19</v>
@@ -7022,11 +7341,12 @@
         <v>94</v>
       </c>
       <c r="G126" s="4"/>
-      <c r="H126" s="20" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H126" s="19" t="s">
+        <v>513</v>
+      </c>
+      <c r="I126" s="4"/>
+    </row>
+    <row r="127" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-20</v>
@@ -7047,11 +7367,12 @@
         <v>95</v>
       </c>
       <c r="G127" s="4"/>
-      <c r="H127" s="20" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" ht="46" x14ac:dyDescent="0.35">
+      <c r="H127" s="19" t="s">
+        <v>514</v>
+      </c>
+      <c r="I127" s="4"/>
+    </row>
+    <row r="128" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A128" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-9</v>
@@ -7074,9 +7395,10 @@
       <c r="G128" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="H128" s="20" t="s">
-        <v>519</v>
-      </c>
+      <c r="H128" s="19" t="s">
+        <v>515</v>
+      </c>
+      <c r="I128" s="4"/>
     </row>
     <row r="129" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="4" t="str">
@@ -7101,9 +7423,10 @@
       <c r="G129" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="H129" s="20" t="s">
-        <v>520</v>
-      </c>
+      <c r="H129" s="19" t="s">
+        <v>516</v>
+      </c>
+      <c r="I129" s="4"/>
     </row>
     <row r="130" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A130" s="4" t="str">
@@ -7129,8 +7452,9 @@
         <v>231</v>
       </c>
       <c r="H130" s="17" t="s">
-        <v>521</v>
-      </c>
+        <v>517</v>
+      </c>
+      <c r="I130" s="4"/>
     </row>
     <row r="131" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A131" s="4" t="str">
@@ -7158,6 +7482,7 @@
       <c r="H131" s="17" t="s">
         <v>352</v>
       </c>
+      <c r="I131" s="4"/>
     </row>
     <row r="132" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A132" s="4" t="str">
@@ -7185,6 +7510,7 @@
       <c r="H132" s="17" t="s">
         <v>352</v>
       </c>
+      <c r="I132" s="4"/>
     </row>
     <row r="133" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A133" s="4" t="str">
@@ -7210,8 +7536,9 @@
         <v>37</v>
       </c>
       <c r="H133" s="13" t="s">
-        <v>522</v>
-      </c>
+        <v>518</v>
+      </c>
+      <c r="I133" s="4"/>
     </row>
     <row r="134" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A134" s="4" t="str">
@@ -7237,8 +7564,9 @@
         <v>39</v>
       </c>
       <c r="H134" s="13" t="s">
-        <v>523</v>
-      </c>
+        <v>519</v>
+      </c>
+      <c r="I134" s="4"/>
     </row>
     <row r="135" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A135" s="4" t="str">
@@ -7263,9 +7591,10 @@
       <c r="G135" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H135" s="20" t="s">
-        <v>524</v>
-      </c>
+      <c r="H135" s="19" t="s">
+        <v>520</v>
+      </c>
+      <c r="I135" s="4"/>
     </row>
     <row r="136" spans="1:9" ht="44" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A136" s="4" t="str">
@@ -7289,8 +7618,9 @@
       </c>
       <c r="G136" s="4"/>
       <c r="H136" s="13" t="s">
-        <v>525</v>
-      </c>
+        <v>521</v>
+      </c>
+      <c r="I136" s="4"/>
     </row>
     <row r="137" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A137" s="4" t="str">
@@ -7316,8 +7646,9 @@
         <v>43</v>
       </c>
       <c r="H137" s="17" t="s">
-        <v>526</v>
-      </c>
+        <v>522</v>
+      </c>
+      <c r="I137" s="4"/>
     </row>
     <row r="138" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A138" s="4" t="str">
@@ -7343,9 +7674,9 @@
         <v>31</v>
       </c>
       <c r="H138" s="13" t="s">
-        <v>527</v>
-      </c>
-      <c r="I138" s="19"/>
+        <v>523</v>
+      </c>
+      <c r="I138" s="23"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Traitement des commentaires "faciles"
</commit_message>
<xml_diff>
--- a/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
+++ b/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Geostandards-Risques\suivi\2024-05_06-Consultation-publique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877C6F1D-6904-41DD-AF51-26087A70F921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A56FB9-4CD3-4F01-8B74-D5711CE6D86F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
+    <workbookView xWindow="60" yWindow="60" windowWidth="28500" windowHeight="15150" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Synthese Modele Commun" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="571">
   <si>
     <t>Organisme</t>
   </si>
@@ -1412,10 +1412,6 @@
   </si>
   <si>
     <t>NOK ?
-Cela doit-être mentionné dans les métadonnées du PPR ou de la table du PPR</t>
-  </si>
-  <si>
-    <t>NOK ?
 Je comprends ici AE = Autorité Environnementale (et non pas Aléa Exceptionnel).
 Le novueau standard ne va pas plus loin que l'ancien au niveau du zonage foncier (il ne fait que le séparer de l'autre). La soumission à l'AE n'est pas du ressort ou non du standard il me semble ?</t>
   </si>
@@ -1428,10 +1424,6 @@
     <t>Cf. précédent</t>
   </si>
   <si>
-    <t>A discuter
-Elles sont identifiées dans les enjeux. Ne peuvent-elles pas alors être représentées comme zones de prescriptions hors zone d'aléa ?</t>
-  </si>
-  <si>
     <t>OK, à regrouper (et peut-être enlever Saint-Barthélémy)</t>
   </si>
   <si>
@@ -1441,14 +1433,6 @@
   </si>
   <si>
     <t>OK sur le principe.
-A harmoniser avec proposition du commentaire suivant</t>
-  </si>
-  <si>
-    <t>OK sur le principe.
-A harmoniser avec proposition du commentaire précédent</t>
-  </si>
-  <si>
-    <t>OK sur le principe.
 Il s'agit de zones particulières (pas de zones d'aléas)
 Un tableau différent est sans doute à proposer (cf. commentaire suviant)</t>
   </si>
@@ -1475,24 +1459,9 @@
 Cf. remarque précédente</t>
   </si>
   <si>
-    <t xml:space="preserve">OK sur le principe.
-Ah, il doit s'agir de ce zonage d'exception là !
-A étudier
-</t>
-  </si>
-  <si>
-    <t>OK sur le principe
-Faisabilité à étudier et décider avec le GT</t>
-  </si>
-  <si>
     <t>NOK,
 GeoIDE n'est pas amené à fermer (il est en train d'évoluer).
 C'ets plutôt le processus de diffusion des PPR qui est  en train d'abandonner GeoIDE.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOK?
-Cela n'est pas du ressort des geostandards mais de l'accomagnement. 
-</t>
   </si>
   <si>
     <t>Cf. ci-dessus</t>
@@ -2173,12 +2142,81 @@
 Reformulation ;  "dont les modalités sont relatives au type d'aléa"
 </t>
   </si>
+  <si>
+    <t>intégré (deux types de bandes particulières)</t>
+  </si>
+  <si>
+    <t>OK, formulation à reprendre (".. dont la date est renseignée ...")</t>
+  </si>
+  <si>
+    <t>intégré (rajout de lien vers les dexcriptions des classes dans le modèle commun)</t>
+  </si>
+  <si>
+    <t>A discuter avec le GT et les demandeurs
+NB : la zone inondable historique ne peut-elle pas être caractérisée par son occurrence ?</t>
+  </si>
+  <si>
+    <t>N.A. ?</t>
+  </si>
+  <si>
+    <t>A discuter
+Elles sont identifiées dans les enjeux. Ne peuvent-elles pas alors être représentées comme zones de prescriptions hors zone d'aléa ou zones de prescription tout-court ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK sur le principe
+Cela doit-être mentionné dans les métadonnées (éléments de généalogie) du PPR  et/ou de la table particulière du PPR (zonage, aléa). Cf.https://github.com/cnigfr/Geostandards-Risques/blob/main/standards/Geostandards-risques-ppr/Document.md#%C3%A9l%C3%A9ments-de-m%C3%A9tadonn%C3%A9es-relatifs-%C3%A0-la-g%C3%A9n%C3%A9alogie-et-r%C3%A9solution-spatiale </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK, à modifier
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK à modifier
+</t>
+  </si>
+  <si>
+    <t>OK sur le principe
+Faisabilité à étudier et décider avec le GT
+NB : là aussi, peut-être que ces différenciations concernent plutôt les représentations à grande échelle (non concernées par cette partie du standard) ?
+NB2: de quel décret 2019 parle-t-on ? Pouvez-vous fournir la référence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK sur le principe.
+Ah, il doit s'agir de ce zonage d'exception là !
+A étudier mais il manque vraiment la référence de ce décret (cf. commentaires précédent)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOK?
+Cela n'est pas du ressort des geostandards mais de l'accompagnement. 
+</t>
+  </si>
+  <si>
+    <t>NOK ? 
+Certes le standard COAVDIS code le CODERISQUE sur sept caractères mais le code alea "utile" ne l'est que sur trois. Il est soit complété par des zéros, soit égal à 9999999 pour le code aléa multirsiques.</t>
+  </si>
+  <si>
+    <t>intégré + idouvrageprotection
++ libellés à 50 minimum aussi</t>
+  </si>
+  <si>
+    <t>intégré (entre 2000 et 25000)</t>
+  </si>
+  <si>
+    <t>intégré (première remarque)</t>
+  </si>
+  <si>
+    <t>intégré (50)</t>
+  </si>
+  <si>
+    <t>N.A. pour le moment</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2271,6 +2309,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="7" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2310,7 +2360,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2383,6 +2433,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3189,25 +3245,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939F5930-30D3-43D0-87E8-B00574FE9CE2}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.36328125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.1796875" style="3" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="21.90625" style="3" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="3" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" style="3" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="3" customWidth="1"/>
-    <col min="5" max="5" width="16.08984375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="49.54296875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="47.6328125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="54.81640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="21.453125" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="10.90625" style="3"/>
+    <col min="5" max="5" width="16.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="49.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="47.5703125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="54.85546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="10.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>349</v>
       </c>
@@ -3233,10 +3289,10 @@
         <v>5</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="73" customHeight="1" x14ac:dyDescent="0.35">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="72.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-1</v>
@@ -3263,10 +3319,10 @@
         <v>351</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-2</v>
@@ -3290,13 +3346,13 @@
         <v>332</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-3</v>
@@ -3323,10 +3379,10 @@
         <v>353</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="75.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-4</v>
@@ -3350,13 +3406,13 @@
         <v>305</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="89" customHeight="1" x14ac:dyDescent="0.35">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="89.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-5</v>
@@ -3383,10 +3439,10 @@
         <v>350</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/DAPP/BIP-11</v>
@@ -3411,10 +3467,10 @@
         <v>352</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="96" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-6</v>
@@ -3441,10 +3497,10 @@
         <v>358</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="96" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-7</v>
@@ -3471,10 +3527,10 @@
         <v>354</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-1</v>
@@ -3501,10 +3557,10 @@
         <v>355</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-2</v>
@@ -3531,10 +3587,10 @@
         <v>355</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-8</v>
@@ -3558,13 +3614,13 @@
         <v>315</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>525</v>
+        <v>518</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>cerema-6</v>
@@ -3591,10 +3647,10 @@
         <v>356</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="96" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-9</v>
@@ -3621,10 +3677,10 @@
         <v>357</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="61" customHeight="1" x14ac:dyDescent="0.35">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="60.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-10</v>
@@ -3651,10 +3707,10 @@
         <v>352</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="68" customHeight="1" x14ac:dyDescent="0.35">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-3</v>
@@ -3678,13 +3734,13 @@
         <v>288</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>526</v>
+        <v>519</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="77" customHeight="1" x14ac:dyDescent="0.35">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="77.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-4</v>
@@ -3711,10 +3767,10 @@
         <v>359</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="111" customHeight="1" x14ac:dyDescent="0.35">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-5</v>
@@ -3738,13 +3794,13 @@
         <v>293</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SDCAP/PONSOH-13</v>
@@ -3768,13 +3824,13 @@
         <v>328</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>546</v>
+        <v>539</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/DAPP/BIP-12</v>
@@ -3799,7 +3855,7 @@
         <v>360</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
     </row>
   </sheetData>
@@ -3815,25 +3871,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815F14A-19BC-4DCE-8D31-81F595A4B0E7}">
   <dimension ref="A1:I138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6328125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="3.81640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="16" style="3" customWidth="1"/>
-    <col min="5" max="5" width="14.36328125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="44.08984375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="44.140625" style="3" customWidth="1"/>
     <col min="7" max="7" width="38" style="3" customWidth="1"/>
-    <col min="8" max="8" width="51.81640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="22.26953125" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="10.90625" style="3"/>
+    <col min="8" max="8" width="51.85546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="10.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>348</v>
       </c>
@@ -3859,10 +3915,10 @@
         <v>5</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-2</v>
@@ -3884,13 +3940,13 @@
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="25" t="s">
-        <v>548</v>
+        <v>541</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-3</v>
@@ -3915,10 +3971,10 @@
         <v>371</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-4</v>
@@ -3943,10 +3999,10 @@
         <v>372</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="65" customHeight="1" x14ac:dyDescent="0.35">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-5</v>
@@ -3968,13 +4024,13 @@
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="22" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="126.5" x14ac:dyDescent="0.35">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="132" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP-0</v>
@@ -3997,10 +4053,10 @@
         <v>373</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-9</v>
@@ -4025,10 +4081,10 @@
         <v>374</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="46" customHeight="1" x14ac:dyDescent="0.35">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-14</v>
@@ -4054,7 +4110,7 @@
       </c>
       <c r="I8" s="24"/>
     </row>
-    <row r="9" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-15</v>
@@ -4080,7 +4136,7 @@
       </c>
       <c r="I9" s="24"/>
     </row>
-    <row r="10" spans="1:9" ht="74" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-2</v>
@@ -4108,7 +4164,7 @@
       </c>
       <c r="I10" s="24"/>
     </row>
-    <row r="11" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-3</v>
@@ -4136,7 +4192,7 @@
       </c>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" spans="1:9" ht="74" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-1</v>
@@ -4163,10 +4219,10 @@
         <v>350</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-1</v>
@@ -4190,13 +4246,13 @@
         <v>166</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>524</v>
+        <v>517</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="161" x14ac:dyDescent="0.35">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="168" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-2</v>
@@ -4220,13 +4276,13 @@
         <v>254</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-3</v>
@@ -4250,13 +4306,13 @@
         <v>62</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-1</v>
@@ -4280,13 +4336,13 @@
         <v>117</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-4</v>
@@ -4313,10 +4369,10 @@
         <v>380</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-4</v>
@@ -4343,10 +4399,10 @@
         <v>381</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-5</v>
@@ -4370,13 +4426,13 @@
         <v>255</v>
       </c>
       <c r="H19" s="19" t="s">
-        <v>551</v>
+        <v>544</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="84" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-6</v>
@@ -4400,13 +4456,13 @@
         <v>256</v>
       </c>
       <c r="H20" s="19" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-2</v>
@@ -4433,10 +4489,10 @@
         <v>382</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-3</v>
@@ -4463,10 +4519,10 @@
         <v>383</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-5</v>
@@ -4493,10 +4549,10 @@
         <v>384</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-4</v>
@@ -4523,10 +4579,10 @@
         <v>385</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-5</v>
@@ -4553,10 +4609,10 @@
         <v>384</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="71.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="71.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-7</v>
@@ -4580,13 +4636,13 @@
         <v>72</v>
       </c>
       <c r="H26" s="19" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-6</v>
@@ -4613,10 +4669,10 @@
         <v>352</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="115" x14ac:dyDescent="0.35">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-</v>
@@ -4638,11 +4694,11 @@
         <v>340</v>
       </c>
       <c r="H28" s="19" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
       <c r="I28" s="24"/>
     </row>
-    <row r="29" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-8</v>
@@ -4666,13 +4722,13 @@
         <v>75</v>
       </c>
       <c r="H29" s="19" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-9</v>
@@ -4698,9 +4754,9 @@
       <c r="H30" s="19" t="s">
         <v>386</v>
       </c>
-      <c r="I30" s="4"/>
-    </row>
-    <row r="31" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+      <c r="I30" s="24"/>
+    </row>
+    <row r="31" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-6</v>
@@ -4723,12 +4779,14 @@
       <c r="G31" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="H31" s="19" t="s">
+      <c r="H31" s="17" t="s">
         <v>387</v>
       </c>
-      <c r="I31" s="4"/>
-    </row>
-    <row r="32" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+      <c r="I31" s="23" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-7</v>
@@ -4754,9 +4812,9 @@
       <c r="H32" s="19" t="s">
         <v>389</v>
       </c>
-      <c r="I32" s="4"/>
-    </row>
-    <row r="33" spans="1:9" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I32" s="24"/>
+    </row>
+    <row r="33" spans="1:9" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-10</v>
@@ -4778,11 +4836,13 @@
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="17" t="s">
-        <v>388</v>
-      </c>
-      <c r="I33" s="4"/>
-    </row>
-    <row r="34" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+        <v>554</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-7</v>
@@ -4808,9 +4868,11 @@
       <c r="H34" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="I34" s="4"/>
-    </row>
-    <row r="35" spans="1:9" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I34" s="23" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-11</v>
@@ -4834,9 +4896,11 @@
       <c r="H35" s="17" t="s">
         <v>388</v>
       </c>
-      <c r="I35" s="4"/>
-    </row>
-    <row r="36" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+      <c r="I35" s="4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="84" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-1</v>
@@ -4862,9 +4926,11 @@
       <c r="H36" s="13" t="s">
         <v>391</v>
       </c>
-      <c r="I36" s="4"/>
-    </row>
-    <row r="37" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I36" s="4" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-21</v>
@@ -4890,9 +4956,11 @@
       <c r="H37" s="13" t="s">
         <v>392</v>
       </c>
-      <c r="I37" s="4"/>
-    </row>
-    <row r="38" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+      <c r="I37" s="4" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-</v>
@@ -4914,11 +4982,11 @@
         <v>338</v>
       </c>
       <c r="H38" s="19" t="s">
-        <v>393</v>
-      </c>
-      <c r="I38" s="4"/>
-    </row>
-    <row r="39" spans="1:9" ht="207" x14ac:dyDescent="0.35">
+        <v>556</v>
+      </c>
+      <c r="I38" s="24"/>
+    </row>
+    <row r="39" spans="1:9" ht="228" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-</v>
@@ -4942,9 +5010,9 @@
       <c r="H39" s="19" t="s">
         <v>393</v>
       </c>
-      <c r="I39" s="4"/>
-    </row>
-    <row r="40" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+      <c r="I39" s="24"/>
+    </row>
+    <row r="40" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-8</v>
@@ -4970,9 +5038,9 @@
       <c r="H40" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="I40" s="4"/>
-    </row>
-    <row r="41" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I40" s="24"/>
+    </row>
+    <row r="41" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-8</v>
@@ -4998,9 +5066,9 @@
       <c r="H41" s="19" t="s">
         <v>397</v>
       </c>
-      <c r="I41" s="4"/>
-    </row>
-    <row r="42" spans="1:9" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I41" s="24"/>
+    </row>
+    <row r="42" spans="1:9" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-12</v>
@@ -5024,9 +5092,11 @@
       <c r="H42" s="19" t="s">
         <v>398</v>
       </c>
-      <c r="I42" s="4"/>
-    </row>
-    <row r="43" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+      <c r="I42" s="23" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-4</v>
@@ -5050,11 +5120,13 @@
         <v>26</v>
       </c>
       <c r="H43" s="13" t="s">
-        <v>400</v>
-      </c>
-      <c r="I43" s="4"/>
-    </row>
-    <row r="44" spans="1:9" ht="38" customHeight="1" x14ac:dyDescent="0.35">
+        <v>399</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-2</v>
@@ -5078,11 +5150,13 @@
         <v>22</v>
       </c>
       <c r="H44" s="19" t="s">
-        <v>401</v>
-      </c>
-      <c r="I44" s="4"/>
-    </row>
-    <row r="45" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+        <v>400</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/BRNT-22</v>
@@ -5104,11 +5178,13 @@
       </c>
       <c r="G45" s="4"/>
       <c r="H45" s="19" t="s">
-        <v>402</v>
-      </c>
-      <c r="I45" s="4"/>
-    </row>
-    <row r="46" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+        <v>401</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-8</v>
@@ -5132,11 +5208,11 @@
         <v>33</v>
       </c>
       <c r="H46" s="19" t="s">
-        <v>403</v>
-      </c>
-      <c r="I46" s="4"/>
-    </row>
-    <row r="47" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>558</v>
+      </c>
+      <c r="I46" s="24"/>
+    </row>
+    <row r="47" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-24</v>
@@ -5160,11 +5236,11 @@
         <v>106</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>402</v>
-      </c>
-      <c r="I47" s="4"/>
-    </row>
-    <row r="48" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>401</v>
+      </c>
+      <c r="I47" s="24"/>
+    </row>
+    <row r="48" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-3</v>
@@ -5188,11 +5264,13 @@
         <v>25</v>
       </c>
       <c r="H48" s="17" t="s">
-        <v>404</v>
-      </c>
-      <c r="I48" s="4"/>
-    </row>
-    <row r="49" spans="1:9" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+        <v>402</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-5</v>
@@ -5215,12 +5293,14 @@
       <c r="G49" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H49" s="13" t="s">
-        <v>399</v>
-      </c>
-      <c r="I49" s="4"/>
-    </row>
-    <row r="50" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+      <c r="H49" s="26" t="s">
+        <v>559</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT07-2</v>
@@ -5244,11 +5324,13 @@
         <v>14</v>
       </c>
       <c r="H50" s="13" t="s">
-        <v>405</v>
-      </c>
-      <c r="I50" s="4"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+        <v>403</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-11</v>
@@ -5274,9 +5356,9 @@
       <c r="H51" s="17" t="s">
         <v>382</v>
       </c>
-      <c r="I51" s="4"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I51" s="24"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-12</v>
@@ -5302,9 +5384,9 @@
       <c r="H52" s="17" t="s">
         <v>382</v>
       </c>
-      <c r="I52" s="4"/>
-    </row>
-    <row r="53" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="I52" s="24"/>
+    </row>
+    <row r="53" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-13</v>
@@ -5327,18 +5409,20 @@
       <c r="G53" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="H53" s="19" t="s">
-        <v>406</v>
-      </c>
-      <c r="I53" s="4"/>
-    </row>
-    <row r="54" spans="1:9" ht="36.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H53" s="17" t="s">
+        <v>560</v>
+      </c>
+      <c r="I53" s="4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DGPR/SRNH/SdcAP/BRIL-14</v>
+        <v>DGPR/SRNH/SdcAP/BRIL-13</v>
       </c>
       <c r="B54" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>55</v>
@@ -5351,20 +5435,22 @@
       </c>
       <c r="F54" s="4"/>
       <c r="G54" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="H54" s="19" t="s">
-        <v>407</v>
-      </c>
-      <c r="I54" s="4"/>
-    </row>
-    <row r="55" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+      <c r="H54" s="17" t="s">
+        <v>379</v>
+      </c>
+      <c r="I54" s="4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DGPR/SRNH/SdcAP/BRIL-13</v>
+        <v>DGPR/SRNH/SdcAP/BRIL-14</v>
       </c>
       <c r="B55" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>55</v>
@@ -5377,14 +5463,16 @@
       </c>
       <c r="F55" s="4"/>
       <c r="G55" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H55" s="17" t="s">
-        <v>379</v>
-      </c>
-      <c r="I55" s="4"/>
-    </row>
-    <row r="56" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+        <v>561</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-15</v>
@@ -5406,11 +5494,13 @@
       </c>
       <c r="G56" s="4"/>
       <c r="H56" s="13" t="s">
-        <v>410</v>
-      </c>
-      <c r="I56" s="4"/>
-    </row>
-    <row r="57" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+        <v>406</v>
+      </c>
+      <c r="I56" s="4" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-9</v>
@@ -5436,9 +5526,11 @@
       <c r="H57" s="17" t="s">
         <v>379</v>
       </c>
-      <c r="I57" s="4"/>
-    </row>
-    <row r="58" spans="1:9" ht="184" x14ac:dyDescent="0.35">
+      <c r="I57" s="4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="216" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5458,11 +5550,11 @@
       </c>
       <c r="G58" s="4"/>
       <c r="H58" s="19" t="s">
-        <v>408</v>
-      </c>
-      <c r="I58" s="4"/>
-    </row>
-    <row r="59" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+        <v>404</v>
+      </c>
+      <c r="I58" s="24"/>
+    </row>
+    <row r="59" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-14</v>
@@ -5486,11 +5578,11 @@
         <v>148</v>
       </c>
       <c r="H59" s="19" t="s">
-        <v>409</v>
-      </c>
-      <c r="I59" s="4"/>
-    </row>
-    <row r="60" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+        <v>405</v>
+      </c>
+      <c r="I59" s="24"/>
+    </row>
+    <row r="60" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5510,11 +5602,11 @@
       </c>
       <c r="G60" s="4"/>
       <c r="H60" s="19" t="s">
-        <v>413</v>
-      </c>
-      <c r="I60" s="4"/>
-    </row>
-    <row r="61" spans="1:9" ht="230" x14ac:dyDescent="0.35">
+        <v>409</v>
+      </c>
+      <c r="I60" s="24"/>
+    </row>
+    <row r="61" spans="1:9" ht="252" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5534,11 +5626,13 @@
       </c>
       <c r="G61" s="4"/>
       <c r="H61" s="13" t="s">
-        <v>411</v>
-      </c>
-      <c r="I61" s="4"/>
-    </row>
-    <row r="62" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+        <v>407</v>
+      </c>
+      <c r="I61" s="4" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="96" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-15</v>
@@ -5562,11 +5656,11 @@
         <v>151</v>
       </c>
       <c r="H62" s="19" t="s">
-        <v>415</v>
-      </c>
-      <c r="I62" s="4"/>
-    </row>
-    <row r="63" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+        <v>562</v>
+      </c>
+      <c r="I62" s="24"/>
+    </row>
+    <row r="63" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5586,11 +5680,11 @@
       </c>
       <c r="G63" s="4"/>
       <c r="H63" s="13" t="s">
-        <v>412</v>
-      </c>
-      <c r="I63" s="4"/>
-    </row>
-    <row r="64" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+        <v>408</v>
+      </c>
+      <c r="I63" s="24"/>
+    </row>
+    <row r="64" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-16</v>
@@ -5614,11 +5708,11 @@
         <v>154</v>
       </c>
       <c r="H64" s="19" t="s">
-        <v>414</v>
-      </c>
-      <c r="I64" s="4"/>
-    </row>
-    <row r="65" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+        <v>563</v>
+      </c>
+      <c r="I64" s="24"/>
+    </row>
+    <row r="65" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT01-3</v>
@@ -5642,11 +5736,13 @@
         <v>50</v>
       </c>
       <c r="H65" s="13" t="s">
-        <v>416</v>
-      </c>
-      <c r="I65" s="4"/>
-    </row>
-    <row r="66" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+        <v>410</v>
+      </c>
+      <c r="I65" s="4" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDTM 83-1</v>
@@ -5670,11 +5766,13 @@
         <v>53</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>417</v>
-      </c>
-      <c r="I66" s="4"/>
-    </row>
-    <row r="67" spans="1:9" ht="174" x14ac:dyDescent="0.35">
+        <v>564</v>
+      </c>
+      <c r="I66" s="4" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-10</v>
@@ -5698,11 +5796,11 @@
         <v>270</v>
       </c>
       <c r="H67" s="19" t="s">
-        <v>481</v>
-      </c>
-      <c r="I67" s="4"/>
-    </row>
-    <row r="68" spans="1:9" ht="88" customHeight="1" x14ac:dyDescent="0.35">
+        <v>474</v>
+      </c>
+      <c r="I67" s="24"/>
+    </row>
+    <row r="68" spans="1:9" ht="87.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-1</v>
@@ -5726,11 +5824,11 @@
         <v>241</v>
       </c>
       <c r="H68" s="19" t="s">
-        <v>418</v>
-      </c>
-      <c r="I68" s="4"/>
-    </row>
-    <row r="69" spans="1:9" ht="103" customHeight="1" x14ac:dyDescent="0.35">
+        <v>411</v>
+      </c>
+      <c r="I68" s="24"/>
+    </row>
+    <row r="69" spans="1:9" ht="102.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-11</v>
@@ -5754,11 +5852,11 @@
         <v>271</v>
       </c>
       <c r="H69" s="19" t="s">
-        <v>482</v>
-      </c>
-      <c r="I69" s="4"/>
-    </row>
-    <row r="70" spans="1:9" ht="111" customHeight="1" x14ac:dyDescent="0.35">
+        <v>475</v>
+      </c>
+      <c r="I69" s="24"/>
+    </row>
+    <row r="70" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-12</v>
@@ -5782,11 +5880,11 @@
         <v>272</v>
       </c>
       <c r="H70" s="19" t="s">
-        <v>529</v>
-      </c>
-      <c r="I70" s="4"/>
-    </row>
-    <row r="71" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+        <v>522</v>
+      </c>
+      <c r="I70" s="24"/>
+    </row>
+    <row r="71" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-13</v>
@@ -5810,11 +5908,13 @@
         <v>197</v>
       </c>
       <c r="H71" s="17" t="s">
-        <v>483</v>
-      </c>
-      <c r="I71" s="4"/>
-    </row>
-    <row r="72" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+        <v>476</v>
+      </c>
+      <c r="I71" s="4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A72" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-14</v>
@@ -5823,26 +5923,28 @@
         <v>14</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="H72" s="19" t="s">
-        <v>484</v>
-      </c>
-      <c r="I72" s="4"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+        <v>477</v>
+      </c>
+      <c r="I72" s="4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A73" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-19</v>
@@ -5851,26 +5953,28 @@
         <v>19</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="H73" s="17" t="s">
-        <v>485</v>
-      </c>
-      <c r="I73" s="4"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+        <v>478</v>
+      </c>
+      <c r="I73" s="4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A74" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-16</v>
@@ -5879,26 +5983,28 @@
         <v>16</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="H74" s="17" t="s">
-        <v>485</v>
-      </c>
-      <c r="I74" s="4"/>
-    </row>
-    <row r="75" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.35">
+        <v>478</v>
+      </c>
+      <c r="I74" s="4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-14</v>
@@ -5922,11 +6028,11 @@
         <v>273</v>
       </c>
       <c r="H75" s="19" t="s">
-        <v>486</v>
-      </c>
-      <c r="I75" s="4"/>
-    </row>
-    <row r="76" spans="1:9" ht="115" customHeight="1" x14ac:dyDescent="0.35">
+        <v>479</v>
+      </c>
+      <c r="I75" s="24"/>
+    </row>
+    <row r="76" spans="1:9" ht="144" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-15</v>
@@ -5950,11 +6056,11 @@
         <v>275</v>
       </c>
       <c r="H76" s="19" t="s">
-        <v>490</v>
-      </c>
-      <c r="I76" s="4"/>
-    </row>
-    <row r="77" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+        <v>483</v>
+      </c>
+      <c r="I76" s="24"/>
+    </row>
+    <row r="77" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-16</v>
@@ -5978,11 +6084,11 @@
         <v>203</v>
       </c>
       <c r="H77" s="19" t="s">
-        <v>487</v>
-      </c>
-      <c r="I77" s="4"/>
-    </row>
-    <row r="78" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+        <v>480</v>
+      </c>
+      <c r="I77" s="24"/>
+    </row>
+    <row r="78" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A78" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-22</v>
@@ -5991,26 +6097,28 @@
         <v>22</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="H78" s="19" t="s">
-        <v>484</v>
-      </c>
-      <c r="I78" s="4"/>
-    </row>
-    <row r="79" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+        <v>477</v>
+      </c>
+      <c r="I78" s="4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="27" x14ac:dyDescent="0.25">
       <c r="A79" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-23</v>
@@ -6019,26 +6127,28 @@
         <v>23</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="H79" s="17" t="s">
-        <v>485</v>
-      </c>
-      <c r="I79" s="4"/>
-    </row>
-    <row r="80" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+        <v>478</v>
+      </c>
+      <c r="I79" s="4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A80" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-24</v>
@@ -6047,26 +6157,28 @@
         <v>24</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>468</v>
-      </c>
-      <c r="H80" s="17" t="s">
-        <v>485</v>
-      </c>
-      <c r="I80" s="4"/>
-    </row>
-    <row r="81" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+        <v>461</v>
+      </c>
+      <c r="H80" s="13" t="s">
+        <v>565</v>
+      </c>
+      <c r="I80" s="4" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-17</v>
@@ -6090,11 +6202,11 @@
         <v>206</v>
       </c>
       <c r="H81" s="19" t="s">
-        <v>488</v>
-      </c>
-      <c r="I81" s="4"/>
-    </row>
-    <row r="82" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+        <v>481</v>
+      </c>
+      <c r="I81" s="24"/>
+    </row>
+    <row r="82" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-18</v>
@@ -6118,11 +6230,11 @@
         <v>209</v>
       </c>
       <c r="H82" s="19" t="s">
-        <v>489</v>
-      </c>
-      <c r="I82" s="4"/>
-    </row>
-    <row r="83" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+        <v>482</v>
+      </c>
+      <c r="I82" s="24"/>
+    </row>
+    <row r="83" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-19</v>
@@ -6146,11 +6258,11 @@
         <v>211</v>
       </c>
       <c r="H83" s="19" t="s">
-        <v>491</v>
-      </c>
-      <c r="I83" s="4"/>
-    </row>
-    <row r="84" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+        <v>484</v>
+      </c>
+      <c r="I83" s="24"/>
+    </row>
+    <row r="84" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-20</v>
@@ -6174,11 +6286,13 @@
         <v>213</v>
       </c>
       <c r="H84" s="17" t="s">
-        <v>492</v>
-      </c>
-      <c r="I84" s="4"/>
-    </row>
-    <row r="85" spans="1:9" ht="36.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>485</v>
+      </c>
+      <c r="I84" s="4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-27</v>
@@ -6187,26 +6301,28 @@
         <v>27</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D85" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E85" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="F85" s="4" t="s">
         <v>473</v>
       </c>
-      <c r="F85" s="4" t="s">
-        <v>480</v>
-      </c>
       <c r="G85" s="4" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="H85" s="19" t="s">
-        <v>484</v>
-      </c>
-      <c r="I85" s="4"/>
-    </row>
-    <row r="86" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+        <v>477</v>
+      </c>
+      <c r="I85" s="4" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-21</v>
@@ -6230,11 +6346,13 @@
         <v>216</v>
       </c>
       <c r="H86" s="19" t="s">
-        <v>493</v>
-      </c>
-      <c r="I86" s="4"/>
-    </row>
-    <row r="87" spans="1:9" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>486</v>
+      </c>
+      <c r="I86" s="4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-26</v>
@@ -6243,26 +6361,28 @@
         <v>26</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E87" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="F87" s="4" t="s">
         <v>472</v>
       </c>
-      <c r="F87" s="4" t="s">
-        <v>479</v>
-      </c>
       <c r="G87" s="4" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="H87" s="19" t="s">
-        <v>484</v>
-      </c>
-      <c r="I87" s="4"/>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+        <v>477</v>
+      </c>
+      <c r="I87" s="4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-17</v>
@@ -6288,9 +6408,11 @@
       <c r="H88" s="17" t="s">
         <v>379</v>
       </c>
-      <c r="I88" s="4"/>
-    </row>
-    <row r="89" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="I88" s="4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-16</v>
@@ -6312,11 +6434,13 @@
         <v>91</v>
       </c>
       <c r="H89" s="17" t="s">
-        <v>494</v>
-      </c>
-      <c r="I89" s="4"/>
-    </row>
-    <row r="90" spans="1:9" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>487</v>
+      </c>
+      <c r="I89" s="4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="77.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-17</v>
@@ -6338,11 +6462,13 @@
       </c>
       <c r="G90" s="4"/>
       <c r="H90" s="13" t="s">
-        <v>495</v>
-      </c>
-      <c r="I90" s="4"/>
-    </row>
-    <row r="91" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+        <v>488</v>
+      </c>
+      <c r="I90" s="4" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-22</v>
@@ -6366,11 +6492,11 @@
         <v>218</v>
       </c>
       <c r="H91" s="19" t="s">
-        <v>496</v>
-      </c>
-      <c r="I91" s="4"/>
-    </row>
-    <row r="92" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+        <v>489</v>
+      </c>
+      <c r="I91" s="24"/>
+    </row>
+    <row r="92" spans="1:9" ht="96" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-23</v>
@@ -6394,11 +6520,13 @@
         <v>278</v>
       </c>
       <c r="H92" s="13" t="s">
-        <v>497</v>
-      </c>
-      <c r="I92" s="4"/>
-    </row>
-    <row r="93" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+        <v>490</v>
+      </c>
+      <c r="I92" s="4" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="96" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-24</v>
@@ -6422,11 +6550,13 @@
         <v>279</v>
       </c>
       <c r="H93" s="21" t="s">
-        <v>498</v>
-      </c>
-      <c r="I93" s="4"/>
-    </row>
-    <row r="94" spans="1:9" ht="113" customHeight="1" x14ac:dyDescent="0.35">
+        <v>491</v>
+      </c>
+      <c r="I93" s="4" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="113.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/PoNSOH-26</v>
@@ -6449,12 +6579,12 @@
       <c r="G94" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="H94" s="9" t="s">
-        <v>528</v>
-      </c>
-      <c r="I94" s="4"/>
-    </row>
-    <row r="95" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H94" s="27" t="s">
+        <v>521</v>
+      </c>
+      <c r="I94" s="24"/>
+    </row>
+    <row r="95" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/PoNSOH-27</v>
@@ -6478,11 +6608,11 @@
         <v>113</v>
       </c>
       <c r="H95" s="19" t="s">
-        <v>499</v>
-      </c>
-      <c r="I95" s="4"/>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+        <v>492</v>
+      </c>
+      <c r="I95" s="24"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-18</v>
@@ -6508,9 +6638,9 @@
       <c r="H96" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="I96" s="4"/>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I96" s="24"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-19</v>
@@ -6536,9 +6666,9 @@
       <c r="H97" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="I97" s="4"/>
-    </row>
-    <row r="98" spans="1:9" ht="96.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I97" s="24"/>
+    </row>
+    <row r="98" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-18</v>
@@ -6560,11 +6690,13 @@
       </c>
       <c r="G98" s="4"/>
       <c r="H98" s="19" t="s">
-        <v>500</v>
-      </c>
-      <c r="I98" s="4"/>
-    </row>
-    <row r="99" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+        <v>493</v>
+      </c>
+      <c r="I98" s="4" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A99" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-15</v>
@@ -6573,26 +6705,28 @@
         <v>15</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D99" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="G99" s="4" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="H99" s="17" t="s">
-        <v>502</v>
-      </c>
-      <c r="I99" s="4"/>
-    </row>
-    <row r="100" spans="1:9" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>495</v>
+      </c>
+      <c r="I99" s="4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-1</v>
@@ -6601,26 +6735,28 @@
         <v>1</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D100" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="G100" s="4" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="H100" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="I100" s="4"/>
-    </row>
-    <row r="101" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="I100" s="4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A101" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-17</v>
@@ -6629,26 +6765,28 @@
         <v>17</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D101" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="F101" s="4" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="G101" s="4" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="H101" s="17" t="s">
-        <v>502</v>
-      </c>
-      <c r="I101" s="4"/>
-    </row>
-    <row r="102" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+        <v>495</v>
+      </c>
+      <c r="I101" s="4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A102" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-20</v>
@@ -6657,26 +6795,28 @@
         <v>20</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D102" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="G102" s="4" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="H102" s="17" t="s">
-        <v>502</v>
-      </c>
-      <c r="I102" s="4"/>
-    </row>
-    <row r="103" spans="1:9" ht="37.5" x14ac:dyDescent="0.35">
+        <v>495</v>
+      </c>
+      <c r="I102" s="4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="39" x14ac:dyDescent="0.25">
       <c r="A103" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-21</v>
@@ -6685,26 +6825,26 @@
         <v>21</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D103" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="F103" s="4" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="G103" s="4" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="H103" s="19" t="s">
-        <v>503</v>
-      </c>
-      <c r="I103" s="4"/>
-    </row>
-    <row r="104" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+        <v>496</v>
+      </c>
+      <c r="I103" s="24"/>
+    </row>
+    <row r="104" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A104" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-18</v>
@@ -6713,26 +6853,28 @@
         <v>18</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D104" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="F104" s="4" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="G104" s="4" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="H104" s="13" t="s">
-        <v>504</v>
-      </c>
-      <c r="I104" s="4"/>
-    </row>
-    <row r="105" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+        <v>497</v>
+      </c>
+      <c r="I104" s="4" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A105" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-25</v>
@@ -6741,26 +6883,28 @@
         <v>25</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D105" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="G105" s="4" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="H105" s="17" t="s">
-        <v>502</v>
-      </c>
-      <c r="I105" s="4"/>
-    </row>
-    <row r="106" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+        <v>495</v>
+      </c>
+      <c r="I105" s="4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A106" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-2</v>
@@ -6769,26 +6913,26 @@
         <v>2</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D106" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="G106" s="4" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="H106" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="I106" s="4"/>
-    </row>
-    <row r="107" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="I106" s="24"/>
+    </row>
+    <row r="107" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A107" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-3</v>
@@ -6797,26 +6941,26 @@
         <v>3</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D107" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="G107" s="4" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="H107" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="I107" s="4"/>
-    </row>
-    <row r="108" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="I107" s="24"/>
+    </row>
+    <row r="108" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A108" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-4</v>
@@ -6825,26 +6969,26 @@
         <v>4</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D108" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="F108" s="4" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="G108" s="4" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="H108" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="I108" s="4"/>
-    </row>
-    <row r="109" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+      <c r="I108" s="24"/>
+    </row>
+    <row r="109" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT01-1</v>
@@ -6868,11 +7012,13 @@
         <v>250</v>
       </c>
       <c r="H109" s="6" t="s">
-        <v>501</v>
-      </c>
-      <c r="I109" s="4"/>
-    </row>
-    <row r="110" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+        <v>494</v>
+      </c>
+      <c r="I109" s="4" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A110" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-5</v>
@@ -6881,26 +7027,26 @@
         <v>5</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D110" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="F110" s="4" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="G110" s="4" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="H110" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="I110" s="4"/>
-    </row>
-    <row r="111" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="I110" s="24"/>
+    </row>
+    <row r="111" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A111" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-6</v>
@@ -6909,26 +7055,26 @@
         <v>6</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D111" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E111" s="5" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="F111" s="4" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="G111" s="4" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="H111" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="I111" s="4"/>
-    </row>
-    <row r="112" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="I111" s="24"/>
+    </row>
+    <row r="112" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A112" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-7</v>
@@ -6937,26 +7083,26 @@
         <v>7</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D112" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="F112" s="4" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="G112" s="4" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="H112" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="I112" s="4"/>
-    </row>
-    <row r="113" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="I112" s="24"/>
+    </row>
+    <row r="113" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A113" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-8</v>
@@ -6965,26 +7111,26 @@
         <v>8</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D113" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="F113" s="4" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="G113" s="4" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="H113" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="I113" s="4"/>
-    </row>
-    <row r="114" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="I113" s="24"/>
+    </row>
+    <row r="114" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A114" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-9</v>
@@ -6993,26 +7139,26 @@
         <v>9</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D114" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="F114" s="4" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="G114" s="4" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="H114" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="I114" s="4"/>
-    </row>
-    <row r="115" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+      <c r="I114" s="24"/>
+    </row>
+    <row r="115" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A115" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-10</v>
@@ -7021,26 +7167,26 @@
         <v>10</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D115" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="G115" s="4" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="H115" s="19" t="s">
-        <v>505</v>
-      </c>
-      <c r="I115" s="4"/>
-    </row>
-    <row r="116" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+        <v>498</v>
+      </c>
+      <c r="I115" s="24"/>
+    </row>
+    <row r="116" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A116" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-11</v>
@@ -7049,26 +7195,28 @@
         <v>11</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D116" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="F116" s="4" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="G116" s="4" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="H116" s="13" t="s">
-        <v>506</v>
-      </c>
-      <c r="I116" s="4"/>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+        <v>499</v>
+      </c>
+      <c r="I116" s="4" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A117" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-12</v>
@@ -7077,26 +7225,26 @@
         <v>12</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D117" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="F117" s="4" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="G117" s="4" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="H117" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="I117" s="4"/>
-    </row>
-    <row r="118" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="I117" s="24"/>
+    </row>
+    <row r="118" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A118" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-13</v>
@@ -7105,26 +7253,26 @@
         <v>13</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="D118" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="F118" s="4" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="G118" s="4" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="H118" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="I118" s="4"/>
-    </row>
-    <row r="119" spans="1:9" ht="119.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I118" s="24"/>
+    </row>
+    <row r="119" spans="1:9" ht="156" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-6</v>
@@ -7148,11 +7296,11 @@
         <v>29</v>
       </c>
       <c r="H119" s="19" t="s">
-        <v>507</v>
-      </c>
-      <c r="I119" s="4"/>
-    </row>
-    <row r="120" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+        <v>500</v>
+      </c>
+      <c r="I119" s="24"/>
+    </row>
+    <row r="120" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT01-2</v>
@@ -7176,11 +7324,11 @@
         <v>252</v>
       </c>
       <c r="H120" s="19" t="s">
-        <v>499</v>
-      </c>
-      <c r="I120" s="4"/>
-    </row>
-    <row r="121" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+        <v>492</v>
+      </c>
+      <c r="I120" s="24"/>
+    </row>
+    <row r="121" spans="1:9" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-23</v>
@@ -7204,11 +7352,11 @@
         <v>104</v>
       </c>
       <c r="H121" s="19" t="s">
-        <v>508</v>
-      </c>
-      <c r="I121" s="4"/>
-    </row>
-    <row r="122" spans="1:9" ht="78" customHeight="1" x14ac:dyDescent="0.35">
+        <v>501</v>
+      </c>
+      <c r="I121" s="24"/>
+    </row>
+    <row r="122" spans="1:9" ht="84" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-20</v>
@@ -7232,11 +7380,11 @@
         <v>162</v>
       </c>
       <c r="H122" s="19" t="s">
-        <v>510</v>
-      </c>
-      <c r="I122" s="4"/>
-    </row>
-    <row r="123" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+        <v>503</v>
+      </c>
+      <c r="I122" s="24"/>
+    </row>
+    <row r="123" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-25</v>
@@ -7260,11 +7408,11 @@
         <v>225</v>
       </c>
       <c r="H123" s="19" t="s">
-        <v>509</v>
-      </c>
-      <c r="I123" s="4"/>
-    </row>
-    <row r="124" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+        <v>502</v>
+      </c>
+      <c r="I123" s="24"/>
+    </row>
+    <row r="124" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-26</v>
@@ -7288,11 +7436,11 @@
         <v>228</v>
       </c>
       <c r="H124" s="19" t="s">
-        <v>511</v>
-      </c>
-      <c r="I124" s="4"/>
-    </row>
-    <row r="125" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+        <v>504</v>
+      </c>
+      <c r="I124" s="24"/>
+    </row>
+    <row r="125" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT07-1</v>
@@ -7316,11 +7464,11 @@
         <v>10</v>
       </c>
       <c r="H125" s="19" t="s">
-        <v>512</v>
-      </c>
-      <c r="I125" s="4"/>
-    </row>
-    <row r="126" spans="1:9" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>505</v>
+      </c>
+      <c r="I125" s="24"/>
+    </row>
+    <row r="126" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-19</v>
@@ -7342,11 +7490,11 @@
       </c>
       <c r="G126" s="4"/>
       <c r="H126" s="19" t="s">
-        <v>513</v>
-      </c>
-      <c r="I126" s="4"/>
-    </row>
-    <row r="127" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+        <v>506</v>
+      </c>
+      <c r="I126" s="24"/>
+    </row>
+    <row r="127" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-20</v>
@@ -7368,11 +7516,11 @@
       </c>
       <c r="G127" s="4"/>
       <c r="H127" s="19" t="s">
-        <v>514</v>
-      </c>
-      <c r="I127" s="4"/>
-    </row>
-    <row r="128" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+        <v>507</v>
+      </c>
+      <c r="I127" s="24"/>
+    </row>
+    <row r="128" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-9</v>
@@ -7396,11 +7544,13 @@
         <v>136</v>
       </c>
       <c r="H128" s="19" t="s">
-        <v>515</v>
-      </c>
-      <c r="I128" s="4"/>
-    </row>
-    <row r="129" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>508</v>
+      </c>
+      <c r="I128" s="4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-10</v>
@@ -7424,11 +7574,11 @@
         <v>139</v>
       </c>
       <c r="H129" s="19" t="s">
-        <v>516</v>
-      </c>
-      <c r="I129" s="4"/>
-    </row>
-    <row r="130" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+        <v>509</v>
+      </c>
+      <c r="I129" s="24"/>
+    </row>
+    <row r="130" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-27</v>
@@ -7452,11 +7602,11 @@
         <v>231</v>
       </c>
       <c r="H130" s="17" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
       <c r="I130" s="4"/>
     </row>
-    <row r="131" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-28</v>
@@ -7482,9 +7632,11 @@
       <c r="H131" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="I131" s="4"/>
-    </row>
-    <row r="132" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="I131" s="4" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-29</v>
@@ -7510,9 +7662,11 @@
       <c r="H132" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="I132" s="4"/>
-    </row>
-    <row r="133" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="I132" s="4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-10</v>
@@ -7536,11 +7690,13 @@
         <v>37</v>
       </c>
       <c r="H133" s="13" t="s">
-        <v>518</v>
-      </c>
-      <c r="I133" s="4"/>
-    </row>
-    <row r="134" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+        <v>511</v>
+      </c>
+      <c r="I133" s="4" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-11</v>
@@ -7564,11 +7720,13 @@
         <v>39</v>
       </c>
       <c r="H134" s="13" t="s">
-        <v>519</v>
-      </c>
-      <c r="I134" s="4"/>
-    </row>
-    <row r="135" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+        <v>512</v>
+      </c>
+      <c r="I134" s="4" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-12</v>
@@ -7592,11 +7750,13 @@
         <v>41</v>
       </c>
       <c r="H135" s="19" t="s">
-        <v>520</v>
-      </c>
-      <c r="I135" s="4"/>
-    </row>
-    <row r="136" spans="1:9" ht="44" customHeight="1" x14ac:dyDescent="0.35">
+        <v>513</v>
+      </c>
+      <c r="I135" s="4" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-25</v>
@@ -7618,11 +7778,13 @@
       </c>
       <c r="G136" s="4"/>
       <c r="H136" s="13" t="s">
-        <v>521</v>
-      </c>
-      <c r="I136" s="4"/>
-    </row>
-    <row r="137" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+      <c r="I136" s="4" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-13</v>
@@ -7646,11 +7808,11 @@
         <v>43</v>
       </c>
       <c r="H137" s="17" t="s">
-        <v>522</v>
-      </c>
-      <c r="I137" s="4"/>
-    </row>
-    <row r="138" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+        <v>515</v>
+      </c>
+      <c r="I137" s="24"/>
+    </row>
+    <row r="138" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-7</v>
@@ -7674,9 +7836,11 @@
         <v>31</v>
       </c>
       <c r="H138" s="13" t="s">
-        <v>523</v>
-      </c>
-      <c r="I138" s="23"/>
+        <v>516</v>
+      </c>
+      <c r="I138" s="23" t="s">
+        <v>529</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
modification tableaux commentaires suite à réunion #1
</commit_message>
<xml_diff>
--- a/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
+++ b/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Geostandards-Risques\suivi\2024-05_06-Consultation-publique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D7CAEE-3403-4955-9979-BBB6F1F9CDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BAFA14-EBC6-4921-84F6-E5DA9404F947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="60" windowWidth="27525" windowHeight="15150" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Synthese Modele Commun" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="592">
   <si>
     <t>Organisme</t>
   </si>
@@ -1344,10 +1344,6 @@
     <t>OK, à modifier</t>
   </si>
   <si>
-    <t>NOK ?
-C'est plutôt un diffuseur de données dérivées des PPR</t>
-  </si>
-  <si>
     <t>OK, à ajouter</t>
   </si>
   <si>
@@ -1373,11 +1369,6 @@
     <t xml:space="preserve">Ok sur le principe
 Elle l'est dans le document modèle commun et n'est pas reprise dans PPR car elle n'est pas modifiée. Il faudrait à minima la mentionner pour rappel dans le document sans réécrire tout.
 </t>
-  </si>
-  <si>
-    <t>NOK ?
-La nomenture des risques GASPAR ne fait pas la distinction entre les différents types d'avalanche. Peut-être faut-il faire des sous-types de l'aléa 14 comme pour l'innondation ?
-Pour l'instant cette information peut être mise dans la description texte libre</t>
   </si>
   <si>
     <t>NOK ?
@@ -2027,21 +2018,6 @@
 </t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">OK, référence à rajouter
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(NB : à vérifier si des éléments du standard sont impactés par cette nouvelle référence) ?</t>
-    </r>
-  </si>
-  <si>
     <t>A priori non pour l'instant. 
 =&gt; Envisager de produire un fichier de métadonnées type</t>
   </si>
@@ -2073,14 +2049,8 @@
     <t>integré</t>
   </si>
   <si>
-    <t>cf. commentaires PPR</t>
-  </si>
-  <si>
     <t>integré (+ carte "approuvée" au lieu de "signée")
 + tables d'énumérations (PPR) + modèle UML + gabarits</t>
-  </si>
-  <si>
-    <t>Vérifier si possibilité de restreindre les valeurs de certains champs au niveau de modèle commun</t>
   </si>
   <si>
     <t xml:space="preserve">OK, à corriger.
@@ -2089,18 +2059,9 @@
 </t>
   </si>
   <si>
-    <t>Typologie des ouvrages de protection à modifier. Proposition BRIL (+BRNT ?) à venir</t>
-  </si>
-  <si>
     <t xml:space="preserve">Non, à moins qu'il n'y ait une volonté de les transformer en PPR (cf. Sweet pepper)?
 NB : certains champs obligatoires non renseignés dans PSS
 </t>
-  </si>
-  <si>
-    <t>Ne rendre obligatoire que les thématiques Procédures, Périmètres et Zonage Réglementaire?</t>
-  </si>
-  <si>
-    <t>something to do ?</t>
   </si>
   <si>
     <t>A vérifier
@@ -2112,9 +2073,6 @@
   <si>
     <t>OK sur le principe, à modifier
 NB : cartographier l'aléa de référence est trop PPRN-centré =&gt; seulement "cartographier les aléas"</t>
-  </si>
-  <si>
-    <t>intégré (pour la première partie)</t>
   </si>
   <si>
     <t>intégré (pour la partie "du PPR")</t>
@@ -2143,9 +2101,6 @@
 </t>
   </si>
   <si>
-    <t>intégré (deux types de bandes particulières)</t>
-  </si>
-  <si>
     <t>OK, formulation à reprendre (".. dont la date est renseignée ...")</t>
   </si>
   <si>
@@ -2247,8 +2202,80 @@
 Les identifiants sont passés à une longueur de 15 (cf. Ineris-22)</t>
   </si>
   <si>
+    <t>cf. commentaires PPR (intégré)</t>
+  </si>
+  <si>
+    <t>Vérifier si possibilité de restreindre les valeurs de certains champs au niveau de modèle commun.
+NB : occurrence = péridoe de retour pour l'aléa naturel
+- Accepté =&gt; à intégrer
+(type: integer)
+- Préciser que 0 équivaut à une valeur nulle</t>
+  </si>
+  <si>
+    <t>Cf. Typologie des ouvrages de protection à modifier. Proposition BRIL (+BRNT)
+Maintenir le terme scénario
+Pas d'accès à SIOUH2 (trouver descriptif)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ne rendre obligatoire que les thématiques Procédures, Périmètres et Zonage Réglementaire?
+Aléa non obligatoire (au niveau diffusion)
+</t>
+  </si>
+  <si>
+    <t>A envisager dans le cadre de l'accompagnement (gabarit XML)</t>
+  </si>
+  <si>
+    <t>Alea 123 pas suffisant ?
+Se rapprocher du BRNT =&gt; comment traiter ce type d'aléa.</t>
+  </si>
+  <si>
+    <t>Rajouter le périmètre d'étude en plus du périmètre administratif (Pour la référence au CE pour le périmètre mis à l'étude : cf article R562-2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voir avec le BIP et le BRNT pour la bonne classification </t>
+  </si>
+  <si>
+    <t>A priori le multi-polygone est autorisé pour les zones d'aléas et le zonage réglementaire (cf. modèle commun). Il est cependant conseillé de produire des géométries simples dans la mesure du possible avec des critères de rejet pour faciliter la diffusion et la consultation.</t>
+  </si>
+  <si>
+    <t>OK, référence à rajouter
+(NB : à vérifier si des éléments du standard sont impactés par cette nouvelle référence) ? =&gt; pad d'impact</t>
+  </si>
+  <si>
+    <t>intégré (pour la première partie)
+=&gt; Supprimer Saint-Barthélémy (Code de l'environnement ne s'applqiue pas)</t>
+  </si>
+  <si>
+    <t>N.A.
+Mentionner la non opposabilité L152-7 (Code urbanisme)</t>
+  </si>
+  <si>
+    <t>OK 
+Rajouter le GPU au sens de L152-7</t>
+  </si>
+  <si>
+    <t>intégré (rajouter princpaux)</t>
+  </si>
+  <si>
+    <t>Mentionner la possibilité de cartographier les PHEC mais sonas les définir + que ça (réf. https://www.reperesdecrues.developpement-durable.gouv.fr/  )</t>
+  </si>
+  <si>
+    <t>remplacer niveau alea par occurrence</t>
+  </si>
+  <si>
+    <t>intégré (deux types de bandes particulières)
+Rajouter la possibilité d'avoir  un type de bande pour les deux</t>
+  </si>
+  <si>
+    <t>changer en zones + mentionner la référence aux espaces du guide PPRN;2016</t>
+  </si>
+  <si>
+    <t>Soumettre la proposition coulante + aérosol + les 2 au BRNT</t>
+  </si>
+  <si>
     <t>NOK ?
-A priori le multi-polygone est autorisé pour les zones d'aléas et le zonage réglementaire (cf. modèle commun). Il est cependant conseillé de produire des géométries simples dans la mesure du possible avec des critères de rejet pour faciliter la diffusion et la consultation.</t>
+La nomenture des risques GASPAR ne fait pas la distinction entre les différents types d'avalanche. Peut-être faut-il faire des sous-types de l'aléa 14 comme pour l'inondation ?
+Pour l'instant cette information peut être mise dans la description texte libre</t>
   </si>
 </sst>
 </file>
@@ -2375,7 +2402,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -2394,12 +2421,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2480,6 +2531,25 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -3284,8 +3354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939F5930-30D3-43D0-87E8-B00574FE9CE2}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3328,7 +3398,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="72.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3358,7 +3428,7 @@
         <v>351</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="108" x14ac:dyDescent="0.25">
@@ -3385,10 +3455,10 @@
         <v>332</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="108" x14ac:dyDescent="0.25">
@@ -3418,7 +3488,7 @@
         <v>353</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3445,10 +3515,10 @@
         <v>305</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="89.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -3478,7 +3548,7 @@
         <v>350</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="24" x14ac:dyDescent="0.25">
@@ -3506,7 +3576,7 @@
         <v>352</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="96" x14ac:dyDescent="0.25">
@@ -3536,10 +3606,10 @@
         <v>358</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="96" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="144" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-7</v>
@@ -3566,7 +3636,7 @@
         <v>354</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>538</v>
+        <v>573</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3596,7 +3666,7 @@
         <v>355</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -3626,7 +3696,7 @@
         <v>355</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="108" x14ac:dyDescent="0.25">
@@ -3653,10 +3723,10 @@
         <v>315</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3686,7 +3756,7 @@
         <v>356</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="96" x14ac:dyDescent="0.25">
@@ -3716,7 +3786,7 @@
         <v>357</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="60.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3746,7 +3816,7 @@
         <v>352</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3773,10 +3843,10 @@
         <v>288</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="77.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3806,7 +3876,7 @@
         <v>359</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="111" customHeight="1" x14ac:dyDescent="0.25">
@@ -3833,13 +3903,13 @@
         <v>293</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="96" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SDCAP/PONSOH-13</v>
@@ -3863,10 +3933,10 @@
         <v>328</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>540</v>
+        <v>574</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3894,7 +3964,7 @@
         <v>360</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
   </sheetData>
@@ -3910,8 +3980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815F14A-19BC-4DCE-8D31-81F595A4B0E7}">
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3954,10 +4024,10 @@
         <v>5</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-2</v>
@@ -3979,10 +4049,10 @@
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="25" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>542</v>
+        <v>575</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4010,7 +4080,7 @@
         <v>371</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4038,7 +4108,7 @@
         <v>372</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4063,10 +4133,10 @@
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="22" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>543</v>
+        <v>576</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="132" x14ac:dyDescent="0.25">
@@ -4092,7 +4162,7 @@
         <v>373</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -4120,10 +4190,10 @@
         <v>374</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="45.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-14</v>
@@ -4144,12 +4214,14 @@
       <c r="G8" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="17" t="s">
         <v>375</v>
       </c>
-      <c r="I8" s="24"/>
-    </row>
-    <row r="9" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+      <c r="I8" s="24" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-15</v>
@@ -4173,7 +4245,9 @@
       <c r="H9" s="19" t="s">
         <v>376</v>
       </c>
-      <c r="I9" s="24"/>
+      <c r="I9" s="23" t="s">
+        <v>579</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="str">
@@ -4184,23 +4258,23 @@
         <v>1</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>571</v>
+        <v>561</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>572</v>
+        <v>562</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="4" t="s">
-        <v>573</v>
+        <v>563</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>574</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>582</v>
+        <v>564</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>580</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4286,7 +4360,7 @@
         <v>350</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4313,10 +4387,10 @@
         <v>166</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="168" x14ac:dyDescent="0.25">
@@ -4343,10 +4417,10 @@
         <v>254</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="36" x14ac:dyDescent="0.25">
@@ -4373,10 +4447,10 @@
         <v>62</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -4403,10 +4477,10 @@
         <v>117</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>525</v>
+        <v>581</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -4436,7 +4510,7 @@
         <v>380</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="36" x14ac:dyDescent="0.25">
@@ -4466,7 +4540,7 @@
         <v>381</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4493,10 +4567,10 @@
         <v>255</v>
       </c>
       <c r="H20" s="19" t="s">
-        <v>544</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>546</v>
+        <v>536</v>
+      </c>
+      <c r="I20" s="24" t="s">
+        <v>582</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="84" x14ac:dyDescent="0.25">
@@ -4523,10 +4597,10 @@
         <v>256</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>545</v>
+        <v>537</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4556,7 +4630,7 @@
         <v>382</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>550</v>
+        <v>541</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -4582,11 +4656,11 @@
       <c r="G23" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="H23" s="13" t="s">
-        <v>383</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>529</v>
+      <c r="H23" s="17" t="s">
+        <v>584</v>
+      </c>
+      <c r="I23" s="24" t="s">
+        <v>583</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -4613,10 +4687,10 @@
         <v>178</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>549</v>
+        <v>540</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -4643,10 +4717,10 @@
         <v>260</v>
       </c>
       <c r="H25" s="19" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>547</v>
+        <v>538</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="24" x14ac:dyDescent="0.25">
@@ -4673,10 +4747,10 @@
         <v>125</v>
       </c>
       <c r="H26" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="71.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4703,10 +4777,10 @@
         <v>72</v>
       </c>
       <c r="H27" s="19" t="s">
-        <v>548</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>530</v>
+        <v>539</v>
+      </c>
+      <c r="I27" s="24" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="36" x14ac:dyDescent="0.25">
@@ -4736,7 +4810,7 @@
         <v>352</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -4761,9 +4835,11 @@
         <v>340</v>
       </c>
       <c r="H29" s="19" t="s">
-        <v>551</v>
-      </c>
-      <c r="I29" s="24"/>
+        <v>542</v>
+      </c>
+      <c r="I29" s="24" t="s">
+        <v>586</v>
+      </c>
     </row>
     <row r="30" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="str">
@@ -4789,10 +4865,10 @@
         <v>75</v>
       </c>
       <c r="H30" s="19" t="s">
-        <v>552</v>
+        <v>543</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="72" x14ac:dyDescent="0.25">
@@ -4818,10 +4894,12 @@
       <c r="G31" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="H31" s="19" t="s">
-        <v>386</v>
-      </c>
-      <c r="I31" s="24"/>
+      <c r="H31" s="17" t="s">
+        <v>385</v>
+      </c>
+      <c r="I31" s="24" t="s">
+        <v>587</v>
+      </c>
     </row>
     <row r="32" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="str">
@@ -4847,10 +4925,10 @@
         <v>128</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>387</v>
-      </c>
-      <c r="I32" s="23" t="s">
-        <v>553</v>
+        <v>386</v>
+      </c>
+      <c r="I32" s="24" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="108" x14ac:dyDescent="0.25">
@@ -4876,10 +4954,12 @@
       <c r="G33" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="H33" s="19" t="s">
-        <v>389</v>
-      </c>
-      <c r="I33" s="24"/>
+      <c r="H33" s="17" t="s">
+        <v>388</v>
+      </c>
+      <c r="I33" s="24" t="s">
+        <v>589</v>
+      </c>
     </row>
     <row r="34" spans="1:9" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="str">
@@ -4903,10 +4983,10 @@
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="17" t="s">
-        <v>554</v>
+        <v>544</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="72" x14ac:dyDescent="0.25">
@@ -4933,13 +5013,13 @@
         <v>184</v>
       </c>
       <c r="H35" s="19" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I35" s="23" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="62.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-11</v>
@@ -4961,43 +5041,43 @@
         <v>82</v>
       </c>
       <c r="H36" s="17" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="84" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="str">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="34" customFormat="1" ht="84.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="28" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-1</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="29">
         <v>1</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E37" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="F37" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="G37" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="H37" s="13" t="s">
-        <v>391</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+      <c r="H37" s="32" t="s">
+        <v>591</v>
+      </c>
+      <c r="I37" s="33" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="48.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-21</v>
@@ -5021,10 +5101,10 @@
         <v>99</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="108" x14ac:dyDescent="0.25">
@@ -5043,13 +5123,13 @@
         <v>369</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>338</v>
       </c>
       <c r="H39" s="19" t="s">
-        <v>556</v>
+        <v>546</v>
       </c>
       <c r="I39" s="24"/>
     </row>
@@ -5069,13 +5149,13 @@
         <v>369</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>338</v>
       </c>
       <c r="H40" s="19" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="I40" s="24"/>
     </row>
@@ -5103,7 +5183,7 @@
         <v>267</v>
       </c>
       <c r="H41" s="19" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="I41" s="24"/>
     </row>
@@ -5131,7 +5211,7 @@
         <v>133</v>
       </c>
       <c r="H42" s="19" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="I42" s="24"/>
     </row>
@@ -5157,10 +5237,10 @@
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="19" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="I43" s="23" t="s">
-        <v>557</v>
+        <v>547</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="108" x14ac:dyDescent="0.25">
@@ -5187,10 +5267,10 @@
         <v>26</v>
       </c>
       <c r="H44" s="13" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5217,10 +5297,10 @@
         <v>22</v>
       </c>
       <c r="H45" s="19" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -5245,10 +5325,10 @@
       </c>
       <c r="G46" s="4"/>
       <c r="H46" s="19" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -5275,7 +5355,7 @@
         <v>33</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>558</v>
+        <v>548</v>
       </c>
       <c r="I47" s="24"/>
     </row>
@@ -5303,7 +5383,7 @@
         <v>106</v>
       </c>
       <c r="H48" s="19" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I48" s="24"/>
     </row>
@@ -5331,13 +5411,13 @@
         <v>25</v>
       </c>
       <c r="H49" s="17" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="96" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-5</v>
@@ -5361,10 +5441,10 @@
         <v>28</v>
       </c>
       <c r="H50" s="26" t="s">
-        <v>559</v>
+        <v>549</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="84" x14ac:dyDescent="0.25">
@@ -5391,10 +5471,10 @@
         <v>14</v>
       </c>
       <c r="H51" s="13" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="24" x14ac:dyDescent="0.25">
@@ -5477,10 +5557,10 @@
         <v>145</v>
       </c>
       <c r="H54" s="17" t="s">
-        <v>560</v>
+        <v>550</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
@@ -5508,7 +5588,7 @@
         <v>379</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5533,10 +5613,10 @@
         <v>87</v>
       </c>
       <c r="H56" s="17" t="s">
-        <v>561</v>
+        <v>551</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="72" x14ac:dyDescent="0.25">
@@ -5561,10 +5641,10 @@
       </c>
       <c r="G57" s="4"/>
       <c r="H57" s="13" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -5594,7 +5674,7 @@
         <v>379</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="216" x14ac:dyDescent="0.25">
@@ -5617,7 +5697,7 @@
       </c>
       <c r="G59" s="4"/>
       <c r="H59" s="19" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="I59" s="24"/>
     </row>
@@ -5645,7 +5725,7 @@
         <v>148</v>
       </c>
       <c r="H60" s="19" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I60" s="24"/>
     </row>
@@ -5669,7 +5749,7 @@
       </c>
       <c r="G61" s="4"/>
       <c r="H61" s="19" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="I61" s="24"/>
     </row>
@@ -5693,10 +5773,10 @@
       </c>
       <c r="G62" s="4"/>
       <c r="H62" s="13" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>557</v>
+        <v>547</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="96" x14ac:dyDescent="0.25">
@@ -5723,7 +5803,7 @@
         <v>151</v>
       </c>
       <c r="H63" s="19" t="s">
-        <v>562</v>
+        <v>552</v>
       </c>
       <c r="I63" s="24"/>
     </row>
@@ -5747,7 +5827,7 @@
       </c>
       <c r="G64" s="4"/>
       <c r="H64" s="13" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="I64" s="24"/>
     </row>
@@ -5775,7 +5855,7 @@
         <v>154</v>
       </c>
       <c r="H65" s="19" t="s">
-        <v>563</v>
+        <v>553</v>
       </c>
       <c r="I65" s="24"/>
     </row>
@@ -5803,10 +5883,10 @@
         <v>50</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -5833,10 +5913,10 @@
         <v>53</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>564</v>
+        <v>554</v>
       </c>
       <c r="I67" s="4" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="195" x14ac:dyDescent="0.25">
@@ -5863,7 +5943,7 @@
         <v>270</v>
       </c>
       <c r="H68" s="19" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="I68" s="24"/>
     </row>
@@ -5891,7 +5971,7 @@
         <v>241</v>
       </c>
       <c r="H69" s="19" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="I69" s="24"/>
     </row>
@@ -5919,7 +5999,7 @@
         <v>271</v>
       </c>
       <c r="H70" s="19" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="I70" s="24"/>
     </row>
@@ -5947,7 +6027,7 @@
         <v>272</v>
       </c>
       <c r="H71" s="19" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="I71" s="24"/>
     </row>
@@ -5975,10 +6055,10 @@
         <v>197</v>
       </c>
       <c r="H72" s="17" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="36" x14ac:dyDescent="0.25">
@@ -5990,25 +6070,25 @@
         <v>14</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E73" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="G73" s="4" t="s">
         <v>442</v>
       </c>
-      <c r="F73" s="4" t="s">
-        <v>443</v>
-      </c>
-      <c r="G73" s="4" t="s">
-        <v>444</v>
-      </c>
       <c r="H73" s="19" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="24" x14ac:dyDescent="0.25">
@@ -6020,25 +6100,25 @@
         <v>19</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E74" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="G74" s="4" t="s">
         <v>442</v>
       </c>
-      <c r="F74" s="4" t="s">
-        <v>443</v>
-      </c>
-      <c r="G74" s="4" t="s">
-        <v>444</v>
-      </c>
       <c r="H74" s="17" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="24" x14ac:dyDescent="0.25">
@@ -6050,25 +6130,25 @@
         <v>16</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="H75" s="17" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="I75" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6095,7 +6175,7 @@
         <v>273</v>
       </c>
       <c r="H76" s="19" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="I76" s="24"/>
     </row>
@@ -6123,7 +6203,7 @@
         <v>275</v>
       </c>
       <c r="H77" s="19" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="I77" s="24"/>
     </row>
@@ -6136,25 +6216,25 @@
         <v>2</v>
       </c>
       <c r="C78" s="4" t="s">
+        <v>561</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>562</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>565</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>566</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="H78" s="19" t="s">
         <v>571</v>
       </c>
-      <c r="D78" s="5" t="s">
-        <v>572</v>
-      </c>
-      <c r="E78" s="5" t="s">
-        <v>575</v>
-      </c>
-      <c r="F78" s="4" t="s">
-        <v>576</v>
-      </c>
-      <c r="G78" s="4" t="s">
-        <v>577</v>
-      </c>
-      <c r="H78" s="19" t="s">
-        <v>581</v>
-      </c>
       <c r="I78" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -6181,7 +6261,7 @@
         <v>203</v>
       </c>
       <c r="H79" s="19" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="I79" s="24"/>
     </row>
@@ -6194,25 +6274,25 @@
         <v>22</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="H80" s="19" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="27" x14ac:dyDescent="0.25">
@@ -6224,25 +6304,25 @@
         <v>23</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="H81" s="17" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="I81" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -6254,25 +6334,25 @@
         <v>24</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="H82" s="13" t="s">
-        <v>565</v>
+        <v>555</v>
       </c>
       <c r="I82" s="4" t="s">
-        <v>557</v>
+        <v>547</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -6299,7 +6379,7 @@
         <v>206</v>
       </c>
       <c r="H83" s="19" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="I83" s="24"/>
     </row>
@@ -6327,7 +6407,7 @@
         <v>209</v>
       </c>
       <c r="H84" s="19" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="I84" s="24"/>
     </row>
@@ -6355,7 +6435,7 @@
         <v>211</v>
       </c>
       <c r="H85" s="19" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="I85" s="24"/>
     </row>
@@ -6383,10 +6463,10 @@
         <v>213</v>
       </c>
       <c r="H86" s="17" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="I86" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -6398,25 +6478,25 @@
         <v>27</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="G87" s="4" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="H87" s="19" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>566</v>
+        <v>556</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -6443,10 +6523,10 @@
         <v>216</v>
       </c>
       <c r="H88" s="19" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -6458,25 +6538,25 @@
         <v>26</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="G89" s="4" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="H89" s="19" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="I89" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -6506,7 +6586,7 @@
         <v>379</v>
       </c>
       <c r="I90" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="36" x14ac:dyDescent="0.25">
@@ -6531,10 +6611,10 @@
         <v>91</v>
       </c>
       <c r="H91" s="17" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="I91" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="77.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6559,10 +6639,10 @@
       </c>
       <c r="G92" s="4"/>
       <c r="H92" s="13" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="I92" s="4" t="s">
-        <v>557</v>
+        <v>547</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="36" x14ac:dyDescent="0.25">
@@ -6589,7 +6669,7 @@
         <v>218</v>
       </c>
       <c r="H93" s="19" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="I93" s="24"/>
     </row>
@@ -6617,10 +6697,10 @@
         <v>278</v>
       </c>
       <c r="H94" s="13" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="I94" s="4" t="s">
-        <v>557</v>
+        <v>547</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="96" x14ac:dyDescent="0.25">
@@ -6647,10 +6727,10 @@
         <v>279</v>
       </c>
       <c r="H95" s="21" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="I95" s="4" t="s">
-        <v>557</v>
+        <v>547</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="113.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -6677,7 +6757,7 @@
         <v>259</v>
       </c>
       <c r="H96" s="27" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="I96" s="24"/>
     </row>
@@ -6705,7 +6785,7 @@
         <v>113</v>
       </c>
       <c r="H97" s="19" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="I97" s="24"/>
     </row>
@@ -6787,10 +6867,10 @@
       </c>
       <c r="G100" s="4"/>
       <c r="H100" s="19" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="I100" s="4" t="s">
-        <v>567</v>
+        <v>557</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="72" x14ac:dyDescent="0.25">
@@ -6802,20 +6882,20 @@
         <v>3</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>571</v>
+        <v>561</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>572</v>
+        <v>562</v>
       </c>
       <c r="E101" s="5"/>
       <c r="F101" s="4" t="s">
-        <v>578</v>
+        <v>568</v>
       </c>
       <c r="G101" s="4" t="s">
-        <v>579</v>
+        <v>569</v>
       </c>
       <c r="H101" s="19" t="s">
-        <v>580</v>
+        <v>570</v>
       </c>
       <c r="I101" s="24"/>
     </row>
@@ -6828,25 +6908,25 @@
         <v>15</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D102" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E102" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="F102" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="G102" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="F102" s="4" t="s">
-        <v>446</v>
-      </c>
-      <c r="G102" s="4" t="s">
-        <v>447</v>
-      </c>
       <c r="H102" s="17" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="I102" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -6858,25 +6938,25 @@
         <v>1</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D103" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E103" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="F103" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="G103" s="4" t="s">
         <v>413</v>
-      </c>
-      <c r="F103" s="4" t="s">
-        <v>414</v>
-      </c>
-      <c r="G103" s="4" t="s">
-        <v>415</v>
       </c>
       <c r="H103" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I103" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="24" x14ac:dyDescent="0.25">
@@ -6888,25 +6968,25 @@
         <v>17</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D104" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="F104" s="4" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="G104" s="4" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="H104" s="17" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="I104" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="24" x14ac:dyDescent="0.25">
@@ -6918,25 +6998,25 @@
         <v>20</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D105" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="G105" s="4" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="H105" s="17" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="I105" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="106" spans="1:9" ht="39" x14ac:dyDescent="0.25">
@@ -6948,22 +7028,22 @@
         <v>21</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D106" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="G106" s="4" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="H106" s="19" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I106" s="24"/>
     </row>
@@ -6976,25 +7056,25 @@
         <v>18</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D107" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E107" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="F107" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="G107" s="4" t="s">
         <v>451</v>
       </c>
-      <c r="F107" s="4" t="s">
-        <v>452</v>
-      </c>
-      <c r="G107" s="4" t="s">
-        <v>453</v>
-      </c>
       <c r="H107" s="13" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I107" s="4" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="108" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -7006,25 +7086,25 @@
         <v>25</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D108" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E108" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="F108" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="G108" s="4" t="s">
         <v>462</v>
       </c>
-      <c r="F108" s="4" t="s">
-        <v>463</v>
-      </c>
-      <c r="G108" s="4" t="s">
-        <v>464</v>
-      </c>
       <c r="H108" s="17" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="I108" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="24" x14ac:dyDescent="0.25">
@@ -7036,19 +7116,19 @@
         <v>2</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D109" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E109" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="F109" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="G109" s="4" t="s">
         <v>416</v>
-      </c>
-      <c r="F109" s="4" t="s">
-        <v>417</v>
-      </c>
-      <c r="G109" s="4" t="s">
-        <v>418</v>
       </c>
       <c r="H109" s="17" t="s">
         <v>352</v>
@@ -7064,19 +7144,19 @@
         <v>3</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D110" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E110" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="F110" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="G110" s="4" t="s">
         <v>419</v>
-      </c>
-      <c r="F110" s="4" t="s">
-        <v>420</v>
-      </c>
-      <c r="G110" s="4" t="s">
-        <v>421</v>
       </c>
       <c r="H110" s="17" t="s">
         <v>352</v>
@@ -7092,19 +7172,19 @@
         <v>4</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D111" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E111" s="5" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F111" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="G111" s="4" t="s">
         <v>420</v>
-      </c>
-      <c r="G111" s="4" t="s">
-        <v>422</v>
       </c>
       <c r="H111" s="17" t="s">
         <v>352</v>
@@ -7135,10 +7215,10 @@
         <v>250</v>
       </c>
       <c r="H112" s="6" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="I112" s="4" t="s">
-        <v>568</v>
+        <v>558</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="24" x14ac:dyDescent="0.25">
@@ -7150,19 +7230,19 @@
         <v>5</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D113" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E113" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="F113" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="G113" s="4" t="s">
         <v>423</v>
-      </c>
-      <c r="F113" s="4" t="s">
-        <v>424</v>
-      </c>
-      <c r="G113" s="4" t="s">
-        <v>425</v>
       </c>
       <c r="H113" s="17" t="s">
         <v>352</v>
@@ -7178,19 +7258,19 @@
         <v>6</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D114" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E114" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="F114" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="G114" s="4" t="s">
         <v>426</v>
-      </c>
-      <c r="F114" s="4" t="s">
-        <v>427</v>
-      </c>
-      <c r="G114" s="4" t="s">
-        <v>428</v>
       </c>
       <c r="H114" s="17" t="s">
         <v>352</v>
@@ -7206,19 +7286,19 @@
         <v>7</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D115" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E115" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="F115" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="G115" s="4" t="s">
         <v>426</v>
-      </c>
-      <c r="F115" s="4" t="s">
-        <v>429</v>
-      </c>
-      <c r="G115" s="4" t="s">
-        <v>428</v>
       </c>
       <c r="H115" s="17" t="s">
         <v>352</v>
@@ -7234,19 +7314,19 @@
         <v>8</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D116" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="F116" s="4" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="G116" s="4" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="H116" s="17" t="s">
         <v>352</v>
@@ -7262,19 +7342,19 @@
         <v>9</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D117" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="F117" s="4" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="G117" s="4" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="H117" s="17" t="s">
         <v>352</v>
@@ -7290,22 +7370,22 @@
         <v>10</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D118" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E118" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="F118" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="F118" s="4" t="s">
-        <v>432</v>
-      </c>
       <c r="G118" s="4" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="H118" s="19" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="I118" s="24"/>
     </row>
@@ -7318,25 +7398,25 @@
         <v>11</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D119" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E119" s="5" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="F119" s="4" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="G119" s="4" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="H119" s="13" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I119" s="4" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="120" spans="1:9" ht="24" x14ac:dyDescent="0.25">
@@ -7348,19 +7428,19 @@
         <v>12</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D120" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E120" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="F120" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="G120" s="4" t="s">
         <v>436</v>
-      </c>
-      <c r="F120" s="4" t="s">
-        <v>437</v>
-      </c>
-      <c r="G120" s="4" t="s">
-        <v>438</v>
       </c>
       <c r="H120" s="17" t="s">
         <v>352</v>
@@ -7376,19 +7456,19 @@
         <v>13</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D121" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E121" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="F121" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="G121" s="4" t="s">
         <v>439</v>
-      </c>
-      <c r="F121" s="4" t="s">
-        <v>440</v>
-      </c>
-      <c r="G121" s="4" t="s">
-        <v>441</v>
       </c>
       <c r="H121" s="17" t="s">
         <v>352</v>
@@ -7419,7 +7499,7 @@
         <v>29</v>
       </c>
       <c r="H122" s="19" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="I122" s="24"/>
     </row>
@@ -7447,7 +7527,7 @@
         <v>252</v>
       </c>
       <c r="H123" s="19" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="I123" s="24"/>
     </row>
@@ -7475,11 +7555,11 @@
         <v>104</v>
       </c>
       <c r="H124" s="19" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="I124" s="24"/>
     </row>
-    <row r="125" spans="1:9" ht="84" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" ht="96" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-20</v>
@@ -7503,7 +7583,7 @@
         <v>162</v>
       </c>
       <c r="H125" s="19" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="I125" s="24"/>
     </row>
@@ -7531,7 +7611,7 @@
         <v>225</v>
       </c>
       <c r="H126" s="19" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="I126" s="24"/>
     </row>
@@ -7559,7 +7639,7 @@
         <v>228</v>
       </c>
       <c r="H127" s="19" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="I127" s="24"/>
     </row>
@@ -7587,7 +7667,7 @@
         <v>10</v>
       </c>
       <c r="H128" s="19" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="I128" s="24"/>
     </row>
@@ -7613,7 +7693,7 @@
       </c>
       <c r="G129" s="4"/>
       <c r="H129" s="19" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="I129" s="24"/>
     </row>
@@ -7639,7 +7719,7 @@
       </c>
       <c r="G130" s="4"/>
       <c r="H130" s="19" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="I130" s="24"/>
     </row>
@@ -7667,10 +7747,10 @@
         <v>136</v>
       </c>
       <c r="H131" s="19" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="I131" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="132" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -7697,7 +7777,7 @@
         <v>139</v>
       </c>
       <c r="H132" s="19" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="I132" s="24"/>
     </row>
@@ -7725,7 +7805,7 @@
         <v>231</v>
       </c>
       <c r="H133" s="17" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="I133" s="4"/>
     </row>
@@ -7756,7 +7836,7 @@
         <v>352</v>
       </c>
       <c r="I134" s="4" t="s">
-        <v>569</v>
+        <v>559</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="24" x14ac:dyDescent="0.25">
@@ -7786,7 +7866,7 @@
         <v>352</v>
       </c>
       <c r="I135" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -7813,10 +7893,10 @@
         <v>37</v>
       </c>
       <c r="H136" s="13" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="I136" s="4" t="s">
-        <v>557</v>
+        <v>547</v>
       </c>
     </row>
     <row r="137" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -7843,10 +7923,10 @@
         <v>39</v>
       </c>
       <c r="H137" s="13" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="I137" s="4" t="s">
-        <v>557</v>
+        <v>547</v>
       </c>
     </row>
     <row r="138" spans="1:9" ht="72" x14ac:dyDescent="0.25">
@@ -7873,10 +7953,10 @@
         <v>41</v>
       </c>
       <c r="H138" s="19" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="I138" s="4" t="s">
-        <v>570</v>
+        <v>560</v>
       </c>
     </row>
     <row r="139" spans="1:9" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -7901,10 +7981,10 @@
       </c>
       <c r="G139" s="4"/>
       <c r="H139" s="13" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="I139" s="4" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="140" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -7931,7 +8011,7 @@
         <v>43</v>
       </c>
       <c r="H140" s="17" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="I140" s="24"/>
     </row>
@@ -7959,10 +8039,10 @@
         <v>31</v>
       </c>
       <c r="H141" s="13" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="I141" s="23" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modif tableau synthèse avant reunion 2 de resolutions
</commit_message>
<xml_diff>
--- a/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
+++ b/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Geostandards-Risques\suivi\2024-05_06-Consultation-publique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BAFA14-EBC6-4921-84F6-E5DA9404F947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5BB7E9-35FB-4545-ABF2-7191EC5C82E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Synthese Modele Commun" sheetId="3" r:id="rId1"/>
@@ -1371,10 +1371,6 @@
 </t>
   </si>
   <si>
-    <t>NOK ?
-avalanche est sous-entendu par la forumlation "Tous PPRN". Sinon il faudrait lister tous les types d'Aléas naturels pour chaque niveau</t>
-  </si>
-  <si>
     <t>A discuter avec le GT et les demandeurs</t>
   </si>
   <si>
@@ -1389,13 +1385,6 @@
  ( dans notre CdC local, c'est  NIVALEA_STD=00  et  NIVALEA=AP )
 Je n'ai pas retrouvé ces types de zones dans les classes ZoneAlea du nouveau standard. Ces zones, bien qu'étant techniquement hors aléa, sont sensibles. Elles ont un impact sur l'urbanisme et sur la conception du zonage réglementaire.
 </t>
-  </si>
-  <si>
-    <t>OK sur le principe. A valider avec le GT</t>
-  </si>
-  <si>
-    <t>OK sur le principe,
-A voir s'il y a moyen d'harmoniser avec la nomenclature PPRN?</t>
   </si>
   <si>
     <t>C'est un héritage du PPR Covadis.
@@ -2276,6 +2265,22 @@
     <t>NOK ?
 La nomenture des risques GASPAR ne fait pas la distinction entre les différents types d'avalanche. Peut-être faut-il faire des sous-types de l'aléa 14 comme pour l'inondation ?
 Pour l'instant cette information peut être mise dans la description texte libre</t>
+  </si>
+  <si>
+    <t>OK sur le principe,
+A voir s'il y a moyen d'harmoniser avec la nomenclature PPRN plutôt que de rajouter une nomenclature?</t>
+  </si>
+  <si>
+    <t>OK sur le principe. A valider avec le GT
+NB : quid des autres aleéas technos (non industriels) ? 
+Risque technologique ; Nucléaire
+Risque technologique ; Rupture de barrage
+Risque technologique ; Transport de marchandises dangereuses
+Risque technologique ; Engins de guerre</t>
+  </si>
+  <si>
+    <t>NOK ?
+avalanche est sous-entendu par la formulation "Tous PPRN". Sinon il faudrait lister tous les types d'Aléas naturels pour chaque niveau</t>
   </si>
 </sst>
 </file>
@@ -3358,21 +3363,21 @@
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="3" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" style="3" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" style="3" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="21.81640625" style="3" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="3" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="49.5703125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="47.5703125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="54.85546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="10.85546875" style="3"/>
+    <col min="5" max="5" width="16.1796875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="49.54296875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="47.54296875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="54.81640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="21.453125" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="10.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>349</v>
       </c>
@@ -3398,10 +3403,10 @@
         <v>5</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="72.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="73" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-1</v>
@@ -3428,10 +3433,10 @@
         <v>351</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="108" x14ac:dyDescent="0.25">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-2</v>
@@ -3455,13 +3460,13 @@
         <v>332</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="108" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-3</v>
@@ -3488,10 +3493,10 @@
         <v>353</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="75.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-4</v>
@@ -3515,13 +3520,13 @@
         <v>305</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="89.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="89.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-5</v>
@@ -3548,10 +3553,10 @@
         <v>350</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/DAPP/BIP-11</v>
@@ -3576,10 +3581,10 @@
         <v>352</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="96" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-6</v>
@@ -3606,10 +3611,10 @@
         <v>358</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="144" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="115" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-7</v>
@@ -3636,10 +3641,10 @@
         <v>354</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-1</v>
@@ -3666,10 +3671,10 @@
         <v>355</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-2</v>
@@ -3696,10 +3701,10 @@
         <v>355</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="108" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-8</v>
@@ -3723,13 +3728,13 @@
         <v>315</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>cerema-6</v>
@@ -3756,10 +3761,10 @@
         <v>356</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="96" x14ac:dyDescent="0.25">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-9</v>
@@ -3786,10 +3791,10 @@
         <v>357</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="60.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="61" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-10</v>
@@ -3816,10 +3821,10 @@
         <v>352</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="68.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-3</v>
@@ -3843,13 +3848,13 @@
         <v>288</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="77.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="77.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-4</v>
@@ -3876,10 +3881,10 @@
         <v>359</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="111" customHeight="1" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="111" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-5</v>
@@ -3903,13 +3908,13 @@
         <v>293</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="96" x14ac:dyDescent="0.25">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SDCAP/PONSOH-13</v>
@@ -3933,13 +3938,13 @@
         <v>328</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/DAPP/BIP-12</v>
@@ -3964,7 +3969,7 @@
         <v>360</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
   </sheetData>
@@ -3980,25 +3985,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815F14A-19BC-4DCE-8D31-81F595A4B0E7}">
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="3.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="3.81640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="3" customWidth="1"/>
     <col min="4" max="4" width="16" style="3" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="44.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="44.1796875" style="3" customWidth="1"/>
     <col min="7" max="7" width="38" style="3" customWidth="1"/>
-    <col min="8" max="8" width="51.85546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="10.85546875" style="3"/>
+    <col min="8" max="8" width="51.81640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="22.26953125" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="10.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>348</v>
       </c>
@@ -4024,10 +4029,10 @@
         <v>5</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-2</v>
@@ -4049,13 +4054,13 @@
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="25" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-3</v>
@@ -4080,10 +4085,10 @@
         <v>371</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-4</v>
@@ -4108,10 +4113,10 @@
         <v>372</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="65.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-5</v>
@@ -4133,13 +4138,13 @@
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="22" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="132" x14ac:dyDescent="0.25">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="126.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP-0</v>
@@ -4162,10 +4167,10 @@
         <v>373</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-9</v>
@@ -4190,10 +4195,10 @@
         <v>374</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-14</v>
@@ -4218,10 +4223,10 @@
         <v>375</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-15</v>
@@ -4246,10 +4251,10 @@
         <v>376</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDTM11-1</v>
@@ -4258,26 +4263,26 @@
         <v>1</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="4" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-2</v>
@@ -4305,7 +4310,7 @@
       </c>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" spans="1:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-3</v>
@@ -4333,7 +4338,7 @@
       </c>
       <c r="I12" s="24"/>
     </row>
-    <row r="13" spans="1:9" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-1</v>
@@ -4360,10 +4365,10 @@
         <v>350</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="66.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-1</v>
@@ -4387,13 +4392,13 @@
         <v>166</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="168" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="161" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-2</v>
@@ -4417,13 +4422,13 @@
         <v>254</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-3</v>
@@ -4447,13 +4452,13 @@
         <v>62</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-1</v>
@@ -4477,13 +4482,13 @@
         <v>117</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-4</v>
@@ -4510,10 +4515,10 @@
         <v>380</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-4</v>
@@ -4540,10 +4545,10 @@
         <v>381</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="84.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-5</v>
@@ -4567,13 +4572,13 @@
         <v>255</v>
       </c>
       <c r="H20" s="19" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="84" x14ac:dyDescent="0.25">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-6</v>
@@ -4597,13 +4602,13 @@
         <v>256</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-2</v>
@@ -4630,10 +4635,10 @@
         <v>382</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-3</v>
@@ -4657,13 +4662,13 @@
         <v>122</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-5</v>
@@ -4690,10 +4695,10 @@
         <v>383</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-4</v>
@@ -4720,10 +4725,10 @@
         <v>384</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-5</v>
@@ -4750,10 +4755,10 @@
         <v>383</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="71.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="71.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-7</v>
@@ -4777,13 +4782,13 @@
         <v>72</v>
       </c>
       <c r="H27" s="19" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="I27" s="24" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-6</v>
@@ -4810,10 +4815,10 @@
         <v>352</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="115" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-</v>
@@ -4835,13 +4840,13 @@
         <v>340</v>
       </c>
       <c r="H29" s="19" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="I29" s="24" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-8</v>
@@ -4865,13 +4870,13 @@
         <v>75</v>
       </c>
       <c r="H30" s="19" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-9</v>
@@ -4898,10 +4903,10 @@
         <v>385</v>
       </c>
       <c r="I31" s="24" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-6</v>
@@ -4928,10 +4933,10 @@
         <v>386</v>
       </c>
       <c r="I32" s="24" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="108" x14ac:dyDescent="0.25">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-7</v>
@@ -4958,10 +4963,10 @@
         <v>388</v>
       </c>
       <c r="I33" s="24" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="41.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-10</v>
@@ -4983,13 +4988,13 @@
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="17" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-7</v>
@@ -5016,10 +5021,10 @@
         <v>389</v>
       </c>
       <c r="I35" s="23" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="62.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="62.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-11</v>
@@ -5044,10 +5049,10 @@
         <v>387</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" s="34" customFormat="1" ht="84.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="34" customFormat="1" ht="81" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="28" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-1</v>
@@ -5071,13 +5076,13 @@
         <v>19</v>
       </c>
       <c r="H37" s="32" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="I37" s="33" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="48.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="44" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-21</v>
@@ -5101,13 +5106,13 @@
         <v>99</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>390</v>
+        <v>591</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="108" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-</v>
@@ -5123,17 +5128,17 @@
         <v>369</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>338</v>
       </c>
       <c r="H39" s="19" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="I39" s="24"/>
     </row>
-    <row r="40" spans="1:9" ht="228" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="207" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-</v>
@@ -5149,17 +5154,17 @@
         <v>369</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>338</v>
       </c>
       <c r="H40" s="19" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I40" s="24"/>
     </row>
-    <row r="41" spans="1:9" ht="108" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-8</v>
@@ -5183,11 +5188,11 @@
         <v>267</v>
       </c>
       <c r="H41" s="19" t="s">
-        <v>394</v>
+        <v>590</v>
       </c>
       <c r="I41" s="24"/>
     </row>
-    <row r="42" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-8</v>
@@ -5211,11 +5216,11 @@
         <v>133</v>
       </c>
       <c r="H42" s="19" t="s">
-        <v>395</v>
+        <v>589</v>
       </c>
       <c r="I42" s="24"/>
     </row>
-    <row r="43" spans="1:9" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-12</v>
@@ -5237,13 +5242,13 @@
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="19" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="I43" s="23" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="108" x14ac:dyDescent="0.25">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-4</v>
@@ -5267,13 +5272,13 @@
         <v>26</v>
       </c>
       <c r="H44" s="13" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="77.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-2</v>
@@ -5297,13 +5302,13 @@
         <v>22</v>
       </c>
       <c r="H45" s="19" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/BRNT-22</v>
@@ -5325,13 +5330,13 @@
       </c>
       <c r="G46" s="4"/>
       <c r="H46" s="19" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-8</v>
@@ -5355,11 +5360,11 @@
         <v>33</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="I47" s="24"/>
     </row>
-    <row r="48" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-24</v>
@@ -5383,11 +5388,11 @@
         <v>106</v>
       </c>
       <c r="H48" s="19" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="I48" s="24"/>
     </row>
-    <row r="49" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-3</v>
@@ -5411,13 +5416,13 @@
         <v>25</v>
       </c>
       <c r="H49" s="17" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="96" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-5</v>
@@ -5441,13 +5446,13 @@
         <v>28</v>
       </c>
       <c r="H50" s="26" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="84" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT07-2</v>
@@ -5471,13 +5476,13 @@
         <v>14</v>
       </c>
       <c r="H51" s="13" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-11</v>
@@ -5505,7 +5510,7 @@
       </c>
       <c r="I52" s="24"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-12</v>
@@ -5533,7 +5538,7 @@
       </c>
       <c r="I53" s="24"/>
     </row>
-    <row r="54" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-13</v>
@@ -5557,13 +5562,13 @@
         <v>145</v>
       </c>
       <c r="H54" s="17" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-13</v>
@@ -5588,10 +5593,10 @@
         <v>379</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-14</v>
@@ -5613,13 +5618,13 @@
         <v>87</v>
       </c>
       <c r="H56" s="17" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-15</v>
@@ -5641,13 +5646,13 @@
       </c>
       <c r="G57" s="4"/>
       <c r="H57" s="13" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-9</v>
@@ -5674,10 +5679,10 @@
         <v>379</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="216" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="184" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5697,11 +5702,11 @@
       </c>
       <c r="G59" s="4"/>
       <c r="H59" s="19" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="I59" s="24"/>
     </row>
-    <row r="60" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-14</v>
@@ -5725,11 +5730,11 @@
         <v>148</v>
       </c>
       <c r="H60" s="19" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="I60" s="24"/>
     </row>
-    <row r="61" spans="1:9" ht="108" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5749,11 +5754,11 @@
       </c>
       <c r="G61" s="4"/>
       <c r="H61" s="19" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="I61" s="24"/>
     </row>
-    <row r="62" spans="1:9" ht="252" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="230" x14ac:dyDescent="0.35">
       <c r="A62" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5773,13 +5778,13 @@
       </c>
       <c r="G62" s="4"/>
       <c r="H62" s="13" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" ht="96" x14ac:dyDescent="0.25">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-15</v>
@@ -5803,11 +5808,11 @@
         <v>151</v>
       </c>
       <c r="H63" s="19" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="I63" s="24"/>
     </row>
-    <row r="64" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A64" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5827,11 +5832,11 @@
       </c>
       <c r="G64" s="4"/>
       <c r="H64" s="13" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="I64" s="24"/>
     </row>
-    <row r="65" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-16</v>
@@ -5855,11 +5860,11 @@
         <v>154</v>
       </c>
       <c r="H65" s="19" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="I65" s="24"/>
     </row>
-    <row r="66" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT01-3</v>
@@ -5883,13 +5888,13 @@
         <v>50</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDTM 83-1</v>
@@ -5913,13 +5918,13 @@
         <v>53</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="I67" s="4" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="174" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-10</v>
@@ -5943,11 +5948,11 @@
         <v>270</v>
       </c>
       <c r="H68" s="19" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="I68" s="24"/>
     </row>
-    <row r="69" spans="1:9" ht="87.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="88" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-1</v>
@@ -5971,11 +5976,11 @@
         <v>241</v>
       </c>
       <c r="H69" s="19" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="I69" s="24"/>
     </row>
-    <row r="70" spans="1:9" ht="102.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="103" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-11</v>
@@ -5999,11 +6004,11 @@
         <v>271</v>
       </c>
       <c r="H70" s="19" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="I70" s="24"/>
     </row>
-    <row r="71" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
       <c r="A71" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-12</v>
@@ -6027,11 +6032,11 @@
         <v>272</v>
       </c>
       <c r="H71" s="19" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="I71" s="24"/>
     </row>
-    <row r="72" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-13</v>
@@ -6055,13 +6060,13 @@
         <v>197</v>
       </c>
       <c r="H72" s="17" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A73" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-14</v>
@@ -6070,28 +6075,28 @@
         <v>14</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="H73" s="19" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-19</v>
@@ -6100,28 +6105,28 @@
         <v>19</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="H74" s="17" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-16</v>
@@ -6130,28 +6135,28 @@
         <v>16</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="H75" s="17" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="I75" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-14</v>
@@ -6175,11 +6180,11 @@
         <v>273</v>
       </c>
       <c r="H76" s="19" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="I76" s="24"/>
     </row>
-    <row r="77" spans="1:9" ht="144" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="126.5" x14ac:dyDescent="0.35">
       <c r="A77" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-15</v>
@@ -6203,11 +6208,11 @@
         <v>275</v>
       </c>
       <c r="H77" s="19" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="I77" s="24"/>
     </row>
-    <row r="78" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A78" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDTM11-2</v>
@@ -6216,28 +6221,28 @@
         <v>2</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="D78" s="5" t="s">
+        <v>559</v>
+      </c>
+      <c r="E78" s="5" t="s">
         <v>562</v>
       </c>
-      <c r="E78" s="5" t="s">
-        <v>565</v>
-      </c>
       <c r="F78" s="4" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="H78" s="19" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A79" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-16</v>
@@ -6261,11 +6266,11 @@
         <v>203</v>
       </c>
       <c r="H79" s="19" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="I79" s="24"/>
     </row>
-    <row r="80" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A80" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-22</v>
@@ -6274,28 +6279,28 @@
         <v>22</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="H80" s="19" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="26" x14ac:dyDescent="0.35">
       <c r="A81" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-23</v>
@@ -6304,28 +6309,28 @@
         <v>23</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="H81" s="17" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="I81" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A82" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-24</v>
@@ -6334,28 +6339,28 @@
         <v>24</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="H82" s="13" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="I82" s="4" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-17</v>
@@ -6379,11 +6384,11 @@
         <v>206</v>
       </c>
       <c r="H83" s="19" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="I83" s="24"/>
     </row>
-    <row r="84" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A84" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-18</v>
@@ -6407,11 +6412,11 @@
         <v>209</v>
       </c>
       <c r="H84" s="19" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="I84" s="24"/>
     </row>
-    <row r="85" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A85" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-19</v>
@@ -6435,11 +6440,11 @@
         <v>211</v>
       </c>
       <c r="H85" s="19" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="I85" s="24"/>
     </row>
-    <row r="86" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-20</v>
@@ -6463,13 +6468,13 @@
         <v>213</v>
       </c>
       <c r="H86" s="17" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="I86" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-27</v>
@@ -6478,28 +6483,28 @@
         <v>27</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="G87" s="4" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="H87" s="19" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A88" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-21</v>
@@ -6523,13 +6528,13 @@
         <v>216</v>
       </c>
       <c r="H88" s="19" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="39.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-26</v>
@@ -6538,28 +6543,28 @@
         <v>26</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="G89" s="4" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="H89" s="19" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="I89" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-17</v>
@@ -6586,10 +6591,10 @@
         <v>379</v>
       </c>
       <c r="I90" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A91" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-16</v>
@@ -6611,13 +6616,13 @@
         <v>91</v>
       </c>
       <c r="H91" s="17" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="I91" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" ht="77.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-17</v>
@@ -6639,13 +6644,13 @@
       </c>
       <c r="G92" s="4"/>
       <c r="H92" s="13" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="I92" s="4" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A93" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-22</v>
@@ -6669,11 +6674,11 @@
         <v>218</v>
       </c>
       <c r="H93" s="19" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="I93" s="24"/>
     </row>
-    <row r="94" spans="1:9" ht="96" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" ht="98" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-23</v>
@@ -6697,13 +6702,13 @@
         <v>278</v>
       </c>
       <c r="H94" s="13" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="I94" s="4" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" ht="96" x14ac:dyDescent="0.25">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A95" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-24</v>
@@ -6727,13 +6732,13 @@
         <v>279</v>
       </c>
       <c r="H95" s="21" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="I95" s="4" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" ht="113.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="113.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/PoNSOH-26</v>
@@ -6757,11 +6762,11 @@
         <v>259</v>
       </c>
       <c r="H96" s="27" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="I96" s="24"/>
     </row>
-    <row r="97" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/PoNSOH-27</v>
@@ -6785,11 +6790,11 @@
         <v>113</v>
       </c>
       <c r="H97" s="19" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="I97" s="24"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-18</v>
@@ -6817,7 +6822,7 @@
       </c>
       <c r="I98" s="24"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-19</v>
@@ -6845,7 +6850,7 @@
       </c>
       <c r="I99" s="24"/>
     </row>
-    <row r="100" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-18</v>
@@ -6867,13 +6872,13 @@
       </c>
       <c r="G100" s="4"/>
       <c r="H100" s="19" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="I100" s="4" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A101" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDTM11-3</v>
@@ -6882,24 +6887,24 @@
         <v>3</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="E101" s="5"/>
       <c r="F101" s="4" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="G101" s="4" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="H101" s="19" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="I101" s="24"/>
     </row>
-    <row r="102" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A102" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-15</v>
@@ -6908,28 +6913,28 @@
         <v>15</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D102" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="G102" s="4" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="H102" s="17" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="I102" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-1</v>
@@ -6938,28 +6943,28 @@
         <v>1</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D103" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="F103" s="4" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="G103" s="4" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="H103" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I103" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A104" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-17</v>
@@ -6968,28 +6973,28 @@
         <v>17</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D104" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="F104" s="4" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="G104" s="4" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="H104" s="17" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="I104" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A105" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-20</v>
@@ -6998,28 +7003,28 @@
         <v>20</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D105" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="G105" s="4" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="H105" s="17" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="I105" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" ht="39" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A106" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-21</v>
@@ -7028,26 +7033,26 @@
         <v>21</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D106" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G106" s="4" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="H106" s="19" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="I106" s="24"/>
     </row>
-    <row r="107" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A107" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-18</v>
@@ -7056,28 +7061,28 @@
         <v>18</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D107" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="G107" s="4" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="H107" s="13" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="I107" s="4" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A108" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-25</v>
@@ -7086,28 +7091,28 @@
         <v>25</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D108" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="F108" s="4" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="G108" s="4" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="H108" s="17" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="I108" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A109" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-2</v>
@@ -7116,26 +7121,26 @@
         <v>2</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D109" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E109" s="5" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="F109" s="4" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="G109" s="4" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="H109" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I109" s="24"/>
     </row>
-    <row r="110" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A110" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-3</v>
@@ -7144,26 +7149,26 @@
         <v>3</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D110" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="F110" s="4" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="G110" s="4" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="H110" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I110" s="24"/>
     </row>
-    <row r="111" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A111" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-4</v>
@@ -7172,26 +7177,26 @@
         <v>4</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D111" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E111" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="F111" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="G111" s="4" t="s">
         <v>417</v>
-      </c>
-      <c r="F111" s="4" t="s">
-        <v>418</v>
-      </c>
-      <c r="G111" s="4" t="s">
-        <v>420</v>
       </c>
       <c r="H111" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I111" s="24"/>
     </row>
-    <row r="112" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A112" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT01-1</v>
@@ -7215,13 +7220,13 @@
         <v>250</v>
       </c>
       <c r="H112" s="6" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="I112" s="4" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A113" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-5</v>
@@ -7230,26 +7235,26 @@
         <v>5</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D113" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="F113" s="4" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="G113" s="4" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="H113" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I113" s="24"/>
     </row>
-    <row r="114" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A114" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-6</v>
@@ -7258,26 +7263,26 @@
         <v>6</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D114" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="F114" s="4" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="G114" s="4" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H114" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I114" s="24"/>
     </row>
-    <row r="115" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A115" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-7</v>
@@ -7286,26 +7291,26 @@
         <v>7</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D115" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E115" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="F115" s="4" t="s">
         <v>424</v>
       </c>
-      <c r="F115" s="4" t="s">
-        <v>427</v>
-      </c>
       <c r="G115" s="4" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H115" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I115" s="24"/>
     </row>
-    <row r="116" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A116" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-8</v>
@@ -7314,26 +7319,26 @@
         <v>8</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D116" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="F116" s="4" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="G116" s="4" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H116" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I116" s="24"/>
     </row>
-    <row r="117" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A117" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-9</v>
@@ -7342,26 +7347,26 @@
         <v>9</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D117" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="F117" s="4" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="G117" s="4" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H117" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I117" s="24"/>
     </row>
-    <row r="118" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A118" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-10</v>
@@ -7370,26 +7375,26 @@
         <v>10</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D118" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E118" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="F118" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="G118" s="4" t="s">
         <v>428</v>
       </c>
-      <c r="F118" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="G118" s="4" t="s">
-        <v>431</v>
-      </c>
       <c r="H118" s="19" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="I118" s="24"/>
     </row>
-    <row r="119" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-11</v>
@@ -7398,28 +7403,28 @@
         <v>11</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D119" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E119" s="5" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="F119" s="4" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="G119" s="4" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="H119" s="13" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="I119" s="4" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-12</v>
@@ -7428,26 +7433,26 @@
         <v>12</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D120" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E120" s="5" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="F120" s="4" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="G120" s="4" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="H120" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I120" s="24"/>
     </row>
-    <row r="121" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A121" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-13</v>
@@ -7456,26 +7461,26 @@
         <v>13</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D121" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E121" s="5" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="F121" s="4" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="G121" s="4" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="H121" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I121" s="24"/>
     </row>
-    <row r="122" spans="1:9" ht="156" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" ht="151.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-6</v>
@@ -7499,11 +7504,11 @@
         <v>29</v>
       </c>
       <c r="H122" s="19" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="I122" s="24"/>
     </row>
-    <row r="123" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A123" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT01-2</v>
@@ -7527,11 +7532,11 @@
         <v>252</v>
       </c>
       <c r="H123" s="19" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="I123" s="24"/>
     </row>
-    <row r="124" spans="1:9" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-23</v>
@@ -7555,11 +7560,11 @@
         <v>104</v>
       </c>
       <c r="H124" s="19" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="I124" s="24"/>
     </row>
-    <row r="125" spans="1:9" ht="96" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A125" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-20</v>
@@ -7583,11 +7588,11 @@
         <v>162</v>
       </c>
       <c r="H125" s="19" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="I125" s="24"/>
     </row>
-    <row r="126" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A126" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-25</v>
@@ -7611,11 +7616,11 @@
         <v>225</v>
       </c>
       <c r="H126" s="19" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="I126" s="24"/>
     </row>
-    <row r="127" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-26</v>
@@ -7639,11 +7644,11 @@
         <v>228</v>
       </c>
       <c r="H127" s="19" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="I127" s="24"/>
     </row>
-    <row r="128" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT07-1</v>
@@ -7667,11 +7672,11 @@
         <v>10</v>
       </c>
       <c r="H128" s="19" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="I128" s="24"/>
     </row>
-    <row r="129" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-19</v>
@@ -7693,11 +7698,11 @@
       </c>
       <c r="G129" s="4"/>
       <c r="H129" s="19" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="I129" s="24"/>
     </row>
-    <row r="130" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-20</v>
@@ -7719,11 +7724,11 @@
       </c>
       <c r="G130" s="4"/>
       <c r="H130" s="19" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="I130" s="24"/>
     </row>
-    <row r="131" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A131" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-9</v>
@@ -7747,13 +7752,13 @@
         <v>136</v>
       </c>
       <c r="H131" s="19" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="I131" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-10</v>
@@ -7777,11 +7782,11 @@
         <v>139</v>
       </c>
       <c r="H132" s="19" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="I132" s="24"/>
     </row>
-    <row r="133" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A133" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-27</v>
@@ -7805,11 +7810,11 @@
         <v>231</v>
       </c>
       <c r="H133" s="17" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="I133" s="4"/>
     </row>
-    <row r="134" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A134" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-28</v>
@@ -7836,10 +7841,10 @@
         <v>352</v>
       </c>
       <c r="I134" s="4" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A135" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-29</v>
@@ -7866,10 +7871,10 @@
         <v>352</v>
       </c>
       <c r="I135" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A136" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-10</v>
@@ -7893,13 +7898,13 @@
         <v>37</v>
       </c>
       <c r="H136" s="13" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="I136" s="4" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A137" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-11</v>
@@ -7923,13 +7928,13 @@
         <v>39</v>
       </c>
       <c r="H137" s="13" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="I137" s="4" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="138" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A138" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-12</v>
@@ -7953,13 +7958,13 @@
         <v>41</v>
       </c>
       <c r="H138" s="19" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="I138" s="4" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" ht="44.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-25</v>
@@ -7981,13 +7986,13 @@
       </c>
       <c r="G139" s="4"/>
       <c r="H139" s="13" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="I139" s="4" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="140" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A140" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-13</v>
@@ -8011,11 +8016,11 @@
         <v>43</v>
       </c>
       <c r="H140" s="17" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="I140" s="24"/>
     </row>
-    <row r="141" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A141" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-7</v>
@@ -8039,10 +8044,10 @@
         <v>31</v>
       </c>
       <c r="H141" s="13" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="I141" s="23" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fichier de commentaires après la réunion de résolution no2
</commit_message>
<xml_diff>
--- a/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
+++ b/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Geostandards-Risques\suivi\2024-05_06-Consultation-publique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5BB7E9-35FB-4545-ABF2-7191EC5C82E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014CA7B2-0C84-4DEF-8781-23CDA5FFEB0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Synthese Modele Commun" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="607">
   <si>
     <t>Organisme</t>
   </si>
@@ -1371,9 +1371,6 @@
 </t>
   </si>
   <si>
-    <t>A discuter avec le GT et les demandeurs</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nous avons ajouté des types de niveaux d'aléa supplémentaires dans les cartes d'aléas de la DDT31 pour répondre à des cas pratiques :
 ## Pour le risque inondation : zone ou remblai hors aléa mais dans la zone inondable historique ( dans notre CdC local, c'est  NIVALEA_STD=00  et  NIVALEA=H )
 </t>
@@ -1387,15 +1384,6 @@
 </t>
   </si>
   <si>
-    <t>C'est un héritage du PPR Covadis.
-"Certains PPR peuvent parfois contenir des règlements associés à des figurés linéaires ou ponctuels (cavités, axe de ruissellement...). Les primitives graphiques linéaire et ponctuelle sont à utiliser respectivement dans ces cas de figure."</t>
-  </si>
-  <si>
-    <t>NOK ?
-Je comprends ici AE = Autorité Environnementale (et non pas Aléa Exceptionnel).
-Le novueau standard ne va pas plus loin que l'ancien au niveau du zonage foncier (il ne fait que le séparer de l'autre). La soumission à l'AE n'est pas du ressort ou non du standard il me semble ?</t>
-  </si>
-  <si>
     <t>A discuter
 Je comprends ici AE = Aléa Exceptionnel
 A priori oui, vu la logique des zones réglementaires AE spécifiques.</t>
@@ -1428,11 +1416,6 @@
     <t>NOK ?
 Cela complexifie les règles de symbologie en fonction des enjeux.
 Plutôt restreindre l'application des styles pour les zones reglementaires à moyenne échelle (départementale) ?</t>
-  </si>
-  <si>
-    <t>NOK?
-Qu'entendez-vous par zonage d'exception ?
-A priori une représentation est proposée pour les zones d'AE. Est-ce cela ?</t>
   </si>
   <si>
     <t>Ok pour sur le principe.
@@ -1785,29 +1768,12 @@
     <t>A discuter en GT (cf aussi commentaires BRIL-9 du modèle commun)</t>
   </si>
   <si>
-    <t>A discuter. Je ne suis pas sur de comprendre si la demande s'applique aux aléas technos ou naturels et ce qui est demandé exactement ?</t>
-  </si>
-  <si>
     <t>OK sur le principe  
 Il faudrait aussi dans ce cas modifier le caractère obligatoire des champs idrefexterne et refexterne (comme pour les enjeu), ainsi que l'énumération typrefexterneouvrage (rajouter valeur "aucun")</t>
   </si>
   <si>
     <t xml:space="preserve">OK sur le principe
 Il faudrait aussi dans ce cas modifier le caractère obligatoire des champs idrefexterne et refexterne </t>
-  </si>
-  <si>
-    <t>OK sur le principe ?
-A discuter :
-- faut-il rajouter un alea "multirisque" ou s'agit-il d'avoir une table qui rassemble toutes les zones d'aléa (avec superposition possibles) ?
-- s'agit-il d'une table toutes zones d'aléas naturels (de référence?)
-- le besoin est-il le même pour les aleéas technos (la strucutre peut varie d'une classe / table à l'autre) ?
-NB : cf. DDT74-6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OK sur le principe.
-Rajouter les tables d'énumération correspondant aux nomenclatures proposées.
-Simplifier les codes : proposition ?
-</t>
   </si>
   <si>
     <t>OK, à renommer</t>
@@ -1826,10 +1792,6 @@
 L'énumération ne propose qu'une seule valeur "Moyen ou modéré" qu'il faut choisir que le risque soit moyen ou modéré selon le type d'aléa considéré. On a essayé d'harmoniser les échelles (cf. p36)
 Cela pose-t-il problème ou faut-il mieux l'expliquer dans le document ?
 </t>
-  </si>
-  <si>
-    <t>OK, sur le principe.
-Peut-on précisier un cas de PPR où nul s'applique et pas très faible ? Ou inversement ?</t>
   </si>
   <si>
     <t>NOK ?
@@ -1907,10 +1869,6 @@
 Proposer une couhce multialea comme dans les commentaires précédents ?</t>
   </si>
   <si>
-    <t>OK, sur le principe
-Par contre, il n'y a pas de procédure PPRT-Multi dans la classification des procédures GASPAR.</t>
-  </si>
-  <si>
     <t xml:space="preserve">OK sur le principe
 Mais le type de Procédure PPR-L vient de la classification GASPAR (au même titre qu'on a des PPRN-S, PPRN-I, etc.. Comme sous catégories de procédures PPRN).
 On peut éventuellement étendre cette partie multirisques aux PPRL ?
@@ -1946,9 +1904,6 @@
   </si>
   <si>
     <t>C'est cité dans le guide PPRN comme enjeu incontournable</t>
-  </si>
-  <si>
-    <t>Le guide PPRN fait cette distinction sans doute pour pouvoir faire la distinction au niveau du zonage…</t>
   </si>
   <si>
     <t xml:space="preserve">OK sur le principe
@@ -2096,15 +2051,7 @@
     <t>intégré (rajout de lien vers les dexcriptions des classes dans le modèle commun)</t>
   </si>
   <si>
-    <t>A discuter avec le GT et les demandeurs
-NB : la zone inondable historique ne peut-elle pas être caractérisée par son occurrence ?</t>
-  </si>
-  <si>
     <t>N.A. ?</t>
-  </si>
-  <si>
-    <t>A discuter
-Elles sont identifiées dans les enjeux. Ne peuvent-elles pas alors être représentées comme zones de prescriptions hors zone d'aléa ou zones de prescription tout-court ?</t>
   </si>
   <si>
     <t xml:space="preserve">OK sur le principe
@@ -2123,12 +2070,6 @@
 Faisabilité à étudier et décider avec le GT
 NB : là aussi, peut-être que ces différenciations concernent plutôt les représentations à grande échelle (non concernées par cette partie du standard) ?
 NB2: de quel décret 2019 parle-t-on ? Pouvez-vous fournir la référence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OK sur le principe.
-Ah, il doit s'agir de ce zonage d'exception là !
-A étudier mais il manque vraiment la référence de ce décret (cf. commentaires précédent)
-</t>
   </si>
   <si>
     <t xml:space="preserve">NOK?
@@ -2235,10 +2176,6 @@
 =&gt; Supprimer Saint-Barthélémy (Code de l'environnement ne s'applqiue pas)</t>
   </si>
   <si>
-    <t>N.A.
-Mentionner la non opposabilité L152-7 (Code urbanisme)</t>
-  </si>
-  <si>
     <t>OK 
 Rajouter le GPU au sens de L152-7</t>
   </si>
@@ -2257,18 +2194,11 @@
   </si>
   <si>
     <t>changer en zones + mentionner la référence aux espaces du guide PPRN;2016</t>
-  </si>
-  <si>
-    <t>Soumettre la proposition coulante + aérosol + les 2 au BRNT</t>
   </si>
   <si>
     <t>NOK ?
 La nomenture des risques GASPAR ne fait pas la distinction entre les différents types d'avalanche. Peut-être faut-il faire des sous-types de l'aléa 14 comme pour l'inondation ?
 Pour l'instant cette information peut être mise dans la description texte libre</t>
-  </si>
-  <si>
-    <t>OK sur le principe,
-A voir s'il y a moyen d'harmoniser avec la nomenclature PPRN plutôt que de rajouter une nomenclature?</t>
   </si>
   <si>
     <t>OK sur le principe. A valider avec le GT
@@ -2282,12 +2212,148 @@
     <t>NOK ?
 avalanche est sous-entendu par la formulation "Tous PPRN". Sinon il faudrait lister tous les types d'Aléas naturels pour chaque niveau</t>
   </si>
+  <si>
+    <t>Mentionner la non opposabilité L152-7 (Code urbanisme)</t>
+  </si>
+  <si>
+    <t>Soumettre la proposition coulante + aérosol + les 2 au BRNT. Cf. réponse BRNT</t>
+  </si>
+  <si>
+    <t>A discuter avec le GT et les demandeurs
+NB : la zone inondable historique ne peut-elle pas être caractérisée par son occurrence ?
+PPRI (code de l'environement) : 4 niveaux
+Quid des PPR historiques ?
+=&gt; niveau : autre
+Libellé : à utiliser pour les anciens PPR (Inondation)</t>
+  </si>
+  <si>
+    <t>A faire remonter au BRNT (à minima par la liste du GT)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A discuter avec le GT et les demandeurs
+Utilisation de "Autre" mais Libellé différent à proposer (non couvert par la classification proposée des niveaux d'aléas, à utiliser de manière exceptionnelle).
+</t>
+  </si>
+  <si>
+    <t>Suppression de l'enumération et du champs effet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK sur le principe,
+Plutôt intégrer nomenclature PPRL dans celle des PPRN qui couvrira naturellement les PPRI
+</t>
+  </si>
+  <si>
+    <t>Fusionner nomenclatures PPRL et PPRN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C'est un héritage du PPR Covadis.
+"Certains PPR peuvent parfois contenir des règlements associés à des figurés linéaires ou ponctuels (cavités, axe de ruissellement...). Les primitives graphiques linéaire et ponctuelle sont à utiliser respectivement dans ces cas de figure."
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conserver les zonages réglementaires et surfaciques mais limiter leur usage à la conversion des anciens PPR et à la gestion des petites surfaces sous les seuils de tolérance.
+</t>
+  </si>
+  <si>
+    <t>NOK ?
+Je comprends ici AE = Autorité Environnementale (et non pas Aléa Exceptionnel).
+Le novueau standard ne va pas plus loin que l'ancien au niveau du zonage foncier (il ne fait que le séparer de l'autre). La soumission à l'AE n'est pas du ressort ou non du standard il me semble ?
+A priori l'expropriation ne concerne que les PPRT, pas les PPRN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pour l'AE : https://www.legifrance.gouv.fr/download/pdf/circ?id=40103 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A discuter
+Elles sont identifiées dans les enjeux. 
+Et déduties dans le Zonage reglementaire comme zones d'interdiction ou prescription avec des mesures particulières.
+</t>
+  </si>
+  <si>
+    <t>N.A.
+(voir si cela peut-être explicité dans le standard)</t>
+  </si>
+  <si>
+    <t>article R 562-11-4 du CE : matérialisation de la bande particulière</t>
+  </si>
+  <si>
+    <t>Symbologie pour les zones proégées également</t>
+  </si>
+  <si>
+    <t>Préciser le caractère synthétique des représentations. Différentes réglementation peuvent s'appliquer dans les zones identifiées dans le principe général d'une même interdiction</t>
+  </si>
+  <si>
+    <t>Pas de nuances supplémentaire au niveau du standard. On précise que la possibilité est laissée à la discretion des DDT.</t>
+  </si>
+  <si>
+    <t>NOK?
+Qu'entendez-vous par zonage d'exception ?
+A priori il s'agit d'identifie les zones où une demande d'exception est faite par rapport à une interdiction…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK sur le principe.
+Ah, il doit s'agir de ce zonage d'exception là !
+A étudier mais il manque vraiment la référence de ce décret (cf. commentaires précédent).
+NB : guide Inondation Cet =&gt; représenté toujours en rouge
+</t>
+  </si>
+  <si>
+    <t>Ces zones d'exception sont une sous partie spécifique  des zones répondant au principe général d'interdiction. (Guide PPRICet (p79) )</t>
+  </si>
+  <si>
+    <t>cf. commentaire #1</t>
+  </si>
+  <si>
+    <t>OK sur le principe ?
+A discuter :
+- faut-il rajouter un alea "multirisque" ou s'agit-il d'avoir une table qui rassemble toutes les zones d'aléa (avec superposition possibles) ?
+=&gt; oui
+- s'agit-il d'une table toutes zones d'aléas naturels (de référence?)
+=&gt; oui
+- le besoin est-il le même pour les aleéas technos (la strucutre peut varie d'une classe / table à l'autre) ? =&gt; oui même principe
+NB : cf. DDT74-6</t>
+  </si>
+  <si>
+    <t>A discuter. Je ne suis pas sur de comprendre si la demande s'applique aux aléas technos ou naturels et ce qui est demandé exactement ?
+Liste pour les avalanches validéée</t>
+  </si>
+  <si>
+    <t>N.A. ?
+Attention aux règles de conversion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK sur le principe.
+Rajouter les tables d'énumération correspondant aux nomenclatures proposées.
+Simplifier les codes : proposition (numérique)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK, sur le principe.
+Peut-on précisier un cas de PPR où nul s'applique et pas très faible ? Ou inversement ?
+</t>
+  </si>
+  <si>
+    <t>N.A.
+Vérifier que le zonage reglementaire lié à l'aléa exceptionnel est bien du domaine reglementaire
+NB : niveau alea optionnel pour les zones d'alea exceptionnel</t>
+  </si>
+  <si>
+    <t>OK, sur le principe
+Par contre, il n'y a pas de procédure PPRT-Multi dans la classification des procédures GASPAR.
+Indiquer, comme pour les PPRL qu'on peut avoir du miultirisques pour les PPRT</t>
+  </si>
+  <si>
+    <t>intégré ?</t>
+  </si>
+  <si>
+    <t>Le guide PPRN fait cette distinction sans doute pour pouvoir faire la distinction au niveau du zonage si besoin…</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2380,18 +2446,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color theme="7" tint="-0.249977111117893"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="5" tint="-0.499984740745262"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2407,7 +2461,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -2450,12 +2504,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2530,12 +2608,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2555,6 +2627,25 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -3359,25 +3450,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939F5930-30D3-43D0-87E8-B00574FE9CE2}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.453125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.1796875" style="3" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="21.81640625" style="3" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="3" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" style="3" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="3" customWidth="1"/>
-    <col min="5" max="5" width="16.1796875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="49.54296875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="47.54296875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="54.81640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="21.453125" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="10.81640625" style="3"/>
+    <col min="5" max="5" width="16.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="49.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="47.5703125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="54.85546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="10.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>349</v>
       </c>
@@ -3403,10 +3494,10 @@
         <v>5</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="73" customHeight="1" x14ac:dyDescent="0.35">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="72.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-1</v>
@@ -3433,10 +3524,10 @@
         <v>351</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-2</v>
@@ -3460,13 +3551,13 @@
         <v>332</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>518</v>
+        <v>508</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-3</v>
@@ -3493,10 +3584,10 @@
         <v>353</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="75.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-4</v>
@@ -3520,13 +3611,13 @@
         <v>305</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>519</v>
+        <v>509</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="89.15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="89.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-5</v>
@@ -3553,10 +3644,10 @@
         <v>350</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/DAPP/BIP-11</v>
@@ -3581,10 +3672,10 @@
         <v>352</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="96" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-6</v>
@@ -3611,10 +3702,10 @@
         <v>358</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="115" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="144" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-7</v>
@@ -3641,10 +3732,10 @@
         <v>354</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-1</v>
@@ -3671,10 +3762,10 @@
         <v>355</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-2</v>
@@ -3701,10 +3792,10 @@
         <v>355</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-8</v>
@@ -3728,13 +3819,13 @@
         <v>315</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>513</v>
+        <v>503</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>cerema-6</v>
@@ -3761,10 +3852,10 @@
         <v>356</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="96" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-9</v>
@@ -3791,10 +3882,10 @@
         <v>357</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="61" customHeight="1" x14ac:dyDescent="0.35">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="60.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-10</v>
@@ -3821,10 +3912,10 @@
         <v>352</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="68.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-3</v>
@@ -3848,13 +3939,13 @@
         <v>288</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>514</v>
+        <v>504</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="77.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="77.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-4</v>
@@ -3881,10 +3972,10 @@
         <v>359</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="111" customHeight="1" x14ac:dyDescent="0.35">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-5</v>
@@ -3908,13 +3999,13 @@
         <v>293</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>515</v>
+        <v>505</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="96" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SDCAP/PONSOH-13</v>
@@ -3938,13 +4029,13 @@
         <v>328</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>531</v>
+        <v>521</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/DAPP/BIP-12</v>
@@ -3969,7 +4060,7 @@
         <v>360</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>528</v>
+        <v>518</v>
       </c>
     </row>
   </sheetData>
@@ -3985,25 +4076,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815F14A-19BC-4DCE-8D31-81F595A4B0E7}">
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView topLeftCell="B141" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G141" sqref="G141"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.54296875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="3.81640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="16" style="3" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="44.1796875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="44.140625" style="3" customWidth="1"/>
     <col min="7" max="7" width="38" style="3" customWidth="1"/>
-    <col min="8" max="8" width="51.81640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="22.26953125" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="10.81640625" style="3"/>
+    <col min="8" max="8" width="51.85546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="10.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>348</v>
       </c>
@@ -4029,10 +4120,10 @@
         <v>5</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-2</v>
@@ -4054,13 +4145,13 @@
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="25" t="s">
-        <v>532</v>
+        <v>522</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-3</v>
@@ -4085,10 +4176,10 @@
         <v>371</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-4</v>
@@ -4113,10 +4204,10 @@
         <v>372</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="65.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-5</v>
@@ -4138,13 +4229,13 @@
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="22" t="s">
-        <v>520</v>
+        <v>510</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="126.5" x14ac:dyDescent="0.35">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="132" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP-0</v>
@@ -4167,10 +4258,10 @@
         <v>373</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-9</v>
@@ -4195,10 +4286,10 @@
         <v>374</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-14</v>
@@ -4223,10 +4314,10 @@
         <v>375</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-15</v>
@@ -4251,10 +4342,10 @@
         <v>376</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDTM11-1</v>
@@ -4263,26 +4354,26 @@
         <v>1</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>558</v>
+        <v>545</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>559</v>
+        <v>546</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="4" t="s">
-        <v>560</v>
+        <v>547</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>561</v>
+        <v>548</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>577</v>
+        <v>564</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-2</v>
@@ -4310,7 +4401,7 @@
       </c>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" spans="1:9" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-3</v>
@@ -4338,7 +4429,7 @@
       </c>
       <c r="I12" s="24"/>
     </row>
-    <row r="13" spans="1:9" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-1</v>
@@ -4365,10 +4456,10 @@
         <v>350</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="66.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-1</v>
@@ -4392,13 +4483,13 @@
         <v>166</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>512</v>
+        <v>502</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="161" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="168" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-2</v>
@@ -4422,13 +4513,13 @@
         <v>254</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>527</v>
+        <v>517</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-3</v>
@@ -4452,13 +4543,13 @@
         <v>62</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>526</v>
+        <v>516</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-1</v>
@@ -4482,13 +4573,13 @@
         <v>117</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>578</v>
+        <v>565</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-4</v>
@@ -4515,10 +4606,10 @@
         <v>380</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-4</v>
@@ -4545,10 +4636,10 @@
         <v>381</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="84.65" customHeight="1" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-5</v>
@@ -4572,13 +4663,13 @@
         <v>255</v>
       </c>
       <c r="H20" s="19" t="s">
-        <v>533</v>
+        <v>523</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="84" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-6</v>
@@ -4602,13 +4693,13 @@
         <v>256</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-2</v>
@@ -4635,10 +4726,10 @@
         <v>382</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-3</v>
@@ -4662,13 +4753,13 @@
         <v>122</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>581</v>
+        <v>567</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-5</v>
@@ -4695,10 +4786,10 @@
         <v>383</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-4</v>
@@ -4725,10 +4816,10 @@
         <v>384</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-5</v>
@@ -4755,10 +4846,10 @@
         <v>383</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="71.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="71.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-7</v>
@@ -4782,13 +4873,13 @@
         <v>72</v>
       </c>
       <c r="H27" s="19" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="I27" s="24" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-6</v>
@@ -4815,10 +4906,10 @@
         <v>352</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="115" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-</v>
@@ -4840,13 +4931,13 @@
         <v>340</v>
       </c>
       <c r="H29" s="19" t="s">
-        <v>539</v>
+        <v>529</v>
       </c>
       <c r="I29" s="24" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-8</v>
@@ -4870,13 +4961,13 @@
         <v>75</v>
       </c>
       <c r="H30" s="19" t="s">
-        <v>540</v>
+        <v>530</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-9</v>
@@ -4903,10 +4994,10 @@
         <v>385</v>
       </c>
       <c r="I31" s="24" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-6</v>
@@ -4933,10 +5024,10 @@
         <v>386</v>
       </c>
       <c r="I32" s="24" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-7</v>
@@ -4963,10 +5054,10 @@
         <v>388</v>
       </c>
       <c r="I33" s="24" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="41.15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-10</v>
@@ -4988,13 +5079,13 @@
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="17" t="s">
-        <v>541</v>
+        <v>531</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-7</v>
@@ -5021,10 +5112,10 @@
         <v>389</v>
       </c>
       <c r="I35" s="23" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="62.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="62.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-11</v>
@@ -5049,40 +5140,40 @@
         <v>387</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" s="34" customFormat="1" ht="81" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="28" t="str">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="32" customFormat="1" ht="84.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="26" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-1</v>
       </c>
-      <c r="B37" s="29">
+      <c r="B37" s="27">
         <v>1</v>
       </c>
-      <c r="C37" s="30" t="s">
+      <c r="C37" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D37" s="31" t="s">
+      <c r="D37" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="E37" s="31" t="s">
+      <c r="E37" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="F37" s="30" t="s">
+      <c r="F37" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="G37" s="30" t="s">
+      <c r="G37" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="H37" s="32" t="s">
-        <v>588</v>
-      </c>
-      <c r="I37" s="33" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="44" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="H37" s="30" t="s">
+        <v>573</v>
+      </c>
+      <c r="I37" s="31" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="44.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-21</v>
@@ -5106,13 +5197,13 @@
         <v>99</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>591</v>
+        <v>575</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.35">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-</v>
@@ -5128,17 +5219,17 @@
         <v>369</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>338</v>
       </c>
       <c r="H39" s="19" t="s">
-        <v>543</v>
+        <v>578</v>
       </c>
       <c r="I39" s="24"/>
     </row>
-    <row r="40" spans="1:9" ht="207" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" ht="228" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-</v>
@@ -5154,17 +5245,19 @@
         <v>369</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>338</v>
       </c>
       <c r="H40" s="19" t="s">
-        <v>390</v>
-      </c>
-      <c r="I40" s="24"/>
-    </row>
-    <row r="41" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+        <v>580</v>
+      </c>
+      <c r="I40" s="24" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-8</v>
@@ -5187,12 +5280,14 @@
       <c r="G41" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="H41" s="19" t="s">
-        <v>590</v>
-      </c>
-      <c r="I41" s="24"/>
-    </row>
-    <row r="42" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+      <c r="H41" s="17" t="s">
+        <v>574</v>
+      </c>
+      <c r="I41" s="24" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-8</v>
@@ -5216,11 +5311,13 @@
         <v>133</v>
       </c>
       <c r="H42" s="19" t="s">
-        <v>589</v>
-      </c>
-      <c r="I42" s="24"/>
-    </row>
-    <row r="43" spans="1:9" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>582</v>
+      </c>
+      <c r="I42" s="24" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="87.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-12</v>
@@ -5241,14 +5338,14 @@
         <v>84</v>
       </c>
       <c r="G43" s="4"/>
-      <c r="H43" s="19" t="s">
-        <v>393</v>
-      </c>
-      <c r="I43" s="23" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+      <c r="H43" s="17" t="s">
+        <v>584</v>
+      </c>
+      <c r="I43" s="24" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-4</v>
@@ -5272,13 +5369,13 @@
         <v>26</v>
       </c>
       <c r="H44" s="13" t="s">
-        <v>394</v>
+        <v>586</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="77.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-2</v>
@@ -5301,14 +5398,14 @@
       <c r="G45" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H45" s="19" t="s">
-        <v>395</v>
+      <c r="H45" s="17" t="s">
+        <v>392</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/BRNT-22</v>
@@ -5329,14 +5426,14 @@
         <v>102</v>
       </c>
       <c r="G46" s="4"/>
-      <c r="H46" s="19" t="s">
-        <v>396</v>
+      <c r="H46" s="17" t="s">
+        <v>393</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-8</v>
@@ -5360,11 +5457,13 @@
         <v>33</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>545</v>
-      </c>
-      <c r="I47" s="24"/>
-    </row>
-    <row r="48" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>588</v>
+      </c>
+      <c r="I47" s="24" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-24</v>
@@ -5388,11 +5487,11 @@
         <v>106</v>
       </c>
       <c r="H48" s="19" t="s">
-        <v>396</v>
-      </c>
-      <c r="I48" s="24"/>
-    </row>
-    <row r="49" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+        <v>393</v>
+      </c>
+      <c r="I48" s="23"/>
+    </row>
+    <row r="49" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-3</v>
@@ -5416,13 +5515,13 @@
         <v>25</v>
       </c>
       <c r="H49" s="17" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="96" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-5</v>
@@ -5445,14 +5544,14 @@
       <c r="G50" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H50" s="26" t="s">
-        <v>546</v>
-      </c>
-      <c r="I50" s="4" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+      <c r="H50" s="17" t="s">
+        <v>534</v>
+      </c>
+      <c r="I50" s="24" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="84" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT07-2</v>
@@ -5476,13 +5575,11 @@
         <v>14</v>
       </c>
       <c r="H51" s="13" t="s">
-        <v>398</v>
-      </c>
-      <c r="I51" s="4" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+        <v>395</v>
+      </c>
+      <c r="I51" s="4"/>
+    </row>
+    <row r="52" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-11</v>
@@ -5510,7 +5607,7 @@
       </c>
       <c r="I52" s="24"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-12</v>
@@ -5538,7 +5635,7 @@
       </c>
       <c r="I53" s="24"/>
     </row>
-    <row r="54" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-13</v>
@@ -5562,13 +5659,13 @@
         <v>145</v>
       </c>
       <c r="H54" s="17" t="s">
-        <v>547</v>
+        <v>535</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-13</v>
@@ -5593,10 +5690,10 @@
         <v>379</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-14</v>
@@ -5618,13 +5715,13 @@
         <v>87</v>
       </c>
       <c r="H56" s="17" t="s">
-        <v>548</v>
+        <v>536</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-15</v>
@@ -5645,14 +5742,14 @@
         <v>89</v>
       </c>
       <c r="G57" s="4"/>
-      <c r="H57" s="13" t="s">
-        <v>401</v>
+      <c r="H57" s="17" t="s">
+        <v>398</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-9</v>
@@ -5679,10 +5776,10 @@
         <v>379</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="184" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="216" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5702,11 +5799,13 @@
       </c>
       <c r="G59" s="4"/>
       <c r="H59" s="19" t="s">
-        <v>399</v>
-      </c>
-      <c r="I59" s="24"/>
-    </row>
-    <row r="60" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+        <v>396</v>
+      </c>
+      <c r="I59" s="24" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-14</v>
@@ -5730,11 +5829,11 @@
         <v>148</v>
       </c>
       <c r="H60" s="19" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="I60" s="24"/>
     </row>
-    <row r="61" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5754,11 +5853,13 @@
       </c>
       <c r="G61" s="4"/>
       <c r="H61" s="19" t="s">
-        <v>404</v>
-      </c>
-      <c r="I61" s="24"/>
-    </row>
-    <row r="62" spans="1:9" ht="230" x14ac:dyDescent="0.35">
+        <v>400</v>
+      </c>
+      <c r="I61" s="24" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="252" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5778,13 +5879,13 @@
       </c>
       <c r="G62" s="4"/>
       <c r="H62" s="13" t="s">
-        <v>402</v>
-      </c>
-      <c r="I62" s="4" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+        <v>399</v>
+      </c>
+      <c r="I62" s="24" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="96" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-15</v>
@@ -5808,11 +5909,13 @@
         <v>151</v>
       </c>
       <c r="H63" s="19" t="s">
-        <v>549</v>
-      </c>
-      <c r="I63" s="24"/>
-    </row>
-    <row r="64" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+        <v>537</v>
+      </c>
+      <c r="I63" s="24" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5832,11 +5935,11 @@
       </c>
       <c r="G64" s="4"/>
       <c r="H64" s="13" t="s">
-        <v>403</v>
+        <v>594</v>
       </c>
       <c r="I64" s="24"/>
     </row>
-    <row r="65" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" ht="84" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-16</v>
@@ -5860,11 +5963,13 @@
         <v>154</v>
       </c>
       <c r="H65" s="19" t="s">
-        <v>550</v>
-      </c>
-      <c r="I65" s="24"/>
-    </row>
-    <row r="66" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+        <v>595</v>
+      </c>
+      <c r="I65" s="24" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT01-3</v>
@@ -5888,13 +5993,13 @@
         <v>50</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDTM 83-1</v>
@@ -5918,13 +6023,13 @@
         <v>53</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>551</v>
+        <v>538</v>
       </c>
       <c r="I67" s="4" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" ht="174" x14ac:dyDescent="0.35">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-10</v>
@@ -5947,12 +6052,12 @@
       <c r="G68" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="H68" s="19" t="s">
-        <v>469</v>
+      <c r="H68" s="17" t="s">
+        <v>465</v>
       </c>
       <c r="I68" s="24"/>
     </row>
-    <row r="69" spans="1:9" ht="88" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" ht="87.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-1</v>
@@ -5975,12 +6080,12 @@
       <c r="G69" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="H69" s="19" t="s">
-        <v>406</v>
+      <c r="H69" s="17" t="s">
+        <v>402</v>
       </c>
       <c r="I69" s="24"/>
     </row>
-    <row r="70" spans="1:9" ht="103" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" ht="102.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-11</v>
@@ -6003,12 +6108,12 @@
       <c r="G70" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="H70" s="19" t="s">
-        <v>470</v>
+      <c r="H70" s="17" t="s">
+        <v>466</v>
       </c>
       <c r="I70" s="24"/>
     </row>
-    <row r="71" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-12</v>
@@ -6031,12 +6136,14 @@
       <c r="G71" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="H71" s="19" t="s">
-        <v>517</v>
-      </c>
-      <c r="I71" s="24"/>
-    </row>
-    <row r="72" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H71" s="17" t="s">
+        <v>507</v>
+      </c>
+      <c r="I71" s="24" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-13</v>
@@ -6060,13 +6167,13 @@
         <v>197</v>
       </c>
       <c r="H72" s="17" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A73" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-14</v>
@@ -6075,28 +6182,28 @@
         <v>14</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="H73" s="19" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A74" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-19</v>
@@ -6105,28 +6212,28 @@
         <v>19</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="H74" s="17" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A75" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-16</v>
@@ -6135,28 +6242,28 @@
         <v>16</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="H75" s="17" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="I75" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-14</v>
@@ -6179,12 +6286,12 @@
       <c r="G76" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="H76" s="19" t="s">
-        <v>474</v>
-      </c>
-      <c r="I76" s="24"/>
-    </row>
-    <row r="77" spans="1:9" ht="126.5" x14ac:dyDescent="0.35">
+      <c r="H76" s="17" t="s">
+        <v>470</v>
+      </c>
+      <c r="I76" s="23"/>
+    </row>
+    <row r="77" spans="1:9" ht="144" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-15</v>
@@ -6207,12 +6314,12 @@
       <c r="G77" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="H77" s="19" t="s">
-        <v>478</v>
+      <c r="H77" s="17" t="s">
+        <v>598</v>
       </c>
       <c r="I77" s="24"/>
     </row>
-    <row r="78" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A78" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDTM11-2</v>
@@ -6221,28 +6328,28 @@
         <v>2</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>558</v>
+        <v>545</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>559</v>
+        <v>546</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>562</v>
+        <v>549</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>563</v>
+        <v>550</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>564</v>
-      </c>
-      <c r="H78" s="19" t="s">
-        <v>568</v>
+        <v>551</v>
+      </c>
+      <c r="H78" s="17" t="s">
+        <v>555</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-16</v>
@@ -6265,12 +6372,12 @@
       <c r="G79" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="H79" s="19" t="s">
-        <v>475</v>
+      <c r="H79" s="17" t="s">
+        <v>599</v>
       </c>
       <c r="I79" s="24"/>
     </row>
-    <row r="80" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A80" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-22</v>
@@ -6279,28 +6386,28 @@
         <v>22</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="H80" s="19" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="27" x14ac:dyDescent="0.25">
       <c r="A81" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-23</v>
@@ -6309,28 +6416,28 @@
         <v>23</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="H81" s="17" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="I81" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A82" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-24</v>
@@ -6339,28 +6446,28 @@
         <v>24</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="H82" s="13" t="s">
-        <v>552</v>
-      </c>
-      <c r="I82" s="4" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" ht="65" customHeight="1" x14ac:dyDescent="0.35">
+        <v>539</v>
+      </c>
+      <c r="I82" s="24" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-17</v>
@@ -6383,12 +6490,12 @@
       <c r="G83" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="H83" s="19" t="s">
-        <v>476</v>
+      <c r="H83" s="17" t="s">
+        <v>471</v>
       </c>
       <c r="I83" s="24"/>
     </row>
-    <row r="84" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-18</v>
@@ -6411,12 +6518,12 @@
       <c r="G84" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="H84" s="19" t="s">
-        <v>477</v>
+      <c r="H84" s="17" t="s">
+        <v>472</v>
       </c>
       <c r="I84" s="24"/>
     </row>
-    <row r="85" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-19</v>
@@ -6440,11 +6547,11 @@
         <v>211</v>
       </c>
       <c r="H85" s="19" t="s">
-        <v>479</v>
+        <v>601</v>
       </c>
       <c r="I85" s="24"/>
     </row>
-    <row r="86" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-20</v>
@@ -6468,13 +6575,13 @@
         <v>213</v>
       </c>
       <c r="H86" s="17" t="s">
-        <v>480</v>
+        <v>473</v>
       </c>
       <c r="I86" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-27</v>
@@ -6483,28 +6590,28 @@
         <v>27</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="F87" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="G87" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="H87" s="19" t="s">
         <v>468</v>
       </c>
-      <c r="G87" s="4" t="s">
-        <v>462</v>
-      </c>
-      <c r="H87" s="19" t="s">
-        <v>472</v>
-      </c>
       <c r="I87" s="4" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-21</v>
@@ -6528,13 +6635,13 @@
         <v>216</v>
       </c>
       <c r="H88" s="19" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" ht="39.65" customHeight="1" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-26</v>
@@ -6543,28 +6650,28 @@
         <v>26</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="G89" s="4" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="H89" s="19" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="I89" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-17</v>
@@ -6591,10 +6698,10 @@
         <v>379</v>
       </c>
       <c r="I90" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-16</v>
@@ -6616,13 +6723,13 @@
         <v>91</v>
       </c>
       <c r="H91" s="17" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
       <c r="I91" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="77.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-17</v>
@@ -6644,13 +6751,13 @@
       </c>
       <c r="G92" s="4"/>
       <c r="H92" s="13" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
       <c r="I92" s="4" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-22</v>
@@ -6673,42 +6780,42 @@
       <c r="G93" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="H93" s="19" t="s">
-        <v>484</v>
+      <c r="H93" s="17" t="s">
+        <v>602</v>
       </c>
       <c r="I93" s="24"/>
     </row>
-    <row r="94" spans="1:9" ht="98" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="4" t="str">
+    <row r="94" spans="1:9" s="39" customFormat="1" ht="98.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="33" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-23</v>
       </c>
-      <c r="B94" s="7">
+      <c r="B94" s="34">
         <v>23</v>
       </c>
-      <c r="C94" s="4" t="s">
+      <c r="C94" s="35" t="s">
         <v>163</v>
       </c>
-      <c r="D94" s="5" t="s">
+      <c r="D94" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="E94" s="5" t="s">
+      <c r="E94" s="36" t="s">
         <v>219</v>
       </c>
-      <c r="F94" s="4" t="s">
+      <c r="F94" s="35" t="s">
         <v>220</v>
       </c>
-      <c r="G94" s="4" t="s">
+      <c r="G94" s="35" t="s">
         <v>278</v>
       </c>
-      <c r="H94" s="13" t="s">
-        <v>485</v>
-      </c>
-      <c r="I94" s="4" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+      <c r="H94" s="37" t="s">
+        <v>477</v>
+      </c>
+      <c r="I94" s="38" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="96.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-24</v>
@@ -6732,13 +6839,13 @@
         <v>279</v>
       </c>
       <c r="H95" s="21" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="I95" s="4" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" ht="113.15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="113.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/PoNSOH-26</v>
@@ -6761,12 +6868,12 @@
       <c r="G96" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="H96" s="27" t="s">
-        <v>516</v>
+      <c r="H96" s="17" t="s">
+        <v>506</v>
       </c>
       <c r="I96" s="24"/>
     </row>
-    <row r="97" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/PoNSOH-27</v>
@@ -6789,12 +6896,12 @@
       <c r="G97" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="H97" s="19" t="s">
-        <v>487</v>
+      <c r="H97" s="17" t="s">
+        <v>479</v>
       </c>
       <c r="I97" s="24"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-18</v>
@@ -6822,7 +6929,7 @@
       </c>
       <c r="I98" s="24"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-19</v>
@@ -6850,7 +6957,7 @@
       </c>
       <c r="I99" s="24"/>
     </row>
-    <row r="100" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-18</v>
@@ -6872,13 +6979,13 @@
       </c>
       <c r="G100" s="4"/>
       <c r="H100" s="19" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="I100" s="4" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A101" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDTM11-3</v>
@@ -6887,24 +6994,24 @@
         <v>3</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>558</v>
+        <v>545</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>559</v>
+        <v>546</v>
       </c>
       <c r="E101" s="5"/>
       <c r="F101" s="4" t="s">
-        <v>565</v>
+        <v>552</v>
       </c>
       <c r="G101" s="4" t="s">
-        <v>566</v>
+        <v>553</v>
       </c>
       <c r="H101" s="19" t="s">
-        <v>567</v>
+        <v>554</v>
       </c>
       <c r="I101" s="24"/>
     </row>
-    <row r="102" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A102" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-15</v>
@@ -6913,28 +7020,28 @@
         <v>15</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D102" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="G102" s="4" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="H102" s="17" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="I102" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-1</v>
@@ -6943,28 +7050,28 @@
         <v>1</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D103" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="F103" s="4" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="G103" s="4" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="H103" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I103" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A104" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-17</v>
@@ -6973,28 +7080,28 @@
         <v>17</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D104" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="F104" s="4" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="G104" s="4" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="H104" s="17" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="I104" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A105" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-20</v>
@@ -7003,28 +7110,28 @@
         <v>20</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D105" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="G105" s="4" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="H105" s="17" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="I105" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" ht="37.5" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" ht="39" x14ac:dyDescent="0.25">
       <c r="A106" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-21</v>
@@ -7033,26 +7140,26 @@
         <v>21</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D106" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="G106" s="4" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="H106" s="19" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="I106" s="24"/>
     </row>
-    <row r="107" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A107" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-18</v>
@@ -7061,28 +7168,28 @@
         <v>18</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D107" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="G107" s="4" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="H107" s="13" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="I107" s="4" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A108" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-25</v>
@@ -7091,28 +7198,28 @@
         <v>25</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D108" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="F108" s="4" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="G108" s="4" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="H108" s="17" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="I108" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A109" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-2</v>
@@ -7121,26 +7228,26 @@
         <v>2</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D109" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E109" s="5" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="F109" s="4" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="G109" s="4" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="H109" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I109" s="24"/>
     </row>
-    <row r="110" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A110" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-3</v>
@@ -7149,26 +7256,26 @@
         <v>3</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D110" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="F110" s="4" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="G110" s="4" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="H110" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I110" s="24"/>
     </row>
-    <row r="111" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A111" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-4</v>
@@ -7177,26 +7284,26 @@
         <v>4</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D111" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E111" s="5" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="F111" s="4" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="G111" s="4" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="H111" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I111" s="24"/>
     </row>
-    <row r="112" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT01-1</v>
@@ -7220,13 +7327,13 @@
         <v>250</v>
       </c>
       <c r="H112" s="6" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="I112" s="4" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A113" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-5</v>
@@ -7235,26 +7342,26 @@
         <v>5</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D113" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="F113" s="4" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="G113" s="4" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="H113" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I113" s="24"/>
     </row>
-    <row r="114" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A114" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-6</v>
@@ -7263,26 +7370,26 @@
         <v>6</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D114" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F114" s="4" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="G114" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="H114" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I114" s="24"/>
     </row>
-    <row r="115" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A115" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-7</v>
@@ -7291,26 +7398,26 @@
         <v>7</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D115" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G115" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="H115" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I115" s="24"/>
     </row>
-    <row r="116" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A116" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-8</v>
@@ -7319,26 +7426,26 @@
         <v>8</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D116" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="F116" s="4" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="G116" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="H116" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I116" s="24"/>
     </row>
-    <row r="117" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A117" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-9</v>
@@ -7347,26 +7454,26 @@
         <v>9</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D117" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="F117" s="4" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G117" s="4" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="H117" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I117" s="24"/>
     </row>
-    <row r="118" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A118" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-10</v>
@@ -7375,26 +7482,26 @@
         <v>10</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D118" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="F118" s="4" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="G118" s="4" t="s">
-        <v>428</v>
-      </c>
-      <c r="H118" s="19" t="s">
-        <v>493</v>
+        <v>424</v>
+      </c>
+      <c r="H118" s="17" t="s">
+        <v>485</v>
       </c>
       <c r="I118" s="24"/>
     </row>
-    <row r="119" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-11</v>
@@ -7403,28 +7510,28 @@
         <v>11</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D119" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E119" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="F119" s="4" t="s">
         <v>425</v>
       </c>
-      <c r="F119" s="4" t="s">
-        <v>429</v>
-      </c>
       <c r="G119" s="4" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="H119" s="13" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="I119" s="4" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A120" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-12</v>
@@ -7433,26 +7540,26 @@
         <v>12</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D120" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E120" s="5" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="F120" s="4" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="G120" s="4" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="H120" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I120" s="24"/>
     </row>
-    <row r="121" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A121" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-13</v>
@@ -7461,26 +7568,26 @@
         <v>13</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D121" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E121" s="5" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="F121" s="4" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="G121" s="4" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="H121" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I121" s="24"/>
     </row>
-    <row r="122" spans="1:9" ht="151.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-6</v>
@@ -7504,11 +7611,11 @@
         <v>29</v>
       </c>
       <c r="H122" s="19" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="I122" s="24"/>
     </row>
-    <row r="123" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT01-2</v>
@@ -7532,11 +7639,11 @@
         <v>252</v>
       </c>
       <c r="H123" s="19" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="I123" s="24"/>
     </row>
-    <row r="124" spans="1:9" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:9" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-23</v>
@@ -7560,11 +7667,11 @@
         <v>104</v>
       </c>
       <c r="H124" s="19" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="I124" s="24"/>
     </row>
-    <row r="125" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:9" ht="96" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-20</v>
@@ -7588,11 +7695,11 @@
         <v>162</v>
       </c>
       <c r="H125" s="19" t="s">
-        <v>498</v>
+        <v>489</v>
       </c>
       <c r="I125" s="24"/>
     </row>
-    <row r="126" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-25</v>
@@ -7616,11 +7723,11 @@
         <v>225</v>
       </c>
       <c r="H126" s="19" t="s">
-        <v>497</v>
+        <v>604</v>
       </c>
       <c r="I126" s="24"/>
     </row>
-    <row r="127" spans="1:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-26</v>
@@ -7644,11 +7751,11 @@
         <v>228</v>
       </c>
       <c r="H127" s="19" t="s">
-        <v>499</v>
+        <v>490</v>
       </c>
       <c r="I127" s="24"/>
     </row>
-    <row r="128" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT07-1</v>
@@ -7672,11 +7779,11 @@
         <v>10</v>
       </c>
       <c r="H128" s="19" t="s">
-        <v>500</v>
+        <v>491</v>
       </c>
       <c r="I128" s="24"/>
     </row>
-    <row r="129" spans="1:9" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-19</v>
@@ -7698,11 +7805,11 @@
       </c>
       <c r="G129" s="4"/>
       <c r="H129" s="19" t="s">
-        <v>501</v>
+        <v>492</v>
       </c>
       <c r="I129" s="24"/>
     </row>
-    <row r="130" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-20</v>
@@ -7724,11 +7831,11 @@
       </c>
       <c r="G130" s="4"/>
       <c r="H130" s="19" t="s">
-        <v>502</v>
+        <v>493</v>
       </c>
       <c r="I130" s="24"/>
     </row>
-    <row r="131" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-9</v>
@@ -7752,13 +7859,13 @@
         <v>136</v>
       </c>
       <c r="H131" s="19" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="I131" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-10</v>
@@ -7782,11 +7889,11 @@
         <v>139</v>
       </c>
       <c r="H132" s="19" t="s">
-        <v>504</v>
+        <v>495</v>
       </c>
       <c r="I132" s="24"/>
     </row>
-    <row r="133" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-27</v>
@@ -7810,11 +7917,13 @@
         <v>231</v>
       </c>
       <c r="H133" s="17" t="s">
-        <v>505</v>
-      </c>
-      <c r="I133" s="4"/>
-    </row>
-    <row r="134" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+        <v>496</v>
+      </c>
+      <c r="I133" s="24" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-28</v>
@@ -7841,10 +7950,10 @@
         <v>352</v>
       </c>
       <c r="I134" s="4" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-29</v>
@@ -7871,10 +7980,10 @@
         <v>352</v>
       </c>
       <c r="I135" s="4" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-10</v>
@@ -7898,13 +8007,13 @@
         <v>37</v>
       </c>
       <c r="H136" s="13" t="s">
-        <v>506</v>
+        <v>497</v>
       </c>
       <c r="I136" s="4" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-11</v>
@@ -7928,13 +8037,13 @@
         <v>39</v>
       </c>
       <c r="H137" s="13" t="s">
-        <v>507</v>
+        <v>606</v>
       </c>
       <c r="I137" s="4" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="138" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-12</v>
@@ -7958,13 +8067,13 @@
         <v>41</v>
       </c>
       <c r="H138" s="19" t="s">
-        <v>508</v>
+        <v>498</v>
       </c>
       <c r="I138" s="4" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9" ht="44.15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-25</v>
@@ -7986,13 +8095,13 @@
       </c>
       <c r="G139" s="4"/>
       <c r="H139" s="13" t="s">
-        <v>509</v>
+        <v>499</v>
       </c>
       <c r="I139" s="4" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="140" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-13</v>
@@ -8016,11 +8125,11 @@
         <v>43</v>
       </c>
       <c r="H140" s="17" t="s">
-        <v>510</v>
+        <v>500</v>
       </c>
       <c r="I140" s="24"/>
     </row>
-    <row r="141" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-7</v>
@@ -8044,10 +8153,10 @@
         <v>31</v>
       </c>
       <c r="H141" s="13" t="s">
-        <v>511</v>
+        <v>501</v>
       </c>
       <c r="I141" s="23" t="s">
-        <v>523</v>
+        <v>513</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Check modifs preceddentes et MaJ XLS en conséquence
</commit_message>
<xml_diff>
--- a/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
+++ b/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Geostandards-Risques\suivi\2024-05_06-Consultation-publique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014CA7B2-0C84-4DEF-8781-23CDA5FFEB0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65989973-F019-48D0-A5E9-ED82031A021E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Synthese Modele Commun" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="603">
   <si>
     <t>Organisme</t>
   </si>
@@ -1244,12 +1244,6 @@
 Mais plutôt dans le standard PPR (cf. remarque précédente)</t>
   </si>
   <si>
-    <t>OK sur le principe
-Mais voir au cas par cas, car dans le modèle commun, certains champs peuvent être spécialisés et implémentées de manière différentes en fonction du type d'aléa. 
-Par exemple : occurrence (classe de probabilité ou période de retour), ou niveau de protection (hauteur dans certains cas, mais pas toujours)
-Cette différenciation est plutôt à envisager dans le profil PPR</t>
-  </si>
-  <si>
     <t>OK sur le principe cf. après</t>
   </si>
   <si>
@@ -1349,14 +1343,6 @@
   <si>
     <t>OK sur le principe
 La formulation "Produire les données métiers des études préalables" ne me semble pas correcte (l'établissement du zonage réglementaire est-il dans la phase d'étude préalable ?)</t>
-  </si>
-  <si>
-    <t>OK sur le principe.
-Peut-être peut-on tout simplement enlever le niveau d'aléa exceptionnel et le caractériser par une période de retour exceptionnellement rare ? (cf. discussion de la dernière plénière)</t>
-  </si>
-  <si>
-    <t>Est-ce une demande de séparer les deux types de bandes particulières ?
-En l'état les deux types de bandes sont couvertes par un seul et même type de suralea : "bande particulière". Il n'y a pas de distinction.</t>
   </si>
   <si>
     <t>OK, formulation à reprendre</t>
@@ -1875,11 +1861,6 @@
 </t>
   </si>
   <si>
-    <t>OK sur le principe.
-La codification proposées se voulait hiérarchique.
-Solution à trouver pour garder cette hiérarchie en simplifiant</t>
-  </si>
-  <si>
     <t>Cf. commentaire précédent</t>
   </si>
   <si>
@@ -1997,22 +1978,9 @@
 + tables d'énumérations (PPR) + modèle UML + gabarits</t>
   </si>
   <si>
-    <t xml:space="preserve">OK, à corriger.
-Cela remet-il en cause la typologie des ouvrages de protection (barrage et digues) ? =&gt; cf. commentaires PPR
-Une référence à la documentation de SIOUH II serait la bienvenue aussi
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Non, à moins qu'il n'y ait une volonté de les transformer en PPR (cf. Sweet pepper)?
 NB : certains champs obligatoires non renseignés dans PSS
 </t>
-  </si>
-  <si>
-    <t>A vérifier
-NB : il existe :
-- des PPRN sur Saint-Martin (risque cyclonique et multirsiques)
-- un PPRT sur la Guadeloupe (Baie Mahault)
-Rien sur Saint-Barthélémy, mais il me semble que le code de l'environnement peut aussi s'appliquer à Saint-Barthélémy, non ?</t>
   </si>
   <si>
     <t>OK sur le principe, à modifier
@@ -2135,18 +2103,6 @@
     <t>cf. commentaires PPR (intégré)</t>
   </si>
   <si>
-    <t>Vérifier si possibilité de restreindre les valeurs de certains champs au niveau de modèle commun.
-NB : occurrence = péridoe de retour pour l'aléa naturel
-- Accepté =&gt; à intégrer
-(type: integer)
-- Préciser que 0 équivaut à une valeur nulle</t>
-  </si>
-  <si>
-    <t>Cf. Typologie des ouvrages de protection à modifier. Proposition BRIL (+BRNT)
-Maintenir le terme scénario
-Pas d'accès à SIOUH2 (trouver descriptif)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ne rendre obligatoire que les thématiques Procédures, Périmètres et Zonage Réglementaire?
 Aléa non obligatoire (au niveau diffusion)
 </t>
@@ -2172,10 +2128,6 @@
 (NB : à vérifier si des éléments du standard sont impactés par cette nouvelle référence) ? =&gt; pad d'impact</t>
   </si>
   <si>
-    <t>intégré (pour la première partie)
-=&gt; Supprimer Saint-Barthélémy (Code de l'environnement ne s'applqiue pas)</t>
-  </si>
-  <si>
     <t>OK 
 Rajouter le GPU au sens de L152-7</t>
   </si>
@@ -2184,13 +2136,6 @@
   </si>
   <si>
     <t>Mentionner la possibilité de cartographier les PHEC mais sonas les définir + que ça (réf. https://www.reperesdecrues.developpement-durable.gouv.fr/  )</t>
-  </si>
-  <si>
-    <t>remplacer niveau alea par occurrence</t>
-  </si>
-  <si>
-    <t>intégré (deux types de bandes particulières)
-Rajouter la possibilité d'avoir  un type de bande pour les deux</t>
   </si>
   <si>
     <t>changer en zones + mentionner la référence aux espaces du guide PPRN;2016</t>
@@ -2233,9 +2178,6 @@
     <t xml:space="preserve">A discuter avec le GT et les demandeurs
 Utilisation de "Autre" mais Libellé différent à proposer (non couvert par la classification proposée des niveaux d'aléas, à utiliser de manière exceptionnelle).
 </t>
-  </si>
-  <si>
-    <t>Suppression de l'enumération et du champs effet.</t>
   </si>
   <si>
     <t xml:space="preserve">OK sur le principe,
@@ -2347,6 +2289,51 @@
   </si>
   <si>
     <t>Le guide PPRN fait cette distinction sans doute pour pouvoir faire la distinction au niveau du zonage si besoin…</t>
+  </si>
+  <si>
+    <t>OK, à corriger.
+Cela remet-il en cause la typologie des ouvrages de protection (barrage et digues) ? =&gt; cf. commentaires PPR
+Une référence à la documentation de SIOUH II serait la bienvenue aussi
+Cf. Typologie des ouvrages de protection à modifier. Proposition BRIL (+BRNT)
+Maintenir le terme scénario Pas d'accès à SIOUH2</t>
+  </si>
+  <si>
+    <t>Traité en partie
+NB : roleProtection dans PPR ou modèle commun ?</t>
+  </si>
+  <si>
+    <t>OK sur le principe
+Mais voir au cas par cas, car dans le modèle commun, certains champs peuvent être spécialisés et implémentées de manière différentes en fonction du type d'aléa. 
+Par exemple : occurrence (classe de probabilité ou période de retour), ou niveau de protection (hauteur dans certains cas, mais pas toujours)
+Cette différenciation est plutôt à envisager dans le profil PPR
+=&gt; Vérifier si possibilité de restreindre les valeurs de certains champs au niveau de modèle commun.
+NB : occurrence = péridoe de retour pour l'aléa naturel
+- Accepté (type: integer). Préciser que 0 équivaut à une valeur nulle</t>
+  </si>
+  <si>
+    <t>intégré (dans proifil PPR)</t>
+  </si>
+  <si>
+    <t>OK sur le principe.
+Peut-être peut-on tout simplement enlever le niveau d'aléa exceptionnel et le caractériser par une période de retour exceptionnellement rare ? (cf. discussion de la dernière plénière)
+=&gt; remplacer niveau alea par occurrence</t>
+  </si>
+  <si>
+    <t>Est-ce une demande de séparer les deux types de bandes particulières ?
+En l'état les deux types de bandes sont couvertes par un seul et même type de suralea : "bande particulière". Il n'y a pas de distinction.
+Faire la distinction des deux types de bandes particulières et garder la possibilité d'avoir  un type de bande pour les deux</t>
+  </si>
+  <si>
+    <t>NB : il existe :
+- des PPRN sur Saint-Martin (risque cyclonique et multirsiques)
+- un PPRT sur la Guadeloupe (Baie Mahault)
+Rien sur Saint-Barthélémy, mais il me semble que le code de l'environnement peut aussi s'appliquer à Saint-Barthélémy, non ?
+Confirmation que le code de l'environnement ne s'applique pas à Saint Barthélémy (un code particulier s'y applique)</t>
+  </si>
+  <si>
+    <t>OK sur le principe.
+La codification proposée se voulait hiérarchique.
+Solution à trouver pour garder cette hiérarchie en simplifiant</t>
   </si>
 </sst>
 </file>
@@ -3450,25 +3437,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939F5930-30D3-43D0-87E8-B00574FE9CE2}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="3" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" style="3" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" style="3" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="21.81640625" style="3" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="3" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="49.5703125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="47.5703125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="54.85546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="10.85546875" style="3"/>
+    <col min="5" max="5" width="16.1796875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="49.54296875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="47.54296875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="54.81640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="21.453125" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="10.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>349</v>
       </c>
@@ -3494,10 +3481,10 @@
         <v>5</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="72.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="73" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-1</v>
@@ -3524,10 +3511,10 @@
         <v>351</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="108" x14ac:dyDescent="0.25">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-2</v>
@@ -3551,13 +3538,13 @@
         <v>332</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="108" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-3</v>
@@ -3584,10 +3571,10 @@
         <v>353</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="75.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-4</v>
@@ -3611,13 +3598,13 @@
         <v>305</v>
       </c>
       <c r="H5" s="13" t="s">
+        <v>505</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>509</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="89.1" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" ht="89.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-5</v>
@@ -3644,10 +3631,10 @@
         <v>350</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/DAPP/BIP-11</v>
@@ -3672,10 +3659,10 @@
         <v>352</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="96" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-6</v>
@@ -3699,13 +3686,13 @@
         <v>334</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="144" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="126.5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-7</v>
@@ -3729,13 +3716,13 @@
         <v>335</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>354</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>597</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-1</v>
@@ -3759,13 +3746,13 @@
         <v>283</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-2</v>
@@ -3789,13 +3776,13 @@
         <v>285</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="108" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-8</v>
@@ -3819,13 +3806,13 @@
         <v>315</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>cerema-6</v>
@@ -3849,13 +3836,13 @@
         <v>297</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="96" x14ac:dyDescent="0.25">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-9</v>
@@ -3879,13 +3866,13 @@
         <v>336</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="60.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="61" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-10</v>
@@ -3912,10 +3899,10 @@
         <v>352</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="68.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-3</v>
@@ -3939,13 +3926,13 @@
         <v>288</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="77.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="77.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-4</v>
@@ -3969,13 +3956,13 @@
         <v>291</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="111" customHeight="1" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="111" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-5</v>
@@ -3999,13 +3986,13 @@
         <v>293</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="96" x14ac:dyDescent="0.25">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SDCAP/PONSOH-13</v>
@@ -4029,13 +4016,13 @@
         <v>328</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>521</v>
+        <v>595</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/DAPP/BIP-12</v>
@@ -4057,10 +4044,10 @@
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="17" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
     </row>
   </sheetData>
@@ -4076,25 +4063,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815F14A-19BC-4DCE-8D31-81F595A4B0E7}">
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView topLeftCell="B141" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G141" sqref="G141"/>
+    <sheetView tabSelected="1" topLeftCell="B131" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I142" sqref="I142"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="3.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="3.81640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="3" customWidth="1"/>
     <col min="4" max="4" width="16" style="3" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="44.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="44.1796875" style="3" customWidth="1"/>
     <col min="7" max="7" width="38" style="3" customWidth="1"/>
-    <col min="8" max="8" width="51.85546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="10.85546875" style="3"/>
+    <col min="8" max="8" width="51.81640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="22.26953125" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="10.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>348</v>
       </c>
@@ -4120,10 +4107,10 @@
         <v>5</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-2</v>
@@ -4145,13 +4132,13 @@
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="25" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-3</v>
@@ -4173,13 +4160,13 @@
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="22" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-4</v>
@@ -4201,13 +4188,13 @@
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="22" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="65.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-5</v>
@@ -4229,13 +4216,13 @@
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="22" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="132" x14ac:dyDescent="0.25">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="126.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP-0</v>
@@ -4255,13 +4242,13 @@
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="17" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-9</v>
@@ -4283,13 +4270,13 @@
         <v>35</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-14</v>
@@ -4311,13 +4298,13 @@
         <v>45</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-15</v>
@@ -4339,13 +4326,13 @@
         <v>47</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDTM11-1</v>
@@ -4354,26 +4341,26 @@
         <v>1</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="4" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>564</v>
+        <v>556</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-2</v>
@@ -4397,11 +4384,11 @@
         <v>263</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" spans="1:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-3</v>
@@ -4425,11 +4412,11 @@
         <v>172</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I12" s="24"/>
     </row>
-    <row r="13" spans="1:9" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-1</v>
@@ -4456,10 +4443,10 @@
         <v>350</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="66.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-1</v>
@@ -4483,13 +4470,13 @@
         <v>166</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="168" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="161" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-2</v>
@@ -4513,13 +4500,13 @@
         <v>254</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-3</v>
@@ -4543,13 +4530,13 @@
         <v>62</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-1</v>
@@ -4573,13 +4560,13 @@
         <v>117</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>565</v>
+        <v>557</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-4</v>
@@ -4603,13 +4590,13 @@
         <v>65</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-4</v>
@@ -4633,13 +4620,13 @@
         <v>175</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="84.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-5</v>
@@ -4663,13 +4650,13 @@
         <v>255</v>
       </c>
       <c r="H20" s="19" t="s">
-        <v>523</v>
-      </c>
-      <c r="I20" s="24" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="84" x14ac:dyDescent="0.25">
+        <v>601</v>
+      </c>
+      <c r="I20" s="23" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-6</v>
@@ -4693,13 +4680,13 @@
         <v>256</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-2</v>
@@ -4723,13 +4710,13 @@
         <v>120</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-3</v>
@@ -4753,13 +4740,13 @@
         <v>122</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>567</v>
+        <v>558</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-5</v>
@@ -4783,13 +4770,13 @@
         <v>178</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-4</v>
@@ -4813,13 +4800,13 @@
         <v>260</v>
       </c>
       <c r="H25" s="19" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-5</v>
@@ -4843,13 +4830,13 @@
         <v>125</v>
       </c>
       <c r="H26" s="17" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="71.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="71.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-7</v>
@@ -4873,13 +4860,13 @@
         <v>72</v>
       </c>
       <c r="H27" s="19" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="I27" s="24" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-6</v>
@@ -4906,10 +4893,10 @@
         <v>352</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="115" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-</v>
@@ -4922,7 +4909,7 @@
         <v>16</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>339</v>
@@ -4931,13 +4918,13 @@
         <v>340</v>
       </c>
       <c r="H29" s="19" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="I29" s="24" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-8</v>
@@ -4961,13 +4948,13 @@
         <v>75</v>
       </c>
       <c r="H30" s="19" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-9</v>
@@ -4991,13 +4978,13 @@
         <v>78</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>385</v>
-      </c>
-      <c r="I31" s="24" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+        <v>599</v>
+      </c>
+      <c r="I31" s="23" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-6</v>
@@ -5021,13 +5008,13 @@
         <v>128</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>386</v>
-      </c>
-      <c r="I32" s="24" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="108" x14ac:dyDescent="0.25">
+        <v>600</v>
+      </c>
+      <c r="I32" s="23" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-7</v>
@@ -5051,13 +5038,13 @@
         <v>130</v>
       </c>
       <c r="H33" s="17" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="I33" s="24" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="41.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-10</v>
@@ -5079,13 +5066,13 @@
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="17" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-7</v>
@@ -5109,13 +5096,13 @@
         <v>184</v>
       </c>
       <c r="H35" s="19" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="I35" s="23" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="62.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="62.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-11</v>
@@ -5137,13 +5124,13 @@
         <v>82</v>
       </c>
       <c r="H36" s="17" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" s="32" customFormat="1" ht="84.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="32" customFormat="1" ht="81" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="26" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-1</v>
@@ -5167,13 +5154,13 @@
         <v>19</v>
       </c>
       <c r="H37" s="30" t="s">
-        <v>573</v>
+        <v>562</v>
       </c>
       <c r="I37" s="31" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="44.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="44.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-21</v>
@@ -5197,13 +5184,13 @@
         <v>99</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>575</v>
+        <v>564</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-</v>
@@ -5216,20 +5203,20 @@
         <v>16</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>338</v>
       </c>
       <c r="H39" s="19" t="s">
-        <v>578</v>
+        <v>567</v>
       </c>
       <c r="I39" s="24"/>
     </row>
-    <row r="40" spans="1:9" ht="228" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="207" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-</v>
@@ -5242,22 +5229,22 @@
         <v>16</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>338</v>
       </c>
       <c r="H40" s="19" t="s">
-        <v>580</v>
+        <v>569</v>
       </c>
       <c r="I40" s="24" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="108" x14ac:dyDescent="0.25">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-8</v>
@@ -5281,13 +5268,13 @@
         <v>267</v>
       </c>
       <c r="H41" s="17" t="s">
-        <v>574</v>
-      </c>
-      <c r="I41" s="24" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>563</v>
+      </c>
+      <c r="I41" s="23" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-8</v>
@@ -5311,13 +5298,13 @@
         <v>133</v>
       </c>
       <c r="H42" s="19" t="s">
-        <v>582</v>
+        <v>570</v>
       </c>
       <c r="I42" s="24" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="87.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="88" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-12</v>
@@ -5339,13 +5326,13 @@
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="17" t="s">
-        <v>584</v>
+        <v>572</v>
       </c>
       <c r="I43" s="24" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="108" x14ac:dyDescent="0.25">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-4</v>
@@ -5369,13 +5356,13 @@
         <v>26</v>
       </c>
       <c r="H44" s="13" t="s">
-        <v>586</v>
+        <v>574</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="77.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-2</v>
@@ -5399,13 +5386,13 @@
         <v>22</v>
       </c>
       <c r="H45" s="17" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/BRNT-22</v>
@@ -5427,13 +5414,13 @@
       </c>
       <c r="G46" s="4"/>
       <c r="H46" s="17" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-8</v>
@@ -5448,7 +5435,7 @@
         <v>16</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>32</v>
@@ -5457,13 +5444,13 @@
         <v>33</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
       <c r="I47" s="24" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-24</v>
@@ -5478,7 +5465,7 @@
         <v>16</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F48" s="4" t="s">
         <v>105</v>
@@ -5487,11 +5474,11 @@
         <v>106</v>
       </c>
       <c r="H48" s="19" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="I48" s="23"/>
     </row>
-    <row r="49" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-3</v>
@@ -5515,13 +5502,13 @@
         <v>25</v>
       </c>
       <c r="H49" s="17" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="96" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-5</v>
@@ -5545,13 +5532,13 @@
         <v>28</v>
       </c>
       <c r="H50" s="17" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="I50" s="24" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="84" x14ac:dyDescent="0.25">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT07-2</v>
@@ -5575,11 +5562,11 @@
         <v>14</v>
       </c>
       <c r="H51" s="13" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="I51" s="4"/>
     </row>
-    <row r="52" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-11</v>
@@ -5603,11 +5590,11 @@
         <v>142</v>
       </c>
       <c r="H52" s="17" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I52" s="24"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-12</v>
@@ -5631,11 +5618,11 @@
         <v>143</v>
       </c>
       <c r="H53" s="17" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I53" s="24"/>
     </row>
-    <row r="54" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-13</v>
@@ -5659,13 +5646,13 @@
         <v>145</v>
       </c>
       <c r="H54" s="17" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-13</v>
@@ -5687,13 +5674,13 @@
         <v>86</v>
       </c>
       <c r="H55" s="17" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-14</v>
@@ -5715,13 +5702,13 @@
         <v>87</v>
       </c>
       <c r="H56" s="17" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-15</v>
@@ -5743,13 +5730,13 @@
       </c>
       <c r="G57" s="4"/>
       <c r="H57" s="17" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-9</v>
@@ -5773,13 +5760,13 @@
         <v>187</v>
       </c>
       <c r="H58" s="17" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="216" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="184" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5799,13 +5786,13 @@
       </c>
       <c r="G59" s="4"/>
       <c r="H59" s="19" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="I59" s="24" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-14</v>
@@ -5829,11 +5816,11 @@
         <v>148</v>
       </c>
       <c r="H60" s="19" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="I60" s="24"/>
     </row>
-    <row r="61" spans="1:9" ht="108" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5853,13 +5840,13 @@
       </c>
       <c r="G61" s="4"/>
       <c r="H61" s="19" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="I61" s="24" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" ht="252" x14ac:dyDescent="0.25">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="230" x14ac:dyDescent="0.35">
       <c r="A62" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5879,13 +5866,13 @@
       </c>
       <c r="G62" s="4"/>
       <c r="H62" s="13" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="I62" s="24" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" ht="96" x14ac:dyDescent="0.25">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-15</v>
@@ -5909,13 +5896,13 @@
         <v>151</v>
       </c>
       <c r="H63" s="19" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="I63" s="24" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A64" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5935,11 +5922,11 @@
       </c>
       <c r="G64" s="4"/>
       <c r="H64" s="13" t="s">
-        <v>594</v>
+        <v>582</v>
       </c>
       <c r="I64" s="24"/>
     </row>
-    <row r="65" spans="1:9" ht="84" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-16</v>
@@ -5963,13 +5950,13 @@
         <v>154</v>
       </c>
       <c r="H65" s="19" t="s">
-        <v>595</v>
+        <v>583</v>
       </c>
       <c r="I65" s="24" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT01-3</v>
@@ -5984,7 +5971,7 @@
         <v>11</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F66" s="4" t="s">
         <v>49</v>
@@ -5993,13 +5980,13 @@
         <v>50</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDTM 83-1</v>
@@ -6014,7 +6001,7 @@
         <v>7</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F67" s="4" t="s">
         <v>52</v>
@@ -6023,13 +6010,13 @@
         <v>53</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="I67" s="4" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="174" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-10</v>
@@ -6053,11 +6040,11 @@
         <v>270</v>
       </c>
       <c r="H68" s="17" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="I68" s="24"/>
     </row>
-    <row r="69" spans="1:9" ht="87.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="88" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-1</v>
@@ -6081,11 +6068,11 @@
         <v>241</v>
       </c>
       <c r="H69" s="17" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="I69" s="24"/>
     </row>
-    <row r="70" spans="1:9" ht="102.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="103" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-11</v>
@@ -6109,11 +6096,11 @@
         <v>271</v>
       </c>
       <c r="H70" s="17" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="I70" s="24"/>
     </row>
-    <row r="71" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
       <c r="A71" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-12</v>
@@ -6137,13 +6124,13 @@
         <v>272</v>
       </c>
       <c r="H71" s="17" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="I71" s="24" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-13</v>
@@ -6167,13 +6154,13 @@
         <v>197</v>
       </c>
       <c r="H72" s="17" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A73" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-14</v>
@@ -6182,28 +6169,28 @@
         <v>14</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="H73" s="19" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-19</v>
@@ -6212,28 +6199,28 @@
         <v>19</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="H74" s="17" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-16</v>
@@ -6242,28 +6229,28 @@
         <v>16</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="H75" s="17" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="I75" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-14</v>
@@ -6287,11 +6274,11 @@
         <v>273</v>
       </c>
       <c r="H76" s="17" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="I76" s="23"/>
     </row>
-    <row r="77" spans="1:9" ht="144" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="126.5" x14ac:dyDescent="0.35">
       <c r="A77" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-15</v>
@@ -6315,11 +6302,11 @@
         <v>275</v>
       </c>
       <c r="H77" s="17" t="s">
-        <v>598</v>
+        <v>586</v>
       </c>
       <c r="I77" s="24"/>
     </row>
-    <row r="78" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A78" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDTM11-2</v>
@@ -6328,28 +6315,28 @@
         <v>2</v>
       </c>
       <c r="C78" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>540</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>543</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="G78" s="4" t="s">
         <v>545</v>
       </c>
-      <c r="D78" s="5" t="s">
-        <v>546</v>
-      </c>
-      <c r="E78" s="5" t="s">
+      <c r="H78" s="17" t="s">
         <v>549</v>
       </c>
-      <c r="F78" s="4" t="s">
-        <v>550</v>
-      </c>
-      <c r="G78" s="4" t="s">
-        <v>551</v>
-      </c>
-      <c r="H78" s="17" t="s">
-        <v>555</v>
-      </c>
       <c r="I78" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A79" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-16</v>
@@ -6373,11 +6360,11 @@
         <v>203</v>
       </c>
       <c r="H79" s="17" t="s">
-        <v>599</v>
+        <v>587</v>
       </c>
       <c r="I79" s="24"/>
     </row>
-    <row r="80" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A80" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-22</v>
@@ -6386,28 +6373,28 @@
         <v>22</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="H80" s="19" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="26" x14ac:dyDescent="0.35">
       <c r="A81" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-23</v>
@@ -6416,28 +6403,28 @@
         <v>23</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="H81" s="17" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="I81" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A82" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-24</v>
@@ -6446,28 +6433,28 @@
         <v>24</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="H82" s="13" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="I82" s="24" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="65.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-17</v>
@@ -6491,11 +6478,11 @@
         <v>206</v>
       </c>
       <c r="H83" s="17" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="I83" s="24"/>
     </row>
-    <row r="84" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A84" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-18</v>
@@ -6519,11 +6506,11 @@
         <v>209</v>
       </c>
       <c r="H84" s="17" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="I84" s="24"/>
     </row>
-    <row r="85" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A85" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-19</v>
@@ -6547,11 +6534,11 @@
         <v>211</v>
       </c>
       <c r="H85" s="19" t="s">
-        <v>601</v>
+        <v>589</v>
       </c>
       <c r="I85" s="24"/>
     </row>
-    <row r="86" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-20</v>
@@ -6575,13 +6562,13 @@
         <v>213</v>
       </c>
       <c r="H86" s="17" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="I86" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-27</v>
@@ -6590,28 +6577,28 @@
         <v>27</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="G87" s="4" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="H87" s="19" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A88" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-21</v>
@@ -6635,13 +6622,13 @@
         <v>216</v>
       </c>
       <c r="H88" s="19" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="39.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-26</v>
@@ -6650,28 +6637,28 @@
         <v>26</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="G89" s="4" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="H89" s="19" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="I89" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-17</v>
@@ -6695,13 +6682,13 @@
         <v>157</v>
       </c>
       <c r="H90" s="17" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I90" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A91" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-16</v>
@@ -6723,13 +6710,13 @@
         <v>91</v>
       </c>
       <c r="H91" s="17" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="I91" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" ht="77.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-17</v>
@@ -6751,13 +6738,13 @@
       </c>
       <c r="G92" s="4"/>
       <c r="H92" s="13" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="I92" s="4" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A93" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-22</v>
@@ -6781,11 +6768,11 @@
         <v>218</v>
       </c>
       <c r="H93" s="17" t="s">
-        <v>602</v>
+        <v>590</v>
       </c>
       <c r="I93" s="24"/>
     </row>
-    <row r="94" spans="1:9" s="39" customFormat="1" ht="98.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" s="39" customFormat="1" ht="98.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A94" s="33" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-23</v>
@@ -6809,13 +6796,13 @@
         <v>278</v>
       </c>
       <c r="H94" s="37" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="I94" s="38" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" ht="96.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="81" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A95" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-24</v>
@@ -6839,13 +6826,13 @@
         <v>279</v>
       </c>
       <c r="H95" s="21" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="I95" s="4" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" ht="113.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="113.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/PoNSOH-26</v>
@@ -6869,11 +6856,13 @@
         <v>259</v>
       </c>
       <c r="H96" s="17" t="s">
-        <v>506</v>
-      </c>
-      <c r="I96" s="24"/>
-    </row>
-    <row r="97" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+      <c r="I96" s="23" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/PoNSOH-27</v>
@@ -6897,11 +6886,11 @@
         <v>113</v>
       </c>
       <c r="H97" s="17" t="s">
-        <v>479</v>
-      </c>
-      <c r="I97" s="24"/>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+        <v>476</v>
+      </c>
+      <c r="I97" s="23"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-18</v>
@@ -6929,7 +6918,7 @@
       </c>
       <c r="I98" s="24"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-19</v>
@@ -6957,7 +6946,7 @@
       </c>
       <c r="I99" s="24"/>
     </row>
-    <row r="100" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-18</v>
@@ -6979,13 +6968,13 @@
       </c>
       <c r="G100" s="4"/>
       <c r="H100" s="19" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="I100" s="4" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A101" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDTM11-3</v>
@@ -6994,24 +6983,24 @@
         <v>3</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="E101" s="5"/>
       <c r="F101" s="4" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
       <c r="G101" s="4" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
       <c r="H101" s="19" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="I101" s="24"/>
     </row>
-    <row r="102" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A102" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-15</v>
@@ -7020,28 +7009,28 @@
         <v>15</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D102" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="F102" s="4" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="G102" s="4" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="H102" s="17" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="I102" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-1</v>
@@ -7050,28 +7039,28 @@
         <v>1</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D103" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="F103" s="4" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="G103" s="4" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="H103" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I103" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A104" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-17</v>
@@ -7080,28 +7069,28 @@
         <v>17</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D104" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="F104" s="4" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="G104" s="4" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="H104" s="17" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="I104" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A105" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-20</v>
@@ -7110,28 +7099,28 @@
         <v>20</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D105" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="F105" s="4" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="G105" s="4" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="H105" s="17" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="I105" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" ht="39" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A106" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-21</v>
@@ -7140,26 +7129,26 @@
         <v>21</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D106" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="G106" s="4" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="H106" s="19" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="I106" s="24"/>
     </row>
-    <row r="107" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A107" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-18</v>
@@ -7168,28 +7157,28 @@
         <v>18</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D107" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="G107" s="4" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H107" s="13" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="I107" s="4" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A108" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-25</v>
@@ -7198,28 +7187,28 @@
         <v>25</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D108" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="F108" s="4" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="G108" s="4" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="H108" s="17" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="I108" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A109" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-2</v>
@@ -7228,26 +7217,26 @@
         <v>2</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D109" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E109" s="5" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="F109" s="4" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="G109" s="4" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="H109" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I109" s="24"/>
     </row>
-    <row r="110" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A110" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-3</v>
@@ -7256,26 +7245,26 @@
         <v>3</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D110" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="F110" s="4" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="G110" s="4" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="H110" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I110" s="24"/>
     </row>
-    <row r="111" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A111" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-4</v>
@@ -7284,26 +7273,26 @@
         <v>4</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D111" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E111" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="F111" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="G111" s="4" t="s">
         <v>410</v>
-      </c>
-      <c r="F111" s="4" t="s">
-        <v>411</v>
-      </c>
-      <c r="G111" s="4" t="s">
-        <v>413</v>
       </c>
       <c r="H111" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I111" s="24"/>
     </row>
-    <row r="112" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A112" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT01-1</v>
@@ -7318,7 +7307,7 @@
         <v>23</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F112" s="6" t="s">
         <v>249</v>
@@ -7327,13 +7316,13 @@
         <v>250</v>
       </c>
       <c r="H112" s="6" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="I112" s="4" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A113" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-5</v>
@@ -7342,26 +7331,26 @@
         <v>5</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D113" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="F113" s="4" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="G113" s="4" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="H113" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I113" s="24"/>
     </row>
-    <row r="114" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A114" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-6</v>
@@ -7370,26 +7359,26 @@
         <v>6</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D114" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="F114" s="4" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="G114" s="4" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="H114" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I114" s="24"/>
     </row>
-    <row r="115" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A115" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-7</v>
@@ -7398,26 +7387,26 @@
         <v>7</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D115" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E115" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="F115" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="F115" s="4" t="s">
-        <v>420</v>
-      </c>
       <c r="G115" s="4" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="H115" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I115" s="24"/>
     </row>
-    <row r="116" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A116" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-8</v>
@@ -7426,26 +7415,26 @@
         <v>8</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D116" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="F116" s="4" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="G116" s="4" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="H116" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I116" s="24"/>
     </row>
-    <row r="117" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A117" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-9</v>
@@ -7454,26 +7443,26 @@
         <v>9</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D117" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="F117" s="4" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="G117" s="4" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="H117" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I117" s="24"/>
     </row>
-    <row r="118" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A118" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-10</v>
@@ -7482,26 +7471,26 @@
         <v>10</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D118" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E118" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="F118" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="G118" s="4" t="s">
         <v>421</v>
       </c>
-      <c r="F118" s="4" t="s">
-        <v>423</v>
-      </c>
-      <c r="G118" s="4" t="s">
-        <v>424</v>
-      </c>
       <c r="H118" s="17" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="I118" s="24"/>
     </row>
-    <row r="119" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-11</v>
@@ -7510,28 +7499,28 @@
         <v>11</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D119" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E119" s="5" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="F119" s="4" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="G119" s="4" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H119" s="13" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="I119" s="4" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-12</v>
@@ -7540,26 +7529,26 @@
         <v>12</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D120" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E120" s="5" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="F120" s="4" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="G120" s="4" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="H120" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I120" s="24"/>
     </row>
-    <row r="121" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A121" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-13</v>
@@ -7568,26 +7557,26 @@
         <v>13</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D121" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E121" s="5" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="F121" s="4" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="G121" s="4" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="H121" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I121" s="24"/>
     </row>
-    <row r="122" spans="1:9" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" ht="151.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-6</v>
@@ -7602,7 +7591,7 @@
         <v>247</v>
       </c>
       <c r="E122" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F122" s="4" t="s">
         <v>248</v>
@@ -7611,11 +7600,11 @@
         <v>29</v>
       </c>
       <c r="H122" s="19" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="I122" s="24"/>
     </row>
-    <row r="123" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A123" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT01-2</v>
@@ -7630,7 +7619,7 @@
         <v>11</v>
       </c>
       <c r="E123" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F123" s="4" t="s">
         <v>251</v>
@@ -7639,11 +7628,11 @@
         <v>252</v>
       </c>
       <c r="H123" s="19" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="I123" s="24"/>
     </row>
-    <row r="124" spans="1:9" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-23</v>
@@ -7658,7 +7647,7 @@
         <v>16</v>
       </c>
       <c r="E124" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F124" s="4" t="s">
         <v>103</v>
@@ -7667,11 +7656,11 @@
         <v>104</v>
       </c>
       <c r="H124" s="19" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="I124" s="24"/>
     </row>
-    <row r="125" spans="1:9" ht="96" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A125" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-20</v>
@@ -7695,11 +7684,11 @@
         <v>162</v>
       </c>
       <c r="H125" s="19" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="I125" s="24"/>
     </row>
-    <row r="126" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A126" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-25</v>
@@ -7723,11 +7712,11 @@
         <v>225</v>
       </c>
       <c r="H126" s="19" t="s">
-        <v>604</v>
+        <v>592</v>
       </c>
       <c r="I126" s="24"/>
     </row>
-    <row r="127" spans="1:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-26</v>
@@ -7751,11 +7740,11 @@
         <v>228</v>
       </c>
       <c r="H127" s="19" t="s">
-        <v>490</v>
+        <v>602</v>
       </c>
       <c r="I127" s="24"/>
     </row>
-    <row r="128" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT07-1</v>
@@ -7779,11 +7768,11 @@
         <v>10</v>
       </c>
       <c r="H128" s="19" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="I128" s="24"/>
     </row>
-    <row r="129" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-19</v>
@@ -7798,18 +7787,18 @@
         <v>16</v>
       </c>
       <c r="E129" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F129" s="4" t="s">
         <v>94</v>
       </c>
       <c r="G129" s="4"/>
       <c r="H129" s="19" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="I129" s="24"/>
     </row>
-    <row r="130" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-20</v>
@@ -7824,18 +7813,18 @@
         <v>16</v>
       </c>
       <c r="E130" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F130" s="4" t="s">
         <v>95</v>
       </c>
       <c r="G130" s="4"/>
       <c r="H130" s="19" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="I130" s="24"/>
     </row>
-    <row r="131" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A131" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-9</v>
@@ -7859,13 +7848,13 @@
         <v>136</v>
       </c>
       <c r="H131" s="19" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="I131" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-10</v>
@@ -7889,11 +7878,11 @@
         <v>139</v>
       </c>
       <c r="H132" s="19" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="I132" s="24"/>
     </row>
-    <row r="133" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-27</v>
@@ -7917,13 +7906,13 @@
         <v>231</v>
       </c>
       <c r="H133" s="17" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="I133" s="24" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A134" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-28</v>
@@ -7950,10 +7939,10 @@
         <v>352</v>
       </c>
       <c r="I134" s="4" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A135" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-29</v>
@@ -7980,10 +7969,10 @@
         <v>352</v>
       </c>
       <c r="I135" s="4" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A136" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-10</v>
@@ -7998,7 +7987,7 @@
         <v>16</v>
       </c>
       <c r="E136" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F136" s="4" t="s">
         <v>36</v>
@@ -8007,13 +7996,13 @@
         <v>37</v>
       </c>
       <c r="H136" s="13" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="I136" s="4" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A137" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-11</v>
@@ -8028,7 +8017,7 @@
         <v>16</v>
       </c>
       <c r="E137" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F137" s="4" t="s">
         <v>38</v>
@@ -8037,13 +8026,13 @@
         <v>39</v>
       </c>
       <c r="H137" s="13" t="s">
-        <v>606</v>
+        <v>594</v>
       </c>
       <c r="I137" s="4" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="138" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A138" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-12</v>
@@ -8058,7 +8047,7 @@
         <v>16</v>
       </c>
       <c r="E138" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F138" s="4" t="s">
         <v>40</v>
@@ -8067,13 +8056,13 @@
         <v>41</v>
       </c>
       <c r="H138" s="19" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="I138" s="4" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" ht="44.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-25</v>
@@ -8095,13 +8084,13 @@
       </c>
       <c r="G139" s="4"/>
       <c r="H139" s="13" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="I139" s="4" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="140" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A140" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-13</v>
@@ -8125,11 +8114,11 @@
         <v>43</v>
       </c>
       <c r="H140" s="17" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="I140" s="24"/>
     </row>
-    <row r="141" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A141" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-7</v>
@@ -8144,7 +8133,7 @@
         <v>7</v>
       </c>
       <c r="E141" s="5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F141" s="4" t="s">
         <v>30</v>
@@ -8153,10 +8142,10 @@
         <v>31</v>
       </c>
       <c r="H141" s="13" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="I141" s="23" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tables enumeration et codes nomenclatures enjeux
</commit_message>
<xml_diff>
--- a/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
+++ b/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Geostandards-Risques\suivi\2024-05_06-Consultation-publique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65989973-F019-48D0-A5E9-ED82031A021E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A521F17-32E4-4FED-9F01-5BB527642F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="604">
   <si>
     <t>Organisme</t>
   </si>
@@ -1868,10 +1868,6 @@
 A-t-on des cas de ce type ?</t>
   </si>
   <si>
-    <t>OK sur le principe
-Quelle règle de fusion adopter ?</t>
-  </si>
-  <si>
     <t>OK sur le principe.
 A voir en fonction du commentaire précédent également</t>
   </si>
@@ -2334,6 +2330,14 @@
     <t>OK sur le principe.
 La codification proposée se voulait hiérarchique.
 Solution à trouver pour garder cette hiérarchie en simplifiant</t>
+  </si>
+  <si>
+    <t>intgéré</t>
+  </si>
+  <si>
+    <t>OK sur le principe
+Quelle règle de fusion adopter
+=&gt; Fusion additionnelle</t>
   </si>
 </sst>
 </file>
@@ -3437,8 +3441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939F5930-30D3-43D0-87E8-B00574FE9CE2}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3481,7 +3485,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="73" customHeight="1" x14ac:dyDescent="0.35">
@@ -3511,7 +3515,7 @@
         <v>351</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="92" x14ac:dyDescent="0.35">
@@ -3538,10 +3542,10 @@
         <v>332</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="92" x14ac:dyDescent="0.35">
@@ -3571,7 +3575,7 @@
         <v>353</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="75.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
@@ -3598,10 +3602,10 @@
         <v>305</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="89.15" customHeight="1" x14ac:dyDescent="0.35">
@@ -3631,7 +3635,7 @@
         <v>350</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="23" x14ac:dyDescent="0.35">
@@ -3659,7 +3663,7 @@
         <v>352</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
@@ -3689,7 +3693,7 @@
         <v>357</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="126.5" x14ac:dyDescent="0.35">
@@ -3716,10 +3720,10 @@
         <v>335</v>
       </c>
       <c r="H9" s="17" t="s">
+        <v>596</v>
+      </c>
+      <c r="I9" s="23" t="s">
         <v>597</v>
-      </c>
-      <c r="I9" s="23" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3749,7 +3753,7 @@
         <v>354</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -3779,7 +3783,7 @@
         <v>354</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
@@ -3806,10 +3810,10 @@
         <v>315</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3839,7 +3843,7 @@
         <v>355</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="92" x14ac:dyDescent="0.35">
@@ -3869,7 +3873,7 @@
         <v>356</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="61" customHeight="1" x14ac:dyDescent="0.35">
@@ -3899,7 +3903,7 @@
         <v>352</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="68.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
@@ -3926,10 +3930,10 @@
         <v>288</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="77.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
@@ -3959,7 +3963,7 @@
         <v>358</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="111" customHeight="1" x14ac:dyDescent="0.35">
@@ -3986,10 +3990,10 @@
         <v>293</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
@@ -4016,10 +4020,10 @@
         <v>328</v>
       </c>
       <c r="H19" s="25" t="s">
+        <v>594</v>
+      </c>
+      <c r="I19" s="24" t="s">
         <v>595</v>
-      </c>
-      <c r="I19" s="24" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4047,7 +4051,7 @@
         <v>359</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
   </sheetData>
@@ -4063,8 +4067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815F14A-19BC-4DCE-8D31-81F595A4B0E7}">
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B131" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I142" sqref="I142"/>
+    <sheetView tabSelected="1" topLeftCell="B124" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G127" sqref="G127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4107,7 +4111,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4132,10 +4136,10 @@
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="25" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4163,7 +4167,7 @@
         <v>370</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4191,7 +4195,7 @@
         <v>371</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="65.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
@@ -4216,10 +4220,10 @@
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="22" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="126.5" x14ac:dyDescent="0.35">
@@ -4245,7 +4249,7 @@
         <v>372</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
@@ -4273,7 +4277,7 @@
         <v>373</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="69" x14ac:dyDescent="0.35">
@@ -4301,7 +4305,7 @@
         <v>374</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4329,7 +4333,7 @@
         <v>375</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
@@ -4341,23 +4345,23 @@
         <v>1</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>538</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>539</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>540</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>541</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>542</v>
-      </c>
       <c r="H10" s="17" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
@@ -4443,7 +4447,7 @@
         <v>350</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="66.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
@@ -4470,10 +4474,10 @@
         <v>166</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="161" x14ac:dyDescent="0.35">
@@ -4500,10 +4504,10 @@
         <v>254</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
@@ -4530,10 +4534,10 @@
         <v>62</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
@@ -4560,10 +4564,10 @@
         <v>117</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
@@ -4593,7 +4597,7 @@
         <v>379</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
@@ -4623,7 +4627,7 @@
         <v>380</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="84.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -4650,10 +4654,10 @@
         <v>255</v>
       </c>
       <c r="H20" s="19" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="I20" s="23" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
@@ -4680,10 +4684,10 @@
         <v>256</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4713,7 +4717,7 @@
         <v>381</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4740,10 +4744,10 @@
         <v>122</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
@@ -4773,7 +4777,7 @@
         <v>382</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="46" x14ac:dyDescent="0.35">
@@ -4803,7 +4807,7 @@
         <v>383</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="23" x14ac:dyDescent="0.35">
@@ -4833,7 +4837,7 @@
         <v>382</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="71.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4860,10 +4864,10 @@
         <v>72</v>
       </c>
       <c r="H27" s="19" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="I27" s="24" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
@@ -4893,7 +4897,7 @@
         <v>352</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="115" x14ac:dyDescent="0.35">
@@ -4918,10 +4922,10 @@
         <v>340</v>
       </c>
       <c r="H29" s="19" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I29" s="24" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4948,10 +4952,10 @@
         <v>75</v>
       </c>
       <c r="H30" s="19" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
@@ -4978,10 +4982,10 @@
         <v>78</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="I31" s="23" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
@@ -5008,10 +5012,10 @@
         <v>128</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="I32" s="23" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="92" x14ac:dyDescent="0.35">
@@ -5041,7 +5045,7 @@
         <v>385</v>
       </c>
       <c r="I33" s="24" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="41.15" customHeight="1" x14ac:dyDescent="0.35">
@@ -5066,10 +5070,10 @@
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="17" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
@@ -5099,7 +5103,7 @@
         <v>386</v>
       </c>
       <c r="I35" s="23" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="62.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -5127,7 +5131,7 @@
         <v>384</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="32" customFormat="1" ht="81" thickBot="1" x14ac:dyDescent="0.4">
@@ -5154,10 +5158,10 @@
         <v>19</v>
       </c>
       <c r="H37" s="30" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="I37" s="31" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="44.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
@@ -5184,10 +5188,10 @@
         <v>99</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.35">
@@ -5212,7 +5216,7 @@
         <v>338</v>
       </c>
       <c r="H39" s="19" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="I39" s="24"/>
     </row>
@@ -5238,10 +5242,10 @@
         <v>338</v>
       </c>
       <c r="H40" s="19" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="I40" s="24" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
@@ -5268,10 +5272,10 @@
         <v>267</v>
       </c>
       <c r="H41" s="17" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="I41" s="23" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
@@ -5298,10 +5302,10 @@
         <v>133</v>
       </c>
       <c r="H42" s="19" t="s">
+        <v>569</v>
+      </c>
+      <c r="I42" s="24" t="s">
         <v>570</v>
-      </c>
-      <c r="I42" s="24" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="88" customHeight="1" x14ac:dyDescent="0.35">
@@ -5326,10 +5330,10 @@
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="17" t="s">
+        <v>571</v>
+      </c>
+      <c r="I43" s="24" t="s">
         <v>572</v>
-      </c>
-      <c r="I43" s="24" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="92" x14ac:dyDescent="0.35">
@@ -5356,10 +5360,10 @@
         <v>26</v>
       </c>
       <c r="H44" s="13" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="77.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5389,7 +5393,7 @@
         <v>389</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
@@ -5417,7 +5421,7 @@
         <v>390</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
@@ -5444,10 +5448,10 @@
         <v>33</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I47" s="24" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5505,7 +5509,7 @@
         <v>391</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="92" x14ac:dyDescent="0.35">
@@ -5532,10 +5536,10 @@
         <v>28</v>
       </c>
       <c r="H50" s="17" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="I50" s="24" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="69" x14ac:dyDescent="0.35">
@@ -5646,10 +5650,10 @@
         <v>145</v>
       </c>
       <c r="H54" s="17" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.35">
@@ -5677,7 +5681,7 @@
         <v>378</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -5702,10 +5706,10 @@
         <v>87</v>
       </c>
       <c r="H56" s="17" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
@@ -5733,7 +5737,7 @@
         <v>395</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="46" x14ac:dyDescent="0.35">
@@ -5763,7 +5767,7 @@
         <v>378</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="184" x14ac:dyDescent="0.35">
@@ -5789,7 +5793,7 @@
         <v>393</v>
       </c>
       <c r="I59" s="24" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="46" x14ac:dyDescent="0.35">
@@ -5843,7 +5847,7 @@
         <v>397</v>
       </c>
       <c r="I61" s="24" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="230" x14ac:dyDescent="0.35">
@@ -5869,7 +5873,7 @@
         <v>396</v>
       </c>
       <c r="I62" s="24" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
@@ -5896,10 +5900,10 @@
         <v>151</v>
       </c>
       <c r="H63" s="19" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="I63" s="24" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="46" x14ac:dyDescent="0.35">
@@ -5922,7 +5926,7 @@
       </c>
       <c r="G64" s="4"/>
       <c r="H64" s="13" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="I64" s="24"/>
     </row>
@@ -5950,10 +5954,10 @@
         <v>154</v>
       </c>
       <c r="H65" s="19" t="s">
+        <v>582</v>
+      </c>
+      <c r="I65" s="24" t="s">
         <v>583</v>
-      </c>
-      <c r="I65" s="24" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="46" x14ac:dyDescent="0.35">
@@ -5983,7 +5987,7 @@
         <v>398</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="46" x14ac:dyDescent="0.35">
@@ -6010,10 +6014,10 @@
         <v>53</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="I67" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="174" x14ac:dyDescent="0.35">
@@ -6124,10 +6128,10 @@
         <v>272</v>
       </c>
       <c r="H71" s="17" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I71" s="24" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
@@ -6157,7 +6161,7 @@
         <v>464</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
@@ -6187,7 +6191,7 @@
         <v>465</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
@@ -6217,7 +6221,7 @@
         <v>466</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.35">
@@ -6247,7 +6251,7 @@
         <v>466</v>
       </c>
       <c r="I75" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6302,7 +6306,7 @@
         <v>275</v>
       </c>
       <c r="H77" s="17" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I77" s="24"/>
     </row>
@@ -6315,25 +6319,25 @@
         <v>2</v>
       </c>
       <c r="C78" s="4" t="s">
+        <v>538</v>
+      </c>
+      <c r="D78" s="5" t="s">
         <v>539</v>
       </c>
-      <c r="D78" s="5" t="s">
-        <v>540</v>
-      </c>
       <c r="E78" s="5" t="s">
+        <v>542</v>
+      </c>
+      <c r="F78" s="4" t="s">
         <v>543</v>
       </c>
-      <c r="F78" s="4" t="s">
+      <c r="G78" s="4" t="s">
         <v>544</v>
       </c>
-      <c r="G78" s="4" t="s">
-        <v>545</v>
-      </c>
       <c r="H78" s="17" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="46" x14ac:dyDescent="0.35">
@@ -6360,7 +6364,7 @@
         <v>203</v>
       </c>
       <c r="H79" s="17" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I79" s="24"/>
     </row>
@@ -6391,7 +6395,7 @@
         <v>465</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="26" x14ac:dyDescent="0.35">
@@ -6421,7 +6425,7 @@
         <v>466</v>
       </c>
       <c r="I81" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
@@ -6448,10 +6452,10 @@
         <v>449</v>
       </c>
       <c r="H82" s="13" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="I82" s="24" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="65.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
@@ -6534,9 +6538,11 @@
         <v>211</v>
       </c>
       <c r="H85" s="19" t="s">
-        <v>589</v>
-      </c>
-      <c r="I85" s="24"/>
+        <v>588</v>
+      </c>
+      <c r="I85" s="23" t="s">
+        <v>509</v>
+      </c>
     </row>
     <row r="86" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="str">
@@ -6565,7 +6571,7 @@
         <v>470</v>
       </c>
       <c r="I86" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -6595,7 +6601,7 @@
         <v>465</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
@@ -6625,7 +6631,7 @@
         <v>471</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="39.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -6655,7 +6661,7 @@
         <v>465</v>
       </c>
       <c r="I89" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.35">
@@ -6685,7 +6691,7 @@
         <v>378</v>
       </c>
       <c r="I90" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
@@ -6713,7 +6719,7 @@
         <v>472</v>
       </c>
       <c r="I91" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6741,7 +6747,7 @@
         <v>473</v>
       </c>
       <c r="I92" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="46" x14ac:dyDescent="0.35">
@@ -6768,7 +6774,7 @@
         <v>218</v>
       </c>
       <c r="H93" s="17" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="I93" s="24"/>
     </row>
@@ -6799,7 +6805,7 @@
         <v>474</v>
       </c>
       <c r="I94" s="38" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="81" thickTop="1" x14ac:dyDescent="0.35">
@@ -6829,7 +6835,7 @@
         <v>475</v>
       </c>
       <c r="I95" s="4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="113.15" customHeight="1" x14ac:dyDescent="0.35">
@@ -6856,10 +6862,10 @@
         <v>259</v>
       </c>
       <c r="H96" s="17" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I96" s="23" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6971,7 +6977,7 @@
         <v>477</v>
       </c>
       <c r="I100" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="69" x14ac:dyDescent="0.35">
@@ -6983,20 +6989,20 @@
         <v>3</v>
       </c>
       <c r="C101" s="4" t="s">
+        <v>538</v>
+      </c>
+      <c r="D101" s="5" t="s">
         <v>539</v>
-      </c>
-      <c r="D101" s="5" t="s">
-        <v>540</v>
       </c>
       <c r="E101" s="5"/>
       <c r="F101" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="G101" s="4" t="s">
         <v>546</v>
       </c>
-      <c r="G101" s="4" t="s">
+      <c r="H101" s="19" t="s">
         <v>547</v>
-      </c>
-      <c r="H101" s="19" t="s">
-        <v>548</v>
       </c>
       <c r="I101" s="24"/>
     </row>
@@ -7027,7 +7033,7 @@
         <v>479</v>
       </c>
       <c r="I102" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -7057,7 +7063,7 @@
         <v>352</v>
       </c>
       <c r="I103" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="23" x14ac:dyDescent="0.35">
@@ -7087,7 +7093,7 @@
         <v>479</v>
       </c>
       <c r="I104" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="23" x14ac:dyDescent="0.35">
@@ -7117,7 +7123,7 @@
         <v>479</v>
       </c>
       <c r="I105" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="106" spans="1:9" ht="37.5" x14ac:dyDescent="0.35">
@@ -7175,7 +7181,7 @@
         <v>481</v>
       </c>
       <c r="I107" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="108" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
@@ -7205,7 +7211,7 @@
         <v>479</v>
       </c>
       <c r="I108" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="23" x14ac:dyDescent="0.35">
@@ -7319,7 +7325,7 @@
         <v>478</v>
       </c>
       <c r="I112" s="4" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="23" x14ac:dyDescent="0.35">
@@ -7517,7 +7523,7 @@
         <v>483</v>
       </c>
       <c r="I119" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.35">
@@ -7712,7 +7718,7 @@
         <v>225</v>
       </c>
       <c r="H126" s="19" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I126" s="24"/>
     </row>
@@ -7739,10 +7745,12 @@
       <c r="G127" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="H127" s="19" t="s">
+      <c r="H127" s="17" t="s">
+        <v>601</v>
+      </c>
+      <c r="I127" s="23" t="s">
         <v>602</v>
       </c>
-      <c r="I127" s="24"/>
     </row>
     <row r="128" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" s="4" t="str">
@@ -7767,10 +7775,12 @@
       <c r="G128" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H128" s="19" t="s">
+      <c r="H128" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="I128" s="24"/>
+      <c r="I128" s="23" t="s">
+        <v>509</v>
+      </c>
     </row>
     <row r="129" spans="1:9" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="4" t="str">
@@ -7819,10 +7829,12 @@
         <v>95</v>
       </c>
       <c r="G130" s="4"/>
-      <c r="H130" s="19" t="s">
-        <v>489</v>
-      </c>
-      <c r="I130" s="24"/>
+      <c r="H130" s="17" t="s">
+        <v>603</v>
+      </c>
+      <c r="I130" s="23" t="s">
+        <v>509</v>
+      </c>
     </row>
     <row r="131" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A131" s="4" t="str">
@@ -7847,11 +7859,11 @@
       <c r="G131" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="H131" s="19" t="s">
-        <v>490</v>
+      <c r="H131" s="17" t="s">
+        <v>489</v>
       </c>
       <c r="I131" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="132" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
@@ -7878,7 +7890,7 @@
         <v>139</v>
       </c>
       <c r="H132" s="19" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I132" s="24"/>
     </row>
@@ -7906,10 +7918,10 @@
         <v>231</v>
       </c>
       <c r="H133" s="17" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I133" s="24" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="23" x14ac:dyDescent="0.35">
@@ -7939,7 +7951,7 @@
         <v>352</v>
       </c>
       <c r="I134" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="23" x14ac:dyDescent="0.35">
@@ -7969,7 +7981,7 @@
         <v>352</v>
       </c>
       <c r="I135" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
@@ -7996,10 +8008,10 @@
         <v>37</v>
       </c>
       <c r="H136" s="13" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="I136" s="4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="137" spans="1:9" ht="46" x14ac:dyDescent="0.35">
@@ -8026,10 +8038,10 @@
         <v>39</v>
       </c>
       <c r="H137" s="13" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="I137" s="4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="138" spans="1:9" ht="69" x14ac:dyDescent="0.35">
@@ -8056,10 +8068,10 @@
         <v>41</v>
       </c>
       <c r="H138" s="19" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I138" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="139" spans="1:9" ht="44.15" customHeight="1" x14ac:dyDescent="0.35">
@@ -8084,10 +8096,10 @@
       </c>
       <c r="G139" s="4"/>
       <c r="H139" s="13" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="I139" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="140" spans="1:9" ht="46" x14ac:dyDescent="0.35">
@@ -8114,9 +8126,11 @@
         <v>43</v>
       </c>
       <c r="H140" s="17" t="s">
-        <v>496</v>
-      </c>
-      <c r="I140" s="24"/>
+        <v>495</v>
+      </c>
+      <c r="I140" s="23" t="s">
+        <v>509</v>
+      </c>
     </row>
     <row r="141" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A141" s="4" t="str">
@@ -8142,10 +8156,10 @@
         <v>31</v>
       </c>
       <c r="H141" s="13" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="I141" s="23" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Traitement commentaires... debut shapefile
</commit_message>
<xml_diff>
--- a/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
+++ b/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Geostandards-Risques\suivi\2024-05_06-Consultation-publique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A521F17-32E4-4FED-9F01-5BB527642F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D8A03A-0B65-44DC-92E3-B8C2114F78E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
+    <workbookView xWindow="6540" yWindow="1395" windowWidth="21600" windowHeight="13035" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Synthese Modele Commun" sheetId="3" r:id="rId1"/>
@@ -2320,24 +2320,24 @@
 Faire la distinction des deux types de bandes particulières et garder la possibilité d'avoir  un type de bande pour les deux</t>
   </si>
   <si>
+    <t>OK sur le principe.
+La codification proposée se voulait hiérarchique.
+Solution à trouver pour garder cette hiérarchie en simplifiant</t>
+  </si>
+  <si>
+    <t>intgéré</t>
+  </si>
+  <si>
+    <t>OK sur le principe
+Quelle règle de fusion adopter
+=&gt; Fusion additionnelle</t>
+  </si>
+  <si>
     <t>NB : il existe :
 - des PPRN sur Saint-Martin (risque cyclonique et multirsiques)
 - un PPRT sur la Guadeloupe (Baie Mahault)
 Rien sur Saint-Barthélémy, mais il me semble que le code de l'environnement peut aussi s'appliquer à Saint-Barthélémy, non ?
 Confirmation que le code de l'environnement ne s'applique pas à Saint Barthélémy (un code particulier s'y applique)</t>
-  </si>
-  <si>
-    <t>OK sur le principe.
-La codification proposée se voulait hiérarchique.
-Solution à trouver pour garder cette hiérarchie en simplifiant</t>
-  </si>
-  <si>
-    <t>intgéré</t>
-  </si>
-  <si>
-    <t>OK sur le principe
-Quelle règle de fusion adopter
-=&gt; Fusion additionnelle</t>
   </si>
 </sst>
 </file>
@@ -3441,25 +3441,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939F5930-30D3-43D0-87E8-B00574FE9CE2}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.453125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.1796875" style="3" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="21.81640625" style="3" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="3" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" style="3" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="3" customWidth="1"/>
-    <col min="5" max="5" width="16.1796875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="49.54296875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="47.54296875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="54.81640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="21.453125" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="10.81640625" style="3"/>
+    <col min="5" max="5" width="16.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="49.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="47.5703125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="54.85546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="10.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>349</v>
       </c>
@@ -3488,7 +3488,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="73" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="72.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-1</v>
@@ -3518,7 +3518,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-2</v>
@@ -3548,7 +3548,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-3</v>
@@ -3578,7 +3578,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="75.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-4</v>
@@ -3608,7 +3608,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="89.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="89.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-5</v>
@@ -3638,7 +3638,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/DAPP/BIP-11</v>
@@ -3666,7 +3666,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="96" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-6</v>
@@ -3696,7 +3696,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="126.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="144" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-7</v>
@@ -3726,7 +3726,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-1</v>
@@ -3756,7 +3756,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-2</v>
@@ -3786,7 +3786,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-8</v>
@@ -3816,7 +3816,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>cerema-6</v>
@@ -3846,7 +3846,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="96" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-9</v>
@@ -3876,7 +3876,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="61" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="60.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-10</v>
@@ -3906,7 +3906,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="68.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-3</v>
@@ -3936,7 +3936,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="77.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="77.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-4</v>
@@ -3966,7 +3966,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="111" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-5</v>
@@ -3996,7 +3996,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="96" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SDCAP/PONSOH-13</v>
@@ -4026,7 +4026,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/DAPP/BIP-12</v>
@@ -4067,25 +4067,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815F14A-19BC-4DCE-8D31-81F595A4B0E7}">
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B124" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G127" sqref="G127"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.54296875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="3.81640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="16" style="3" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="44.1796875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="44.140625" style="3" customWidth="1"/>
     <col min="7" max="7" width="38" style="3" customWidth="1"/>
-    <col min="8" max="8" width="51.81640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="22.26953125" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="10.81640625" style="3"/>
+    <col min="8" max="8" width="51.85546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="10.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>348</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-2</v>
@@ -4142,7 +4142,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-3</v>
@@ -4170,7 +4170,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-4</v>
@@ -4198,7 +4198,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="65.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-5</v>
@@ -4226,7 +4226,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="126.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="132" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP-0</v>
@@ -4252,7 +4252,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-9</v>
@@ -4280,7 +4280,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-14</v>
@@ -4308,7 +4308,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-15</v>
@@ -4336,7 +4336,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDTM11-1</v>
@@ -4364,7 +4364,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-2</v>
@@ -4392,7 +4392,7 @@
       </c>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" spans="1:9" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-3</v>
@@ -4420,7 +4420,7 @@
       </c>
       <c r="I12" s="24"/>
     </row>
-    <row r="13" spans="1:9" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-1</v>
@@ -4450,7 +4450,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="66.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-1</v>
@@ -4480,7 +4480,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="161" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="168" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-2</v>
@@ -4510,7 +4510,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-3</v>
@@ -4540,7 +4540,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-1</v>
@@ -4570,7 +4570,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-4</v>
@@ -4600,7 +4600,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-4</v>
@@ -4630,7 +4630,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="84.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-5</v>
@@ -4653,14 +4653,14 @@
       <c r="G20" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="H20" s="19" t="s">
-        <v>600</v>
+      <c r="H20" s="17" t="s">
+        <v>603</v>
       </c>
       <c r="I20" s="23" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="84" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-6</v>
@@ -4690,7 +4690,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-2</v>
@@ -4720,7 +4720,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-3</v>
@@ -4750,7 +4750,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-5</v>
@@ -4780,7 +4780,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-4</v>
@@ -4810,7 +4810,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-5</v>
@@ -4840,7 +4840,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="71.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="71.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-7</v>
@@ -4870,7 +4870,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-6</v>
@@ -4900,7 +4900,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="115" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-</v>
@@ -4928,7 +4928,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-8</v>
@@ -4958,7 +4958,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-9</v>
@@ -4988,7 +4988,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="84" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-6</v>
@@ -5018,7 +5018,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-7</v>
@@ -5048,7 +5048,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="41.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-10</v>
@@ -5076,7 +5076,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-7</v>
@@ -5106,7 +5106,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="62.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:9" ht="62.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-11</v>
@@ -5134,7 +5134,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="32" customFormat="1" ht="81" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:9" s="32" customFormat="1" ht="84.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="26" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-1</v>
@@ -5164,7 +5164,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="44.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" ht="44.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-21</v>
@@ -5194,7 +5194,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-</v>
@@ -5220,7 +5220,7 @@
       </c>
       <c r="I39" s="24"/>
     </row>
-    <row r="40" spans="1:9" ht="207" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" ht="228" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-</v>
@@ -5248,7 +5248,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-8</v>
@@ -5278,7 +5278,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-8</v>
@@ -5308,7 +5308,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="88" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" ht="87.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-12</v>
@@ -5336,7 +5336,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-4</v>
@@ -5366,7 +5366,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="77.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-2</v>
@@ -5396,7 +5396,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/BRNT-22</v>
@@ -5424,7 +5424,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-8</v>
@@ -5454,7 +5454,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-24</v>
@@ -5482,7 +5482,7 @@
       </c>
       <c r="I48" s="23"/>
     </row>
-    <row r="49" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-3</v>
@@ -5512,7 +5512,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" ht="96" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-5</v>
@@ -5542,7 +5542,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" ht="84" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT07-2</v>
@@ -5570,7 +5570,7 @@
       </c>
       <c r="I51" s="4"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-11</v>
@@ -5598,7 +5598,7 @@
       </c>
       <c r="I52" s="24"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-12</v>
@@ -5626,7 +5626,7 @@
       </c>
       <c r="I53" s="24"/>
     </row>
-    <row r="54" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-13</v>
@@ -5656,7 +5656,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-13</v>
@@ -5684,7 +5684,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-14</v>
@@ -5712,7 +5712,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-15</v>
@@ -5740,7 +5740,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-9</v>
@@ -5770,7 +5770,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="184" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" ht="216" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5796,7 +5796,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-14</v>
@@ -5824,7 +5824,7 @@
       </c>
       <c r="I60" s="24"/>
     </row>
-    <row r="61" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5850,7 +5850,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="230" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" ht="252" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5876,7 +5876,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" ht="96" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-15</v>
@@ -5906,7 +5906,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -</v>
@@ -5930,7 +5930,7 @@
       </c>
       <c r="I64" s="24"/>
     </row>
-    <row r="65" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" ht="84" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-16</v>
@@ -5960,7 +5960,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT01-3</v>
@@ -5990,7 +5990,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDTM 83-1</v>
@@ -6020,7 +6020,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="174" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-10</v>
@@ -6048,7 +6048,7 @@
       </c>
       <c r="I68" s="24"/>
     </row>
-    <row r="69" spans="1:9" ht="88" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" ht="87.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-1</v>
@@ -6076,7 +6076,7 @@
       </c>
       <c r="I69" s="24"/>
     </row>
-    <row r="70" spans="1:9" ht="103" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" ht="102.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-11</v>
@@ -6104,7 +6104,7 @@
       </c>
       <c r="I70" s="24"/>
     </row>
-    <row r="71" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-12</v>
@@ -6134,7 +6134,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-13</v>
@@ -6164,7 +6164,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A73" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-14</v>
@@ -6194,7 +6194,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A74" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-19</v>
@@ -6224,7 +6224,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A75" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-16</v>
@@ -6254,7 +6254,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-14</v>
@@ -6282,7 +6282,7 @@
       </c>
       <c r="I76" s="23"/>
     </row>
-    <row r="77" spans="1:9" ht="126.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" ht="144" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-15</v>
@@ -6310,7 +6310,7 @@
       </c>
       <c r="I77" s="24"/>
     </row>
-    <row r="78" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A78" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDTM11-2</v>
@@ -6340,7 +6340,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-16</v>
@@ -6368,7 +6368,7 @@
       </c>
       <c r="I79" s="24"/>
     </row>
-    <row r="80" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A80" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-22</v>
@@ -6398,7 +6398,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" ht="27" x14ac:dyDescent="0.25">
       <c r="A81" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-23</v>
@@ -6428,7 +6428,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A82" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-24</v>
@@ -6458,7 +6458,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="65.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-17</v>
@@ -6486,7 +6486,7 @@
       </c>
       <c r="I83" s="24"/>
     </row>
-    <row r="84" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-18</v>
@@ -6514,7 +6514,7 @@
       </c>
       <c r="I84" s="24"/>
     </row>
-    <row r="85" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-19</v>
@@ -6544,7 +6544,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-20</v>
@@ -6574,7 +6574,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-27</v>
@@ -6604,7 +6604,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-21</v>
@@ -6634,7 +6634,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="39.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-26</v>
@@ -6664,7 +6664,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-17</v>
@@ -6694,7 +6694,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-16</v>
@@ -6722,7 +6722,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:9" ht="77.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-17</v>
@@ -6750,7 +6750,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-22</v>
@@ -6778,7 +6778,7 @@
       </c>
       <c r="I93" s="24"/>
     </row>
-    <row r="94" spans="1:9" s="39" customFormat="1" ht="98.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:9" s="39" customFormat="1" ht="98.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="33" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-23</v>
@@ -6808,7 +6808,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="81" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9" ht="96.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-24</v>
@@ -6838,7 +6838,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="113.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9" ht="113.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/PoNSOH-26</v>
@@ -6868,7 +6868,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/PoNSOH-27</v>
@@ -6896,7 +6896,7 @@
       </c>
       <c r="I97" s="23"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-18</v>
@@ -6924,7 +6924,7 @@
       </c>
       <c r="I98" s="24"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-19</v>
@@ -6952,7 +6952,7 @@
       </c>
       <c r="I99" s="24"/>
     </row>
-    <row r="100" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-18</v>
@@ -6980,7 +6980,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A101" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDTM11-3</v>
@@ -7006,7 +7006,7 @@
       </c>
       <c r="I101" s="24"/>
     </row>
-    <row r="102" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A102" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-15</v>
@@ -7036,7 +7036,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-1</v>
@@ -7066,7 +7066,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A104" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-17</v>
@@ -7096,7 +7096,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A105" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-20</v>
@@ -7126,7 +7126,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9" ht="39" x14ac:dyDescent="0.25">
       <c r="A106" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-21</v>
@@ -7154,7 +7154,7 @@
       </c>
       <c r="I106" s="24"/>
     </row>
-    <row r="107" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A107" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-18</v>
@@ -7184,7 +7184,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A108" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-25</v>
@@ -7214,7 +7214,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A109" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-2</v>
@@ -7242,7 +7242,7 @@
       </c>
       <c r="I109" s="24"/>
     </row>
-    <row r="110" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A110" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-3</v>
@@ -7270,7 +7270,7 @@
       </c>
       <c r="I110" s="24"/>
     </row>
-    <row r="111" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A111" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-4</v>
@@ -7298,7 +7298,7 @@
       </c>
       <c r="I111" s="24"/>
     </row>
-    <row r="112" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT01-1</v>
@@ -7328,7 +7328,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A113" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-5</v>
@@ -7356,7 +7356,7 @@
       </c>
       <c r="I113" s="24"/>
     </row>
-    <row r="114" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A114" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-6</v>
@@ -7384,7 +7384,7 @@
       </c>
       <c r="I114" s="24"/>
     </row>
-    <row r="115" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A115" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-7</v>
@@ -7412,7 +7412,7 @@
       </c>
       <c r="I115" s="24"/>
     </row>
-    <row r="116" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A116" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-8</v>
@@ -7440,7 +7440,7 @@
       </c>
       <c r="I116" s="24"/>
     </row>
-    <row r="117" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A117" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-9</v>
@@ -7468,7 +7468,7 @@
       </c>
       <c r="I117" s="24"/>
     </row>
-    <row r="118" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A118" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-10</v>
@@ -7496,7 +7496,7 @@
       </c>
       <c r="I118" s="24"/>
     </row>
-    <row r="119" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-11</v>
@@ -7526,7 +7526,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A120" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-12</v>
@@ -7554,7 +7554,7 @@
       </c>
       <c r="I120" s="24"/>
     </row>
-    <row r="121" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A121" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-13</v>
@@ -7582,7 +7582,7 @@
       </c>
       <c r="I121" s="24"/>
     </row>
-    <row r="122" spans="1:9" ht="151.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-6</v>
@@ -7610,7 +7610,7 @@
       </c>
       <c r="I122" s="24"/>
     </row>
-    <row r="123" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT01-2</v>
@@ -7638,7 +7638,7 @@
       </c>
       <c r="I123" s="24"/>
     </row>
-    <row r="124" spans="1:9" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:9" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-23</v>
@@ -7666,7 +7666,7 @@
       </c>
       <c r="I124" s="24"/>
     </row>
-    <row r="125" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:9" ht="96" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-20</v>
@@ -7694,7 +7694,7 @@
       </c>
       <c r="I125" s="24"/>
     </row>
-    <row r="126" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-25</v>
@@ -7722,7 +7722,7 @@
       </c>
       <c r="I126" s="24"/>
     </row>
-    <row r="127" spans="1:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-26</v>
@@ -7746,13 +7746,13 @@
         <v>228</v>
       </c>
       <c r="H127" s="17" t="s">
+        <v>600</v>
+      </c>
+      <c r="I127" s="23" t="s">
         <v>601</v>
       </c>
-      <c r="I127" s="23" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="128" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT07-1</v>
@@ -7782,7 +7782,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-19</v>
@@ -7808,7 +7808,7 @@
       </c>
       <c r="I129" s="24"/>
     </row>
-    <row r="130" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-20</v>
@@ -7830,13 +7830,13 @@
       </c>
       <c r="G130" s="4"/>
       <c r="H130" s="17" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="I130" s="23" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="131" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-9</v>
@@ -7866,7 +7866,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="132" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-10</v>
@@ -7894,7 +7894,7 @@
       </c>
       <c r="I132" s="24"/>
     </row>
-    <row r="133" spans="1:9" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-27</v>
@@ -7924,7 +7924,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="134" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-28</v>
@@ -7954,7 +7954,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="135" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-29</v>
@@ -7984,7 +7984,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="136" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-10</v>
@@ -8014,7 +8014,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="137" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-11</v>
@@ -8044,7 +8044,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-12</v>
@@ -8074,7 +8074,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="139" spans="1:9" ht="44.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:9" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-25</v>
@@ -8102,7 +8102,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="140" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-13</v>
@@ -8132,7 +8132,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="141" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-7</v>

</xml_diff>

<commit_message>
Traitement OuvrageProtecteur et roleProtection
</commit_message>
<xml_diff>
--- a/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
+++ b/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Geostandards-Risques\suivi\2024-05_06-Consultation-publique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE2692C-B4E4-4AFB-A063-AE1F2440AE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87828D0F-9BFE-4B6F-951D-12296027CF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="870" yWindow="1140" windowWidth="25065" windowHeight="13035" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Synthese Modele Commun" sheetId="3" r:id="rId1"/>
@@ -2276,10 +2276,6 @@
 Maintenir le terme scénario Pas d'accès à SIOUH2</t>
   </si>
   <si>
-    <t>Traité en partie
-NB : roleProtection dans PPR ou modèle commun ?</t>
-  </si>
-  <si>
     <t>OK sur le principe
 Mais voir au cas par cas, car dans le modèle commun, certains champs peuvent être spécialisés et implémentées de manière différentes en fonction du type d'aléa. 
 Par exemple : occurrence (classe de probabilité ou période de retour), ou niveau de protection (hauteur dans certains cas, mais pas toujours)
@@ -2341,6 +2337,11 @@
   <si>
     <t>NOK.
 D'après le decret 2019, ces informations relèvent plutôt du règlement (interdiction sur les contructions pouvant engendrer des pollutions) et non des enjeux.</t>
+  </si>
+  <si>
+    <t>Traité
+NB : roleProtection + occurrence dans modèle commun
+OuvrageProtection =&gt; OuvrageProtecteur</t>
   </si>
 </sst>
 </file>
@@ -3444,8 +3445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939F5930-30D3-43D0-87E8-B00574FE9CE2}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="G19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3723,10 +3724,10 @@
         <v>335</v>
       </c>
       <c r="H9" s="17" t="s">
+        <v>590</v>
+      </c>
+      <c r="I9" s="23" t="s">
         <v>591</v>
-      </c>
-      <c r="I9" s="23" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4025,8 +4026,8 @@
       <c r="H19" s="25" t="s">
         <v>589</v>
       </c>
-      <c r="I19" s="24" t="s">
-        <v>590</v>
+      <c r="I19" s="23" t="s">
+        <v>603</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4070,8 +4071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815F14A-19BC-4DCE-8D31-81F595A4B0E7}">
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D135" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G142" sqref="G142"/>
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4657,7 +4658,7 @@
         <v>255</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="I20" s="23" t="s">
         <v>508</v>
@@ -4747,10 +4748,10 @@
         <v>122</v>
       </c>
       <c r="H23" s="13" t="s">
+        <v>598</v>
+      </c>
+      <c r="I23" s="24" t="s">
         <v>599</v>
-      </c>
-      <c r="I23" s="24" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -4985,7 +4986,7 @@
         <v>78</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="I31" s="23" t="s">
         <v>508</v>
@@ -5015,7 +5016,7 @@
         <v>128</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="I32" s="23" t="s">
         <v>508</v>
@@ -7005,7 +7006,7 @@
         <v>544</v>
       </c>
       <c r="H101" s="19" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="I101" s="24"/>
     </row>
@@ -7328,7 +7329,7 @@
         <v>478</v>
       </c>
       <c r="I112" s="24" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="24" x14ac:dyDescent="0.25">
@@ -7749,10 +7750,10 @@
         <v>228</v>
       </c>
       <c r="H127" s="17" t="s">
+        <v>594</v>
+      </c>
+      <c r="I127" s="23" t="s">
         <v>595</v>
-      </c>
-      <c r="I127" s="23" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="128" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
@@ -7833,7 +7834,7 @@
       </c>
       <c r="G130" s="4"/>
       <c r="H130" s="17" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="I130" s="23" t="s">
         <v>508</v>
@@ -7893,7 +7894,7 @@
         <v>139</v>
       </c>
       <c r="H132" s="13" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="I132" s="23" t="s">
         <v>507</v>

</xml_diff>

<commit_message>
Traitement commentaires DGPR/SRNH/SdcAP/BRIL-7 et Cerema-7
</commit_message>
<xml_diff>
--- a/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
+++ b/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Geostandards-Risques\suivi\2024-05_06-Consultation-publique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87828D0F-9BFE-4B6F-951D-12296027CF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E131303C-E28F-4B68-A2F9-E893DB3F3878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
+    <workbookView xWindow="6765" yWindow="4785" windowWidth="21600" windowHeight="10395" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Synthese Modele Commun" sheetId="3" r:id="rId1"/>
@@ -2119,9 +2119,6 @@
     <t>Mentionner la possibilité de cartographier les PHEC mais sonas les définir + que ça (réf. https://www.reperesdecrues.developpement-durable.gouv.fr/  )</t>
   </si>
   <si>
-    <t>changer en zones + mentionner la référence aux espaces du guide PPRN;2016</t>
-  </si>
-  <si>
     <t>NOK ?
 La nomenture des risques GASPAR ne fait pas la distinction entre les différents types d'avalanche. Peut-être faut-il faire des sous-types de l'aléa 14 comme pour l'inondation ?
 Pour l'instant cette information peut être mise dans la description texte libre</t>
@@ -2342,6 +2339,10 @@
     <t>Traité
 NB : roleProtection + occurrence dans modèle commun
 OuvrageProtection =&gt; OuvrageProtecteur</t>
+  </si>
+  <si>
+    <t>intégré 
+changer en zones + mentionner la référence aux espaces du guide PPRN;2016</t>
   </si>
 </sst>
 </file>
@@ -3445,8 +3446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939F5930-30D3-43D0-87E8-B00574FE9CE2}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3724,10 +3725,10 @@
         <v>335</v>
       </c>
       <c r="H9" s="17" t="s">
+        <v>589</v>
+      </c>
+      <c r="I9" s="23" t="s">
         <v>590</v>
-      </c>
-      <c r="I9" s="23" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4024,10 +4025,10 @@
         <v>328</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4071,8 +4072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815F14A-19BC-4DCE-8D31-81F595A4B0E7}">
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4658,7 +4659,7 @@
         <v>255</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="I20" s="23" t="s">
         <v>508</v>
@@ -4748,10 +4749,10 @@
         <v>122</v>
       </c>
       <c r="H23" s="13" t="s">
+        <v>597</v>
+      </c>
+      <c r="I23" s="24" t="s">
         <v>598</v>
-      </c>
-      <c r="I23" s="24" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -4867,10 +4868,10 @@
       <c r="G27" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="H27" s="19" t="s">
+      <c r="H27" s="17" t="s">
         <v>518</v>
       </c>
-      <c r="I27" s="24" t="s">
+      <c r="I27" s="23" t="s">
         <v>554</v>
       </c>
     </row>
@@ -4986,7 +4987,7 @@
         <v>78</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I31" s="23" t="s">
         <v>508</v>
@@ -5016,7 +5017,7 @@
         <v>128</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="I32" s="23" t="s">
         <v>508</v>
@@ -5048,8 +5049,8 @@
       <c r="H33" s="17" t="s">
         <v>385</v>
       </c>
-      <c r="I33" s="24" t="s">
-        <v>556</v>
+      <c r="I33" s="23" t="s">
+        <v>603</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -5162,10 +5163,10 @@
         <v>19</v>
       </c>
       <c r="H37" s="30" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I37" s="31" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="44.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -5192,7 +5193,7 @@
         <v>99</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="I38" s="4" t="s">
         <v>507</v>
@@ -5220,7 +5221,7 @@
         <v>338</v>
       </c>
       <c r="H39" s="19" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="I39" s="24"/>
     </row>
@@ -5246,10 +5247,10 @@
         <v>338</v>
       </c>
       <c r="H40" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="I40" s="24" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="108" x14ac:dyDescent="0.25">
@@ -5276,7 +5277,7 @@
         <v>267</v>
       </c>
       <c r="H41" s="17" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="I41" s="23" t="s">
         <v>508</v>
@@ -5306,10 +5307,10 @@
         <v>133</v>
       </c>
       <c r="H42" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="I42" s="24" t="s">
         <v>564</v>
-      </c>
-      <c r="I42" s="24" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="87.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -5334,10 +5335,10 @@
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="17" t="s">
+        <v>565</v>
+      </c>
+      <c r="I43" s="24" t="s">
         <v>566</v>
-      </c>
-      <c r="I43" s="24" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="108" x14ac:dyDescent="0.25">
@@ -5364,7 +5365,7 @@
         <v>26</v>
       </c>
       <c r="H44" s="13" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="I44" s="4" t="s">
         <v>507</v>
@@ -5452,10 +5453,10 @@
         <v>33</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="I47" s="24" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5543,7 +5544,7 @@
         <v>526</v>
       </c>
       <c r="I50" s="24" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="84" x14ac:dyDescent="0.25">
@@ -5797,7 +5798,7 @@
         <v>393</v>
       </c>
       <c r="I59" s="24" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -5851,7 +5852,7 @@
         <v>397</v>
       </c>
       <c r="I61" s="24" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="252" x14ac:dyDescent="0.25">
@@ -5877,7 +5878,7 @@
         <v>396</v>
       </c>
       <c r="I62" s="24" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="96" x14ac:dyDescent="0.25">
@@ -5907,7 +5908,7 @@
         <v>529</v>
       </c>
       <c r="I63" s="24" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -5930,7 +5931,7 @@
       </c>
       <c r="G64" s="4"/>
       <c r="H64" s="13" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I64" s="24"/>
     </row>
@@ -5958,10 +5959,10 @@
         <v>154</v>
       </c>
       <c r="H65" s="19" t="s">
+        <v>576</v>
+      </c>
+      <c r="I65" s="24" t="s">
         <v>577</v>
-      </c>
-      <c r="I65" s="24" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -6135,7 +6136,7 @@
         <v>501</v>
       </c>
       <c r="I71" s="24" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -6310,7 +6311,7 @@
         <v>275</v>
       </c>
       <c r="H77" s="17" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I77" s="24"/>
     </row>
@@ -6368,7 +6369,7 @@
         <v>203</v>
       </c>
       <c r="H79" s="17" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I79" s="24"/>
     </row>
@@ -6459,7 +6460,7 @@
         <v>531</v>
       </c>
       <c r="I82" s="24" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -6542,7 +6543,7 @@
         <v>211</v>
       </c>
       <c r="H85" s="19" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="I85" s="23" t="s">
         <v>508</v>
@@ -6778,7 +6779,7 @@
         <v>218</v>
       </c>
       <c r="H93" s="17" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="I93" s="24"/>
     </row>
@@ -6809,7 +6810,7 @@
         <v>474</v>
       </c>
       <c r="I94" s="38" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="96.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -7006,7 +7007,7 @@
         <v>544</v>
       </c>
       <c r="H101" s="19" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="I101" s="24"/>
     </row>
@@ -7329,7 +7330,7 @@
         <v>478</v>
       </c>
       <c r="I112" s="24" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="24" x14ac:dyDescent="0.25">
@@ -7722,7 +7723,7 @@
         <v>225</v>
       </c>
       <c r="H126" s="19" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I126" s="24"/>
     </row>
@@ -7750,10 +7751,10 @@
         <v>228</v>
       </c>
       <c r="H127" s="17" t="s">
+        <v>593</v>
+      </c>
+      <c r="I127" s="23" t="s">
         <v>594</v>
-      </c>
-      <c r="I127" s="23" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="128" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
@@ -7834,7 +7835,7 @@
       </c>
       <c r="G130" s="4"/>
       <c r="H130" s="17" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="I130" s="23" t="s">
         <v>508</v>
@@ -7894,7 +7895,7 @@
         <v>139</v>
       </c>
       <c r="H132" s="13" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="I132" s="23" t="s">
         <v>507</v>
@@ -7927,7 +7928,7 @@
         <v>490</v>
       </c>
       <c r="I133" s="24" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="24" x14ac:dyDescent="0.25">
@@ -8044,7 +8045,7 @@
         <v>39</v>
       </c>
       <c r="H137" s="13" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="I137" s="4" t="s">
         <v>525</v>

</xml_diff>

<commit_message>
Traitement commentaire DDT74-14 (Périmetre d'étude)
</commit_message>
<xml_diff>
--- a/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
+++ b/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Geostandards-Risques\suivi\2024-05_06-Consultation-publique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E131303C-E28F-4B68-A2F9-E893DB3F3878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04872FCC-1C58-46F0-81AC-9641B65A0F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6765" yWindow="4785" windowWidth="21600" windowHeight="10395" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
+    <workbookView xWindow="3390" yWindow="420" windowWidth="21600" windowHeight="12630" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Synthese Modele Commun" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="603">
   <si>
     <t>Organisme</t>
   </si>
@@ -1312,9 +1312,6 @@
 A ce stade le standard s'appuie sur les nomenclatures et guides existants. Pour l'instant, pas d'aléa spécifique "effondrement de montagne"</t>
   </si>
   <si>
-    <t>Cela n'est effectivement pas prévu à part par défaut en déduisant les zones d'aléas du périmètre de procédure. Est-ce suffisant ?</t>
-  </si>
-  <si>
     <t>Le standard s'appuie sur la nomenclature des risques GASPAR. Est-ce que l'aléa "Glissement de terrain" correspond ?</t>
   </si>
   <si>
@@ -2100,9 +2097,6 @@
 Se rapprocher du BRNT =&gt; comment traiter ce type d'aléa.</t>
   </si>
   <si>
-    <t>Rajouter le périmètre d'étude en plus du périmètre administratif (Pour la référence au CE pour le périmètre mis à l'étude : cf article R562-2)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Voir avec le BIP et le BRNT pour la bonne classification </t>
   </si>
   <si>
@@ -2158,9 +2152,6 @@
     <t xml:space="preserve">OK sur le principe,
 Plutôt intégrer nomenclature PPRL dans celle des PPRN qui couvrira naturellement les PPRI
 </t>
-  </si>
-  <si>
-    <t>Fusionner nomenclatures PPRL et PPRN</t>
   </si>
   <si>
     <t xml:space="preserve">C'est un héritage du PPR Covadis.
@@ -2343,6 +2334,14 @@
   <si>
     <t>intégré 
 changer en zones + mentionner la référence aux espaces du guide PPRN;2016</t>
+  </si>
+  <si>
+    <t>Intégré
+Fusionner nomenclatures PPRL et PPRN</t>
+  </si>
+  <si>
+    <t>Cela n'est effectivement pas prévu à part par défaut en déduisant les zones d'aléas du périmètre de procédure. Est-ce suffisant ?
+=&gt; Rajouter le périmètre d'étude en plus du périmètre administratif (Pour la référence au CE pour le périmètre mis à l'étude : cf article R562-2)</t>
   </si>
 </sst>
 </file>
@@ -3490,7 +3489,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="72.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3520,7 +3519,7 @@
         <v>351</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="108" x14ac:dyDescent="0.25">
@@ -3547,10 +3546,10 @@
         <v>332</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="108" x14ac:dyDescent="0.25">
@@ -3580,7 +3579,7 @@
         <v>353</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3607,10 +3606,10 @@
         <v>305</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="89.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -3640,7 +3639,7 @@
         <v>350</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="24" x14ac:dyDescent="0.25">
@@ -3668,7 +3667,7 @@
         <v>352</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="96" x14ac:dyDescent="0.25">
@@ -3698,7 +3697,7 @@
         <v>357</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="144" x14ac:dyDescent="0.25">
@@ -3725,10 +3724,10 @@
         <v>335</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3758,7 +3757,7 @@
         <v>354</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -3788,7 +3787,7 @@
         <v>354</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="108" x14ac:dyDescent="0.25">
@@ -3815,10 +3814,10 @@
         <v>315</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3848,7 +3847,7 @@
         <v>355</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="96" x14ac:dyDescent="0.25">
@@ -3878,7 +3877,7 @@
         <v>356</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="60.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3908,7 +3907,7 @@
         <v>352</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3935,10 +3934,10 @@
         <v>288</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="77.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3968,7 +3967,7 @@
         <v>358</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="111" customHeight="1" x14ac:dyDescent="0.25">
@@ -3995,10 +3994,10 @@
         <v>293</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="96" x14ac:dyDescent="0.25">
@@ -4025,10 +4024,10 @@
         <v>328</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4056,7 +4055,7 @@
         <v>359</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
   </sheetData>
@@ -4072,8 +4071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815F14A-19BC-4DCE-8D31-81F595A4B0E7}">
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4116,7 +4115,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4141,10 +4140,10 @@
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="25" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4172,7 +4171,7 @@
         <v>370</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4200,7 +4199,7 @@
         <v>371</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4225,10 +4224,10 @@
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="22" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="132" x14ac:dyDescent="0.25">
@@ -4254,7 +4253,7 @@
         <v>372</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -4282,10 +4281,10 @@
         <v>373</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="84" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-14</v>
@@ -4307,10 +4306,10 @@
         <v>45</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>374</v>
-      </c>
-      <c r="I8" s="24" t="s">
-        <v>550</v>
+        <v>602</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4335,10 +4334,10 @@
         <v>47</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="72" x14ac:dyDescent="0.25">
@@ -4350,23 +4349,23 @@
         <v>1</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>535</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>536</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>537</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="4" t="s">
+        <v>537</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>538</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>539</v>
-      </c>
       <c r="H10" s="17" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4393,7 +4392,7 @@
         <v>263</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I11" s="24"/>
     </row>
@@ -4421,7 +4420,7 @@
         <v>172</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I12" s="24"/>
     </row>
@@ -4452,7 +4451,7 @@
         <v>350</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4479,10 +4478,10 @@
         <v>166</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="168" x14ac:dyDescent="0.25">
@@ -4509,10 +4508,10 @@
         <v>254</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="36" x14ac:dyDescent="0.25">
@@ -4539,10 +4538,10 @@
         <v>62</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -4569,10 +4568,10 @@
         <v>117</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -4599,10 +4598,10 @@
         <v>65</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="36" x14ac:dyDescent="0.25">
@@ -4629,10 +4628,10 @@
         <v>175</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="108" x14ac:dyDescent="0.25">
@@ -4659,10 +4658,10 @@
         <v>255</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="I20" s="23" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="84" x14ac:dyDescent="0.25">
@@ -4689,10 +4688,10 @@
         <v>256</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4719,10 +4718,10 @@
         <v>120</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="84" x14ac:dyDescent="0.25">
@@ -4749,10 +4748,10 @@
         <v>122</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -4779,10 +4778,10 @@
         <v>178</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -4809,10 +4808,10 @@
         <v>260</v>
       </c>
       <c r="H25" s="19" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="24" x14ac:dyDescent="0.25">
@@ -4839,10 +4838,10 @@
         <v>125</v>
       </c>
       <c r="H26" s="17" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="71.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4869,10 +4868,10 @@
         <v>72</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="I27" s="23" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="36" x14ac:dyDescent="0.25">
@@ -4902,7 +4901,7 @@
         <v>352</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -4927,10 +4926,10 @@
         <v>340</v>
       </c>
       <c r="H29" s="19" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="I29" s="24" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4957,10 +4956,10 @@
         <v>75</v>
       </c>
       <c r="H30" s="19" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="72" x14ac:dyDescent="0.25">
@@ -4987,10 +4986,10 @@
         <v>78</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="I31" s="23" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="84" x14ac:dyDescent="0.25">
@@ -5017,10 +5016,10 @@
         <v>128</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="I32" s="23" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="108" x14ac:dyDescent="0.25">
@@ -5047,10 +5046,10 @@
         <v>130</v>
       </c>
       <c r="H33" s="17" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I33" s="23" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -5075,10 +5074,10 @@
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="17" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="72" x14ac:dyDescent="0.25">
@@ -5105,10 +5104,10 @@
         <v>184</v>
       </c>
       <c r="H35" s="19" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I35" s="23" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="62.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5133,10 +5132,10 @@
         <v>82</v>
       </c>
       <c r="H36" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="32" customFormat="1" ht="84.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5163,10 +5162,10 @@
         <v>19</v>
       </c>
       <c r="H37" s="30" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="I37" s="31" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="44.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -5193,10 +5192,10 @@
         <v>99</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.25">
@@ -5215,13 +5214,13 @@
         <v>368</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>338</v>
       </c>
       <c r="H39" s="19" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="I39" s="24"/>
     </row>
@@ -5241,16 +5240,16 @@
         <v>368</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>338</v>
       </c>
       <c r="H40" s="19" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="I40" s="24" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="108" x14ac:dyDescent="0.25">
@@ -5277,13 +5276,13 @@
         <v>267</v>
       </c>
       <c r="H41" s="17" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="I41" s="23" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-8</v>
@@ -5307,13 +5306,13 @@
         <v>133</v>
       </c>
       <c r="H42" s="19" t="s">
-        <v>563</v>
-      </c>
-      <c r="I42" s="24" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="87.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="I42" s="23" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-12</v>
@@ -5335,10 +5334,10 @@
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="17" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="I43" s="24" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="108" x14ac:dyDescent="0.25">
@@ -5365,10 +5364,10 @@
         <v>26</v>
       </c>
       <c r="H44" s="13" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5395,10 +5394,10 @@
         <v>22</v>
       </c>
       <c r="H45" s="17" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -5423,10 +5422,10 @@
       </c>
       <c r="G46" s="4"/>
       <c r="H46" s="17" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -5453,10 +5452,10 @@
         <v>33</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="I47" s="24" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5483,7 +5482,7 @@
         <v>106</v>
       </c>
       <c r="H48" s="19" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I48" s="23"/>
     </row>
@@ -5511,10 +5510,10 @@
         <v>25</v>
       </c>
       <c r="H49" s="17" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="96" x14ac:dyDescent="0.25">
@@ -5541,10 +5540,10 @@
         <v>28</v>
       </c>
       <c r="H50" s="17" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="I50" s="24" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="84" x14ac:dyDescent="0.25">
@@ -5571,7 +5570,7 @@
         <v>14</v>
       </c>
       <c r="H51" s="13" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I51" s="4"/>
     </row>
@@ -5599,7 +5598,7 @@
         <v>142</v>
       </c>
       <c r="H52" s="17" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I52" s="24"/>
     </row>
@@ -5627,7 +5626,7 @@
         <v>143</v>
       </c>
       <c r="H53" s="17" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I53" s="24"/>
     </row>
@@ -5655,10 +5654,10 @@
         <v>145</v>
       </c>
       <c r="H54" s="17" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
@@ -5683,10 +5682,10 @@
         <v>86</v>
       </c>
       <c r="H55" s="17" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -5711,10 +5710,10 @@
         <v>87</v>
       </c>
       <c r="H56" s="17" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="72" x14ac:dyDescent="0.25">
@@ -5739,10 +5738,10 @@
       </c>
       <c r="G57" s="4"/>
       <c r="H57" s="17" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -5769,10 +5768,10 @@
         <v>187</v>
       </c>
       <c r="H58" s="17" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="216" x14ac:dyDescent="0.25">
@@ -5795,10 +5794,10 @@
       </c>
       <c r="G59" s="4"/>
       <c r="H59" s="19" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I59" s="24" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -5825,7 +5824,7 @@
         <v>148</v>
       </c>
       <c r="H60" s="19" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I60" s="24"/>
     </row>
@@ -5849,10 +5848,10 @@
       </c>
       <c r="G61" s="4"/>
       <c r="H61" s="19" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="I61" s="24" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="252" x14ac:dyDescent="0.25">
@@ -5875,10 +5874,10 @@
       </c>
       <c r="G62" s="4"/>
       <c r="H62" s="13" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I62" s="24" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="96" x14ac:dyDescent="0.25">
@@ -5905,10 +5904,10 @@
         <v>151</v>
       </c>
       <c r="H63" s="19" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I63" s="24" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -5931,7 +5930,7 @@
       </c>
       <c r="G64" s="4"/>
       <c r="H64" s="13" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="I64" s="24"/>
     </row>
@@ -5959,10 +5958,10 @@
         <v>154</v>
       </c>
       <c r="H65" s="19" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="I65" s="24" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -5989,10 +5988,10 @@
         <v>50</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -6019,10 +6018,10 @@
         <v>53</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="I67" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="195" x14ac:dyDescent="0.25">
@@ -6049,7 +6048,7 @@
         <v>270</v>
       </c>
       <c r="H68" s="17" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I68" s="24"/>
     </row>
@@ -6077,7 +6076,7 @@
         <v>241</v>
       </c>
       <c r="H69" s="17" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I69" s="24"/>
     </row>
@@ -6105,7 +6104,7 @@
         <v>271</v>
       </c>
       <c r="H70" s="17" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="I70" s="24"/>
     </row>
@@ -6133,10 +6132,10 @@
         <v>272</v>
       </c>
       <c r="H71" s="17" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="I71" s="24" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -6163,10 +6162,10 @@
         <v>197</v>
       </c>
       <c r="H72" s="17" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="36" x14ac:dyDescent="0.25">
@@ -6178,25 +6177,25 @@
         <v>14</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E73" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="F73" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="F73" s="4" t="s">
+      <c r="G73" s="4" t="s">
         <v>431</v>
       </c>
-      <c r="G73" s="4" t="s">
-        <v>432</v>
-      </c>
       <c r="H73" s="19" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="24" x14ac:dyDescent="0.25">
@@ -6208,25 +6207,25 @@
         <v>19</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E74" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="F74" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="F74" s="4" t="s">
+      <c r="G74" s="4" t="s">
         <v>431</v>
       </c>
-      <c r="G74" s="4" t="s">
-        <v>432</v>
-      </c>
       <c r="H74" s="17" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="24" x14ac:dyDescent="0.25">
@@ -6238,25 +6237,25 @@
         <v>16</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F75" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="G75" s="4" t="s">
         <v>431</v>
       </c>
-      <c r="G75" s="4" t="s">
-        <v>432</v>
-      </c>
       <c r="H75" s="17" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I75" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6283,7 +6282,7 @@
         <v>273</v>
       </c>
       <c r="H76" s="17" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="I76" s="23"/>
     </row>
@@ -6311,7 +6310,7 @@
         <v>275</v>
       </c>
       <c r="H77" s="17" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="I77" s="24"/>
     </row>
@@ -6324,25 +6323,25 @@
         <v>2</v>
       </c>
       <c r="C78" s="4" t="s">
+        <v>535</v>
+      </c>
+      <c r="D78" s="5" t="s">
         <v>536</v>
       </c>
-      <c r="D78" s="5" t="s">
-        <v>537</v>
-      </c>
       <c r="E78" s="5" t="s">
+        <v>539</v>
+      </c>
+      <c r="F78" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="F78" s="4" t="s">
+      <c r="G78" s="4" t="s">
         <v>541</v>
       </c>
-      <c r="G78" s="4" t="s">
-        <v>542</v>
-      </c>
       <c r="H78" s="17" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -6369,7 +6368,7 @@
         <v>203</v>
       </c>
       <c r="H79" s="17" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="I79" s="24"/>
     </row>
@@ -6382,25 +6381,25 @@
         <v>22</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E80" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>456</v>
+      </c>
+      <c r="G80" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="F80" s="4" t="s">
-        <v>457</v>
-      </c>
-      <c r="G80" s="4" t="s">
-        <v>446</v>
-      </c>
       <c r="H80" s="19" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="27" x14ac:dyDescent="0.25">
@@ -6412,25 +6411,25 @@
         <v>23</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H81" s="17" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I81" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -6442,25 +6441,25 @@
         <v>24</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E82" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="G82" s="4" t="s">
         <v>448</v>
       </c>
-      <c r="F82" s="4" t="s">
-        <v>459</v>
-      </c>
-      <c r="G82" s="4" t="s">
-        <v>449</v>
-      </c>
       <c r="H82" s="13" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="I82" s="24" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -6487,7 +6486,7 @@
         <v>206</v>
       </c>
       <c r="H83" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="I83" s="24"/>
     </row>
@@ -6515,7 +6514,7 @@
         <v>209</v>
       </c>
       <c r="H84" s="17" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="I84" s="24"/>
     </row>
@@ -6543,10 +6542,10 @@
         <v>211</v>
       </c>
       <c r="H85" s="19" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="I85" s="23" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="36" x14ac:dyDescent="0.25">
@@ -6573,10 +6572,10 @@
         <v>213</v>
       </c>
       <c r="H86" s="17" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I86" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -6588,25 +6587,25 @@
         <v>27</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E87" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="G87" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="F87" s="4" t="s">
-        <v>461</v>
-      </c>
-      <c r="G87" s="4" t="s">
-        <v>455</v>
-      </c>
       <c r="H87" s="19" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -6633,10 +6632,10 @@
         <v>216</v>
       </c>
       <c r="H88" s="19" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -6648,25 +6647,25 @@
         <v>26</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G89" s="4" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H89" s="19" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="I89" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -6693,10 +6692,10 @@
         <v>157</v>
       </c>
       <c r="H90" s="17" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I90" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="36" x14ac:dyDescent="0.25">
@@ -6721,10 +6720,10 @@
         <v>91</v>
       </c>
       <c r="H91" s="17" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="I91" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="77.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6749,10 +6748,10 @@
       </c>
       <c r="G92" s="4"/>
       <c r="H92" s="13" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="I92" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -6779,7 +6778,7 @@
         <v>218</v>
       </c>
       <c r="H93" s="17" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="I93" s="24"/>
     </row>
@@ -6807,10 +6806,10 @@
         <v>278</v>
       </c>
       <c r="H94" s="37" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="I94" s="38" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="96.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -6837,10 +6836,10 @@
         <v>279</v>
       </c>
       <c r="H95" s="21" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I95" s="4" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="113.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -6867,10 +6866,10 @@
         <v>259</v>
       </c>
       <c r="H96" s="17" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I96" s="23" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6897,7 +6896,7 @@
         <v>113</v>
       </c>
       <c r="H97" s="17" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="I97" s="23"/>
     </row>
@@ -6979,10 +6978,10 @@
       </c>
       <c r="G100" s="4"/>
       <c r="H100" s="19" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="I100" s="4" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="72" x14ac:dyDescent="0.25">
@@ -6994,20 +6993,20 @@
         <v>3</v>
       </c>
       <c r="C101" s="4" t="s">
+        <v>535</v>
+      </c>
+      <c r="D101" s="5" t="s">
         <v>536</v>
-      </c>
-      <c r="D101" s="5" t="s">
-        <v>537</v>
       </c>
       <c r="E101" s="5"/>
       <c r="F101" s="4" t="s">
+        <v>542</v>
+      </c>
+      <c r="G101" s="4" t="s">
         <v>543</v>
       </c>
-      <c r="G101" s="4" t="s">
-        <v>544</v>
-      </c>
       <c r="H101" s="19" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="I101" s="24"/>
     </row>
@@ -7020,25 +7019,25 @@
         <v>15</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D102" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E102" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="F102" s="4" t="s">
         <v>433</v>
       </c>
-      <c r="F102" s="4" t="s">
+      <c r="G102" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="G102" s="4" t="s">
-        <v>435</v>
-      </c>
       <c r="H102" s="17" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="I102" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -7050,25 +7049,25 @@
         <v>1</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D103" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E103" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="F103" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="F103" s="4" t="s">
+      <c r="G103" s="4" t="s">
         <v>402</v>
-      </c>
-      <c r="G103" s="4" t="s">
-        <v>403</v>
       </c>
       <c r="H103" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I103" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="24" x14ac:dyDescent="0.25">
@@ -7080,25 +7079,25 @@
         <v>17</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D104" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F104" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="G104" s="4" t="s">
         <v>437</v>
       </c>
-      <c r="G104" s="4" t="s">
-        <v>438</v>
-      </c>
       <c r="H104" s="17" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="I104" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="24" x14ac:dyDescent="0.25">
@@ -7110,25 +7109,25 @@
         <v>20</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D105" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F105" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="G105" s="4" t="s">
         <v>442</v>
       </c>
-      <c r="G105" s="4" t="s">
-        <v>443</v>
-      </c>
       <c r="H105" s="17" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="I105" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="106" spans="1:9" ht="39" x14ac:dyDescent="0.25">
@@ -7140,22 +7139,22 @@
         <v>21</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D106" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G106" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H106" s="19" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="I106" s="24"/>
     </row>
@@ -7168,25 +7167,25 @@
         <v>18</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D107" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E107" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="F107" s="4" t="s">
         <v>439</v>
       </c>
-      <c r="F107" s="4" t="s">
+      <c r="G107" s="4" t="s">
         <v>440</v>
       </c>
-      <c r="G107" s="4" t="s">
-        <v>441</v>
-      </c>
       <c r="H107" s="13" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I107" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="108" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -7198,25 +7197,25 @@
         <v>25</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D108" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E108" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="F108" s="4" t="s">
         <v>450</v>
       </c>
-      <c r="F108" s="4" t="s">
+      <c r="G108" s="4" t="s">
         <v>451</v>
       </c>
-      <c r="G108" s="4" t="s">
-        <v>452</v>
-      </c>
       <c r="H108" s="17" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="I108" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="24" x14ac:dyDescent="0.25">
@@ -7228,19 +7227,19 @@
         <v>2</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D109" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E109" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="F109" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="F109" s="4" t="s">
+      <c r="G109" s="4" t="s">
         <v>405</v>
-      </c>
-      <c r="G109" s="4" t="s">
-        <v>406</v>
       </c>
       <c r="H109" s="17" t="s">
         <v>352</v>
@@ -7256,19 +7255,19 @@
         <v>3</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D110" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E110" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="F110" s="4" t="s">
         <v>407</v>
       </c>
-      <c r="F110" s="4" t="s">
+      <c r="G110" s="4" t="s">
         <v>408</v>
-      </c>
-      <c r="G110" s="4" t="s">
-        <v>409</v>
       </c>
       <c r="H110" s="17" t="s">
         <v>352</v>
@@ -7284,19 +7283,19 @@
         <v>4</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D111" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E111" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="F111" s="4" t="s">
         <v>407</v>
       </c>
-      <c r="F111" s="4" t="s">
-        <v>408</v>
-      </c>
       <c r="G111" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="H111" s="17" t="s">
         <v>352</v>
@@ -7327,10 +7326,10 @@
         <v>250</v>
       </c>
       <c r="H112" s="6" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="I112" s="24" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="24" x14ac:dyDescent="0.25">
@@ -7342,19 +7341,19 @@
         <v>5</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D113" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E113" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="F113" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="F113" s="4" t="s">
+      <c r="G113" s="4" t="s">
         <v>412</v>
-      </c>
-      <c r="G113" s="4" t="s">
-        <v>413</v>
       </c>
       <c r="H113" s="17" t="s">
         <v>352</v>
@@ -7370,19 +7369,19 @@
         <v>6</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D114" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E114" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="F114" s="4" t="s">
         <v>414</v>
       </c>
-      <c r="F114" s="4" t="s">
+      <c r="G114" s="4" t="s">
         <v>415</v>
-      </c>
-      <c r="G114" s="4" t="s">
-        <v>416</v>
       </c>
       <c r="H114" s="17" t="s">
         <v>352</v>
@@ -7398,19 +7397,19 @@
         <v>7</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D115" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G115" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H115" s="17" t="s">
         <v>352</v>
@@ -7426,19 +7425,19 @@
         <v>8</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D116" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E116" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="F116" s="4" t="s">
         <v>418</v>
       </c>
-      <c r="F116" s="4" t="s">
-        <v>419</v>
-      </c>
       <c r="G116" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H116" s="17" t="s">
         <v>352</v>
@@ -7454,19 +7453,19 @@
         <v>9</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D117" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F117" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G117" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H117" s="17" t="s">
         <v>352</v>
@@ -7482,22 +7481,22 @@
         <v>10</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D118" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F118" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="G118" s="4" t="s">
         <v>420</v>
       </c>
-      <c r="G118" s="4" t="s">
-        <v>421</v>
-      </c>
       <c r="H118" s="17" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="I118" s="24"/>
     </row>
@@ -7510,25 +7509,25 @@
         <v>11</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D119" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E119" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F119" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="G119" s="4" t="s">
         <v>422</v>
       </c>
-      <c r="G119" s="4" t="s">
-        <v>423</v>
-      </c>
       <c r="H119" s="13" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I119" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="120" spans="1:9" ht="24" x14ac:dyDescent="0.25">
@@ -7540,19 +7539,19 @@
         <v>12</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D120" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E120" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="F120" s="4" t="s">
         <v>424</v>
       </c>
-      <c r="F120" s="4" t="s">
+      <c r="G120" s="4" t="s">
         <v>425</v>
-      </c>
-      <c r="G120" s="4" t="s">
-        <v>426</v>
       </c>
       <c r="H120" s="17" t="s">
         <v>352</v>
@@ -7568,19 +7567,19 @@
         <v>13</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D121" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E121" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="F121" s="4" t="s">
         <v>427</v>
       </c>
-      <c r="F121" s="4" t="s">
+      <c r="G121" s="4" t="s">
         <v>428</v>
-      </c>
-      <c r="G121" s="4" t="s">
-        <v>429</v>
       </c>
       <c r="H121" s="17" t="s">
         <v>352</v>
@@ -7611,7 +7610,7 @@
         <v>29</v>
       </c>
       <c r="H122" s="19" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I122" s="24"/>
     </row>
@@ -7639,7 +7638,7 @@
         <v>252</v>
       </c>
       <c r="H123" s="19" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="I123" s="24"/>
     </row>
@@ -7667,7 +7666,7 @@
         <v>104</v>
       </c>
       <c r="H124" s="19" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="I124" s="24"/>
     </row>
@@ -7695,7 +7694,7 @@
         <v>162</v>
       </c>
       <c r="H125" s="19" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I125" s="24"/>
     </row>
@@ -7723,7 +7722,7 @@
         <v>225</v>
       </c>
       <c r="H126" s="19" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="I126" s="24"/>
     </row>
@@ -7751,10 +7750,10 @@
         <v>228</v>
       </c>
       <c r="H127" s="17" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="I127" s="23" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="128" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
@@ -7781,10 +7780,10 @@
         <v>10</v>
       </c>
       <c r="H128" s="17" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="I128" s="23" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="129" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -7809,7 +7808,7 @@
       </c>
       <c r="G129" s="4"/>
       <c r="H129" s="19" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I129" s="24"/>
     </row>
@@ -7835,10 +7834,10 @@
       </c>
       <c r="G130" s="4"/>
       <c r="H130" s="17" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="I130" s="23" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="131" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -7865,10 +7864,10 @@
         <v>136</v>
       </c>
       <c r="H131" s="17" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="I131" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="132" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -7895,10 +7894,10 @@
         <v>139</v>
       </c>
       <c r="H132" s="13" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="I132" s="23" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="133" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -7925,10 +7924,10 @@
         <v>231</v>
       </c>
       <c r="H133" s="17" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I133" s="24" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="24" x14ac:dyDescent="0.25">
@@ -7958,7 +7957,7 @@
         <v>352</v>
       </c>
       <c r="I134" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="24" x14ac:dyDescent="0.25">
@@ -7988,7 +7987,7 @@
         <v>352</v>
       </c>
       <c r="I135" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -8015,10 +8014,10 @@
         <v>37</v>
       </c>
       <c r="H136" s="13" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I136" s="4" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="137" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -8045,10 +8044,10 @@
         <v>39</v>
       </c>
       <c r="H137" s="13" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="I137" s="4" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="138" spans="1:9" ht="72" x14ac:dyDescent="0.25">
@@ -8075,10 +8074,10 @@
         <v>41</v>
       </c>
       <c r="H138" s="19" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I138" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="139" spans="1:9" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -8103,10 +8102,10 @@
       </c>
       <c r="G139" s="4"/>
       <c r="H139" s="13" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="I139" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="140" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -8133,10 +8132,10 @@
         <v>43</v>
       </c>
       <c r="H140" s="17" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I140" s="23" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="141" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -8163,10 +8162,10 @@
         <v>31</v>
       </c>
       <c r="H141" s="13" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="I141" s="23" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Traitement DDT 31-2 et DDT 31-3 (Niveau aléa "Autre")
</commit_message>
<xml_diff>
--- a/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
+++ b/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Geostandards-Risques\suivi\2024-05_06-Consultation-publique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04872FCC-1C58-46F0-81AC-9641B65A0F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3F1DD7-96A9-4181-8559-CD8012E268AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3390" yWindow="420" windowWidth="21600" windowHeight="12630" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
+    <workbookView xWindow="5400" yWindow="1110" windowWidth="21600" windowHeight="12630" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Synthese Modele Commun" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="603">
   <si>
     <t>Organisme</t>
   </si>
@@ -2141,14 +2141,6 @@
 Libellé : à utiliser pour les anciens PPR (Inondation)</t>
   </si>
   <si>
-    <t>A faire remonter au BRNT (à minima par la liste du GT)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A discuter avec le GT et les demandeurs
-Utilisation de "Autre" mais Libellé différent à proposer (non couvert par la classification proposée des niveaux d'aléas, à utiliser de manière exceptionnelle).
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">OK sur le principe,
 Plutôt intégrer nomenclature PPRL dans celle des PPRN qui couvrira naturellement les PPRI
 </t>
@@ -2342,6 +2334,14 @@
   <si>
     <t>Cela n'est effectivement pas prévu à part par défaut en déduisant les zones d'aléas du périmètre de procédure. Est-ce suffisant ?
 =&gt; Rajouter le périmètre d'étude en plus du périmètre administratif (Pour la référence au CE pour le périmètre mis à l'étude : cf article R562-2)</t>
+  </si>
+  <si>
+    <t>intégré : niveau aléa autre</t>
+  </si>
+  <si>
+    <t>A discuter avec le GT et les demandeurs
+Utilisation de "Autre" mais Libellé différent à proposer (non couvert par la classification proposée des niveaux d'aléas, à utiliser de manière exceptionnelle).
+A faire remonter au BRNT (à minima par la liste du GT)</t>
   </si>
 </sst>
 </file>
@@ -3724,10 +3724,10 @@
         <v>335</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4024,10 +4024,10 @@
         <v>328</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4071,8 +4071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815F14A-19BC-4DCE-8D31-81F595A4B0E7}">
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4306,7 +4306,7 @@
         <v>45</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="I8" s="23" t="s">
         <v>507</v>
@@ -4658,7 +4658,7 @@
         <v>255</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="I20" s="23" t="s">
         <v>507</v>
@@ -4748,10 +4748,10 @@
         <v>122</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -4986,7 +4986,7 @@
         <v>78</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="I31" s="23" t="s">
         <v>507</v>
@@ -5016,7 +5016,7 @@
         <v>128</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="I32" s="23" t="s">
         <v>507</v>
@@ -5049,7 +5049,7 @@
         <v>384</v>
       </c>
       <c r="I33" s="23" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -5222,7 +5222,9 @@
       <c r="H39" s="19" t="s">
         <v>558</v>
       </c>
-      <c r="I39" s="24"/>
+      <c r="I39" s="23" t="s">
+        <v>601</v>
+      </c>
     </row>
     <row r="40" spans="1:9" ht="228" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="str">
@@ -5246,10 +5248,10 @@
         <v>338</v>
       </c>
       <c r="H40" s="19" t="s">
-        <v>560</v>
-      </c>
-      <c r="I40" s="24" t="s">
-        <v>559</v>
+        <v>602</v>
+      </c>
+      <c r="I40" s="23" t="s">
+        <v>601</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="108" x14ac:dyDescent="0.25">
@@ -5306,10 +5308,10 @@
         <v>133</v>
       </c>
       <c r="H42" s="19" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="I42" s="23" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5334,10 +5336,10 @@
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="17" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="I43" s="24" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="108" x14ac:dyDescent="0.25">
@@ -5364,7 +5366,7 @@
         <v>26</v>
       </c>
       <c r="H44" s="13" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="I44" s="4" t="s">
         <v>506</v>
@@ -5452,10 +5454,10 @@
         <v>33</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="I47" s="24" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5543,7 +5545,7 @@
         <v>525</v>
       </c>
       <c r="I50" s="24" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="84" x14ac:dyDescent="0.25">
@@ -5797,7 +5799,7 @@
         <v>392</v>
       </c>
       <c r="I59" s="24" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -5851,7 +5853,7 @@
         <v>396</v>
       </c>
       <c r="I61" s="24" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="252" x14ac:dyDescent="0.25">
@@ -5877,7 +5879,7 @@
         <v>395</v>
       </c>
       <c r="I62" s="24" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="96" x14ac:dyDescent="0.25">
@@ -5907,7 +5909,7 @@
         <v>528</v>
       </c>
       <c r="I63" s="24" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -5930,7 +5932,7 @@
       </c>
       <c r="G64" s="4"/>
       <c r="H64" s="13" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="I64" s="24"/>
     </row>
@@ -5958,10 +5960,10 @@
         <v>154</v>
       </c>
       <c r="H65" s="19" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="I65" s="24" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -6135,7 +6137,7 @@
         <v>500</v>
       </c>
       <c r="I71" s="24" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -6310,7 +6312,7 @@
         <v>275</v>
       </c>
       <c r="H77" s="17" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="I77" s="24"/>
     </row>
@@ -6368,7 +6370,7 @@
         <v>203</v>
       </c>
       <c r="H79" s="17" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="I79" s="24"/>
     </row>
@@ -6459,7 +6461,7 @@
         <v>530</v>
       </c>
       <c r="I82" s="24" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -6542,7 +6544,7 @@
         <v>211</v>
       </c>
       <c r="H85" s="19" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="I85" s="23" t="s">
         <v>507</v>
@@ -6778,7 +6780,7 @@
         <v>218</v>
       </c>
       <c r="H93" s="17" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="I93" s="24"/>
     </row>
@@ -6809,7 +6811,7 @@
         <v>473</v>
       </c>
       <c r="I94" s="38" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="96.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -7006,7 +7008,7 @@
         <v>543</v>
       </c>
       <c r="H101" s="19" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="I101" s="24"/>
     </row>
@@ -7329,7 +7331,7 @@
         <v>477</v>
       </c>
       <c r="I112" s="24" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="24" x14ac:dyDescent="0.25">
@@ -7722,7 +7724,7 @@
         <v>225</v>
       </c>
       <c r="H126" s="19" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="I126" s="24"/>
     </row>
@@ -7750,10 +7752,10 @@
         <v>228</v>
       </c>
       <c r="H127" s="17" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="I127" s="23" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="128" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
@@ -7834,7 +7836,7 @@
       </c>
       <c r="G130" s="4"/>
       <c r="H130" s="17" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="I130" s="23" t="s">
         <v>507</v>
@@ -7894,7 +7896,7 @@
         <v>139</v>
       </c>
       <c r="H132" s="13" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="I132" s="23" t="s">
         <v>506</v>
@@ -7927,7 +7929,7 @@
         <v>489</v>
       </c>
       <c r="I133" s="24" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="24" x14ac:dyDescent="0.25">
@@ -8044,7 +8046,7 @@
         <v>39</v>
       </c>
       <c r="H137" s="13" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="I137" s="4" t="s">
         <v>524</v>

</xml_diff>

<commit_message>
Traitement DGPR/SRNH/SdcAP/BRIL-19 (Enjeu "Autre")
</commit_message>
<xml_diff>
--- a/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
+++ b/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Geostandards-Risques\suivi\2024-05_06-Consultation-publique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3F1DD7-96A9-4181-8559-CD8012E268AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29E5259-12CE-4A81-B25E-BDF9099F6B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5400" yWindow="1110" windowWidth="21600" windowHeight="12630" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="604">
   <si>
     <t>Organisme</t>
   </si>
@@ -2342,6 +2342,9 @@
     <t>A discuter avec le GT et les demandeurs
 Utilisation de "Autre" mais Libellé différent à proposer (non couvert par la classification proposée des niveaux d'aléas, à utiliser de manière exceptionnelle).
 A faire remonter au BRNT (à minima par la liste du GT)</t>
+  </si>
+  <si>
+    <t>intgégré</t>
   </si>
 </sst>
 </file>
@@ -4071,8 +4074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815F14A-19BC-4DCE-8D31-81F595A4B0E7}">
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A129" sqref="A129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4907,9 +4910,11 @@
     <row r="29" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DDT 31-</v>
-      </c>
-      <c r="B29" s="1"/>
+        <v>DDT 31-1</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
       <c r="C29" s="4" t="s">
         <v>337</v>
       </c>
@@ -5201,9 +5206,11 @@
     <row r="39" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DDT 31-</v>
-      </c>
-      <c r="B39" s="1"/>
+        <v>DDT 31-2</v>
+      </c>
+      <c r="B39" s="1">
+        <v>2</v>
+      </c>
       <c r="C39" s="4" t="s">
         <v>337</v>
       </c>
@@ -5229,9 +5236,11 @@
     <row r="40" spans="1:9" ht="228" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>DDT 31-</v>
-      </c>
-      <c r="B40" s="1"/>
+        <v>DDT 31-3</v>
+      </c>
+      <c r="B40" s="1">
+        <v>3</v>
+      </c>
       <c r="C40" s="4" t="s">
         <v>337</v>
       </c>
@@ -5779,9 +5788,11 @@
     <row r="59" spans="1:9" ht="216" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>CEREMA/DTerHdF/ASQT/MET -</v>
-      </c>
-      <c r="B59" s="1"/>
+        <v>CEREMA/DTerHdF/ASQT/MET -1</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1</v>
+      </c>
       <c r="C59" s="15" t="s">
         <v>341</v>
       </c>
@@ -5833,9 +5844,11 @@
     <row r="61" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>CEREMA/DTerHdF/ASQT/MET -</v>
-      </c>
-      <c r="B61" s="1"/>
+        <v>CEREMA/DTerHdF/ASQT/MET -2</v>
+      </c>
+      <c r="B61" s="1">
+        <v>2</v>
+      </c>
       <c r="C61" s="15" t="s">
         <v>341</v>
       </c>
@@ -5859,9 +5872,11 @@
     <row r="62" spans="1:9" ht="252" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>CEREMA/DTerHdF/ASQT/MET -</v>
-      </c>
-      <c r="B62" s="1"/>
+        <v>CEREMA/DTerHdF/ASQT/MET -3</v>
+      </c>
+      <c r="B62" s="1">
+        <v>3</v>
+      </c>
       <c r="C62" s="15" t="s">
         <v>341</v>
       </c>
@@ -5915,9 +5930,11 @@
     <row r="64" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
-        <v>CEREMA/DTerHdF/ASQT/MET -</v>
-      </c>
-      <c r="B64" s="1"/>
+        <v>CEREMA/DTerHdF/ASQT/MET -4</v>
+      </c>
+      <c r="B64" s="1">
+        <v>4</v>
+      </c>
       <c r="C64" s="15" t="s">
         <v>341</v>
       </c>
@@ -7812,7 +7829,9 @@
       <c r="H129" s="19" t="s">
         <v>487</v>
       </c>
-      <c r="I129" s="24"/>
+      <c r="I129" s="23" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="130" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="str">

</xml_diff>

<commit_message>
traitement commentaires :DDT88-15, DDT38-25, DDT74-6; DDT01-2, BRNT-23 et Cerema-20 (multirisques)
</commit_message>
<xml_diff>
--- a/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
+++ b/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Geostandards-Risques\suivi\2024-05_06-Consultation-publique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29E5259-12CE-4A81-B25E-BDF9099F6B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8352BC-3867-4F13-9481-CF5E4C3533D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="1110" windowWidth="21600" windowHeight="12630" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
+    <workbookView xWindow="-26520" yWindow="2280" windowWidth="21600" windowHeight="11265" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Synthese Modele Commun" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="607">
   <si>
     <t>Organisme</t>
   </si>
@@ -2345,6 +2345,15 @@
   </si>
   <si>
     <t>intgégré</t>
+  </si>
+  <si>
+    <t>intégré (couche de synthèse des aléas)</t>
+  </si>
+  <si>
+    <t>intégré (mention des PPRL dans l'annexe multirisques)</t>
+  </si>
+  <si>
+    <t>intégré (mention des PPRT dans l'annexe multirisques et couche de synthèse PPRT pour les aléas techno multiples)</t>
   </si>
 </sst>
 </file>
@@ -3452,21 +3461,21 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="3" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" style="3" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" style="3" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="21.81640625" style="3" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="3" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="49.5703125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="47.5703125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="54.85546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="10.85546875" style="3"/>
+    <col min="5" max="5" width="16.1796875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="49.54296875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="47.54296875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="54.81640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="21.453125" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="10.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>349</v>
       </c>
@@ -3495,7 +3504,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="72.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="73" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-1</v>
@@ -3525,7 +3534,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="108" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-2</v>
@@ -3555,7 +3564,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="108" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-3</v>
@@ -3585,7 +3594,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="75.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-4</v>
@@ -3615,7 +3624,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="89.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="89.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-5</v>
@@ -3645,7 +3654,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/DAPP/BIP-11</v>
@@ -3673,7 +3682,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="96" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-6</v>
@@ -3703,7 +3712,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="144" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="126.5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-7</v>
@@ -3733,7 +3742,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-1</v>
@@ -3763,7 +3772,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-2</v>
@@ -3793,7 +3802,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="108" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-8</v>
@@ -3823,7 +3832,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>cerema-6</v>
@@ -3853,7 +3862,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="96" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-9</v>
@@ -3883,7 +3892,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="60.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="61" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-10</v>
@@ -3913,7 +3922,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="68.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-3</v>
@@ -3943,7 +3952,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="77.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="77.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-4</v>
@@ -3973,7 +3982,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="111" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="111" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-5</v>
@@ -4003,7 +4012,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="96" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SDCAP/PONSOH-13</v>
@@ -4033,7 +4042,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/DAPP/BIP-12</v>
@@ -4074,25 +4083,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815F14A-19BC-4DCE-8D31-81F595A4B0E7}">
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A129" sqref="A129"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I133" sqref="I133"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="3.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="3.81640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="3" customWidth="1"/>
     <col min="4" max="4" width="16" style="3" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="44.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="44.1796875" style="3" customWidth="1"/>
     <col min="7" max="7" width="38" style="3" customWidth="1"/>
-    <col min="8" max="8" width="51.85546875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="10.85546875" style="3"/>
+    <col min="8" max="8" width="51.81640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="22.26953125" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="10.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>348</v>
       </c>
@@ -4121,7 +4130,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-2</v>
@@ -4149,7 +4158,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-3</v>
@@ -4177,7 +4186,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-4</v>
@@ -4205,7 +4214,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="65.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-5</v>
@@ -4233,7 +4242,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="132" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="126.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP-0</v>
@@ -4259,7 +4268,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-9</v>
@@ -4287,7 +4296,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="84" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-14</v>
@@ -4315,7 +4324,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-15</v>
@@ -4343,7 +4352,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDTM11-1</v>
@@ -4371,7 +4380,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-2</v>
@@ -4399,7 +4408,7 @@
       </c>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" spans="1:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-3</v>
@@ -4427,7 +4436,7 @@
       </c>
       <c r="I12" s="24"/>
     </row>
-    <row r="13" spans="1:9" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-1</v>
@@ -4457,7 +4466,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="66.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-1</v>
@@ -4487,7 +4496,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="168" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="161" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-2</v>
@@ -4517,7 +4526,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-3</v>
@@ -4547,7 +4556,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-1</v>
@@ -4577,7 +4586,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-4</v>
@@ -4607,7 +4616,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-4</v>
@@ -4637,7 +4646,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="108" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-5</v>
@@ -4667,7 +4676,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="84" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-6</v>
@@ -4697,7 +4706,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-2</v>
@@ -4727,7 +4736,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="84" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-3</v>
@@ -4757,7 +4766,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-5</v>
@@ -4787,7 +4796,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-4</v>
@@ -4817,7 +4826,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-5</v>
@@ -4847,7 +4856,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="71.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="71.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-7</v>
@@ -4877,7 +4886,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-6</v>
@@ -4907,7 +4916,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="115" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-1</v>
@@ -4937,7 +4946,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-8</v>
@@ -4967,7 +4976,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-9</v>
@@ -4997,7 +5006,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="84" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-6</v>
@@ -5027,7 +5036,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="108" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-7</v>
@@ -5057,7 +5066,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="41.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-10</v>
@@ -5085,7 +5094,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-7</v>
@@ -5115,7 +5124,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="62.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="62.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-11</v>
@@ -5143,7 +5152,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="32" customFormat="1" ht="84.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" s="32" customFormat="1" ht="81" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="26" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-1</v>
@@ -5173,7 +5182,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="44.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="44.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-21</v>
@@ -5203,7 +5212,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-2</v>
@@ -5233,7 +5242,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="228" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="207" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-3</v>
@@ -5263,7 +5272,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="108" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-8</v>
@@ -5293,7 +5302,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-8</v>
@@ -5323,7 +5332,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="111.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-12</v>
@@ -5351,7 +5360,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="108" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-4</v>
@@ -5381,7 +5390,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="77.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-2</v>
@@ -5411,7 +5420,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/BRNT-22</v>
@@ -5439,7 +5448,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-8</v>
@@ -5469,7 +5478,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-24</v>
@@ -5497,7 +5506,7 @@
       </c>
       <c r="I48" s="23"/>
     </row>
-    <row r="49" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-3</v>
@@ -5527,7 +5536,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="96" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-5</v>
@@ -5557,7 +5566,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="84" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT07-2</v>
@@ -5585,7 +5594,7 @@
       </c>
       <c r="I51" s="4"/>
     </row>
-    <row r="52" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-11</v>
@@ -5613,7 +5622,7 @@
       </c>
       <c r="I52" s="24"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-12</v>
@@ -5641,7 +5650,7 @@
       </c>
       <c r="I53" s="24"/>
     </row>
-    <row r="54" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-13</v>
@@ -5671,7 +5680,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-13</v>
@@ -5699,7 +5708,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-14</v>
@@ -5727,7 +5736,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-15</v>
@@ -5755,7 +5764,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-9</v>
@@ -5785,7 +5794,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="216" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="184" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -1</v>
@@ -5813,7 +5822,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-14</v>
@@ -5841,7 +5850,7 @@
       </c>
       <c r="I60" s="24"/>
     </row>
-    <row r="61" spans="1:9" ht="108" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -2</v>
@@ -5869,7 +5878,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="252" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="230" x14ac:dyDescent="0.35">
       <c r="A62" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -3</v>
@@ -5897,7 +5906,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="96" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-15</v>
@@ -5927,7 +5936,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A64" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -4</v>
@@ -5953,7 +5962,7 @@
       </c>
       <c r="I64" s="24"/>
     </row>
-    <row r="65" spans="1:9" ht="84" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-16</v>
@@ -5983,7 +5992,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT01-3</v>
@@ -6013,7 +6022,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDTM 83-1</v>
@@ -6043,7 +6052,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="195" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="174" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-10</v>
@@ -6071,7 +6080,7 @@
       </c>
       <c r="I68" s="24"/>
     </row>
-    <row r="69" spans="1:9" ht="87.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="88" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-1</v>
@@ -6099,7 +6108,7 @@
       </c>
       <c r="I69" s="24"/>
     </row>
-    <row r="70" spans="1:9" ht="102.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="103" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-11</v>
@@ -6127,7 +6136,7 @@
       </c>
       <c r="I70" s="24"/>
     </row>
-    <row r="71" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
       <c r="A71" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-12</v>
@@ -6157,7 +6166,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-13</v>
@@ -6187,7 +6196,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A73" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-14</v>
@@ -6217,7 +6226,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-19</v>
@@ -6247,7 +6256,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-16</v>
@@ -6277,7 +6286,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-14</v>
@@ -6305,7 +6314,7 @@
       </c>
       <c r="I76" s="23"/>
     </row>
-    <row r="77" spans="1:9" ht="144" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="126.5" x14ac:dyDescent="0.35">
       <c r="A77" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-15</v>
@@ -6331,9 +6340,11 @@
       <c r="H77" s="17" t="s">
         <v>574</v>
       </c>
-      <c r="I77" s="24"/>
-    </row>
-    <row r="78" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+      <c r="I77" s="23" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A78" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDTM11-2</v>
@@ -6363,7 +6374,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A79" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-16</v>
@@ -6391,7 +6402,7 @@
       </c>
       <c r="I79" s="24"/>
     </row>
-    <row r="80" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A80" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-22</v>
@@ -6421,7 +6432,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="27" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" ht="26" x14ac:dyDescent="0.35">
       <c r="A81" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-23</v>
@@ -6451,7 +6462,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A82" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-24</v>
@@ -6481,7 +6492,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" ht="65.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-17</v>
@@ -6509,7 +6520,7 @@
       </c>
       <c r="I83" s="24"/>
     </row>
-    <row r="84" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A84" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-18</v>
@@ -6537,7 +6548,7 @@
       </c>
       <c r="I84" s="24"/>
     </row>
-    <row r="85" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A85" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-19</v>
@@ -6567,7 +6578,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-20</v>
@@ -6597,7 +6608,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-27</v>
@@ -6627,7 +6638,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A88" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-21</v>
@@ -6657,7 +6668,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" ht="39.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-26</v>
@@ -6687,7 +6698,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-17</v>
@@ -6717,7 +6728,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A91" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-16</v>
@@ -6745,7 +6756,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="77.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-17</v>
@@ -6773,7 +6784,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A93" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-22</v>
@@ -6801,7 +6812,7 @@
       </c>
       <c r="I93" s="24"/>
     </row>
-    <row r="94" spans="1:9" s="39" customFormat="1" ht="98.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" s="39" customFormat="1" ht="98.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A94" s="33" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-23</v>
@@ -6831,7 +6842,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="96.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" ht="81" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A95" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-24</v>
@@ -6861,7 +6872,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="113.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" ht="113.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/PoNSOH-26</v>
@@ -6891,7 +6902,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/PoNSOH-27</v>
@@ -6919,7 +6930,7 @@
       </c>
       <c r="I97" s="23"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-18</v>
@@ -6947,7 +6958,7 @@
       </c>
       <c r="I98" s="24"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-19</v>
@@ -6975,7 +6986,7 @@
       </c>
       <c r="I99" s="24"/>
     </row>
-    <row r="100" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-18</v>
@@ -7003,7 +7014,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A101" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDTM11-3</v>
@@ -7029,7 +7040,7 @@
       </c>
       <c r="I101" s="24"/>
     </row>
-    <row r="102" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A102" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-15</v>
@@ -7059,7 +7070,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-1</v>
@@ -7089,7 +7100,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A104" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-17</v>
@@ -7119,7 +7130,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A105" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-20</v>
@@ -7149,7 +7160,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="39" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" ht="37.5" x14ac:dyDescent="0.35">
       <c r="A106" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-21</v>
@@ -7177,7 +7188,7 @@
       </c>
       <c r="I106" s="24"/>
     </row>
-    <row r="107" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A107" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-18</v>
@@ -7207,7 +7218,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A108" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-25</v>
@@ -7237,7 +7248,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A109" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-2</v>
@@ -7265,7 +7276,7 @@
       </c>
       <c r="I109" s="24"/>
     </row>
-    <row r="110" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A110" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-3</v>
@@ -7293,7 +7304,7 @@
       </c>
       <c r="I110" s="24"/>
     </row>
-    <row r="111" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A111" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-4</v>
@@ -7321,7 +7332,7 @@
       </c>
       <c r="I111" s="24"/>
     </row>
-    <row r="112" spans="1:9" ht="84" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A112" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT01-1</v>
@@ -7351,7 +7362,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A113" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-5</v>
@@ -7379,7 +7390,7 @@
       </c>
       <c r="I113" s="24"/>
     </row>
-    <row r="114" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A114" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-6</v>
@@ -7407,7 +7418,7 @@
       </c>
       <c r="I114" s="24"/>
     </row>
-    <row r="115" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A115" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-7</v>
@@ -7435,7 +7446,7 @@
       </c>
       <c r="I115" s="24"/>
     </row>
-    <row r="116" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A116" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-8</v>
@@ -7463,7 +7474,7 @@
       </c>
       <c r="I116" s="24"/>
     </row>
-    <row r="117" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A117" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-9</v>
@@ -7491,7 +7502,7 @@
       </c>
       <c r="I117" s="24"/>
     </row>
-    <row r="118" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A118" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-10</v>
@@ -7519,7 +7530,7 @@
       </c>
       <c r="I118" s="24"/>
     </row>
-    <row r="119" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-11</v>
@@ -7549,7 +7560,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-12</v>
@@ -7577,7 +7588,7 @@
       </c>
       <c r="I120" s="24"/>
     </row>
-    <row r="121" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A121" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-13</v>
@@ -7605,7 +7616,7 @@
       </c>
       <c r="I121" s="24"/>
     </row>
-    <row r="122" spans="1:9" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" ht="151.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-6</v>
@@ -7631,9 +7642,11 @@
       <c r="H122" s="19" t="s">
         <v>483</v>
       </c>
-      <c r="I122" s="24"/>
-    </row>
-    <row r="123" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+      <c r="I122" s="23" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A123" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT01-2</v>
@@ -7659,9 +7672,11 @@
       <c r="H123" s="19" t="s">
         <v>475</v>
       </c>
-      <c r="I123" s="24"/>
-    </row>
-    <row r="124" spans="1:9" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I123" s="23" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-23</v>
@@ -7687,9 +7702,11 @@
       <c r="H124" s="19" t="s">
         <v>484</v>
       </c>
-      <c r="I124" s="24"/>
-    </row>
-    <row r="125" spans="1:9" ht="96" x14ac:dyDescent="0.25">
+      <c r="I124" s="23" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A125" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-20</v>
@@ -7715,9 +7732,11 @@
       <c r="H125" s="19" t="s">
         <v>485</v>
       </c>
-      <c r="I125" s="24"/>
-    </row>
-    <row r="126" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="I125" s="23" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
       <c r="A126" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-25</v>
@@ -7743,9 +7762,11 @@
       <c r="H126" s="19" t="s">
         <v>580</v>
       </c>
-      <c r="I126" s="24"/>
-    </row>
-    <row r="127" spans="1:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I126" s="23" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-26</v>
@@ -7775,7 +7796,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT07-1</v>
@@ -7805,7 +7826,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-19</v>
@@ -7833,7 +7854,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="130" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-20</v>
@@ -7861,7 +7882,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="131" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A131" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-9</v>
@@ -7891,7 +7912,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="132" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A132" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-10</v>
@@ -7921,7 +7942,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="133" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-27</v>
@@ -7951,7 +7972,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="134" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A134" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-28</v>
@@ -7981,7 +8002,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="135" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" ht="23" x14ac:dyDescent="0.35">
       <c r="A135" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-29</v>
@@ -8011,7 +8032,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="136" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A136" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-10</v>
@@ -8041,7 +8062,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="137" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A137" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-11</v>
@@ -8071,7 +8092,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="72" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" ht="69" x14ac:dyDescent="0.35">
       <c r="A138" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-12</v>
@@ -8101,7 +8122,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="139" spans="1:9" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" ht="44.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-25</v>
@@ -8129,7 +8150,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="140" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A140" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-13</v>
@@ -8159,7 +8180,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="141" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A141" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-7</v>

</xml_diff>

<commit_message>
traitement commentaires DDT38-10, DDT42-1 (Livraison Shaefile)
</commit_message>
<xml_diff>
--- a/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
+++ b/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Geostandards-Risques\suivi\2024-05_06-Consultation-publique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8352BC-3867-4F13-9481-CF5E4C3533D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31EE03F-849A-4074-9D7A-A4E2D0BE5CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-26520" yWindow="2280" windowWidth="21600" windowHeight="11265" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="607">
   <si>
     <t>Organisme</t>
   </si>
@@ -2113,11 +2113,6 @@
     <t>Mentionner la possibilité de cartographier les PHEC mais sonas les définir + que ça (réf. https://www.reperesdecrues.developpement-durable.gouv.fr/  )</t>
   </si>
   <si>
-    <t>NOK ?
-La nomenture des risques GASPAR ne fait pas la distinction entre les différents types d'avalanche. Peut-être faut-il faire des sous-types de l'aléa 14 comme pour l'inondation ?
-Pour l'instant cette information peut être mise dans la description texte libre</t>
-  </si>
-  <si>
     <t>OK sur le principe. A valider avec le GT
 NB : quid des autres aleéas technos (non industriels) ? 
 Risque technologique ; Nucléaire
@@ -2128,9 +2123,6 @@
   <si>
     <t>NOK ?
 avalanche est sous-entendu par la formulation "Tous PPRN". Sinon il faudrait lister tous les types d'Aléas naturels pour chaque niveau</t>
-  </si>
-  <si>
-    <t>Soumettre la proposition coulante + aérosol + les 2 au BRNT. Cf. réponse BRNT</t>
   </si>
   <si>
     <t>A discuter avec le GT et les demandeurs
@@ -2354,6 +2346,16 @@
   </si>
   <si>
     <t>intégré (mention des PPRT dans l'annexe multirisques et couche de synthèse PPRT pour les aléas techno multiples)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intégré (énumération informative)
+</t>
+  </si>
+  <si>
+    <t>NOK ?
+La nomenture des risques GASPAR ne fait pas la distinction entre les différents types d'avalanche. Peut-être faut-il faire des sous-types de l'aléa 14 comme pour l'inondation ?
+Pour l'instant cette information peut être mise dans la description texte libre
+Soumettre la proposition coulante + aérosol + les 2 au BRNT. Cf. réponse BRNT</t>
   </si>
 </sst>
 </file>
@@ -2630,9 +2632,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2653,6 +2652,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -3736,10 +3738,10 @@
         <v>335</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4036,10 +4038,10 @@
         <v>328</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4083,8 +4085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815F14A-19BC-4DCE-8D31-81F595A4B0E7}">
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I133" sqref="I133"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I69" sqref="I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4318,7 +4320,7 @@
         <v>45</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="I8" s="23" t="s">
         <v>507</v>
@@ -4670,7 +4672,7 @@
         <v>255</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="I20" s="23" t="s">
         <v>507</v>
@@ -4760,10 +4762,10 @@
         <v>122</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
@@ -5000,7 +5002,7 @@
         <v>78</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="I31" s="23" t="s">
         <v>507</v>
@@ -5030,7 +5032,7 @@
         <v>128</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="I32" s="23" t="s">
         <v>507</v>
@@ -5063,7 +5065,7 @@
         <v>384</v>
       </c>
       <c r="I33" s="23" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="41.15" customHeight="1" x14ac:dyDescent="0.35">
@@ -5152,7 +5154,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="32" customFormat="1" ht="81" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:9" s="31" customFormat="1" ht="115.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="26" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-1</v>
@@ -5176,10 +5178,10 @@
         <v>19</v>
       </c>
       <c r="H37" s="30" t="s">
-        <v>554</v>
-      </c>
-      <c r="I37" s="31" t="s">
-        <v>557</v>
+        <v>606</v>
+      </c>
+      <c r="I37" s="39" t="s">
+        <v>605</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="44.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
@@ -5206,7 +5208,7 @@
         <v>99</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I38" s="4" t="s">
         <v>506</v>
@@ -5236,10 +5238,10 @@
         <v>338</v>
       </c>
       <c r="H39" s="19" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="I39" s="23" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="207" x14ac:dyDescent="0.35">
@@ -5266,10 +5268,10 @@
         <v>338</v>
       </c>
       <c r="H40" s="19" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="I40" s="23" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
@@ -5296,7 +5298,7 @@
         <v>267</v>
       </c>
       <c r="H41" s="17" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I41" s="23" t="s">
         <v>507</v>
@@ -5326,10 +5328,10 @@
         <v>133</v>
       </c>
       <c r="H42" s="19" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="I42" s="23" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="111.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5354,10 +5356,10 @@
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="17" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="I43" s="24" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="92" x14ac:dyDescent="0.35">
@@ -5384,7 +5386,7 @@
         <v>26</v>
       </c>
       <c r="H44" s="13" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="I44" s="4" t="s">
         <v>506</v>
@@ -5472,10 +5474,10 @@
         <v>33</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="I47" s="24" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5563,7 +5565,7 @@
         <v>525</v>
       </c>
       <c r="I50" s="24" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="69" x14ac:dyDescent="0.35">
@@ -5819,7 +5821,7 @@
         <v>392</v>
       </c>
       <c r="I59" s="24" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="46" x14ac:dyDescent="0.35">
@@ -5875,7 +5877,7 @@
         <v>396</v>
       </c>
       <c r="I61" s="24" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="230" x14ac:dyDescent="0.35">
@@ -5903,7 +5905,7 @@
         <v>395</v>
       </c>
       <c r="I62" s="24" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
@@ -5933,7 +5935,7 @@
         <v>528</v>
       </c>
       <c r="I63" s="24" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="46" x14ac:dyDescent="0.35">
@@ -5958,7 +5960,7 @@
       </c>
       <c r="G64" s="4"/>
       <c r="H64" s="13" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="I64" s="24"/>
     </row>
@@ -5986,10 +5988,10 @@
         <v>154</v>
       </c>
       <c r="H65" s="19" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="I65" s="24" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="46" x14ac:dyDescent="0.35">
@@ -6078,7 +6080,9 @@
       <c r="H68" s="17" t="s">
         <v>461</v>
       </c>
-      <c r="I68" s="24"/>
+      <c r="I68" s="23" t="s">
+        <v>507</v>
+      </c>
     </row>
     <row r="69" spans="1:9" ht="88" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="4" t="str">
@@ -6106,7 +6110,9 @@
       <c r="H69" s="17" t="s">
         <v>398</v>
       </c>
-      <c r="I69" s="24"/>
+      <c r="I69" s="23" t="s">
+        <v>507</v>
+      </c>
     </row>
     <row r="70" spans="1:9" ht="103" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="str">
@@ -6134,7 +6140,9 @@
       <c r="H70" s="17" t="s">
         <v>462</v>
       </c>
-      <c r="I70" s="24"/>
+      <c r="I70" s="23" t="s">
+        <v>507</v>
+      </c>
     </row>
     <row r="71" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
       <c r="A71" s="4" t="str">
@@ -6163,7 +6171,7 @@
         <v>500</v>
       </c>
       <c r="I71" s="24" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
@@ -6338,7 +6346,7 @@
         <v>275</v>
       </c>
       <c r="H77" s="17" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="I77" s="23" t="s">
         <v>507</v>
@@ -6398,7 +6406,7 @@
         <v>203</v>
       </c>
       <c r="H79" s="17" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="I79" s="24"/>
     </row>
@@ -6489,7 +6497,7 @@
         <v>530</v>
       </c>
       <c r="I82" s="24" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="65.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
@@ -6572,7 +6580,7 @@
         <v>211</v>
       </c>
       <c r="H85" s="19" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="I85" s="23" t="s">
         <v>507</v>
@@ -6808,38 +6816,38 @@
         <v>218</v>
       </c>
       <c r="H93" s="17" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="I93" s="24"/>
     </row>
-    <row r="94" spans="1:9" s="39" customFormat="1" ht="98.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A94" s="33" t="str">
+    <row r="94" spans="1:9" s="38" customFormat="1" ht="98.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A94" s="32" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-23</v>
       </c>
-      <c r="B94" s="34">
+      <c r="B94" s="33">
         <v>23</v>
       </c>
-      <c r="C94" s="35" t="s">
+      <c r="C94" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="D94" s="36" t="s">
+      <c r="D94" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="E94" s="36" t="s">
+      <c r="E94" s="35" t="s">
         <v>219</v>
       </c>
-      <c r="F94" s="35" t="s">
+      <c r="F94" s="34" t="s">
         <v>220</v>
       </c>
-      <c r="G94" s="35" t="s">
+      <c r="G94" s="34" t="s">
         <v>278</v>
       </c>
-      <c r="H94" s="37" t="s">
+      <c r="H94" s="36" t="s">
         <v>473</v>
       </c>
-      <c r="I94" s="38" t="s">
-        <v>579</v>
+      <c r="I94" s="37" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="81" thickTop="1" x14ac:dyDescent="0.35">
@@ -7036,7 +7044,7 @@
         <v>543</v>
       </c>
       <c r="H101" s="19" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="I101" s="24"/>
     </row>
@@ -7359,7 +7367,7 @@
         <v>477</v>
       </c>
       <c r="I112" s="24" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="23" x14ac:dyDescent="0.35">
@@ -7703,7 +7711,7 @@
         <v>484</v>
       </c>
       <c r="I124" s="23" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="125" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
@@ -7733,7 +7741,7 @@
         <v>485</v>
       </c>
       <c r="I125" s="23" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="126" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
@@ -7760,10 +7768,10 @@
         <v>225</v>
       </c>
       <c r="H126" s="19" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="I126" s="23" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="127" spans="1:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7790,10 +7798,10 @@
         <v>228</v>
       </c>
       <c r="H127" s="17" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="I127" s="23" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="128" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.35">
@@ -7851,7 +7859,7 @@
         <v>487</v>
       </c>
       <c r="I129" s="23" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="130" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
@@ -7876,7 +7884,7 @@
       </c>
       <c r="G130" s="4"/>
       <c r="H130" s="17" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="I130" s="23" t="s">
         <v>507</v>
@@ -7936,7 +7944,7 @@
         <v>139</v>
       </c>
       <c r="H132" s="13" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="I132" s="23" t="s">
         <v>506</v>
@@ -7969,7 +7977,7 @@
         <v>489</v>
       </c>
       <c r="I133" s="24" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="23" x14ac:dyDescent="0.35">
@@ -8086,7 +8094,7 @@
         <v>39</v>
       </c>
       <c r="H137" s="13" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="I137" s="4" t="s">
         <v>524</v>

</xml_diff>

<commit_message>
traitement commentaires dans tableau XLS
</commit_message>
<xml_diff>
--- a/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
+++ b/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Geostandards-Risques\suivi\2024-05_06-Consultation-publique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31EE03F-849A-4074-9D7A-A4E2D0BE5CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6D0513-F3EC-4465-BFCB-8D30B21C0437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26520" yWindow="2280" windowWidth="21600" windowHeight="11265" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
+    <workbookView xWindow="-25875" yWindow="855" windowWidth="21600" windowHeight="11265" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Synthese Modele Commun" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="605">
   <si>
     <t>Organisme</t>
   </si>
@@ -1383,11 +1383,6 @@
 NB : si des traitements sont appliqués pour traiter ce problème, cela peut (doit) être mentionné dans les métadonnées</t>
   </si>
   <si>
-    <t>OK sur le principe.
-Il s'agit de zones particulières (pas de zones d'aléas)
-Un tableau différent est sans doute à proposer (cf. commentaire suviant)</t>
-  </si>
-  <si>
     <t>Ok sur le principe. 
 Symobologie à trouver. Cf. commentaire précédent.</t>
   </si>
@@ -1914,12 +1909,6 @@
 - Proposition BRIL (en cours): ouvrages de protection (inondations)" décomposé en AH et SE, et "Autres ouvrages faisant obstacle aux écoulements". A valider avec PONSOH</t>
   </si>
   <si>
-    <t xml:space="preserve">OK sur le principe. 
-A valdier en GT 
-NB : A vérifier avec le DAGSI (rendre obligatoire les aléas à partir d'une certaine date) ?
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">NOK
 Cette référence est citée dans le standard PPR
 Les références aux Guides PPR dans le modèle commun sont essentiellement dues aux défintiions.
@@ -1965,11 +1954,6 @@
   <si>
     <t>integré (+ carte "approuvée" au lieu de "signée")
 + tables d'énumérations (PPR) + modèle UML + gabarits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non, à moins qu'il n'y ait une volonté de les transformer en PPR (cf. Sweet pepper)?
-NB : certains champs obligatoires non renseignés dans PSS
-</t>
   </si>
   <si>
     <t>OK sur le principe, à modifier
@@ -2085,11 +2069,6 @@
     <t>cf. commentaires PPR (intégré)</t>
   </si>
   <si>
-    <t xml:space="preserve">Ne rendre obligatoire que les thématiques Procédures, Périmètres et Zonage Réglementaire?
-Aléa non obligatoire (au niveau diffusion)
-</t>
-  </si>
-  <si>
     <t>A envisager dans le cadre de l'accompagnement (gabarit XML)</t>
   </si>
   <si>
@@ -2153,23 +2132,8 @@
 A priori l'expropriation ne concerne que les PPRT, pas les PPRN</t>
   </si>
   <si>
-    <t xml:space="preserve">pour l'AE : https://www.legifrance.gouv.fr/download/pdf/circ?id=40103 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">A discuter
-Elles sont identifiées dans les enjeux. 
-Et déduties dans le Zonage reglementaire comme zones d'interdiction ou prescription avec des mesures particulières.
-</t>
-  </si>
-  <si>
     <t>N.A.
 (voir si cela peut-être explicité dans le standard)</t>
-  </si>
-  <si>
-    <t>article R 562-11-4 du CE : matérialisation de la bande particulière</t>
-  </si>
-  <si>
-    <t>Symbologie pour les zones proégées également</t>
   </si>
   <si>
     <t>Préciser le caractère synthétique des représentations. Différentes réglementation peuvent s'appliquer dans les zones identifiées dans le principe général d'une même interdiction</t>
@@ -2191,9 +2155,6 @@
   </si>
   <si>
     <t>Ces zones d'exception sont une sous partie spécifique  des zones répondant au principe général d'interdiction. (Guide PPRICet (p79) )</t>
-  </si>
-  <si>
-    <t>cf. commentaire #1</t>
   </si>
   <si>
     <t>OK sur le principe ?
@@ -2356,6 +2317,41 @@
 La nomenture des risques GASPAR ne fait pas la distinction entre les différents types d'avalanche. Peut-être faut-il faire des sous-types de l'aléa 14 comme pour l'inondation ?
 Pour l'instant cette information peut être mise dans la description texte libre
 Soumettre la proposition coulante + aérosol + les 2 au BRNT. Cf. réponse BRNT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non, à moins qu'il n'y ait une volonté de les transformer en PPR (cf. Sweet pepper)?
+NB : certains champs obligatoires non renseignés dans PSS
+=&gt; Ne rendre obligatoire que les thématiques Procédures, Périmètres et Zonage Réglementaire?
+Aléa non obligatoire (au niveau diffusion)
+</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A discuter
+Elles sont identifiées dans les enjeux. 
+Et déduties dans le Zonage reglementaire comme zones d'interdiction ou prescription avec des mesures particulières.
+(Pas de modification)
+</t>
+  </si>
+  <si>
+    <t>OK sur le principe.
+Il s'agit de zones particulières (pas de zones d'aléas)
+Un tableau différent est sans doute à proposer (cf. commentaire suviant).
+article R 562-11-4 du CE : matérialisation de la bande particulière</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intégré </t>
+  </si>
+  <si>
+    <t>OK sur le principe. 
+A valdier en GT 
+NB : A vérifier avec le DAGSI (rendre obligatoire les aléas à partir d'une certaine date) ?
+cf. commentaire #1</t>
+  </si>
+  <si>
+    <t>inétgré (en partie pour avalanches)</t>
   </si>
 </sst>
 </file>
@@ -2456,7 +2452,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2466,6 +2462,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2542,7 +2544,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2653,6 +2655,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3503,7 +3508,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="73" customHeight="1" x14ac:dyDescent="0.35">
@@ -3533,7 +3538,7 @@
         <v>351</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="92" x14ac:dyDescent="0.35">
@@ -3560,10 +3565,10 @@
         <v>332</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="92" x14ac:dyDescent="0.35">
@@ -3593,7 +3598,7 @@
         <v>353</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="75.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
@@ -3620,10 +3625,10 @@
         <v>305</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="89.15" customHeight="1" x14ac:dyDescent="0.35">
@@ -3653,7 +3658,7 @@
         <v>350</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="23" x14ac:dyDescent="0.35">
@@ -3681,7 +3686,7 @@
         <v>352</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
@@ -3711,7 +3716,7 @@
         <v>357</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="126.5" x14ac:dyDescent="0.35">
@@ -3738,10 +3743,10 @@
         <v>335</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>582</v>
+        <v>573</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>583</v>
+        <v>574</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3771,7 +3776,7 @@
         <v>354</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -3801,7 +3806,7 @@
         <v>354</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
@@ -3828,10 +3833,10 @@
         <v>315</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3861,7 +3866,7 @@
         <v>355</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="92" x14ac:dyDescent="0.35">
@@ -3891,7 +3896,7 @@
         <v>356</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="61" customHeight="1" x14ac:dyDescent="0.35">
@@ -3921,7 +3926,7 @@
         <v>352</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="68.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
@@ -3948,10 +3953,10 @@
         <v>288</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="77.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
@@ -3981,7 +3986,7 @@
         <v>358</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="111" customHeight="1" x14ac:dyDescent="0.35">
@@ -4008,10 +4013,10 @@
         <v>293</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
@@ -4038,10 +4043,10 @@
         <v>328</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>581</v>
+        <v>572</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>595</v>
+        <v>586</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4069,7 +4074,7 @@
         <v>359</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
   </sheetData>
@@ -4085,8 +4090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815F14A-19BC-4DCE-8D31-81F595A4B0E7}">
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I69" sqref="I69"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H133" sqref="H133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4129,7 +4134,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4154,10 +4159,10 @@
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="25" t="s">
-        <v>514</v>
-      </c>
-      <c r="I2" s="24" t="s">
-        <v>546</v>
+        <v>598</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4185,7 +4190,7 @@
         <v>370</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4213,7 +4218,7 @@
         <v>371</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="65.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
@@ -4238,10 +4243,10 @@
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="22" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="126.5" x14ac:dyDescent="0.35">
@@ -4267,7 +4272,7 @@
         <v>372</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
@@ -4295,7 +4300,7 @@
         <v>373</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="69" x14ac:dyDescent="0.35">
@@ -4320,10 +4325,10 @@
         <v>45</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>598</v>
+        <v>589</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4351,7 +4356,7 @@
         <v>374</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
@@ -4363,23 +4368,23 @@
         <v>1</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="4" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
@@ -4465,7 +4470,7 @@
         <v>350</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="66.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
@@ -4492,10 +4497,10 @@
         <v>166</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="161" x14ac:dyDescent="0.35">
@@ -4522,10 +4527,10 @@
         <v>254</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
@@ -4552,10 +4557,10 @@
         <v>62</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
@@ -4582,10 +4587,10 @@
         <v>117</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
@@ -4615,7 +4620,7 @@
         <v>378</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
@@ -4645,7 +4650,7 @@
         <v>379</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="92" x14ac:dyDescent="0.35">
@@ -4672,10 +4677,10 @@
         <v>255</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>589</v>
+        <v>580</v>
       </c>
       <c r="I20" s="23" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
@@ -4702,10 +4707,10 @@
         <v>256</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4735,7 +4740,7 @@
         <v>380</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="69" x14ac:dyDescent="0.35">
@@ -4762,10 +4767,10 @@
         <v>122</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>590</v>
+        <v>581</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>591</v>
+        <v>582</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
@@ -4795,7 +4800,7 @@
         <v>381</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="46" x14ac:dyDescent="0.35">
@@ -4825,7 +4830,7 @@
         <v>382</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="23" x14ac:dyDescent="0.35">
@@ -4855,7 +4860,7 @@
         <v>381</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="71.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4882,10 +4887,10 @@
         <v>72</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="I27" s="23" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
@@ -4915,7 +4920,7 @@
         <v>352</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="115" x14ac:dyDescent="0.35">
@@ -4942,10 +4947,10 @@
         <v>340</v>
       </c>
       <c r="H29" s="19" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="I29" s="24" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4972,10 +4977,10 @@
         <v>75</v>
       </c>
       <c r="H30" s="19" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
@@ -5002,10 +5007,10 @@
         <v>78</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>584</v>
+        <v>575</v>
       </c>
       <c r="I31" s="23" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
@@ -5032,10 +5037,10 @@
         <v>128</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>585</v>
+        <v>576</v>
       </c>
       <c r="I32" s="23" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="92" x14ac:dyDescent="0.35">
@@ -5065,7 +5070,7 @@
         <v>384</v>
       </c>
       <c r="I33" s="23" t="s">
-        <v>596</v>
+        <v>587</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="41.15" customHeight="1" x14ac:dyDescent="0.35">
@@ -5090,10 +5095,10 @@
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="17" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
@@ -5123,7 +5128,7 @@
         <v>385</v>
       </c>
       <c r="I35" s="23" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="62.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -5151,7 +5156,7 @@
         <v>383</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="31" customFormat="1" ht="115.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -5178,10 +5183,10 @@
         <v>19</v>
       </c>
       <c r="H37" s="30" t="s">
-        <v>606</v>
+        <v>597</v>
       </c>
       <c r="I37" s="39" t="s">
-        <v>605</v>
+        <v>596</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="44.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
@@ -5208,10 +5213,10 @@
         <v>99</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.35">
@@ -5238,10 +5243,10 @@
         <v>338</v>
       </c>
       <c r="H39" s="19" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="I39" s="23" t="s">
-        <v>599</v>
+        <v>590</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="207" x14ac:dyDescent="0.35">
@@ -5268,10 +5273,10 @@
         <v>338</v>
       </c>
       <c r="H40" s="19" t="s">
-        <v>600</v>
+        <v>591</v>
       </c>
       <c r="I40" s="23" t="s">
-        <v>599</v>
+        <v>590</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
@@ -5298,10 +5303,10 @@
         <v>267</v>
       </c>
       <c r="H41" s="17" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="I41" s="23" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5328,10 +5333,10 @@
         <v>133</v>
       </c>
       <c r="H42" s="19" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="I42" s="23" t="s">
-        <v>597</v>
+        <v>588</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="111.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5356,10 +5361,10 @@
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="17" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="I43" s="24" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="92" x14ac:dyDescent="0.35">
@@ -5386,10 +5391,10 @@
         <v>26</v>
       </c>
       <c r="H44" s="13" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="77.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5419,7 +5424,7 @@
         <v>388</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
@@ -5447,10 +5452,10 @@
         <v>389</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-8</v>
@@ -5474,10 +5479,10 @@
         <v>33</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>562</v>
-      </c>
-      <c r="I47" s="24" t="s">
-        <v>561</v>
+        <v>600</v>
+      </c>
+      <c r="I47" s="23" t="s">
+        <v>599</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5506,7 +5511,9 @@
       <c r="H48" s="19" t="s">
         <v>389</v>
       </c>
-      <c r="I48" s="23"/>
+      <c r="I48" s="23" t="s">
+        <v>599</v>
+      </c>
     </row>
     <row r="49" spans="1:9" ht="46" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="str">
@@ -5535,10 +5542,10 @@
         <v>390</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="117.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-5</v>
@@ -5562,10 +5569,10 @@
         <v>28</v>
       </c>
       <c r="H50" s="17" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="I50" s="24" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="69" x14ac:dyDescent="0.35">
@@ -5594,7 +5601,9 @@
       <c r="H51" s="13" t="s">
         <v>391</v>
       </c>
-      <c r="I51" s="4"/>
+      <c r="I51" s="4" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="str">
@@ -5676,10 +5685,10 @@
         <v>145</v>
       </c>
       <c r="H54" s="17" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.35">
@@ -5707,7 +5716,7 @@
         <v>377</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -5732,10 +5741,10 @@
         <v>87</v>
       </c>
       <c r="H56" s="17" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
@@ -5760,10 +5769,10 @@
       </c>
       <c r="G57" s="4"/>
       <c r="H57" s="17" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="46" x14ac:dyDescent="0.35">
@@ -5793,7 +5802,7 @@
         <v>377</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="184" x14ac:dyDescent="0.35">
@@ -5818,13 +5827,13 @@
       </c>
       <c r="G59" s="4"/>
       <c r="H59" s="19" t="s">
-        <v>392</v>
-      </c>
-      <c r="I59" s="24" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+        <v>601</v>
+      </c>
+      <c r="I59" s="23" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="61" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-14</v>
@@ -5848,9 +5857,11 @@
         <v>148</v>
       </c>
       <c r="H60" s="19" t="s">
-        <v>393</v>
-      </c>
-      <c r="I60" s="24"/>
+        <v>392</v>
+      </c>
+      <c r="I60" s="23" t="s">
+        <v>602</v>
+      </c>
     </row>
     <row r="61" spans="1:9" ht="92" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="str">
@@ -5874,10 +5885,10 @@
       </c>
       <c r="G61" s="4"/>
       <c r="H61" s="19" t="s">
-        <v>396</v>
-      </c>
-      <c r="I61" s="24" t="s">
-        <v>565</v>
+        <v>395</v>
+      </c>
+      <c r="I61" s="23" t="s">
+        <v>602</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="230" x14ac:dyDescent="0.35">
@@ -5902,10 +5913,10 @@
       </c>
       <c r="G62" s="4"/>
       <c r="H62" s="13" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I62" s="24" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
@@ -5932,10 +5943,10 @@
         <v>151</v>
       </c>
       <c r="H63" s="19" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="I63" s="24" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="46" x14ac:dyDescent="0.35">
@@ -5960,9 +5971,11 @@
       </c>
       <c r="G64" s="4"/>
       <c r="H64" s="13" t="s">
-        <v>568</v>
-      </c>
-      <c r="I64" s="24"/>
+        <v>560</v>
+      </c>
+      <c r="I64" s="23" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="65" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="str">
@@ -5988,10 +6001,10 @@
         <v>154</v>
       </c>
       <c r="H65" s="19" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="I65" s="24" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="46" x14ac:dyDescent="0.35">
@@ -6018,10 +6031,10 @@
         <v>50</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="46" x14ac:dyDescent="0.35">
@@ -6048,10 +6061,10 @@
         <v>53</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="I67" s="4" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="174" x14ac:dyDescent="0.35">
@@ -6078,10 +6091,10 @@
         <v>270</v>
       </c>
       <c r="H68" s="17" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="I68" s="23" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="88" customHeight="1" x14ac:dyDescent="0.35">
@@ -6108,10 +6121,10 @@
         <v>241</v>
       </c>
       <c r="H69" s="17" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I69" s="23" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="103" customHeight="1" x14ac:dyDescent="0.35">
@@ -6138,10 +6151,10 @@
         <v>271</v>
       </c>
       <c r="H70" s="17" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I70" s="23" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
@@ -6168,10 +6181,10 @@
         <v>272</v>
       </c>
       <c r="H71" s="17" t="s">
-        <v>500</v>
-      </c>
-      <c r="I71" s="24" t="s">
-        <v>571</v>
+        <v>603</v>
+      </c>
+      <c r="I71" s="23" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
@@ -6198,10 +6211,10 @@
         <v>197</v>
       </c>
       <c r="H72" s="17" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
@@ -6213,25 +6226,25 @@
         <v>14</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E73" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="F73" s="4" t="s">
         <v>429</v>
       </c>
-      <c r="F73" s="4" t="s">
+      <c r="G73" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="G73" s="4" t="s">
-        <v>431</v>
-      </c>
       <c r="H73" s="19" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
@@ -6243,25 +6256,25 @@
         <v>19</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E74" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="F74" s="4" t="s">
         <v>429</v>
       </c>
-      <c r="F74" s="4" t="s">
+      <c r="G74" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="G74" s="4" t="s">
-        <v>431</v>
-      </c>
       <c r="H74" s="17" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.35">
@@ -6273,25 +6286,25 @@
         <v>16</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F75" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="G75" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="G75" s="4" t="s">
-        <v>431</v>
-      </c>
       <c r="H75" s="17" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="I75" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6318,7 +6331,7 @@
         <v>273</v>
       </c>
       <c r="H76" s="17" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I76" s="23"/>
     </row>
@@ -6346,10 +6359,10 @@
         <v>275</v>
       </c>
       <c r="H77" s="17" t="s">
-        <v>572</v>
+        <v>563</v>
       </c>
       <c r="I77" s="23" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
@@ -6361,25 +6374,25 @@
         <v>2</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="D78" s="5" t="s">
+        <v>533</v>
+      </c>
+      <c r="E78" s="5" t="s">
         <v>536</v>
       </c>
-      <c r="E78" s="5" t="s">
-        <v>539</v>
-      </c>
       <c r="F78" s="4" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="G78" s="4" t="s">
+        <v>538</v>
+      </c>
+      <c r="H78" s="17" t="s">
         <v>541</v>
       </c>
-      <c r="H78" s="17" t="s">
-        <v>544</v>
-      </c>
       <c r="I78" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="46" x14ac:dyDescent="0.35">
@@ -6406,9 +6419,11 @@
         <v>203</v>
       </c>
       <c r="H79" s="17" t="s">
-        <v>573</v>
-      </c>
-      <c r="I79" s="24"/>
+        <v>564</v>
+      </c>
+      <c r="I79" s="40" t="s">
+        <v>604</v>
+      </c>
     </row>
     <row r="80" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A80" s="20" t="str">
@@ -6419,25 +6434,25 @@
         <v>22</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E80" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="G80" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="F80" s="4" t="s">
-        <v>456</v>
-      </c>
-      <c r="G80" s="4" t="s">
-        <v>445</v>
-      </c>
       <c r="H80" s="19" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="26" x14ac:dyDescent="0.35">
@@ -6449,25 +6464,25 @@
         <v>23</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H81" s="17" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="I81" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
@@ -6479,25 +6494,25 @@
         <v>24</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E82" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>457</v>
+      </c>
+      <c r="G82" s="4" t="s">
         <v>447</v>
       </c>
-      <c r="F82" s="4" t="s">
-        <v>458</v>
-      </c>
-      <c r="G82" s="4" t="s">
-        <v>448</v>
-      </c>
       <c r="H82" s="13" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="I82" s="24" t="s">
-        <v>574</v>
+        <v>565</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="65.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
@@ -6524,7 +6539,7 @@
         <v>206</v>
       </c>
       <c r="H83" s="17" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="I83" s="24"/>
     </row>
@@ -6552,7 +6567,7 @@
         <v>209</v>
       </c>
       <c r="H84" s="17" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="I84" s="24"/>
     </row>
@@ -6580,10 +6595,10 @@
         <v>211</v>
       </c>
       <c r="H85" s="19" t="s">
-        <v>575</v>
+        <v>566</v>
       </c>
       <c r="I85" s="23" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="23" x14ac:dyDescent="0.35">
@@ -6610,10 +6625,10 @@
         <v>213</v>
       </c>
       <c r="H86" s="17" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="I86" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -6625,25 +6640,25 @@
         <v>27</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E87" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="G87" s="4" t="s">
         <v>453</v>
       </c>
-      <c r="F87" s="4" t="s">
-        <v>460</v>
-      </c>
-      <c r="G87" s="4" t="s">
-        <v>454</v>
-      </c>
       <c r="H87" s="19" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
@@ -6670,10 +6685,10 @@
         <v>216</v>
       </c>
       <c r="H88" s="19" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="39.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -6685,25 +6700,25 @@
         <v>26</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="G89" s="4" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H89" s="19" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I89" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.35">
@@ -6733,7 +6748,7 @@
         <v>377</v>
       </c>
       <c r="I90" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
@@ -6758,10 +6773,10 @@
         <v>91</v>
       </c>
       <c r="H91" s="17" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="I91" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6786,10 +6801,10 @@
       </c>
       <c r="G92" s="4"/>
       <c r="H92" s="13" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="I92" s="4" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="46" x14ac:dyDescent="0.35">
@@ -6816,7 +6831,7 @@
         <v>218</v>
       </c>
       <c r="H93" s="17" t="s">
-        <v>576</v>
+        <v>567</v>
       </c>
       <c r="I93" s="24"/>
     </row>
@@ -6844,10 +6859,10 @@
         <v>278</v>
       </c>
       <c r="H94" s="36" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="I94" s="37" t="s">
-        <v>577</v>
+        <v>568</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="81" thickTop="1" x14ac:dyDescent="0.35">
@@ -6874,10 +6889,10 @@
         <v>279</v>
       </c>
       <c r="H95" s="21" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="I95" s="4" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="113.15" customHeight="1" x14ac:dyDescent="0.35">
@@ -6904,10 +6919,10 @@
         <v>259</v>
       </c>
       <c r="H96" s="17" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="I96" s="23" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6934,7 +6949,7 @@
         <v>113</v>
       </c>
       <c r="H97" s="17" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I97" s="23"/>
     </row>
@@ -7016,10 +7031,10 @@
       </c>
       <c r="G100" s="4"/>
       <c r="H100" s="19" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="I100" s="4" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="69" x14ac:dyDescent="0.35">
@@ -7031,20 +7046,20 @@
         <v>3</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="E101" s="5"/>
       <c r="F101" s="4" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="G101" s="4" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="H101" s="19" t="s">
-        <v>592</v>
+        <v>583</v>
       </c>
       <c r="I101" s="24"/>
     </row>
@@ -7057,25 +7072,25 @@
         <v>15</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D102" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E102" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="F102" s="4" t="s">
         <v>432</v>
       </c>
-      <c r="F102" s="4" t="s">
+      <c r="G102" s="4" t="s">
         <v>433</v>
       </c>
-      <c r="G102" s="4" t="s">
-        <v>434</v>
-      </c>
       <c r="H102" s="17" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="I102" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -7087,25 +7102,25 @@
         <v>1</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D103" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E103" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="F103" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="F103" s="4" t="s">
+      <c r="G103" s="4" t="s">
         <v>401</v>
-      </c>
-      <c r="G103" s="4" t="s">
-        <v>402</v>
       </c>
       <c r="H103" s="17" t="s">
         <v>352</v>
       </c>
       <c r="I103" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="23" x14ac:dyDescent="0.35">
@@ -7117,25 +7132,25 @@
         <v>17</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D104" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F104" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="G104" s="4" t="s">
         <v>436</v>
       </c>
-      <c r="G104" s="4" t="s">
-        <v>437</v>
-      </c>
       <c r="H104" s="17" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="I104" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="23" x14ac:dyDescent="0.35">
@@ -7147,25 +7162,25 @@
         <v>20</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D105" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F105" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="G105" s="4" t="s">
         <v>441</v>
       </c>
-      <c r="G105" s="4" t="s">
-        <v>442</v>
-      </c>
       <c r="H105" s="17" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="I105" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="106" spans="1:9" ht="37.5" x14ac:dyDescent="0.35">
@@ -7177,22 +7192,22 @@
         <v>21</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D106" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F106" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G106" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H106" s="19" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="I106" s="24"/>
     </row>
@@ -7205,25 +7220,25 @@
         <v>18</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D107" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E107" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="F107" s="4" t="s">
         <v>438</v>
       </c>
-      <c r="F107" s="4" t="s">
+      <c r="G107" s="4" t="s">
         <v>439</v>
       </c>
-      <c r="G107" s="4" t="s">
-        <v>440</v>
-      </c>
       <c r="H107" s="13" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="I107" s="4" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="108" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
@@ -7235,25 +7250,25 @@
         <v>25</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D108" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E108" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="F108" s="4" t="s">
         <v>449</v>
       </c>
-      <c r="F108" s="4" t="s">
+      <c r="G108" s="4" t="s">
         <v>450</v>
       </c>
-      <c r="G108" s="4" t="s">
-        <v>451</v>
-      </c>
       <c r="H108" s="17" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="I108" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="23" x14ac:dyDescent="0.35">
@@ -7265,19 +7280,19 @@
         <v>2</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D109" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E109" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="F109" s="4" t="s">
         <v>403</v>
       </c>
-      <c r="F109" s="4" t="s">
+      <c r="G109" s="4" t="s">
         <v>404</v>
-      </c>
-      <c r="G109" s="4" t="s">
-        <v>405</v>
       </c>
       <c r="H109" s="17" t="s">
         <v>352</v>
@@ -7293,19 +7308,19 @@
         <v>3</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D110" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E110" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="F110" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="F110" s="4" t="s">
+      <c r="G110" s="4" t="s">
         <v>407</v>
-      </c>
-      <c r="G110" s="4" t="s">
-        <v>408</v>
       </c>
       <c r="H110" s="17" t="s">
         <v>352</v>
@@ -7321,19 +7336,19 @@
         <v>4</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D111" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E111" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="F111" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="F111" s="4" t="s">
-        <v>407</v>
-      </c>
       <c r="G111" s="4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="H111" s="17" t="s">
         <v>352</v>
@@ -7364,10 +7379,10 @@
         <v>250</v>
       </c>
       <c r="H112" s="6" t="s">
-        <v>477</v>
-      </c>
-      <c r="I112" s="24" t="s">
-        <v>593</v>
+        <v>476</v>
+      </c>
+      <c r="I112" s="40" t="s">
+        <v>584</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="23" x14ac:dyDescent="0.35">
@@ -7379,19 +7394,19 @@
         <v>5</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D113" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E113" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="F113" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="F113" s="4" t="s">
+      <c r="G113" s="4" t="s">
         <v>411</v>
-      </c>
-      <c r="G113" s="4" t="s">
-        <v>412</v>
       </c>
       <c r="H113" s="17" t="s">
         <v>352</v>
@@ -7407,19 +7422,19 @@
         <v>6</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D114" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E114" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="F114" s="4" t="s">
         <v>413</v>
       </c>
-      <c r="F114" s="4" t="s">
+      <c r="G114" s="4" t="s">
         <v>414</v>
-      </c>
-      <c r="G114" s="4" t="s">
-        <v>415</v>
       </c>
       <c r="H114" s="17" t="s">
         <v>352</v>
@@ -7435,19 +7450,19 @@
         <v>7</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D115" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G115" s="4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="H115" s="17" t="s">
         <v>352</v>
@@ -7463,19 +7478,19 @@
         <v>8</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D116" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E116" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="F116" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="F116" s="4" t="s">
-        <v>418</v>
-      </c>
       <c r="G116" s="4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="H116" s="17" t="s">
         <v>352</v>
@@ -7491,19 +7506,19 @@
         <v>9</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D117" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F117" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G117" s="4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="H117" s="17" t="s">
         <v>352</v>
@@ -7519,22 +7534,22 @@
         <v>10</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D118" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F118" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="G118" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="G118" s="4" t="s">
-        <v>420</v>
-      </c>
       <c r="H118" s="17" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I118" s="24"/>
     </row>
@@ -7547,25 +7562,25 @@
         <v>11</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D119" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E119" s="5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F119" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="G119" s="4" t="s">
         <v>421</v>
       </c>
-      <c r="G119" s="4" t="s">
-        <v>422</v>
-      </c>
       <c r="H119" s="13" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="I119" s="4" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.35">
@@ -7577,19 +7592,19 @@
         <v>12</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D120" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E120" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="F120" s="4" t="s">
         <v>423</v>
       </c>
-      <c r="F120" s="4" t="s">
+      <c r="G120" s="4" t="s">
         <v>424</v>
-      </c>
-      <c r="G120" s="4" t="s">
-        <v>425</v>
       </c>
       <c r="H120" s="17" t="s">
         <v>352</v>
@@ -7605,19 +7620,19 @@
         <v>13</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D121" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E121" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="F121" s="4" t="s">
         <v>426</v>
       </c>
-      <c r="F121" s="4" t="s">
+      <c r="G121" s="4" t="s">
         <v>427</v>
-      </c>
-      <c r="G121" s="4" t="s">
-        <v>428</v>
       </c>
       <c r="H121" s="17" t="s">
         <v>352</v>
@@ -7648,10 +7663,10 @@
         <v>29</v>
       </c>
       <c r="H122" s="19" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I122" s="23" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="123" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
@@ -7678,10 +7693,10 @@
         <v>252</v>
       </c>
       <c r="H123" s="19" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I123" s="23" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="124" spans="1:9" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -7708,10 +7723,10 @@
         <v>104</v>
       </c>
       <c r="H124" s="19" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I124" s="23" t="s">
-        <v>602</v>
+        <v>593</v>
       </c>
     </row>
     <row r="125" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
@@ -7738,10 +7753,10 @@
         <v>162</v>
       </c>
       <c r="H125" s="19" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="I125" s="23" t="s">
-        <v>603</v>
+        <v>594</v>
       </c>
     </row>
     <row r="126" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
@@ -7768,10 +7783,10 @@
         <v>225</v>
       </c>
       <c r="H126" s="19" t="s">
-        <v>578</v>
+        <v>569</v>
       </c>
       <c r="I126" s="23" t="s">
-        <v>604</v>
+        <v>595</v>
       </c>
     </row>
     <row r="127" spans="1:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7798,10 +7813,10 @@
         <v>228</v>
       </c>
       <c r="H127" s="17" t="s">
-        <v>586</v>
+        <v>577</v>
       </c>
       <c r="I127" s="23" t="s">
-        <v>587</v>
+        <v>578</v>
       </c>
     </row>
     <row r="128" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.35">
@@ -7828,10 +7843,10 @@
         <v>10</v>
       </c>
       <c r="H128" s="17" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I128" s="23" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="129" spans="1:9" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -7856,10 +7871,10 @@
       </c>
       <c r="G129" s="4"/>
       <c r="H129" s="19" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="I129" s="23" t="s">
-        <v>601</v>
+        <v>592</v>
       </c>
     </row>
     <row r="130" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
@@ -7884,10 +7899,10 @@
       </c>
       <c r="G130" s="4"/>
       <c r="H130" s="17" t="s">
-        <v>588</v>
+        <v>579</v>
       </c>
       <c r="I130" s="23" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="131" spans="1:9" ht="46" x14ac:dyDescent="0.35">
@@ -7914,10 +7929,10 @@
         <v>136</v>
       </c>
       <c r="H131" s="17" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I131" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="132" spans="1:9" ht="46" x14ac:dyDescent="0.35">
@@ -7944,10 +7959,10 @@
         <v>139</v>
       </c>
       <c r="H132" s="13" t="s">
-        <v>594</v>
+        <v>585</v>
       </c>
       <c r="I132" s="23" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="133" spans="1:9" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -7974,10 +7989,10 @@
         <v>231</v>
       </c>
       <c r="H133" s="17" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="I133" s="24" t="s">
-        <v>579</v>
+        <v>570</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="23" x14ac:dyDescent="0.35">
@@ -8007,7 +8022,7 @@
         <v>352</v>
       </c>
       <c r="I134" s="4" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="23" x14ac:dyDescent="0.35">
@@ -8037,7 +8052,7 @@
         <v>352</v>
       </c>
       <c r="I135" s="4" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
@@ -8064,10 +8079,10 @@
         <v>37</v>
       </c>
       <c r="H136" s="13" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I136" s="4" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="137" spans="1:9" ht="46" x14ac:dyDescent="0.35">
@@ -8094,10 +8109,10 @@
         <v>39</v>
       </c>
       <c r="H137" s="13" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
       <c r="I137" s="4" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="138" spans="1:9" ht="69" x14ac:dyDescent="0.35">
@@ -8124,10 +8139,10 @@
         <v>41</v>
       </c>
       <c r="H138" s="19" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I138" s="4" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="139" spans="1:9" ht="44.15" customHeight="1" x14ac:dyDescent="0.35">
@@ -8152,10 +8167,10 @@
       </c>
       <c r="G139" s="4"/>
       <c r="H139" s="13" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I139" s="4" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="140" spans="1:9" ht="46" x14ac:dyDescent="0.35">
@@ -8182,10 +8197,10 @@
         <v>43</v>
       </c>
       <c r="H140" s="17" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="I140" s="23" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="141" spans="1:9" ht="46" x14ac:dyDescent="0.35">
@@ -8212,10 +8227,10 @@
         <v>31</v>
       </c>
       <c r="H141" s="13" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I141" s="23" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Traitement commentaire DGPR/SRNH/SdcAP/BRIL-12 (reglement ponctuel ou lineaire)
</commit_message>
<xml_diff>
--- a/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
+++ b/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Geostandards-Risques\suivi\2024-05_06-Consultation-publique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6D0513-F3EC-4465-BFCB-8D30B21C0437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C45D0D-C9ED-48CE-85AC-1374FD2E7B44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25875" yWindow="855" windowWidth="21600" windowHeight="11265" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
   </bookViews>
@@ -2117,15 +2117,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">C'est un héritage du PPR Covadis.
-"Certains PPR peuvent parfois contenir des règlements associés à des figurés linéaires ou ponctuels (cavités, axe de ruissellement...). Les primitives graphiques linéaire et ponctuelle sont à utiliser respectivement dans ces cas de figure."
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conserver les zonages réglementaires et surfaciques mais limiter leur usage à la conversion des anciens PPR et à la gestion des petites surfaces sous les seuils de tolérance.
-</t>
-  </si>
-  <si>
     <t>NOK ?
 Je comprends ici AE = Autorité Environnementale (et non pas Aléa Exceptionnel).
 Le novueau standard ne va pas plus loin que l'ancien au niveau du zonage foncier (il ne fait que le séparer de l'autre). La soumission à l'AE n'est pas du ressort ou non du standard il me semble ?
@@ -2352,6 +2343,16 @@
   </si>
   <si>
     <t>inétgré (en partie pour avalanches)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C'est un héritage du PPR Covadis.
+"Certains PPR peuvent parfois contenir des règlements associés à des figurés linéaires ou ponctuels (cavités, axe de ruissellement...). Les primitives graphiques linéaire et ponctuelle sont à utiliser respectivement dans ces cas de figure."
+=&gt; Conserver les zonages réglementaires et surfaciques mais limiter leur usage à la conversion des anciens PPR et à la gestion des petites surfaces sous les seuils de tolérance.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intégré
+</t>
   </si>
 </sst>
 </file>
@@ -3743,10 +3744,10 @@
         <v>335</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4043,10 +4044,10 @@
         <v>328</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4090,8 +4091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815F14A-19BC-4DCE-8D31-81F595A4B0E7}">
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H133" sqref="H133"/>
+    <sheetView tabSelected="1" topLeftCell="B40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4159,7 +4160,7 @@
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="25" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="I2" s="23" t="s">
         <v>505</v>
@@ -4325,7 +4326,7 @@
         <v>45</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="I8" s="23" t="s">
         <v>505</v>
@@ -4677,7 +4678,7 @@
         <v>255</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="I20" s="23" t="s">
         <v>505</v>
@@ -4767,10 +4768,10 @@
         <v>122</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
@@ -5007,7 +5008,7 @@
         <v>78</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="I31" s="23" t="s">
         <v>505</v>
@@ -5037,7 +5038,7 @@
         <v>128</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="I32" s="23" t="s">
         <v>505</v>
@@ -5070,7 +5071,7 @@
         <v>384</v>
       </c>
       <c r="I33" s="23" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="41.15" customHeight="1" x14ac:dyDescent="0.35">
@@ -5183,10 +5184,10 @@
         <v>19</v>
       </c>
       <c r="H37" s="30" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="I37" s="39" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="44.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
@@ -5246,7 +5247,7 @@
         <v>552</v>
       </c>
       <c r="I39" s="23" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="207" x14ac:dyDescent="0.35">
@@ -5273,10 +5274,10 @@
         <v>338</v>
       </c>
       <c r="H40" s="19" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="I40" s="23" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
@@ -5336,7 +5337,7 @@
         <v>553</v>
       </c>
       <c r="I42" s="23" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="111.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5361,10 +5362,10 @@
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="17" t="s">
-        <v>554</v>
-      </c>
-      <c r="I43" s="24" t="s">
-        <v>555</v>
+        <v>603</v>
+      </c>
+      <c r="I43" s="23" t="s">
+        <v>604</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="92" x14ac:dyDescent="0.35">
@@ -5391,7 +5392,7 @@
         <v>26</v>
       </c>
       <c r="H44" s="13" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="I44" s="4" t="s">
         <v>504</v>
@@ -5479,10 +5480,10 @@
         <v>33</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="I47" s="23" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5512,7 +5513,7 @@
         <v>389</v>
       </c>
       <c r="I48" s="23" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="46" x14ac:dyDescent="0.35">
@@ -5572,7 +5573,7 @@
         <v>522</v>
       </c>
       <c r="I50" s="24" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="69" x14ac:dyDescent="0.35">
@@ -5827,10 +5828,10 @@
       </c>
       <c r="G59" s="4"/>
       <c r="H59" s="19" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="I59" s="23" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="61" customHeight="1" x14ac:dyDescent="0.35">
@@ -5860,7 +5861,7 @@
         <v>392</v>
       </c>
       <c r="I60" s="23" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="92" x14ac:dyDescent="0.35">
@@ -5888,7 +5889,7 @@
         <v>395</v>
       </c>
       <c r="I61" s="23" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="230" x14ac:dyDescent="0.35">
@@ -5916,7 +5917,7 @@
         <v>394</v>
       </c>
       <c r="I62" s="24" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
@@ -5946,7 +5947,7 @@
         <v>525</v>
       </c>
       <c r="I63" s="24" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="46" x14ac:dyDescent="0.35">
@@ -5971,7 +5972,7 @@
       </c>
       <c r="G64" s="4"/>
       <c r="H64" s="13" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="I64" s="23" t="s">
         <v>504</v>
@@ -6001,10 +6002,10 @@
         <v>154</v>
       </c>
       <c r="H65" s="19" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="I65" s="24" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="46" x14ac:dyDescent="0.35">
@@ -6181,7 +6182,7 @@
         <v>272</v>
       </c>
       <c r="H71" s="17" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="I71" s="23" t="s">
         <v>505</v>
@@ -6359,7 +6360,7 @@
         <v>275</v>
       </c>
       <c r="H77" s="17" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="I77" s="23" t="s">
         <v>505</v>
@@ -6419,10 +6420,10 @@
         <v>203</v>
       </c>
       <c r="H79" s="17" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="I79" s="40" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
@@ -6512,7 +6513,7 @@
         <v>527</v>
       </c>
       <c r="I82" s="24" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="65.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
@@ -6595,7 +6596,7 @@
         <v>211</v>
       </c>
       <c r="H85" s="19" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="I85" s="23" t="s">
         <v>505</v>
@@ -6831,7 +6832,7 @@
         <v>218</v>
       </c>
       <c r="H93" s="17" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="I93" s="24"/>
     </row>
@@ -6862,7 +6863,7 @@
         <v>472</v>
       </c>
       <c r="I94" s="37" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="81" thickTop="1" x14ac:dyDescent="0.35">
@@ -7059,7 +7060,7 @@
         <v>540</v>
       </c>
       <c r="H101" s="19" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="I101" s="24"/>
     </row>
@@ -7382,7 +7383,7 @@
         <v>476</v>
       </c>
       <c r="I112" s="40" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="23" x14ac:dyDescent="0.35">
@@ -7726,7 +7727,7 @@
         <v>483</v>
       </c>
       <c r="I124" s="23" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="125" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
@@ -7756,7 +7757,7 @@
         <v>484</v>
       </c>
       <c r="I125" s="23" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="126" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
@@ -7783,10 +7784,10 @@
         <v>225</v>
       </c>
       <c r="H126" s="19" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="I126" s="23" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="127" spans="1:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -7813,10 +7814,10 @@
         <v>228</v>
       </c>
       <c r="H127" s="17" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="I127" s="23" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="128" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.35">
@@ -7874,7 +7875,7 @@
         <v>486</v>
       </c>
       <c r="I129" s="23" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="130" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
@@ -7899,7 +7900,7 @@
       </c>
       <c r="G130" s="4"/>
       <c r="H130" s="17" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="I130" s="23" t="s">
         <v>505</v>
@@ -7959,7 +7960,7 @@
         <v>139</v>
       </c>
       <c r="H132" s="13" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I132" s="23" t="s">
         <v>504</v>
@@ -7992,7 +7993,7 @@
         <v>488</v>
       </c>
       <c r="I133" s="24" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="23" x14ac:dyDescent="0.35">
@@ -8109,7 +8110,7 @@
         <v>39</v>
       </c>
       <c r="H137" s="13" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="I137" s="4" t="s">
         <v>521</v>

</xml_diff>

<commit_message>
Traitement : Cerema-15, CEREMA/DTerHdF/ASQT/MET-3, Cerema-16, CEREMA/DTerHdF/ASQT/MET-4 (nuances sur représentation zonage réglementaire)
</commit_message>
<xml_diff>
--- a/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
+++ b/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Geostandards-Risques\suivi\2024-05_06-Consultation-publique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C45D0D-C9ED-48CE-85AC-1374FD2E7B44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4E26B3-D2AE-49AE-B055-F972D3065F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25875" yWindow="855" windowWidth="21600" windowHeight="11265" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Synthese Modele Commun" sheetId="3" r:id="rId1"/>
@@ -2089,9 +2089,6 @@
     <t>intégré (rajouter princpaux)</t>
   </si>
   <si>
-    <t>Mentionner la possibilité de cartographier les PHEC mais sonas les définir + que ça (réf. https://www.reperesdecrues.developpement-durable.gouv.fr/  )</t>
-  </si>
-  <si>
     <t>OK sur le principe. A valider avec le GT
 NB : quid des autres aleéas technos (non industriels) ? 
 Risque technologique ; Nucléaire
@@ -2127,25 +2124,9 @@
 (voir si cela peut-être explicité dans le standard)</t>
   </si>
   <si>
-    <t>Préciser le caractère synthétique des représentations. Différentes réglementation peuvent s'appliquer dans les zones identifiées dans le principe général d'une même interdiction</t>
-  </si>
-  <si>
-    <t>Pas de nuances supplémentaire au niveau du standard. On précise que la possibilité est laissée à la discretion des DDT.</t>
-  </si>
-  <si>
     <t>NOK?
 Qu'entendez-vous par zonage d'exception ?
 A priori il s'agit d'identifie les zones où une demande d'exception est faite par rapport à une interdiction…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OK sur le principe.
-Ah, il doit s'agir de ce zonage d'exception là !
-A étudier mais il manque vraiment la référence de ce décret (cf. commentaires précédent).
-NB : guide Inondation Cet =&gt; représenté toujours en rouge
-</t>
-  </si>
-  <si>
-    <t>Ces zones d'exception sont une sous partie spécifique  des zones répondant au principe général d'interdiction. (Guide PPRICet (p79) )</t>
   </si>
   <si>
     <t>OK sur le principe ?
@@ -2353,6 +2334,28 @@
   <si>
     <t xml:space="preserve">intégré
 </t>
+  </si>
+  <si>
+    <t>Mentionner la possibilité de cartographier les PHEC mais sans les définir + que ça (réf. https://www.reperesdecrues.developpement-durable.gouv.fr/  )</t>
+  </si>
+  <si>
+    <t>intégré (rajout de la mention d'exceptions dans la caégorie).</t>
+  </si>
+  <si>
+    <t>OK sur le principe.
+Ah, il doit s'agir de ce zonage d'exception là !
+A étudier mais il manque vraiment la référence de ce décret (cf. commentaires précédent).
+NB : guide Inondation Cet =&gt; représenté toujours en rouge
+Ces zones d'exception sont une sous partie spécifique  des zones répondant au principe général d'interdiction. (Guide PPRICet (p79) )
+=&gt; NOK (caractère synthétique de la représentation du zonage reglementaire au niveau du standard) =&gt; cf. commentaires précédents</t>
+  </si>
+  <si>
+    <t>Intégré :
+Préciser le caractère synthétique des représentations. Différentes réglementation peuvent s'appliquer dans les zones identifiées dans le principe général d'une même interdiction</t>
+  </si>
+  <si>
+    <t>Intégré :
+Pas de nuances supplémentaire au niveau du standard. On précise que la possibilité est laissée à la discretion des DDT.</t>
   </si>
 </sst>
 </file>
@@ -3469,21 +3472,21 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.453125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.1796875" style="3" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="21.81640625" style="3" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="3" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" style="3" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="3" customWidth="1"/>
-    <col min="5" max="5" width="16.1796875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="49.54296875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="47.54296875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="54.81640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="21.453125" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="10.81640625" style="3"/>
+    <col min="5" max="5" width="16.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="49.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="47.5703125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="54.85546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="10.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>349</v>
       </c>
@@ -3512,7 +3515,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="73" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="72.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-1</v>
@@ -3542,7 +3545,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-2</v>
@@ -3572,7 +3575,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-3</v>
@@ -3602,7 +3605,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="75.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-4</v>
@@ -3632,7 +3635,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="89.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="89.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-5</v>
@@ -3662,7 +3665,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/DAPP/BIP-11</v>
@@ -3690,7 +3693,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="96" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-6</v>
@@ -3720,7 +3723,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="126.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="144" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-7</v>
@@ -3744,13 +3747,13 @@
         <v>335</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-1</v>
@@ -3780,7 +3783,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-2</v>
@@ -3810,7 +3813,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-8</v>
@@ -3840,7 +3843,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>cerema-6</v>
@@ -3870,7 +3873,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="96" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-9</v>
@@ -3900,7 +3903,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="61" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="60.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-10</v>
@@ -3930,7 +3933,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="68.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="68.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-3</v>
@@ -3960,7 +3963,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="77.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="77.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-4</v>
@@ -3990,7 +3993,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="111" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>Cerema-5</v>
@@ -4020,7 +4023,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="96" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SDCAP/PONSOH-13</v>
@@ -4044,13 +4047,13 @@
         <v>328</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau3[[#This Row],[Organisme]],"-",Tableau3[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/DAPP/BIP-12</v>
@@ -4091,25 +4094,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815F14A-19BC-4DCE-8D31-81F595A4B0E7}">
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="B62" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I62" sqref="I62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.54296875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="3.81640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="16" style="3" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="44.1796875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="44.140625" style="3" customWidth="1"/>
     <col min="7" max="7" width="38" style="3" customWidth="1"/>
-    <col min="8" max="8" width="51.81640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="22.26953125" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="10.81640625" style="3"/>
+    <col min="8" max="8" width="51.85546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="10.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>348</v>
       </c>
@@ -4138,7 +4141,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-2</v>
@@ -4160,13 +4163,13 @@
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="25" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="I2" s="23" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-3</v>
@@ -4194,7 +4197,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-4</v>
@@ -4222,7 +4225,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="65.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-5</v>
@@ -4246,11 +4249,11 @@
       <c r="H5" s="22" t="s">
         <v>501</v>
       </c>
-      <c r="I5" s="24" t="s">
+      <c r="I5" s="40" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="126.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="132" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP-0</v>
@@ -4276,7 +4279,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-9</v>
@@ -4304,7 +4307,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="84" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-14</v>
@@ -4326,13 +4329,13 @@
         <v>45</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="I8" s="23" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-15</v>
@@ -4360,7 +4363,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDTM11-1</v>
@@ -4388,7 +4391,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-2</v>
@@ -4416,7 +4419,7 @@
       </c>
       <c r="I11" s="24"/>
     </row>
-    <row r="12" spans="1:9" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-3</v>
@@ -4444,7 +4447,7 @@
       </c>
       <c r="I12" s="24"/>
     </row>
-    <row r="13" spans="1:9" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-1</v>
@@ -4474,7 +4477,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="66.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-1</v>
@@ -4504,7 +4507,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="161" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="168" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-2</v>
@@ -4534,7 +4537,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-3</v>
@@ -4564,7 +4567,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-1</v>
@@ -4594,7 +4597,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-4</v>
@@ -4624,7 +4627,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-4</v>
@@ -4654,7 +4657,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-5</v>
@@ -4678,13 +4681,13 @@
         <v>255</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="I20" s="23" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="84" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-6</v>
@@ -4714,7 +4717,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-2</v>
@@ -4744,7 +4747,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="84" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-3</v>
@@ -4768,13 +4771,13 @@
         <v>122</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-5</v>
@@ -4804,7 +4807,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-4</v>
@@ -4834,7 +4837,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-5</v>
@@ -4864,7 +4867,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="71.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="71.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-7</v>
@@ -4894,7 +4897,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-6</v>
@@ -4924,7 +4927,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="115" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-1</v>
@@ -4951,10 +4954,10 @@
         <v>517</v>
       </c>
       <c r="I29" s="24" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-8</v>
@@ -4984,7 +4987,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-9</v>
@@ -5008,13 +5011,13 @@
         <v>78</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="I31" s="23" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="84" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-6</v>
@@ -5038,13 +5041,13 @@
         <v>128</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="I32" s="23" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-7</v>
@@ -5071,10 +5074,10 @@
         <v>384</v>
       </c>
       <c r="I33" s="23" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="41.15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-10</v>
@@ -5102,7 +5105,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-7</v>
@@ -5132,7 +5135,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="62.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:9" ht="62.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-11</v>
@@ -5160,7 +5163,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="31" customFormat="1" ht="115.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:9" s="31" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="26" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-1</v>
@@ -5184,13 +5187,13 @@
         <v>19</v>
       </c>
       <c r="H37" s="30" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="I37" s="39" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="44.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="44.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-21</v>
@@ -5214,13 +5217,13 @@
         <v>99</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I38" s="4" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-2</v>
@@ -5244,13 +5247,13 @@
         <v>338</v>
       </c>
       <c r="H39" s="19" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="I39" s="23" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="207" x14ac:dyDescent="0.35">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="228" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 31-3</v>
@@ -5274,13 +5277,13 @@
         <v>338</v>
       </c>
       <c r="H40" s="19" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="I40" s="23" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-8</v>
@@ -5304,13 +5307,13 @@
         <v>267</v>
       </c>
       <c r="H41" s="17" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I41" s="23" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-8</v>
@@ -5334,13 +5337,13 @@
         <v>133</v>
       </c>
       <c r="H42" s="19" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="I42" s="23" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="111.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-12</v>
@@ -5362,13 +5365,13 @@
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="17" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
       <c r="I43" s="23" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-4</v>
@@ -5392,13 +5395,13 @@
         <v>26</v>
       </c>
       <c r="H44" s="13" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="I44" s="4" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="77.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-2</v>
@@ -5428,7 +5431,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/BRNT-22</v>
@@ -5456,7 +5459,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" ht="84" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-8</v>
@@ -5480,13 +5483,13 @@
         <v>33</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="I47" s="23" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-24</v>
@@ -5513,10 +5516,10 @@
         <v>389</v>
       </c>
       <c r="I48" s="23" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-3</v>
@@ -5546,7 +5549,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="117.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" ht="117.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-5</v>
@@ -5573,10 +5576,10 @@
         <v>522</v>
       </c>
       <c r="I50" s="24" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="84" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT07-2</v>
@@ -5606,7 +5609,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-11</v>
@@ -5634,7 +5637,7 @@
       </c>
       <c r="I52" s="24"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-12</v>
@@ -5662,7 +5665,7 @@
       </c>
       <c r="I53" s="24"/>
     </row>
-    <row r="54" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-13</v>
@@ -5692,7 +5695,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-13</v>
@@ -5720,7 +5723,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-14</v>
@@ -5748,7 +5751,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-15</v>
@@ -5776,7 +5779,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-9</v>
@@ -5806,7 +5809,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="184" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" ht="216" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -1</v>
@@ -5828,13 +5831,13 @@
       </c>
       <c r="G59" s="4"/>
       <c r="H59" s="19" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="I59" s="23" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" ht="61" customHeight="1" x14ac:dyDescent="0.35">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="60.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-14</v>
@@ -5861,10 +5864,10 @@
         <v>392</v>
       </c>
       <c r="I60" s="23" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" ht="92" x14ac:dyDescent="0.35">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="108" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -2</v>
@@ -5889,10 +5892,10 @@
         <v>395</v>
       </c>
       <c r="I61" s="23" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" ht="230" x14ac:dyDescent="0.35">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="252" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -3</v>
@@ -5916,11 +5919,11 @@
       <c r="H62" s="13" t="s">
         <v>394</v>
       </c>
-      <c r="I62" s="24" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+      <c r="I62" s="23" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="96" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-15</v>
@@ -5946,11 +5949,11 @@
       <c r="H63" s="19" t="s">
         <v>525</v>
       </c>
-      <c r="I63" s="24" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+      <c r="I63" s="23" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>CEREMA/DTerHdF/ASQT/MET -4</v>
@@ -5972,13 +5975,13 @@
       </c>
       <c r="G64" s="4"/>
       <c r="H64" s="13" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="I64" s="23" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" ht="132" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-16</v>
@@ -6002,13 +6005,13 @@
         <v>154</v>
       </c>
       <c r="H65" s="19" t="s">
-        <v>559</v>
-      </c>
-      <c r="I65" s="24" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+        <v>602</v>
+      </c>
+      <c r="I65" s="23" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT01-3</v>
@@ -6038,7 +6041,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDTM 83-1</v>
@@ -6068,7 +6071,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="174" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-10</v>
@@ -6098,7 +6101,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="88" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" ht="87.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT 42-1</v>
@@ -6128,7 +6131,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="103" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" ht="102.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-11</v>
@@ -6158,7 +6161,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="103.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-12</v>
@@ -6182,13 +6185,13 @@
         <v>272</v>
       </c>
       <c r="H71" s="17" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="I71" s="23" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-13</v>
@@ -6218,7 +6221,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A73" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-14</v>
@@ -6248,7 +6251,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A74" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-19</v>
@@ -6278,7 +6281,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A75" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-16</v>
@@ -6308,7 +6311,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-14</v>
@@ -6336,7 +6339,7 @@
       </c>
       <c r="I76" s="23"/>
     </row>
-    <row r="77" spans="1:9" ht="126.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" ht="144" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-15</v>
@@ -6360,13 +6363,13 @@
         <v>275</v>
       </c>
       <c r="H77" s="17" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="I77" s="23" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A78" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDTM11-2</v>
@@ -6396,7 +6399,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-16</v>
@@ -6420,13 +6423,13 @@
         <v>203</v>
       </c>
       <c r="H79" s="17" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="I79" s="40" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A80" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-22</v>
@@ -6456,7 +6459,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="26" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" ht="27" x14ac:dyDescent="0.25">
       <c r="A81" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-23</v>
@@ -6486,7 +6489,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A82" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-24</v>
@@ -6513,10 +6516,10 @@
         <v>527</v>
       </c>
       <c r="I82" s="24" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" ht="65.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-17</v>
@@ -6544,7 +6547,7 @@
       </c>
       <c r="I83" s="24"/>
     </row>
-    <row r="84" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-18</v>
@@ -6572,7 +6575,7 @@
       </c>
       <c r="I84" s="24"/>
     </row>
-    <row r="85" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-19</v>
@@ -6596,13 +6599,13 @@
         <v>211</v>
       </c>
       <c r="H85" s="19" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="I85" s="23" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-20</v>
@@ -6632,7 +6635,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="36.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-27</v>
@@ -6662,7 +6665,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-21</v>
@@ -6692,7 +6695,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="39.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-26</v>
@@ -6722,7 +6725,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-17</v>
@@ -6752,7 +6755,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-16</v>
@@ -6780,7 +6783,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:9" ht="77.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-17</v>
@@ -6808,7 +6811,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-22</v>
@@ -6832,11 +6835,11 @@
         <v>218</v>
       </c>
       <c r="H93" s="17" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="I93" s="24"/>
     </row>
-    <row r="94" spans="1:9" s="38" customFormat="1" ht="98.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:9" s="38" customFormat="1" ht="98.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="32" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-23</v>
@@ -6863,10 +6866,10 @@
         <v>472</v>
       </c>
       <c r="I94" s="37" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" ht="81" thickTop="1" x14ac:dyDescent="0.35">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="96.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-24</v>
@@ -6896,7 +6899,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="113.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9" ht="113.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/PoNSOH-26</v>
@@ -6926,7 +6929,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/PoNSOH-27</v>
@@ -6954,7 +6957,7 @@
       </c>
       <c r="I97" s="23"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-18</v>
@@ -6982,7 +6985,7 @@
       </c>
       <c r="I98" s="24"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-19</v>
@@ -7010,7 +7013,7 @@
       </c>
       <c r="I99" s="24"/>
     </row>
-    <row r="100" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-18</v>
@@ -7038,7 +7041,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A101" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDTM11-3</v>
@@ -7060,11 +7063,11 @@
         <v>540</v>
       </c>
       <c r="H101" s="19" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="I101" s="24"/>
     </row>
-    <row r="102" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A102" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-15</v>
@@ -7094,7 +7097,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-1</v>
@@ -7124,7 +7127,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A104" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-17</v>
@@ -7154,7 +7157,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A105" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-20</v>
@@ -7184,7 +7187,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="37.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9" ht="39" x14ac:dyDescent="0.25">
       <c r="A106" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-21</v>
@@ -7212,7 +7215,7 @@
       </c>
       <c r="I106" s="24"/>
     </row>
-    <row r="107" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A107" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-18</v>
@@ -7242,7 +7245,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A108" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-25</v>
@@ -7272,7 +7275,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A109" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-2</v>
@@ -7300,7 +7303,7 @@
       </c>
       <c r="I109" s="24"/>
     </row>
-    <row r="110" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A110" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-3</v>
@@ -7328,7 +7331,7 @@
       </c>
       <c r="I110" s="24"/>
     </row>
-    <row r="111" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A111" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-4</v>
@@ -7356,7 +7359,7 @@
       </c>
       <c r="I111" s="24"/>
     </row>
-    <row r="112" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:9" ht="84" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT01-1</v>
@@ -7383,10 +7386,10 @@
         <v>476</v>
       </c>
       <c r="I112" s="40" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A113" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-5</v>
@@ -7414,7 +7417,7 @@
       </c>
       <c r="I113" s="24"/>
     </row>
-    <row r="114" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A114" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-6</v>
@@ -7442,7 +7445,7 @@
       </c>
       <c r="I114" s="24"/>
     </row>
-    <row r="115" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A115" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-7</v>
@@ -7470,7 +7473,7 @@
       </c>
       <c r="I115" s="24"/>
     </row>
-    <row r="116" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A116" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-8</v>
@@ -7498,7 +7501,7 @@
       </c>
       <c r="I116" s="24"/>
     </row>
-    <row r="117" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A117" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-9</v>
@@ -7526,7 +7529,7 @@
       </c>
       <c r="I117" s="24"/>
     </row>
-    <row r="118" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A118" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-10</v>
@@ -7554,7 +7557,7 @@
       </c>
       <c r="I118" s="24"/>
     </row>
-    <row r="119" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-11</v>
@@ -7584,7 +7587,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A120" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-12</v>
@@ -7612,7 +7615,7 @@
       </c>
       <c r="I120" s="24"/>
     </row>
-    <row r="121" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A121" s="20" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Ineris-13</v>
@@ -7640,7 +7643,7 @@
       </c>
       <c r="I121" s="24"/>
     </row>
-    <row r="122" spans="1:9" ht="151.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-6</v>
@@ -7670,7 +7673,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="123" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT01-2</v>
@@ -7700,7 +7703,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="124" spans="1:9" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:9" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-23</v>
@@ -7727,10 +7730,10 @@
         <v>483</v>
       </c>
       <c r="I124" s="23" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9" ht="80.5" x14ac:dyDescent="0.35">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" ht="96" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-20</v>
@@ -7757,10 +7760,10 @@
         <v>484</v>
       </c>
       <c r="I125" s="23" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9" ht="57.5" x14ac:dyDescent="0.35">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-25</v>
@@ -7784,13 +7787,13 @@
         <v>225</v>
       </c>
       <c r="H126" s="19" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="I126" s="23" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-26</v>
@@ -7814,13 +7817,13 @@
         <v>228</v>
       </c>
       <c r="H127" s="17" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="I127" s="23" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT07-1</v>
@@ -7850,7 +7853,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-19</v>
@@ -7875,10 +7878,10 @@
         <v>486</v>
       </c>
       <c r="I129" s="23" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdcAP/BRIL-20</v>
@@ -7900,13 +7903,13 @@
       </c>
       <c r="G130" s="4"/>
       <c r="H130" s="17" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="I130" s="23" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="131" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-9</v>
@@ -7936,7 +7939,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="132" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-10</v>
@@ -7960,13 +7963,13 @@
         <v>139</v>
       </c>
       <c r="H132" s="13" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="I132" s="23" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="133" spans="1:9" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-27</v>
@@ -7993,10 +7996,10 @@
         <v>488</v>
       </c>
       <c r="I133" s="24" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-28</v>
@@ -8026,7 +8029,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="135" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-29</v>
@@ -8056,7 +8059,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="136" spans="1:9" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-10</v>
@@ -8086,7 +8089,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="137" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-11</v>
@@ -8110,13 +8113,13 @@
         <v>39</v>
       </c>
       <c r="H137" s="13" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="I137" s="4" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="69" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-12</v>
@@ -8146,7 +8149,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="139" spans="1:9" ht="44.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:9" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DGPR/SRNH/SdCAP/BRNT-25</v>
@@ -8174,7 +8177,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="140" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-13</v>
@@ -8204,7 +8207,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="141" spans="1:9" ht="46" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:9" ht="48" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-7</v>

</xml_diff>

<commit_message>
Traitement DDT38-17 et DDT38-18 (clefs primaires)
</commit_message>
<xml_diff>
--- a/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
+++ b/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Geostandards-Risques\suivi\2024-05_06-Consultation-publique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B96DF8D-BA63-4DDA-8EEC-6F2ECFD681DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BB07C6-DEC1-4896-BAD2-7653204B9812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="605">
   <si>
     <t>Organisme</t>
   </si>
@@ -4094,8 +4094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815F14A-19BC-4DCE-8D31-81F595A4B0E7}">
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H85" sqref="H85"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6545,7 +6545,9 @@
       <c r="H83" s="17" t="s">
         <v>466</v>
       </c>
-      <c r="I83" s="24"/>
+      <c r="I83" s="23" t="s">
+        <v>505</v>
+      </c>
     </row>
     <row r="84" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="str">
@@ -6573,7 +6575,9 @@
       <c r="H84" s="17" t="s">
         <v>467</v>
       </c>
-      <c r="I84" s="24"/>
+      <c r="I84" s="23" t="s">
+        <v>505</v>
+      </c>
     </row>
     <row r="85" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="str">

</xml_diff>

<commit_message>
Traitement DDT 31-1 (PHEC)
</commit_message>
<xml_diff>
--- a/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
+++ b/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Geostandards-Risques\suivi\2024-05_06-Consultation-publique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A3E3AD-70BB-4EAC-B085-3743B015CDE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A94BFDB-EE0E-4985-B1E6-C98FEF8B645B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
   </bookViews>
@@ -2219,9 +2219,6 @@
 Le GPU diffuse des servitudes d'utilité publiques (SUP) au sens de l'article L152-7 du code de l'irbanisme. Ces documents ont leur structure et standard propre. Certaines peuvent être dérivées de PPR auxquelles elles peuvent faire référence. Mais les ces PPR ne sont pas sur le GPU (plutôt sur Georisques)</t>
   </si>
   <si>
-    <t>Expliciter cette différence GPU SUP et PPR et faire référence à l'annexe sur le passage PPR -&gt; SUP PM1/PM3)</t>
-  </si>
-  <si>
     <t>OK sur le principe
 A voir au cas par cas. 
 Préciser ce qui relève de la valeur "nulle" et la valeur "inconnue".</t>
@@ -2326,9 +2323,6 @@
   <si>
     <t xml:space="preserve">intégré
 </t>
-  </si>
-  <si>
-    <t>Mentionner la possibilité de cartographier les PHEC mais sans les définir + que ça (réf. https://www.reperesdecrues.developpement-durable.gouv.fr/  )</t>
   </si>
   <si>
     <t>intégré (rajout de la mention d'exceptions dans la caégorie).</t>
@@ -2359,6 +2353,13 @@
   </si>
   <si>
     <t>Intégré : nul ou négligeable</t>
+  </si>
+  <si>
+    <t>intégré : Expliciter cette différence GPU SUP et PPR et faire référence à l'annexe sur le passage PPR -&gt; SUP PM1/PM3)</t>
+  </si>
+  <si>
+    <t>Intégré :
+Mentionner la possibilité de cartographier les PHEC mais sans les définir + que ça (réf. https://www.reperesdecrues.developpement-durable.gouv.fr/  )</t>
   </si>
 </sst>
 </file>
@@ -2551,7 +2552,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2665,6 +2666,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4053,7 +4057,7 @@
         <v>563</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4097,8 +4101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815F14A-19BC-4DCE-8D31-81F595A4B0E7}">
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H94" sqref="H94"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4166,7 +4170,7 @@
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="25" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="I2" s="23" t="s">
         <v>505</v>
@@ -4332,7 +4336,7 @@
         <v>45</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I8" s="23" t="s">
         <v>505</v>
@@ -4750,7 +4754,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="84" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>Cerema-3</v>
@@ -4776,8 +4780,8 @@
       <c r="H23" s="13" t="s">
         <v>572</v>
       </c>
-      <c r="I23" s="24" t="s">
-        <v>573</v>
+      <c r="I23" s="23" t="s">
+        <v>604</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -4953,11 +4957,11 @@
       <c r="G29" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="H29" s="19" t="s">
+      <c r="H29" s="41" t="s">
         <v>517</v>
       </c>
-      <c r="I29" s="24" t="s">
-        <v>598</v>
+      <c r="I29" s="23" t="s">
+        <v>605</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5077,7 +5081,7 @@
         <v>384</v>
       </c>
       <c r="I33" s="23" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -5190,10 +5194,10 @@
         <v>19</v>
       </c>
       <c r="H37" s="30" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="I37" s="38" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="44.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -5253,7 +5257,7 @@
         <v>550</v>
       </c>
       <c r="I39" s="23" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="228" x14ac:dyDescent="0.25">
@@ -5280,10 +5284,10 @@
         <v>338</v>
       </c>
       <c r="H40" s="19" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="I40" s="23" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="108" x14ac:dyDescent="0.25">
@@ -5343,7 +5347,7 @@
         <v>551</v>
       </c>
       <c r="I42" s="23" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5368,10 +5372,10 @@
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="17" t="s">
+        <v>595</v>
+      </c>
+      <c r="I43" s="23" t="s">
         <v>596</v>
-      </c>
-      <c r="I43" s="23" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="108" x14ac:dyDescent="0.25">
@@ -5486,10 +5490,10 @@
         <v>33</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="I47" s="23" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5519,7 +5523,7 @@
         <v>389</v>
       </c>
       <c r="I48" s="23" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -5834,10 +5838,10 @@
       </c>
       <c r="G59" s="4"/>
       <c r="H59" s="19" t="s">
+        <v>591</v>
+      </c>
+      <c r="I59" s="23" t="s">
         <v>592</v>
-      </c>
-      <c r="I59" s="23" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="60.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -5867,7 +5871,7 @@
         <v>392</v>
       </c>
       <c r="I60" s="23" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="108" x14ac:dyDescent="0.25">
@@ -5895,7 +5899,7 @@
         <v>395</v>
       </c>
       <c r="I61" s="23" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="252" x14ac:dyDescent="0.25">
@@ -5923,7 +5927,7 @@
         <v>394</v>
       </c>
       <c r="I62" s="23" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="96" x14ac:dyDescent="0.25">
@@ -5953,7 +5957,7 @@
         <v>525</v>
       </c>
       <c r="I63" s="23" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -6008,10 +6012,10 @@
         <v>154</v>
       </c>
       <c r="H65" s="19" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="I65" s="23" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -6188,7 +6192,7 @@
         <v>272</v>
       </c>
       <c r="H71" s="17" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="I71" s="23" t="s">
         <v>505</v>
@@ -6429,7 +6433,7 @@
         <v>556</v>
       </c>
       <c r="I79" s="39" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="36" x14ac:dyDescent="0.25">
@@ -6516,10 +6520,10 @@
         <v>447</v>
       </c>
       <c r="H82" s="19" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="I82" s="23" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -6845,7 +6849,7 @@
         <v>558</v>
       </c>
       <c r="I93" s="23" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="94" spans="1:9" s="37" customFormat="1" ht="98.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7072,7 +7076,7 @@
         <v>539</v>
       </c>
       <c r="H101" s="19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I101" s="24"/>
     </row>
@@ -7222,7 +7226,7 @@
       <c r="H106" s="19" t="s">
         <v>478</v>
       </c>
-      <c r="I106" s="24"/>
+      <c r="I106" s="39"/>
     </row>
     <row r="107" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A107" s="20" t="str">
@@ -7395,7 +7399,7 @@
         <v>476</v>
       </c>
       <c r="I112" s="39" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="24" x14ac:dyDescent="0.25">
@@ -7739,7 +7743,7 @@
         <v>483</v>
       </c>
       <c r="I124" s="23" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="125" spans="1:9" ht="96" x14ac:dyDescent="0.25">
@@ -7769,7 +7773,7 @@
         <v>484</v>
       </c>
       <c r="I125" s="23" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="126" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -7799,7 +7803,7 @@
         <v>560</v>
       </c>
       <c r="I126" s="23" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="127" spans="1:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7887,7 +7891,7 @@
         <v>486</v>
       </c>
       <c r="I129" s="23" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="130" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -7972,7 +7976,7 @@
         <v>139</v>
       </c>
       <c r="H132" s="13" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I132" s="23" t="s">
         <v>504</v>

</xml_diff>

<commit_message>
Traitement DDT74-5 (millésime données sources)
</commit_message>
<xml_diff>
--- a/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
+++ b/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Geostandards-Risques\suivi\2024-05_06-Consultation-publique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA565A70-302E-41D2-A7AA-E420C32D9BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E07E3C3-9EF6-48FA-A90B-DAFF0D2FB961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
   </bookViews>
@@ -2112,10 +2112,6 @@
 A priori l'expropriation ne concerne que les PPRT, pas les PPRN</t>
   </si>
   <si>
-    <t>N.A.
-(voir si cela peut-être explicité dans le standard)</t>
-  </si>
-  <si>
     <t>NOK?
 Qu'entendez-vous par zonage d'exception ?
 A priori il s'agit d'identifie les zones où une demande d'exception est faite par rapport à une interdiction…</t>
@@ -2361,6 +2357,9 @@
   </si>
   <si>
     <t>intégré : ajout d'un champ identifiant dans le gabarit SQL</t>
+  </si>
+  <si>
+    <t>intégré : mention du millésime du référentiel source dans la parti métadonnées</t>
   </si>
 </sst>
 </file>
@@ -3755,10 +3754,10 @@
         <v>335</v>
       </c>
       <c r="H9" s="17" t="s">
+        <v>561</v>
+      </c>
+      <c r="I9" s="23" t="s">
         <v>562</v>
-      </c>
-      <c r="I9" s="23" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4055,10 +4054,10 @@
         <v>328</v>
       </c>
       <c r="H19" s="25" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4102,8 +4101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815F14A-19BC-4DCE-8D31-81F595A4B0E7}">
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G135" sqref="G135"/>
+    <sheetView tabSelected="1" topLeftCell="B49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4171,7 +4170,7 @@
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="25" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I2" s="23" t="s">
         <v>504</v>
@@ -4337,7 +4336,7 @@
         <v>45</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="I8" s="23" t="s">
         <v>504</v>
@@ -4689,7 +4688,7 @@
         <v>255</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="I20" s="23" t="s">
         <v>504</v>
@@ -4779,10 +4778,10 @@
         <v>122</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="I23" s="23" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -4962,7 +4961,7 @@
         <v>516</v>
       </c>
       <c r="I29" s="23" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5019,7 +5018,7 @@
         <v>78</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="I31" s="23" t="s">
         <v>504</v>
@@ -5049,7 +5048,7 @@
         <v>128</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="I32" s="23" t="s">
         <v>504</v>
@@ -5082,7 +5081,7 @@
         <v>384</v>
       </c>
       <c r="I33" s="23" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -5195,10 +5194,10 @@
         <v>19</v>
       </c>
       <c r="H37" s="30" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="I37" s="38" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="44.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -5258,7 +5257,7 @@
         <v>549</v>
       </c>
       <c r="I39" s="23" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="228" x14ac:dyDescent="0.25">
@@ -5285,10 +5284,10 @@
         <v>338</v>
       </c>
       <c r="H40" s="19" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="I40" s="23" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="108" x14ac:dyDescent="0.25">
@@ -5348,7 +5347,7 @@
         <v>550</v>
       </c>
       <c r="I42" s="23" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5373,10 +5372,10 @@
       </c>
       <c r="G43" s="4"/>
       <c r="H43" s="17" t="s">
+        <v>592</v>
+      </c>
+      <c r="I43" s="23" t="s">
         <v>593</v>
-      </c>
-      <c r="I43" s="23" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="108" x14ac:dyDescent="0.25">
@@ -5491,10 +5490,10 @@
         <v>33</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="I47" s="23" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5524,7 +5523,7 @@
         <v>389</v>
       </c>
       <c r="I48" s="23" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -5583,8 +5582,8 @@
       <c r="H50" s="17" t="s">
         <v>521</v>
       </c>
-      <c r="I50" s="24" t="s">
-        <v>552</v>
+      <c r="I50" s="23" t="s">
+        <v>605</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="84" x14ac:dyDescent="0.25">
@@ -5839,10 +5838,10 @@
       </c>
       <c r="G59" s="4"/>
       <c r="H59" s="19" t="s">
+        <v>588</v>
+      </c>
+      <c r="I59" s="23" t="s">
         <v>589</v>
-      </c>
-      <c r="I59" s="23" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="60.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -5872,7 +5871,7 @@
         <v>392</v>
       </c>
       <c r="I60" s="23" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="108" x14ac:dyDescent="0.25">
@@ -5900,7 +5899,7 @@
         <v>395</v>
       </c>
       <c r="I61" s="23" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="252" x14ac:dyDescent="0.25">
@@ -5928,7 +5927,7 @@
         <v>394</v>
       </c>
       <c r="I62" s="23" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="96" x14ac:dyDescent="0.25">
@@ -5958,7 +5957,7 @@
         <v>524</v>
       </c>
       <c r="I63" s="23" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -5983,7 +5982,7 @@
       </c>
       <c r="G64" s="4"/>
       <c r="H64" s="13" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="I64" s="23" t="s">
         <v>503</v>
@@ -6013,10 +6012,10 @@
         <v>154</v>
       </c>
       <c r="H65" s="19" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="I65" s="23" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="48" x14ac:dyDescent="0.25">
@@ -6193,7 +6192,7 @@
         <v>272</v>
       </c>
       <c r="H71" s="17" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="I71" s="23" t="s">
         <v>504</v>
@@ -6371,7 +6370,7 @@
         <v>275</v>
       </c>
       <c r="H77" s="17" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="I77" s="23" t="s">
         <v>504</v>
@@ -6431,10 +6430,10 @@
         <v>203</v>
       </c>
       <c r="H79" s="17" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I79" s="39" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="36" x14ac:dyDescent="0.25">
@@ -6521,10 +6520,10 @@
         <v>447</v>
       </c>
       <c r="H82" s="19" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="I82" s="23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -6611,7 +6610,7 @@
         <v>211</v>
       </c>
       <c r="H85" s="19" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I85" s="23" t="s">
         <v>504</v>
@@ -6847,10 +6846,10 @@
         <v>218</v>
       </c>
       <c r="H93" s="17" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I93" s="23" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="94" spans="1:9" s="37" customFormat="1" ht="98.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6880,7 +6879,7 @@
         <v>472</v>
       </c>
       <c r="I94" s="40" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="96.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -7077,7 +7076,7 @@
         <v>538</v>
       </c>
       <c r="H101" s="19" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="I101" s="24"/>
     </row>
@@ -7400,7 +7399,7 @@
         <v>476</v>
       </c>
       <c r="I112" s="39" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="24" x14ac:dyDescent="0.25">
@@ -7744,7 +7743,7 @@
         <v>483</v>
       </c>
       <c r="I124" s="23" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="125" spans="1:9" ht="96" x14ac:dyDescent="0.25">
@@ -7774,7 +7773,7 @@
         <v>484</v>
       </c>
       <c r="I125" s="23" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="126" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -7801,10 +7800,10 @@
         <v>225</v>
       </c>
       <c r="H126" s="19" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="I126" s="23" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="127" spans="1:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7831,10 +7830,10 @@
         <v>228</v>
       </c>
       <c r="H127" s="17" t="s">
+        <v>565</v>
+      </c>
+      <c r="I127" s="23" t="s">
         <v>566</v>
-      </c>
-      <c r="I127" s="23" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="128" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
@@ -7892,7 +7891,7 @@
         <v>486</v>
       </c>
       <c r="I129" s="23" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="130" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -7917,7 +7916,7 @@
       </c>
       <c r="G130" s="4"/>
       <c r="H130" s="17" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="I130" s="23" t="s">
         <v>504</v>
@@ -7977,7 +7976,7 @@
         <v>139</v>
       </c>
       <c r="H132" s="13" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="I132" s="23" t="s">
         <v>503</v>
@@ -8007,10 +8006,10 @@
         <v>231</v>
       </c>
       <c r="H133" s="19" t="s">
+        <v>603</v>
+      </c>
+      <c r="I133" s="23" t="s">
         <v>604</v>
-      </c>
-      <c r="I133" s="23" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="24" x14ac:dyDescent="0.25">
@@ -8127,7 +8126,7 @@
         <v>39</v>
       </c>
       <c r="H137" s="13" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="I137" s="4" t="s">
         <v>520</v>

</xml_diff>

<commit_message>
génération version PPR v0.3 pour validation CNIG
</commit_message>
<xml_diff>
--- a/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
+++ b/suivi/2024-05_06-Consultation-publique/Synthes-Commentaires-ModeleCommun-PPR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Geostandards-Risques\suivi\2024-05_06-Consultation-publique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E07E3C3-9EF6-48FA-A90B-DAFF0D2FB961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{343219E2-0AAE-4372-89DE-D219925D6113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{1EA775A6-9D8D-4CA4-9DA3-4042083F20FC}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="607">
   <si>
     <t>Organisme</t>
   </si>
@@ -2360,6 +2360,9 @@
   </si>
   <si>
     <t>intégré : mention du millésime du référentiel source dans la parti métadonnées</t>
+  </si>
+  <si>
+    <t>Désolé PB de numérotation</t>
   </si>
 </sst>
 </file>
@@ -2460,18 +2463,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -2552,7 +2549,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2621,9 +2618,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2662,7 +2656,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4053,7 +4047,7 @@
       <c r="G19" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="H19" s="25" t="s">
+      <c r="H19" s="24" t="s">
         <v>560</v>
       </c>
       <c r="I19" s="23" t="s">
@@ -4101,8 +4095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815F14A-19BC-4DCE-8D31-81F595A4B0E7}">
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+    <sheetView tabSelected="1" topLeftCell="B124" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4169,7 +4163,7 @@
         <v>242</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="24" t="s">
         <v>585</v>
       </c>
       <c r="I2" s="23" t="s">
@@ -4256,7 +4250,7 @@
       <c r="H5" s="22" t="s">
         <v>500</v>
       </c>
-      <c r="I5" s="39" t="s">
+      <c r="I5" s="38" t="s">
         <v>541</v>
       </c>
     </row>
@@ -4424,7 +4418,9 @@
       <c r="H11" s="17" t="s">
         <v>375</v>
       </c>
-      <c r="I11" s="24"/>
+      <c r="I11" s="38" t="s">
+        <v>606</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="str">
@@ -4452,7 +4448,9 @@
       <c r="H12" s="17" t="s">
         <v>376</v>
       </c>
-      <c r="I12" s="24"/>
+      <c r="I12" s="4" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="str">
@@ -4957,7 +4955,7 @@
       <c r="G29" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="H29" s="41" t="s">
+      <c r="H29" s="40" t="s">
         <v>516</v>
       </c>
       <c r="I29" s="23" t="s">
@@ -5170,33 +5168,33 @@
         <v>504</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="31" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="26" t="str">
+    <row r="37" spans="1:9" s="30" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="25" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT74-1</v>
       </c>
-      <c r="B37" s="27">
+      <c r="B37" s="26">
         <v>1</v>
       </c>
-      <c r="C37" s="28" t="s">
+      <c r="C37" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D37" s="29" t="s">
+      <c r="D37" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E37" s="29" t="s">
+      <c r="E37" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="F37" s="28" t="s">
+      <c r="F37" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="G37" s="28" t="s">
+      <c r="G37" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="H37" s="30" t="s">
+      <c r="H37" s="29" t="s">
         <v>584</v>
       </c>
-      <c r="I37" s="38" t="s">
+      <c r="I37" s="37" t="s">
         <v>583</v>
       </c>
     </row>
@@ -5642,7 +5640,9 @@
       <c r="H52" s="17" t="s">
         <v>380</v>
       </c>
-      <c r="I52" s="24"/>
+      <c r="I52" s="4" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="str">
@@ -5670,7 +5670,9 @@
       <c r="H53" s="17" t="s">
         <v>380</v>
       </c>
-      <c r="I53" s="24"/>
+      <c r="I53" s="4" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="54" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="str">
@@ -6432,7 +6434,7 @@
       <c r="H79" s="17" t="s">
         <v>554</v>
       </c>
-      <c r="I79" s="39" t="s">
+      <c r="I79" s="38" t="s">
         <v>591</v>
       </c>
     </row>
@@ -6852,33 +6854,33 @@
         <v>600</v>
       </c>
     </row>
-    <row r="94" spans="1:9" s="37" customFormat="1" ht="98.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="32" t="str">
+    <row r="94" spans="1:9" s="36" customFormat="1" ht="98.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="31" t="str">
         <f>_xlfn.CONCAT(Tableau2[[#This Row],[Organisme]],"-",Tableau2[[#This Row],[Colonne1]])</f>
         <v>DDT38-23</v>
       </c>
-      <c r="B94" s="33">
+      <c r="B94" s="32">
         <v>23</v>
       </c>
-      <c r="C94" s="34" t="s">
+      <c r="C94" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="D94" s="35" t="s">
+      <c r="D94" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="E94" s="35" t="s">
+      <c r="E94" s="34" t="s">
         <v>219</v>
       </c>
-      <c r="F94" s="34" t="s">
+      <c r="F94" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="G94" s="34" t="s">
+      <c r="G94" s="33" t="s">
         <v>278</v>
       </c>
-      <c r="H94" s="36" t="s">
+      <c r="H94" s="35" t="s">
         <v>472</v>
       </c>
-      <c r="I94" s="40" t="s">
+      <c r="I94" s="39" t="s">
         <v>557</v>
       </c>
     </row>
@@ -6968,7 +6970,9 @@
       <c r="H97" s="17" t="s">
         <v>474</v>
       </c>
-      <c r="I97" s="23"/>
+      <c r="I97" s="23" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="str">
@@ -6996,7 +7000,9 @@
       <c r="H98" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="I98" s="24"/>
+      <c r="I98" s="23" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="str">
@@ -7024,7 +7030,9 @@
       <c r="H99" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="I99" s="24"/>
+      <c r="I99" s="23" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="100" spans="1:9" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="str">
@@ -7078,7 +7086,7 @@
       <c r="H101" s="19" t="s">
         <v>570</v>
       </c>
-      <c r="I101" s="24"/>
+      <c r="I101" s="38"/>
     </row>
     <row r="102" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A102" s="20" t="str">
@@ -7226,7 +7234,7 @@
       <c r="H106" s="19" t="s">
         <v>478</v>
       </c>
-      <c r="I106" s="39"/>
+      <c r="I106" s="38"/>
     </row>
     <row r="107" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A107" s="20" t="str">
@@ -7314,7 +7322,9 @@
       <c r="H109" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="I109" s="24"/>
+      <c r="I109" s="23" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="110" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A110" s="20" t="str">
@@ -7342,7 +7352,9 @@
       <c r="H110" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="I110" s="24"/>
+      <c r="I110" s="23" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="111" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A111" s="20" t="str">
@@ -7370,7 +7382,9 @@
       <c r="H111" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="I111" s="24"/>
+      <c r="I111" s="23" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="112" spans="1:9" ht="84" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="str">
@@ -7398,7 +7412,7 @@
       <c r="H112" s="6" t="s">
         <v>476</v>
       </c>
-      <c r="I112" s="39" t="s">
+      <c r="I112" s="38" t="s">
         <v>571</v>
       </c>
     </row>
@@ -7428,7 +7442,9 @@
       <c r="H113" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="I113" s="24"/>
+      <c r="I113" s="23" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="114" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A114" s="20" t="str">
@@ -7456,7 +7472,9 @@
       <c r="H114" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="I114" s="24"/>
+      <c r="I114" s="23" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="115" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A115" s="20" t="str">
@@ -7484,7 +7502,9 @@
       <c r="H115" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="I115" s="24"/>
+      <c r="I115" s="23" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="116" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A116" s="20" t="str">
@@ -7512,7 +7532,9 @@
       <c r="H116" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="I116" s="24"/>
+      <c r="I116" s="23" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="117" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A117" s="20" t="str">
@@ -7540,7 +7562,9 @@
       <c r="H117" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="I117" s="24"/>
+      <c r="I117" s="23" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="118" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A118" s="20" t="str">
@@ -7568,7 +7592,7 @@
       <c r="H118" s="17" t="s">
         <v>480</v>
       </c>
-      <c r="I118" s="24"/>
+      <c r="I118" s="38"/>
     </row>
     <row r="119" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="20" t="str">
@@ -7626,7 +7650,9 @@
       <c r="H120" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="I120" s="24"/>
+      <c r="I120" s="23" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="121" spans="1:9" ht="24" x14ac:dyDescent="0.25">
       <c r="A121" s="20" t="str">
@@ -7654,7 +7680,9 @@
       <c r="H121" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="I121" s="24"/>
+      <c r="I121" s="23" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="122" spans="1:9" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="str">

</xml_diff>